<commit_message>
Update Gantt Diagram: Amine
</commit_message>
<xml_diff>
--- a/Gantt_Diagram_Robot_Project_2018.xlsx
+++ b/Gantt_Diagram_Robot_Project_2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evaux\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaizi\Desktop\Robot_Project_IFX\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
     <definedName name="vertex42_id" hidden="1">"gantt-chart_L.xlsx"</definedName>
     <definedName name="vertex42_title" hidden="1">"Gantt Chart Template"</definedName>
   </definedNames>
-  <calcPr calcId="162913" refMode="R1C1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -442,7 +442,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="158">
   <si>
     <t>WBS</t>
   </si>
@@ -1553,6 +1553,27 @@
   </si>
   <si>
     <t>M. ZROUMBA</t>
+  </si>
+  <si>
+    <t>Movements</t>
+  </si>
+  <si>
+    <t>M. Amine Gaizi</t>
+  </si>
+  <si>
+    <t>M. Jeannin</t>
+  </si>
+  <si>
+    <t>Motor control</t>
+  </si>
+  <si>
+    <t>Soldered circuit</t>
+  </si>
+  <si>
+    <t>Proportional correction</t>
+  </si>
+  <si>
+    <t>M.Amine Gaizi</t>
   </si>
 </sst>
 </file>
@@ -2906,6 +2927,24 @@
     </xf>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2913,27 +2952,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3110,7 +3131,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="3"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3118,13 +3139,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>185208</xdr:rowOff>
     </xdr:to>
@@ -3770,13 +3791,13 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" style="6" customWidth="1"/>
     <col min="5" max="6" width="12" style="1" customWidth="1"/>
@@ -3798,29 +3819,29 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
       <c r="I1" s="132"/>
-      <c r="K1" s="163" t="s">
+      <c r="K1" s="169" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
-      <c r="P1" s="163"/>
-      <c r="Q1" s="163"/>
-      <c r="R1" s="163"/>
-      <c r="S1" s="163"/>
-      <c r="T1" s="163"/>
-      <c r="U1" s="163"/>
-      <c r="V1" s="163"/>
-      <c r="W1" s="163"/>
-      <c r="X1" s="163"/>
-      <c r="Y1" s="163"/>
-      <c r="Z1" s="163"/>
-      <c r="AA1" s="163"/>
-      <c r="AB1" s="163"/>
-      <c r="AC1" s="163"/>
-      <c r="AD1" s="163"/>
-      <c r="AE1" s="163"/>
+      <c r="L1" s="169"/>
+      <c r="M1" s="169"/>
+      <c r="N1" s="169"/>
+      <c r="O1" s="169"/>
+      <c r="P1" s="169"/>
+      <c r="Q1" s="169"/>
+      <c r="R1" s="169"/>
+      <c r="S1" s="169"/>
+      <c r="T1" s="169"/>
+      <c r="U1" s="169"/>
+      <c r="V1" s="169"/>
+      <c r="W1" s="169"/>
+      <c r="X1" s="169"/>
+      <c r="Y1" s="169"/>
+      <c r="Z1" s="169"/>
+      <c r="AA1" s="169"/>
+      <c r="AB1" s="169"/>
+      <c r="AC1" s="169"/>
+      <c r="AD1" s="169"/>
+      <c r="AE1" s="169"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
@@ -3865,196 +3886,196 @@
       <c r="B4" s="114" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="168">
+      <c r="C4" s="171">
         <v>43340</v>
       </c>
-      <c r="D4" s="168"/>
-      <c r="E4" s="168"/>
+      <c r="D4" s="171"/>
+      <c r="E4" s="171"/>
       <c r="F4" s="111"/>
       <c r="G4" s="114" t="s">
         <v>75</v>
       </c>
       <c r="H4" s="129">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I4" s="112"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="165" t="str">
+      <c r="K4" s="163" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 1</v>
+      </c>
+      <c r="L4" s="164"/>
+      <c r="M4" s="164"/>
+      <c r="N4" s="164"/>
+      <c r="O4" s="164"/>
+      <c r="P4" s="164"/>
+      <c r="Q4" s="165"/>
+      <c r="R4" s="163" t="str">
+        <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 2</v>
+      </c>
+      <c r="S4" s="164"/>
+      <c r="T4" s="164"/>
+      <c r="U4" s="164"/>
+      <c r="V4" s="164"/>
+      <c r="W4" s="164"/>
+      <c r="X4" s="165"/>
+      <c r="Y4" s="163" t="str">
+        <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="L4" s="166"/>
-      <c r="M4" s="166"/>
-      <c r="N4" s="166"/>
-      <c r="O4" s="166"/>
-      <c r="P4" s="166"/>
-      <c r="Q4" s="167"/>
-      <c r="R4" s="165" t="str">
-        <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="Z4" s="164"/>
+      <c r="AA4" s="164"/>
+      <c r="AB4" s="164"/>
+      <c r="AC4" s="164"/>
+      <c r="AD4" s="164"/>
+      <c r="AE4" s="165"/>
+      <c r="AF4" s="163" t="str">
+        <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="S4" s="166"/>
-      <c r="T4" s="166"/>
-      <c r="U4" s="166"/>
-      <c r="V4" s="166"/>
-      <c r="W4" s="166"/>
-      <c r="X4" s="167"/>
-      <c r="Y4" s="165" t="str">
-        <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AG4" s="164"/>
+      <c r="AH4" s="164"/>
+      <c r="AI4" s="164"/>
+      <c r="AJ4" s="164"/>
+      <c r="AK4" s="164"/>
+      <c r="AL4" s="165"/>
+      <c r="AM4" s="163" t="str">
+        <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="Z4" s="166"/>
-      <c r="AA4" s="166"/>
-      <c r="AB4" s="166"/>
-      <c r="AC4" s="166"/>
-      <c r="AD4" s="166"/>
-      <c r="AE4" s="167"/>
-      <c r="AF4" s="165" t="str">
-        <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AN4" s="164"/>
+      <c r="AO4" s="164"/>
+      <c r="AP4" s="164"/>
+      <c r="AQ4" s="164"/>
+      <c r="AR4" s="164"/>
+      <c r="AS4" s="165"/>
+      <c r="AT4" s="163" t="str">
+        <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AG4" s="166"/>
-      <c r="AH4" s="166"/>
-      <c r="AI4" s="166"/>
-      <c r="AJ4" s="166"/>
-      <c r="AK4" s="166"/>
-      <c r="AL4" s="167"/>
-      <c r="AM4" s="165" t="str">
-        <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AU4" s="164"/>
+      <c r="AV4" s="164"/>
+      <c r="AW4" s="164"/>
+      <c r="AX4" s="164"/>
+      <c r="AY4" s="164"/>
+      <c r="AZ4" s="165"/>
+      <c r="BA4" s="163" t="str">
+        <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="AN4" s="166"/>
-      <c r="AO4" s="166"/>
-      <c r="AP4" s="166"/>
-      <c r="AQ4" s="166"/>
-      <c r="AR4" s="166"/>
-      <c r="AS4" s="167"/>
-      <c r="AT4" s="165" t="str">
-        <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="BB4" s="164"/>
+      <c r="BC4" s="164"/>
+      <c r="BD4" s="164"/>
+      <c r="BE4" s="164"/>
+      <c r="BF4" s="164"/>
+      <c r="BG4" s="165"/>
+      <c r="BH4" s="163" t="str">
+        <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="AU4" s="166"/>
-      <c r="AV4" s="166"/>
-      <c r="AW4" s="166"/>
-      <c r="AX4" s="166"/>
-      <c r="AY4" s="166"/>
-      <c r="AZ4" s="167"/>
-      <c r="BA4" s="165" t="str">
-        <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 9</v>
-      </c>
-      <c r="BB4" s="166"/>
-      <c r="BC4" s="166"/>
-      <c r="BD4" s="166"/>
-      <c r="BE4" s="166"/>
-      <c r="BF4" s="166"/>
-      <c r="BG4" s="167"/>
-      <c r="BH4" s="165" t="str">
-        <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 10</v>
-      </c>
-      <c r="BI4" s="166"/>
-      <c r="BJ4" s="166"/>
-      <c r="BK4" s="166"/>
-      <c r="BL4" s="166"/>
-      <c r="BM4" s="166"/>
-      <c r="BN4" s="167"/>
+      <c r="BI4" s="164"/>
+      <c r="BJ4" s="164"/>
+      <c r="BK4" s="164"/>
+      <c r="BL4" s="164"/>
+      <c r="BM4" s="164"/>
+      <c r="BN4" s="165"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="110"/>
       <c r="B5" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="164" t="s">
+      <c r="C5" s="170" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="164"/>
-      <c r="E5" s="164"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
       <c r="F5" s="113"/>
       <c r="G5" s="113"/>
       <c r="H5" s="113"/>
       <c r="I5" s="113"/>
       <c r="J5" s="50"/>
-      <c r="K5" s="169">
+      <c r="K5" s="166">
         <f>K6</f>
+        <v>43339</v>
+      </c>
+      <c r="L5" s="167"/>
+      <c r="M5" s="167"/>
+      <c r="N5" s="167"/>
+      <c r="O5" s="167"/>
+      <c r="P5" s="167"/>
+      <c r="Q5" s="168"/>
+      <c r="R5" s="166">
+        <f>R6</f>
+        <v>43346</v>
+      </c>
+      <c r="S5" s="167"/>
+      <c r="T5" s="167"/>
+      <c r="U5" s="167"/>
+      <c r="V5" s="167"/>
+      <c r="W5" s="167"/>
+      <c r="X5" s="168"/>
+      <c r="Y5" s="166">
+        <f>Y6</f>
         <v>43353</v>
       </c>
-      <c r="L5" s="170"/>
-      <c r="M5" s="170"/>
-      <c r="N5" s="170"/>
-      <c r="O5" s="170"/>
-      <c r="P5" s="170"/>
-      <c r="Q5" s="171"/>
-      <c r="R5" s="169">
-        <f>R6</f>
+      <c r="Z5" s="167"/>
+      <c r="AA5" s="167"/>
+      <c r="AB5" s="167"/>
+      <c r="AC5" s="167"/>
+      <c r="AD5" s="167"/>
+      <c r="AE5" s="168"/>
+      <c r="AF5" s="166">
+        <f>AF6</f>
         <v>43360</v>
       </c>
-      <c r="S5" s="170"/>
-      <c r="T5" s="170"/>
-      <c r="U5" s="170"/>
-      <c r="V5" s="170"/>
-      <c r="W5" s="170"/>
-      <c r="X5" s="171"/>
-      <c r="Y5" s="169">
-        <f>Y6</f>
+      <c r="AG5" s="167"/>
+      <c r="AH5" s="167"/>
+      <c r="AI5" s="167"/>
+      <c r="AJ5" s="167"/>
+      <c r="AK5" s="167"/>
+      <c r="AL5" s="168"/>
+      <c r="AM5" s="166">
+        <f>AM6</f>
         <v>43367</v>
       </c>
-      <c r="Z5" s="170"/>
-      <c r="AA5" s="170"/>
-      <c r="AB5" s="170"/>
-      <c r="AC5" s="170"/>
-      <c r="AD5" s="170"/>
-      <c r="AE5" s="171"/>
-      <c r="AF5" s="169">
-        <f>AF6</f>
+      <c r="AN5" s="167"/>
+      <c r="AO5" s="167"/>
+      <c r="AP5" s="167"/>
+      <c r="AQ5" s="167"/>
+      <c r="AR5" s="167"/>
+      <c r="AS5" s="168"/>
+      <c r="AT5" s="166">
+        <f>AT6</f>
         <v>43374</v>
       </c>
-      <c r="AG5" s="170"/>
-      <c r="AH5" s="170"/>
-      <c r="AI5" s="170"/>
-      <c r="AJ5" s="170"/>
-      <c r="AK5" s="170"/>
-      <c r="AL5" s="171"/>
-      <c r="AM5" s="169">
-        <f>AM6</f>
+      <c r="AU5" s="167"/>
+      <c r="AV5" s="167"/>
+      <c r="AW5" s="167"/>
+      <c r="AX5" s="167"/>
+      <c r="AY5" s="167"/>
+      <c r="AZ5" s="168"/>
+      <c r="BA5" s="166">
+        <f>BA6</f>
         <v>43381</v>
       </c>
-      <c r="AN5" s="170"/>
-      <c r="AO5" s="170"/>
-      <c r="AP5" s="170"/>
-      <c r="AQ5" s="170"/>
-      <c r="AR5" s="170"/>
-      <c r="AS5" s="171"/>
-      <c r="AT5" s="169">
-        <f>AT6</f>
+      <c r="BB5" s="167"/>
+      <c r="BC5" s="167"/>
+      <c r="BD5" s="167"/>
+      <c r="BE5" s="167"/>
+      <c r="BF5" s="167"/>
+      <c r="BG5" s="168"/>
+      <c r="BH5" s="166">
+        <f>BH6</f>
         <v>43388</v>
       </c>
-      <c r="AU5" s="170"/>
-      <c r="AV5" s="170"/>
-      <c r="AW5" s="170"/>
-      <c r="AX5" s="170"/>
-      <c r="AY5" s="170"/>
-      <c r="AZ5" s="171"/>
-      <c r="BA5" s="169">
-        <f>BA6</f>
-        <v>43395</v>
-      </c>
-      <c r="BB5" s="170"/>
-      <c r="BC5" s="170"/>
-      <c r="BD5" s="170"/>
-      <c r="BE5" s="170"/>
-      <c r="BF5" s="170"/>
-      <c r="BG5" s="171"/>
-      <c r="BH5" s="169">
-        <f>BH6</f>
-        <v>43402</v>
-      </c>
-      <c r="BI5" s="170"/>
-      <c r="BJ5" s="170"/>
-      <c r="BK5" s="170"/>
-      <c r="BL5" s="170"/>
-      <c r="BM5" s="170"/>
-      <c r="BN5" s="171"/>
+      <c r="BI5" s="167"/>
+      <c r="BJ5" s="167"/>
+      <c r="BK5" s="167"/>
+      <c r="BL5" s="167"/>
+      <c r="BM5" s="167"/>
+      <c r="BN5" s="168"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="49"/>
@@ -4069,230 +4090,230 @@
       <c r="J6" s="50"/>
       <c r="K6" s="92">
         <f>C4-WEEKDAY(C4,1)+2+7*(H4-1)</f>
-        <v>43353</v>
+        <v>43339</v>
       </c>
       <c r="L6" s="83">
         <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
-        <v>43354</v>
+        <v>43340</v>
       </c>
       <c r="M6" s="83">
         <f t="shared" si="0"/>
-        <v>43355</v>
+        <v>43341</v>
       </c>
       <c r="N6" s="83">
         <f t="shared" si="0"/>
-        <v>43356</v>
+        <v>43342</v>
       </c>
       <c r="O6" s="83">
         <f t="shared" si="0"/>
-        <v>43357</v>
+        <v>43343</v>
       </c>
       <c r="P6" s="83">
         <f t="shared" si="0"/>
-        <v>43358</v>
+        <v>43344</v>
       </c>
       <c r="Q6" s="93">
         <f t="shared" si="0"/>
-        <v>43359</v>
+        <v>43345</v>
       </c>
       <c r="R6" s="92">
         <f t="shared" si="0"/>
-        <v>43360</v>
+        <v>43346</v>
       </c>
       <c r="S6" s="83">
         <f t="shared" si="0"/>
-        <v>43361</v>
+        <v>43347</v>
       </c>
       <c r="T6" s="83">
         <f t="shared" si="0"/>
-        <v>43362</v>
+        <v>43348</v>
       </c>
       <c r="U6" s="83">
         <f t="shared" si="0"/>
-        <v>43363</v>
+        <v>43349</v>
       </c>
       <c r="V6" s="83">
         <f t="shared" si="0"/>
-        <v>43364</v>
+        <v>43350</v>
       </c>
       <c r="W6" s="83">
         <f t="shared" si="0"/>
-        <v>43365</v>
+        <v>43351</v>
       </c>
       <c r="X6" s="93">
         <f t="shared" si="0"/>
-        <v>43366</v>
+        <v>43352</v>
       </c>
       <c r="Y6" s="92">
         <f t="shared" si="0"/>
-        <v>43367</v>
+        <v>43353</v>
       </c>
       <c r="Z6" s="83">
         <f t="shared" si="0"/>
-        <v>43368</v>
+        <v>43354</v>
       </c>
       <c r="AA6" s="83">
         <f t="shared" si="0"/>
-        <v>43369</v>
+        <v>43355</v>
       </c>
       <c r="AB6" s="83">
         <f t="shared" si="0"/>
-        <v>43370</v>
+        <v>43356</v>
       </c>
       <c r="AC6" s="83">
         <f t="shared" si="0"/>
-        <v>43371</v>
+        <v>43357</v>
       </c>
       <c r="AD6" s="83">
         <f t="shared" si="0"/>
-        <v>43372</v>
+        <v>43358</v>
       </c>
       <c r="AE6" s="93">
         <f t="shared" si="0"/>
-        <v>43373</v>
+        <v>43359</v>
       </c>
       <c r="AF6" s="92">
         <f t="shared" si="0"/>
-        <v>43374</v>
+        <v>43360</v>
       </c>
       <c r="AG6" s="83">
         <f t="shared" si="0"/>
-        <v>43375</v>
+        <v>43361</v>
       </c>
       <c r="AH6" s="83">
         <f t="shared" si="0"/>
-        <v>43376</v>
+        <v>43362</v>
       </c>
       <c r="AI6" s="83">
         <f t="shared" si="0"/>
-        <v>43377</v>
+        <v>43363</v>
       </c>
       <c r="AJ6" s="83">
         <f t="shared" si="0"/>
-        <v>43378</v>
+        <v>43364</v>
       </c>
       <c r="AK6" s="83">
         <f t="shared" si="0"/>
-        <v>43379</v>
+        <v>43365</v>
       </c>
       <c r="AL6" s="93">
         <f t="shared" si="0"/>
-        <v>43380</v>
+        <v>43366</v>
       </c>
       <c r="AM6" s="92">
         <f t="shared" si="0"/>
-        <v>43381</v>
+        <v>43367</v>
       </c>
       <c r="AN6" s="83">
         <f t="shared" si="0"/>
-        <v>43382</v>
+        <v>43368</v>
       </c>
       <c r="AO6" s="83">
         <f t="shared" si="0"/>
-        <v>43383</v>
+        <v>43369</v>
       </c>
       <c r="AP6" s="83">
         <f t="shared" si="0"/>
-        <v>43384</v>
+        <v>43370</v>
       </c>
       <c r="AQ6" s="83">
         <f t="shared" si="0"/>
-        <v>43385</v>
+        <v>43371</v>
       </c>
       <c r="AR6" s="83">
         <f t="shared" ref="AR6:BN6" si="1">AQ6+1</f>
-        <v>43386</v>
+        <v>43372</v>
       </c>
       <c r="AS6" s="93">
         <f t="shared" si="1"/>
-        <v>43387</v>
+        <v>43373</v>
       </c>
       <c r="AT6" s="92">
         <f t="shared" si="1"/>
-        <v>43388</v>
+        <v>43374</v>
       </c>
       <c r="AU6" s="83">
         <f t="shared" si="1"/>
-        <v>43389</v>
+        <v>43375</v>
       </c>
       <c r="AV6" s="83">
         <f t="shared" si="1"/>
-        <v>43390</v>
+        <v>43376</v>
       </c>
       <c r="AW6" s="83">
         <f t="shared" si="1"/>
-        <v>43391</v>
+        <v>43377</v>
       </c>
       <c r="AX6" s="83">
         <f t="shared" si="1"/>
-        <v>43392</v>
+        <v>43378</v>
       </c>
       <c r="AY6" s="83">
         <f t="shared" si="1"/>
-        <v>43393</v>
+        <v>43379</v>
       </c>
       <c r="AZ6" s="93">
         <f t="shared" si="1"/>
-        <v>43394</v>
+        <v>43380</v>
       </c>
       <c r="BA6" s="92">
         <f t="shared" si="1"/>
-        <v>43395</v>
+        <v>43381</v>
       </c>
       <c r="BB6" s="83">
         <f t="shared" si="1"/>
-        <v>43396</v>
+        <v>43382</v>
       </c>
       <c r="BC6" s="83">
         <f t="shared" si="1"/>
-        <v>43397</v>
+        <v>43383</v>
       </c>
       <c r="BD6" s="83">
         <f t="shared" si="1"/>
-        <v>43398</v>
+        <v>43384</v>
       </c>
       <c r="BE6" s="83">
         <f t="shared" si="1"/>
-        <v>43399</v>
+        <v>43385</v>
       </c>
       <c r="BF6" s="83">
         <f t="shared" si="1"/>
-        <v>43400</v>
+        <v>43386</v>
       </c>
       <c r="BG6" s="93">
         <f t="shared" si="1"/>
-        <v>43401</v>
+        <v>43387</v>
       </c>
       <c r="BH6" s="92">
         <f t="shared" si="1"/>
-        <v>43402</v>
+        <v>43388</v>
       </c>
       <c r="BI6" s="83">
         <f t="shared" si="1"/>
-        <v>43403</v>
+        <v>43389</v>
       </c>
       <c r="BJ6" s="83">
         <f t="shared" si="1"/>
-        <v>43404</v>
+        <v>43390</v>
       </c>
       <c r="BK6" s="83">
         <f t="shared" si="1"/>
-        <v>43405</v>
+        <v>43391</v>
       </c>
       <c r="BL6" s="83">
         <f t="shared" si="1"/>
-        <v>43406</v>
+        <v>43392</v>
       </c>
       <c r="BM6" s="83">
         <f t="shared" si="1"/>
-        <v>43407</v>
+        <v>43393</v>
       </c>
       <c r="BN6" s="93">
         <f t="shared" si="1"/>
-        <v>43408</v>
-      </c>
-    </row>
-    <row r="7" spans="1:66" s="124" customFormat="1" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>43394</v>
+      </c>
+    </row>
+    <row r="7" spans="1:66" s="124" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="116" t="s">
         <v>0</v>
       </c>
@@ -5236,7 +5257,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="54" t="s">
-        <v>8</v>
+        <v>151</v>
       </c>
       <c r="D16" s="56"/>
       <c r="E16" s="102"/>
@@ -5314,25 +5335,29 @@
         <v>2.1</v>
       </c>
       <c r="B17" s="126" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="127"/>
+        <v>154</v>
+      </c>
+      <c r="C17" s="61" t="s">
+        <v>152</v>
+      </c>
+      <c r="D17" s="127" t="s">
+        <v>153</v>
+      </c>
       <c r="E17" s="100">
-        <v>43141</v>
+        <v>43329</v>
       </c>
       <c r="F17" s="101">
-        <f t="shared" si="6"/>
-        <v>43144</v>
+        <f>IF(ISBLANK(E17)," - ",IF(G17=0,E17,E17+G17-1))</f>
+        <v>43353</v>
       </c>
       <c r="G17" s="62">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="H17" s="63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="64">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="J17" s="95"/>
       <c r="K17" s="107"/>
@@ -5398,25 +5423,28 @@
         <v>2.2</v>
       </c>
       <c r="B18" s="126" t="s">
-        <v>9</v>
+        <v>155</v>
+      </c>
+      <c r="C18" s="61" t="s">
+        <v>152</v>
       </c>
       <c r="D18" s="127"/>
       <c r="E18" s="100">
-        <v>43145</v>
+        <v>43354</v>
       </c>
       <c r="F18" s="101">
         <f t="shared" si="6"/>
-        <v>43147</v>
+        <v>43367</v>
       </c>
       <c r="G18" s="62">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="H18" s="63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="64">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J18" s="95"/>
       <c r="K18" s="107"/>
@@ -5482,25 +5510,28 @@
         <v>2.3</v>
       </c>
       <c r="B19" s="126" t="s">
-        <v>9</v>
+        <v>156</v>
+      </c>
+      <c r="C19" s="61" t="s">
+        <v>157</v>
       </c>
       <c r="D19" s="127"/>
       <c r="E19" s="100">
-        <v>43145</v>
+        <v>43374</v>
       </c>
       <c r="F19" s="101">
         <f t="shared" si="6"/>
-        <v>43147</v>
+        <v>43392</v>
       </c>
       <c r="G19" s="62">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="H19" s="63">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="I19" s="64">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="J19" s="95"/>
       <c r="K19" s="107"/>
@@ -5566,25 +5597,28 @@
         <v>2.4</v>
       </c>
       <c r="B20" s="126" t="s">
-        <v>9</v>
+        <v>149</v>
+      </c>
+      <c r="C20" s="61" t="s">
+        <v>152</v>
       </c>
       <c r="D20" s="127"/>
       <c r="E20" s="100">
-        <v>43148</v>
+        <v>43364</v>
       </c>
       <c r="F20" s="101">
         <f t="shared" si="6"/>
-        <v>43153</v>
+        <v>43367</v>
       </c>
       <c r="G20" s="62">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H20" s="63">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="I20" s="64">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J20" s="95"/>
       <c r="K20" s="107"/>
@@ -7393,6 +7427,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -7403,15 +7446,6 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8:H41">
@@ -7456,7 +7490,7 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 A34:B35 B29 B30:B32 B23:B26 B17:B20 A37:B37 B36 E16 E22 E28 E34:H37 G14 G11 G16:H16 G22:H22 G28:H32 H20 G38 G39:G40 G41 H18 H19 H23:H26" unlockedFormula="1"/>
+    <ignoredError sqref="H9 A34:B35 B29 B30:B32 B23:B26 A37:B37 B36 E16 E22 E28 E34:H37 G14 G11 G16:H16 G22:H22 G28:H32 G38 G39:G40 G41 H23:H26" unlockedFormula="1"/>
     <ignoredError sqref="A28 A22 A16" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>

</xml_diff>

<commit_message>
Add Gant Gyroscope stuff
</commit_message>
<xml_diff>
--- a/Gantt_Diagram_Robot_Project_2018.xlsx
+++ b/Gantt_Diagram_Robot_Project_2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaizi\Desktop\Robot_Project_IFX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolle\Documents\Robot_Project_IFX\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -442,7 +442,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="164">
   <si>
     <t>WBS</t>
   </si>
@@ -1574,6 +1574,24 @@
   </si>
   <si>
     <t>M.Amine Gaizi</t>
+  </si>
+  <si>
+    <t>Gyroscope/Accelerometer</t>
+  </si>
+  <si>
+    <t>I2C protocol</t>
+  </si>
+  <si>
+    <t>Data Treatment</t>
+  </si>
+  <si>
+    <t>Integration to Amine's program</t>
+  </si>
+  <si>
+    <t>Noise treatment</t>
+  </si>
+  <si>
+    <t>M,Guillaume Nicolle</t>
   </si>
 </sst>
 </file>
@@ -2927,24 +2945,6 @@
     </xf>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2952,9 +2952,27 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3006,7 +3024,95 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="12">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -3787,11 +3893,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN42"/>
+  <dimension ref="A1:CP42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <pane ySplit="7" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BO23" sqref="BO23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3806,10 +3912,34 @@
     <col min="9" max="9" width="6.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="1.85546875" style="1" customWidth="1"/>
     <col min="11" max="66" width="2.42578125" style="1" customWidth="1"/>
-    <col min="67" max="16384" width="9.140625" style="3"/>
+    <col min="67" max="67" width="2.7109375" style="3" customWidth="1"/>
+    <col min="68" max="68" width="2.5703125" style="3" customWidth="1"/>
+    <col min="69" max="70" width="3" style="3" customWidth="1"/>
+    <col min="71" max="71" width="3.28515625" style="3" customWidth="1"/>
+    <col min="72" max="72" width="2.7109375" style="3" customWidth="1"/>
+    <col min="73" max="73" width="2.5703125" style="3" customWidth="1"/>
+    <col min="74" max="74" width="2.7109375" style="3" customWidth="1"/>
+    <col min="75" max="76" width="2.85546875" style="3" customWidth="1"/>
+    <col min="77" max="77" width="3" style="3" customWidth="1"/>
+    <col min="78" max="78" width="2.5703125" style="3" customWidth="1"/>
+    <col min="79" max="79" width="2.42578125" style="3" customWidth="1"/>
+    <col min="80" max="80" width="2.7109375" style="3" customWidth="1"/>
+    <col min="81" max="81" width="2.42578125" style="3" customWidth="1"/>
+    <col min="82" max="82" width="3" style="3" customWidth="1"/>
+    <col min="83" max="83" width="2.42578125" style="3" customWidth="1"/>
+    <col min="84" max="84" width="2.7109375" style="3" customWidth="1"/>
+    <col min="85" max="85" width="2.85546875" style="3" customWidth="1"/>
+    <col min="86" max="86" width="2.42578125" style="3" customWidth="1"/>
+    <col min="87" max="88" width="2.5703125" style="3" customWidth="1"/>
+    <col min="89" max="89" width="3" style="3" customWidth="1"/>
+    <col min="90" max="90" width="2.5703125" style="3" customWidth="1"/>
+    <col min="91" max="92" width="3.140625" style="3" customWidth="1"/>
+    <col min="93" max="93" width="2.7109375" style="3" customWidth="1"/>
+    <col min="94" max="94" width="2.85546875" style="3" customWidth="1"/>
+    <col min="95" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:94" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="125" t="s">
         <v>138</v>
       </c>
@@ -3819,31 +3949,31 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
       <c r="I1" s="132"/>
-      <c r="K1" s="169" t="s">
+      <c r="K1" s="163" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="169"/>
-      <c r="M1" s="169"/>
-      <c r="N1" s="169"/>
-      <c r="O1" s="169"/>
-      <c r="P1" s="169"/>
-      <c r="Q1" s="169"/>
-      <c r="R1" s="169"/>
-      <c r="S1" s="169"/>
-      <c r="T1" s="169"/>
-      <c r="U1" s="169"/>
-      <c r="V1" s="169"/>
-      <c r="W1" s="169"/>
-      <c r="X1" s="169"/>
-      <c r="Y1" s="169"/>
-      <c r="Z1" s="169"/>
-      <c r="AA1" s="169"/>
-      <c r="AB1" s="169"/>
-      <c r="AC1" s="169"/>
-      <c r="AD1" s="169"/>
-      <c r="AE1" s="169"/>
-    </row>
-    <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L1" s="163"/>
+      <c r="M1" s="163"/>
+      <c r="N1" s="163"/>
+      <c r="O1" s="163"/>
+      <c r="P1" s="163"/>
+      <c r="Q1" s="163"/>
+      <c r="R1" s="163"/>
+      <c r="S1" s="163"/>
+      <c r="T1" s="163"/>
+      <c r="U1" s="163"/>
+      <c r="V1" s="163"/>
+      <c r="W1" s="163"/>
+      <c r="X1" s="163"/>
+      <c r="Y1" s="163"/>
+      <c r="Z1" s="163"/>
+      <c r="AA1" s="163"/>
+      <c r="AB1" s="163"/>
+      <c r="AC1" s="163"/>
+      <c r="AD1" s="163"/>
+      <c r="AE1" s="163"/>
+    </row>
+    <row r="2" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
         <v>139</v>
       </c>
@@ -3854,7 +3984,7 @@
       <c r="F2" s="160"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:66" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:94" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="52"/>
       <c r="B3" s="48"/>
       <c r="C3" s="4"/>
@@ -3881,16 +4011,16 @@
       <c r="Z3" s="29"/>
       <c r="AA3" s="29"/>
     </row>
-    <row r="4" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:94" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="110"/>
       <c r="B4" s="114" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="171">
+      <c r="C4" s="168">
         <v>43340</v>
       </c>
-      <c r="D4" s="171"/>
-      <c r="E4" s="171"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="168"/>
       <c r="F4" s="111"/>
       <c r="G4" s="114" t="s">
         <v>75</v>
@@ -3900,184 +4030,264 @@
       </c>
       <c r="I4" s="112"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="163" t="str">
+      <c r="K4" s="165" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="164"/>
-      <c r="M4" s="164"/>
-      <c r="N4" s="164"/>
-      <c r="O4" s="164"/>
-      <c r="P4" s="164"/>
-      <c r="Q4" s="165"/>
-      <c r="R4" s="163" t="str">
+      <c r="L4" s="166"/>
+      <c r="M4" s="166"/>
+      <c r="N4" s="166"/>
+      <c r="O4" s="166"/>
+      <c r="P4" s="166"/>
+      <c r="Q4" s="167"/>
+      <c r="R4" s="165" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="164"/>
-      <c r="T4" s="164"/>
-      <c r="U4" s="164"/>
-      <c r="V4" s="164"/>
-      <c r="W4" s="164"/>
-      <c r="X4" s="165"/>
-      <c r="Y4" s="163" t="str">
+      <c r="S4" s="166"/>
+      <c r="T4" s="166"/>
+      <c r="U4" s="166"/>
+      <c r="V4" s="166"/>
+      <c r="W4" s="166"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="165" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="164"/>
-      <c r="AA4" s="164"/>
-      <c r="AB4" s="164"/>
-      <c r="AC4" s="164"/>
-      <c r="AD4" s="164"/>
-      <c r="AE4" s="165"/>
-      <c r="AF4" s="163" t="str">
+      <c r="Z4" s="166"/>
+      <c r="AA4" s="166"/>
+      <c r="AB4" s="166"/>
+      <c r="AC4" s="166"/>
+      <c r="AD4" s="166"/>
+      <c r="AE4" s="167"/>
+      <c r="AF4" s="165" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="164"/>
-      <c r="AH4" s="164"/>
-      <c r="AI4" s="164"/>
-      <c r="AJ4" s="164"/>
-      <c r="AK4" s="164"/>
-      <c r="AL4" s="165"/>
-      <c r="AM4" s="163" t="str">
+      <c r="AG4" s="166"/>
+      <c r="AH4" s="166"/>
+      <c r="AI4" s="166"/>
+      <c r="AJ4" s="166"/>
+      <c r="AK4" s="166"/>
+      <c r="AL4" s="167"/>
+      <c r="AM4" s="165" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="164"/>
-      <c r="AO4" s="164"/>
-      <c r="AP4" s="164"/>
-      <c r="AQ4" s="164"/>
-      <c r="AR4" s="164"/>
-      <c r="AS4" s="165"/>
-      <c r="AT4" s="163" t="str">
+      <c r="AN4" s="166"/>
+      <c r="AO4" s="166"/>
+      <c r="AP4" s="166"/>
+      <c r="AQ4" s="166"/>
+      <c r="AR4" s="166"/>
+      <c r="AS4" s="167"/>
+      <c r="AT4" s="165" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="164"/>
-      <c r="AV4" s="164"/>
-      <c r="AW4" s="164"/>
-      <c r="AX4" s="164"/>
-      <c r="AY4" s="164"/>
-      <c r="AZ4" s="165"/>
-      <c r="BA4" s="163" t="str">
+      <c r="AU4" s="166"/>
+      <c r="AV4" s="166"/>
+      <c r="AW4" s="166"/>
+      <c r="AX4" s="166"/>
+      <c r="AY4" s="166"/>
+      <c r="AZ4" s="167"/>
+      <c r="BA4" s="165" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="164"/>
-      <c r="BC4" s="164"/>
-      <c r="BD4" s="164"/>
-      <c r="BE4" s="164"/>
-      <c r="BF4" s="164"/>
-      <c r="BG4" s="165"/>
-      <c r="BH4" s="163" t="str">
+      <c r="BB4" s="166"/>
+      <c r="BC4" s="166"/>
+      <c r="BD4" s="166"/>
+      <c r="BE4" s="166"/>
+      <c r="BF4" s="166"/>
+      <c r="BG4" s="167"/>
+      <c r="BH4" s="165" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="164"/>
-      <c r="BJ4" s="164"/>
-      <c r="BK4" s="164"/>
-      <c r="BL4" s="164"/>
-      <c r="BM4" s="164"/>
-      <c r="BN4" s="165"/>
-    </row>
-    <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BI4" s="166"/>
+      <c r="BJ4" s="166"/>
+      <c r="BK4" s="166"/>
+      <c r="BL4" s="166"/>
+      <c r="BM4" s="166"/>
+      <c r="BN4" s="167"/>
+      <c r="BO4" s="165" t="str">
+        <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 9</v>
+      </c>
+      <c r="BP4" s="166"/>
+      <c r="BQ4" s="166"/>
+      <c r="BR4" s="166"/>
+      <c r="BS4" s="166"/>
+      <c r="BT4" s="166"/>
+      <c r="BU4" s="167"/>
+      <c r="BV4" s="165" t="str">
+        <f>"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 10</v>
+      </c>
+      <c r="BW4" s="166"/>
+      <c r="BX4" s="166"/>
+      <c r="BY4" s="166"/>
+      <c r="BZ4" s="166"/>
+      <c r="CA4" s="166"/>
+      <c r="CB4" s="167"/>
+      <c r="CC4" s="165" t="str">
+        <f>"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 11</v>
+      </c>
+      <c r="CD4" s="166"/>
+      <c r="CE4" s="166"/>
+      <c r="CF4" s="166"/>
+      <c r="CG4" s="166"/>
+      <c r="CH4" s="166"/>
+      <c r="CI4" s="167"/>
+      <c r="CJ4" s="165" t="str">
+        <f>"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 12</v>
+      </c>
+      <c r="CK4" s="166"/>
+      <c r="CL4" s="166"/>
+      <c r="CM4" s="166"/>
+      <c r="CN4" s="166"/>
+      <c r="CO4" s="166"/>
+      <c r="CP4" s="167"/>
+    </row>
+    <row r="5" spans="1:94" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="110"/>
       <c r="B5" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="170" t="s">
+      <c r="C5" s="164" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
+      <c r="D5" s="164"/>
+      <c r="E5" s="164"/>
       <c r="F5" s="113"/>
       <c r="G5" s="113"/>
       <c r="H5" s="113"/>
       <c r="I5" s="113"/>
       <c r="J5" s="50"/>
-      <c r="K5" s="166">
+      <c r="K5" s="169">
         <f>K6</f>
         <v>43339</v>
       </c>
-      <c r="L5" s="167"/>
-      <c r="M5" s="167"/>
-      <c r="N5" s="167"/>
-      <c r="O5" s="167"/>
-      <c r="P5" s="167"/>
-      <c r="Q5" s="168"/>
-      <c r="R5" s="166">
+      <c r="L5" s="170"/>
+      <c r="M5" s="170"/>
+      <c r="N5" s="170"/>
+      <c r="O5" s="170"/>
+      <c r="P5" s="170"/>
+      <c r="Q5" s="171"/>
+      <c r="R5" s="169">
         <f>R6</f>
         <v>43346</v>
       </c>
-      <c r="S5" s="167"/>
-      <c r="T5" s="167"/>
-      <c r="U5" s="167"/>
-      <c r="V5" s="167"/>
-      <c r="W5" s="167"/>
-      <c r="X5" s="168"/>
-      <c r="Y5" s="166">
+      <c r="S5" s="170"/>
+      <c r="T5" s="170"/>
+      <c r="U5" s="170"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
+      <c r="X5" s="171"/>
+      <c r="Y5" s="169">
         <f>Y6</f>
         <v>43353</v>
       </c>
-      <c r="Z5" s="167"/>
-      <c r="AA5" s="167"/>
-      <c r="AB5" s="167"/>
-      <c r="AC5" s="167"/>
-      <c r="AD5" s="167"/>
-      <c r="AE5" s="168"/>
-      <c r="AF5" s="166">
+      <c r="Z5" s="170"/>
+      <c r="AA5" s="170"/>
+      <c r="AB5" s="170"/>
+      <c r="AC5" s="170"/>
+      <c r="AD5" s="170"/>
+      <c r="AE5" s="171"/>
+      <c r="AF5" s="169">
         <f>AF6</f>
         <v>43360</v>
       </c>
-      <c r="AG5" s="167"/>
-      <c r="AH5" s="167"/>
-      <c r="AI5" s="167"/>
-      <c r="AJ5" s="167"/>
-      <c r="AK5" s="167"/>
-      <c r="AL5" s="168"/>
-      <c r="AM5" s="166">
+      <c r="AG5" s="170"/>
+      <c r="AH5" s="170"/>
+      <c r="AI5" s="170"/>
+      <c r="AJ5" s="170"/>
+      <c r="AK5" s="170"/>
+      <c r="AL5" s="171"/>
+      <c r="AM5" s="169">
         <f>AM6</f>
         <v>43367</v>
       </c>
-      <c r="AN5" s="167"/>
-      <c r="AO5" s="167"/>
-      <c r="AP5" s="167"/>
-      <c r="AQ5" s="167"/>
-      <c r="AR5" s="167"/>
-      <c r="AS5" s="168"/>
-      <c r="AT5" s="166">
+      <c r="AN5" s="170"/>
+      <c r="AO5" s="170"/>
+      <c r="AP5" s="170"/>
+      <c r="AQ5" s="170"/>
+      <c r="AR5" s="170"/>
+      <c r="AS5" s="171"/>
+      <c r="AT5" s="169">
         <f>AT6</f>
         <v>43374</v>
       </c>
-      <c r="AU5" s="167"/>
-      <c r="AV5" s="167"/>
-      <c r="AW5" s="167"/>
-      <c r="AX5" s="167"/>
-      <c r="AY5" s="167"/>
-      <c r="AZ5" s="168"/>
-      <c r="BA5" s="166">
+      <c r="AU5" s="170"/>
+      <c r="AV5" s="170"/>
+      <c r="AW5" s="170"/>
+      <c r="AX5" s="170"/>
+      <c r="AY5" s="170"/>
+      <c r="AZ5" s="171"/>
+      <c r="BA5" s="169">
         <f>BA6</f>
         <v>43381</v>
       </c>
-      <c r="BB5" s="167"/>
-      <c r="BC5" s="167"/>
-      <c r="BD5" s="167"/>
-      <c r="BE5" s="167"/>
-      <c r="BF5" s="167"/>
-      <c r="BG5" s="168"/>
-      <c r="BH5" s="166">
+      <c r="BB5" s="170"/>
+      <c r="BC5" s="170"/>
+      <c r="BD5" s="170"/>
+      <c r="BE5" s="170"/>
+      <c r="BF5" s="170"/>
+      <c r="BG5" s="171"/>
+      <c r="BH5" s="169">
         <f>BH6</f>
         <v>43388</v>
       </c>
-      <c r="BI5" s="167"/>
-      <c r="BJ5" s="167"/>
-      <c r="BK5" s="167"/>
-      <c r="BL5" s="167"/>
-      <c r="BM5" s="167"/>
-      <c r="BN5" s="168"/>
-    </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="BI5" s="170"/>
+      <c r="BJ5" s="170"/>
+      <c r="BK5" s="170"/>
+      <c r="BL5" s="170"/>
+      <c r="BM5" s="170"/>
+      <c r="BN5" s="171"/>
+      <c r="BO5" s="169">
+        <f>BO6</f>
+        <v>43395</v>
+      </c>
+      <c r="BP5" s="170"/>
+      <c r="BQ5" s="170"/>
+      <c r="BR5" s="170"/>
+      <c r="BS5" s="170"/>
+      <c r="BT5" s="170"/>
+      <c r="BU5" s="171"/>
+      <c r="BV5" s="169">
+        <f>BV6</f>
+        <v>43402</v>
+      </c>
+      <c r="BW5" s="170"/>
+      <c r="BX5" s="170"/>
+      <c r="BY5" s="170"/>
+      <c r="BZ5" s="170"/>
+      <c r="CA5" s="170"/>
+      <c r="CB5" s="171"/>
+      <c r="CC5" s="169">
+        <f>CC6</f>
+        <v>43409</v>
+      </c>
+      <c r="CD5" s="170"/>
+      <c r="CE5" s="170"/>
+      <c r="CF5" s="170"/>
+      <c r="CG5" s="170"/>
+      <c r="CH5" s="170"/>
+      <c r="CI5" s="171"/>
+      <c r="CJ5" s="169">
+        <f>CJ6</f>
+        <v>43416</v>
+      </c>
+      <c r="CK5" s="170"/>
+      <c r="CL5" s="170"/>
+      <c r="CM5" s="170"/>
+      <c r="CN5" s="170"/>
+      <c r="CO5" s="170"/>
+      <c r="CP5" s="171"/>
+    </row>
+    <row r="6" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A6" s="49"/>
       <c r="B6" s="50"/>
       <c r="C6" s="50"/>
@@ -4312,8 +4522,120 @@
         <f t="shared" si="1"/>
         <v>43394</v>
       </c>
-    </row>
-    <row r="7" spans="1:66" s="124" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="BO6" s="92">
+        <f t="shared" ref="BO6" si="2">BN6+1</f>
+        <v>43395</v>
+      </c>
+      <c r="BP6" s="83">
+        <f t="shared" ref="BP6" si="3">BO6+1</f>
+        <v>43396</v>
+      </c>
+      <c r="BQ6" s="83">
+        <f t="shared" ref="BQ6" si="4">BP6+1</f>
+        <v>43397</v>
+      </c>
+      <c r="BR6" s="83">
+        <f t="shared" ref="BR6" si="5">BQ6+1</f>
+        <v>43398</v>
+      </c>
+      <c r="BS6" s="83">
+        <f t="shared" ref="BS6" si="6">BR6+1</f>
+        <v>43399</v>
+      </c>
+      <c r="BT6" s="83">
+        <f t="shared" ref="BT6" si="7">BS6+1</f>
+        <v>43400</v>
+      </c>
+      <c r="BU6" s="93">
+        <f t="shared" ref="BU6" si="8">BT6+1</f>
+        <v>43401</v>
+      </c>
+      <c r="BV6" s="92">
+        <f t="shared" ref="BV6" si="9">BU6+1</f>
+        <v>43402</v>
+      </c>
+      <c r="BW6" s="83">
+        <f t="shared" ref="BW6" si="10">BV6+1</f>
+        <v>43403</v>
+      </c>
+      <c r="BX6" s="83">
+        <f t="shared" ref="BX6" si="11">BW6+1</f>
+        <v>43404</v>
+      </c>
+      <c r="BY6" s="83">
+        <f t="shared" ref="BY6" si="12">BX6+1</f>
+        <v>43405</v>
+      </c>
+      <c r="BZ6" s="83">
+        <f t="shared" ref="BZ6" si="13">BY6+1</f>
+        <v>43406</v>
+      </c>
+      <c r="CA6" s="83">
+        <f t="shared" ref="CA6" si="14">BZ6+1</f>
+        <v>43407</v>
+      </c>
+      <c r="CB6" s="93">
+        <f t="shared" ref="CB6" si="15">CA6+1</f>
+        <v>43408</v>
+      </c>
+      <c r="CC6" s="92">
+        <f t="shared" ref="CC6" si="16">CB6+1</f>
+        <v>43409</v>
+      </c>
+      <c r="CD6" s="83">
+        <f t="shared" ref="CD6" si="17">CC6+1</f>
+        <v>43410</v>
+      </c>
+      <c r="CE6" s="83">
+        <f t="shared" ref="CE6" si="18">CD6+1</f>
+        <v>43411</v>
+      </c>
+      <c r="CF6" s="83">
+        <f t="shared" ref="CF6" si="19">CE6+1</f>
+        <v>43412</v>
+      </c>
+      <c r="CG6" s="83">
+        <f t="shared" ref="CG6" si="20">CF6+1</f>
+        <v>43413</v>
+      </c>
+      <c r="CH6" s="83">
+        <f t="shared" ref="CH6" si="21">CG6+1</f>
+        <v>43414</v>
+      </c>
+      <c r="CI6" s="93">
+        <f t="shared" ref="CI6" si="22">CH6+1</f>
+        <v>43415</v>
+      </c>
+      <c r="CJ6" s="92">
+        <f t="shared" ref="CJ6" si="23">CI6+1</f>
+        <v>43416</v>
+      </c>
+      <c r="CK6" s="83">
+        <f t="shared" ref="CK6" si="24">CJ6+1</f>
+        <v>43417</v>
+      </c>
+      <c r="CL6" s="83">
+        <f t="shared" ref="CL6" si="25">CK6+1</f>
+        <v>43418</v>
+      </c>
+      <c r="CM6" s="83">
+        <f t="shared" ref="CM6" si="26">CL6+1</f>
+        <v>43419</v>
+      </c>
+      <c r="CN6" s="83">
+        <f t="shared" ref="CN6" si="27">CM6+1</f>
+        <v>43420</v>
+      </c>
+      <c r="CO6" s="83">
+        <f t="shared" ref="CO6" si="28">CN6+1</f>
+        <v>43421</v>
+      </c>
+      <c r="CP6" s="93">
+        <f t="shared" ref="CP6" si="29">CO6+1</f>
+        <v>43422</v>
+      </c>
+    </row>
+    <row r="7" spans="1:94" s="124" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="116" t="s">
         <v>0</v>
       </c>
@@ -4343,231 +4665,343 @@
       </c>
       <c r="J7" s="118"/>
       <c r="K7" s="121" t="str">
-        <f t="shared" ref="K7:AP7" si="2">CHOOSE(WEEKDAY(K6,1),"S","M","T","W","T","F","S")</f>
+        <f t="shared" ref="K7:AP7" si="30">CHOOSE(WEEKDAY(K6,1),"S","M","T","W","T","F","S")</f>
         <v>M</v>
       </c>
       <c r="L7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>T</v>
       </c>
       <c r="M7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>W</v>
       </c>
       <c r="N7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>T</v>
       </c>
       <c r="O7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>F</v>
       </c>
       <c r="P7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>S</v>
       </c>
       <c r="Q7" s="123" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>S</v>
       </c>
       <c r="R7" s="121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>M</v>
       </c>
       <c r="S7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>T</v>
       </c>
       <c r="T7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>W</v>
       </c>
       <c r="U7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>T</v>
       </c>
       <c r="V7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>F</v>
       </c>
       <c r="W7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>S</v>
       </c>
       <c r="X7" s="123" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>S</v>
       </c>
       <c r="Y7" s="121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>M</v>
       </c>
       <c r="Z7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>T</v>
       </c>
       <c r="AA7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>W</v>
       </c>
       <c r="AB7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>T</v>
       </c>
       <c r="AC7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>F</v>
       </c>
       <c r="AD7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>S</v>
       </c>
       <c r="AE7" s="123" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>S</v>
       </c>
       <c r="AF7" s="121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>M</v>
       </c>
       <c r="AG7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>T</v>
       </c>
       <c r="AH7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>W</v>
       </c>
       <c r="AI7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>T</v>
       </c>
       <c r="AJ7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>F</v>
       </c>
       <c r="AK7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>S</v>
       </c>
       <c r="AL7" s="123" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>S</v>
       </c>
       <c r="AM7" s="121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>M</v>
       </c>
       <c r="AN7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>T</v>
       </c>
       <c r="AO7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>W</v>
       </c>
       <c r="AP7" s="122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="30"/>
         <v>T</v>
       </c>
       <c r="AQ7" s="122" t="str">
-        <f t="shared" ref="AQ7:BN7" si="3">CHOOSE(WEEKDAY(AQ6,1),"S","M","T","W","T","F","S")</f>
+        <f t="shared" ref="AQ7:BN7" si="31">CHOOSE(WEEKDAY(AQ6,1),"S","M","T","W","T","F","S")</f>
         <v>F</v>
       </c>
       <c r="AR7" s="122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>S</v>
       </c>
       <c r="AS7" s="123" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>S</v>
       </c>
       <c r="AT7" s="121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>M</v>
       </c>
       <c r="AU7" s="122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>T</v>
       </c>
       <c r="AV7" s="122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>W</v>
       </c>
       <c r="AW7" s="122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>T</v>
       </c>
       <c r="AX7" s="122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>F</v>
       </c>
       <c r="AY7" s="122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>S</v>
       </c>
       <c r="AZ7" s="123" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>S</v>
       </c>
       <c r="BA7" s="121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>M</v>
       </c>
       <c r="BB7" s="122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>T</v>
       </c>
       <c r="BC7" s="122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>W</v>
       </c>
       <c r="BD7" s="122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>T</v>
       </c>
       <c r="BE7" s="122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>F</v>
       </c>
       <c r="BF7" s="122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>S</v>
       </c>
       <c r="BG7" s="123" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>S</v>
       </c>
       <c r="BH7" s="121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>M</v>
       </c>
       <c r="BI7" s="122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>T</v>
       </c>
       <c r="BJ7" s="122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>W</v>
       </c>
       <c r="BK7" s="122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>T</v>
       </c>
       <c r="BL7" s="122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>F</v>
       </c>
       <c r="BM7" s="122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>S</v>
       </c>
       <c r="BN7" s="123" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="31"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="8" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="BO7" s="121" t="str">
+        <f t="shared" ref="BO7:CP7" si="32">CHOOSE(WEEKDAY(BO6,1),"S","M","T","W","T","F","S")</f>
+        <v>M</v>
+      </c>
+      <c r="BP7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>T</v>
+      </c>
+      <c r="BQ7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>W</v>
+      </c>
+      <c r="BR7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>T</v>
+      </c>
+      <c r="BS7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>F</v>
+      </c>
+      <c r="BT7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>S</v>
+      </c>
+      <c r="BU7" s="123" t="str">
+        <f t="shared" si="32"/>
+        <v>S</v>
+      </c>
+      <c r="BV7" s="121" t="str">
+        <f t="shared" si="32"/>
+        <v>M</v>
+      </c>
+      <c r="BW7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>T</v>
+      </c>
+      <c r="BX7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>W</v>
+      </c>
+      <c r="BY7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>T</v>
+      </c>
+      <c r="BZ7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>F</v>
+      </c>
+      <c r="CA7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>S</v>
+      </c>
+      <c r="CB7" s="123" t="str">
+        <f t="shared" si="32"/>
+        <v>S</v>
+      </c>
+      <c r="CC7" s="121" t="str">
+        <f t="shared" si="32"/>
+        <v>M</v>
+      </c>
+      <c r="CD7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>T</v>
+      </c>
+      <c r="CE7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>W</v>
+      </c>
+      <c r="CF7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>T</v>
+      </c>
+      <c r="CG7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>F</v>
+      </c>
+      <c r="CH7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>S</v>
+      </c>
+      <c r="CI7" s="123" t="str">
+        <f t="shared" si="32"/>
+        <v>S</v>
+      </c>
+      <c r="CJ7" s="121" t="str">
+        <f t="shared" si="32"/>
+        <v>M</v>
+      </c>
+      <c r="CK7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>T</v>
+      </c>
+      <c r="CL7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>W</v>
+      </c>
+      <c r="CM7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>T</v>
+      </c>
+      <c r="CN7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>F</v>
+      </c>
+      <c r="CO7" s="122" t="str">
+        <f t="shared" si="32"/>
+        <v>S</v>
+      </c>
+      <c r="CP7" s="123" t="str">
+        <f t="shared" si="32"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="8" spans="1:94" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="84" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -4585,7 +5019,7 @@
       <c r="G8" s="89"/>
       <c r="H8" s="90"/>
       <c r="I8" s="91" t="str">
-        <f t="shared" ref="I8:I35" si="4">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
+        <f t="shared" ref="I8:I35" si="33">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J8" s="94"/>
@@ -4646,9 +5080,9 @@
       <c r="BM8" s="106"/>
       <c r="BN8" s="106"/>
     </row>
-    <row r="9" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:94" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="60" t="str">
-        <f t="shared" ref="A9:A15" si="5">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A9:A15" si="34">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
       </c>
       <c r="B9" s="126" t="s">
@@ -4674,7 +5108,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v>10</v>
       </c>
       <c r="J9" s="95"/>
@@ -4735,9 +5169,9 @@
       <c r="BM9" s="107"/>
       <c r="BN9" s="107"/>
     </row>
-    <row r="10" spans="1:66" s="61" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:94" s="61" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A10" s="60" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="34"/>
         <v>1.2</v>
       </c>
       <c r="B10" s="126" t="s">
@@ -4761,7 +5195,7 @@
         <v>0.8</v>
       </c>
       <c r="I10" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v>23</v>
       </c>
       <c r="J10" s="95"/>
@@ -4822,9 +5256,9 @@
       <c r="BM10" s="107"/>
       <c r="BN10" s="107"/>
     </row>
-    <row r="11" spans="1:66" s="61" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:94" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="60" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="34"/>
         <v>1.3</v>
       </c>
       <c r="B11" s="126" t="s">
@@ -4838,7 +5272,7 @@
         <v>43139</v>
       </c>
       <c r="F11" s="101">
-        <f t="shared" ref="F11:F33" si="6">IF(ISBLANK(E11)," - ",IF(G11=0,E11,E11+G11-1))</f>
+        <f t="shared" ref="F11:F33" si="35">IF(ISBLANK(E11)," - ",IF(G11=0,E11,E11+G11-1))</f>
         <v>43142</v>
       </c>
       <c r="G11" s="62">
@@ -4848,7 +5282,7 @@
         <v>0.5</v>
       </c>
       <c r="I11" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v>2</v>
       </c>
       <c r="J11" s="95"/>
@@ -4909,7 +5343,7 @@
       <c r="BM11" s="107"/>
       <c r="BN11" s="107"/>
     </row>
-    <row r="12" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:94" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.3.1</v>
@@ -4932,7 +5366,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="J12" s="95"/>
@@ -4993,7 +5427,7 @@
       <c r="BM12" s="107"/>
       <c r="BN12" s="107"/>
     </row>
-    <row r="13" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:94" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.3.2</v>
@@ -5006,7 +5440,7 @@
         <v>43384</v>
       </c>
       <c r="F13" s="101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="35"/>
         <v>43403</v>
       </c>
       <c r="G13" s="62">
@@ -5016,7 +5450,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v>14</v>
       </c>
       <c r="J13" s="95"/>
@@ -5077,9 +5511,9 @@
       <c r="BM13" s="107"/>
       <c r="BN13" s="107"/>
     </row>
-    <row r="14" spans="1:66" s="61" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:94" s="61" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="60" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="34"/>
         <v>1.4</v>
       </c>
       <c r="B14" s="126" t="s">
@@ -5093,7 +5527,7 @@
         <v>43405</v>
       </c>
       <c r="F14" s="101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="35"/>
         <v>43409</v>
       </c>
       <c r="G14" s="62">
@@ -5103,7 +5537,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v>3</v>
       </c>
       <c r="J14" s="95"/>
@@ -5164,9 +5598,9 @@
       <c r="BM14" s="107"/>
       <c r="BN14" s="107"/>
     </row>
-    <row r="15" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:94" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="60" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="34"/>
         <v>1.5</v>
       </c>
       <c r="B15" s="126" t="s">
@@ -5190,7 +5624,7 @@
         <v>0.95</v>
       </c>
       <c r="I15" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v>22</v>
       </c>
       <c r="J15" s="95"/>
@@ -5251,7 +5685,7 @@
       <c r="BM15" s="107"/>
       <c r="BN15" s="107"/>
     </row>
-    <row r="16" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:94" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>2</v>
@@ -5262,13 +5696,13 @@
       <c r="D16" s="56"/>
       <c r="E16" s="102"/>
       <c r="F16" s="102" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="35"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G16" s="57"/>
       <c r="H16" s="58"/>
       <c r="I16" s="59" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J16" s="96"/>
@@ -5433,7 +5867,7 @@
         <v>43354</v>
       </c>
       <c r="F18" s="101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="35"/>
         <v>43367</v>
       </c>
       <c r="G18" s="62">
@@ -5443,7 +5877,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v>10</v>
       </c>
       <c r="J18" s="95"/>
@@ -5520,7 +5954,7 @@
         <v>43374</v>
       </c>
       <c r="F19" s="101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="35"/>
         <v>43392</v>
       </c>
       <c r="G19" s="62">
@@ -5530,7 +5964,7 @@
         <v>0.9</v>
       </c>
       <c r="I19" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v>15</v>
       </c>
       <c r="J19" s="95"/>
@@ -5607,7 +6041,7 @@
         <v>43364</v>
       </c>
       <c r="F20" s="101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="35"/>
         <v>43367</v>
       </c>
       <c r="G20" s="62">
@@ -5617,7 +6051,7 @@
         <v>0.6</v>
       </c>
       <c r="I20" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v>2</v>
       </c>
       <c r="J20" s="95"/>
@@ -5691,7 +6125,7 @@
         <v>43154</v>
       </c>
       <c r="F21" s="101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="35"/>
         <v>43156</v>
       </c>
       <c r="G21" s="62">
@@ -5701,7 +6135,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="J21" s="95"/>
@@ -5768,18 +6202,18 @@
         <v>3</v>
       </c>
       <c r="B22" s="54" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="D22" s="56"/>
       <c r="E22" s="102"/>
       <c r="F22" s="102" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="35"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G22" s="57"/>
       <c r="H22" s="58"/>
       <c r="I22" s="59" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J22" s="96"/>
@@ -5846,25 +6280,28 @@
         <v>3.1</v>
       </c>
       <c r="B23" s="126" t="s">
-        <v>9</v>
+        <v>159</v>
+      </c>
+      <c r="C23" s="61" t="s">
+        <v>163</v>
       </c>
       <c r="D23" s="127"/>
       <c r="E23" s="100">
-        <v>43141</v>
+        <v>43384</v>
       </c>
       <c r="F23" s="101">
-        <f t="shared" si="6"/>
-        <v>43144</v>
+        <f t="shared" si="35"/>
+        <v>43408</v>
       </c>
       <c r="G23" s="62">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="H23" s="63">
         <v>0</v>
       </c>
       <c r="I23" s="64">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <f t="shared" si="33"/>
+        <v>17</v>
       </c>
       <c r="J23" s="95"/>
       <c r="K23" s="107"/>
@@ -5930,25 +6367,28 @@
         <v>3.2</v>
       </c>
       <c r="B24" s="126" t="s">
-        <v>9</v>
+        <v>160</v>
+      </c>
+      <c r="C24" s="61" t="s">
+        <v>163</v>
       </c>
       <c r="D24" s="127"/>
       <c r="E24" s="100">
-        <v>43145</v>
+        <v>43384</v>
       </c>
       <c r="F24" s="101">
-        <f t="shared" si="6"/>
-        <v>43147</v>
+        <f t="shared" si="35"/>
+        <v>43385</v>
       </c>
       <c r="G24" s="62">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H24" s="63">
         <v>0</v>
       </c>
       <c r="I24" s="64">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <f t="shared" si="33"/>
+        <v>2</v>
       </c>
       <c r="J24" s="95"/>
       <c r="K24" s="107"/>
@@ -6014,25 +6454,28 @@
         <v>3.3</v>
       </c>
       <c r="B25" s="126" t="s">
-        <v>9</v>
+        <v>161</v>
+      </c>
+      <c r="C25" s="61" t="s">
+        <v>163</v>
       </c>
       <c r="D25" s="127"/>
       <c r="E25" s="100">
-        <v>43145</v>
+        <v>43384</v>
       </c>
       <c r="F25" s="101">
-        <f t="shared" si="6"/>
-        <v>43147</v>
+        <f t="shared" si="35"/>
+        <v>43390</v>
       </c>
       <c r="G25" s="62">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H25" s="63">
         <v>0</v>
       </c>
       <c r="I25" s="64">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <f t="shared" si="33"/>
+        <v>5</v>
       </c>
       <c r="J25" s="95"/>
       <c r="K25" s="107"/>
@@ -6098,25 +6541,28 @@
         <v>3.4</v>
       </c>
       <c r="B26" s="126" t="s">
-        <v>9</v>
+        <v>162</v>
+      </c>
+      <c r="C26" s="61" t="s">
+        <v>163</v>
       </c>
       <c r="D26" s="127"/>
       <c r="E26" s="100">
-        <v>43148</v>
+        <v>43384</v>
       </c>
       <c r="F26" s="101">
-        <f t="shared" si="6"/>
-        <v>43153</v>
+        <f t="shared" si="35"/>
+        <v>43397</v>
       </c>
       <c r="G26" s="62">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H26" s="63">
         <v>0</v>
       </c>
       <c r="I26" s="64">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f t="shared" si="33"/>
+        <v>10</v>
       </c>
       <c r="J26" s="95"/>
       <c r="K26" s="107"/>
@@ -6182,24 +6628,27 @@
         <v>3.5</v>
       </c>
       <c r="B27" s="126" t="s">
-        <v>9</v>
+        <v>149</v>
+      </c>
+      <c r="C27" s="61" t="s">
+        <v>163</v>
       </c>
       <c r="D27" s="127"/>
       <c r="E27" s="100">
-        <v>43154</v>
+        <v>43384</v>
       </c>
       <c r="F27" s="101">
-        <f t="shared" si="6"/>
-        <v>43156</v>
+        <f t="shared" si="35"/>
+        <v>43384</v>
       </c>
       <c r="G27" s="62">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H27" s="63">
         <v>0</v>
       </c>
       <c r="I27" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="J27" s="95"/>
@@ -6271,13 +6720,13 @@
       <c r="D28" s="56"/>
       <c r="E28" s="102"/>
       <c r="F28" s="102" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="35"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G28" s="57"/>
       <c r="H28" s="58"/>
       <c r="I28" s="59" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J28" s="96"/>
@@ -6351,7 +6800,7 @@
         <v>43129</v>
       </c>
       <c r="F29" s="101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="35"/>
         <v>43129</v>
       </c>
       <c r="G29" s="62">
@@ -6361,7 +6810,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="J29" s="95"/>
@@ -6435,7 +6884,7 @@
         <v>43130</v>
       </c>
       <c r="F30" s="101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="35"/>
         <v>43130</v>
       </c>
       <c r="G30" s="62">
@@ -6445,7 +6894,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="J30" s="95"/>
@@ -6519,7 +6968,7 @@
         <v>43131</v>
       </c>
       <c r="F31" s="101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="35"/>
         <v>43131</v>
       </c>
       <c r="G31" s="62">
@@ -6529,7 +6978,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="J31" s="95"/>
@@ -6603,7 +7052,7 @@
         <v>43132</v>
       </c>
       <c r="F32" s="101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="35"/>
         <v>43132</v>
       </c>
       <c r="G32" s="62">
@@ -6613,7 +7062,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="J32" s="95"/>
@@ -6687,7 +7136,7 @@
         <v>43133</v>
       </c>
       <c r="F33" s="101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="35"/>
         <v>43133</v>
       </c>
       <c r="G33" s="62">
@@ -6697,7 +7146,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="J33" s="95"/>
@@ -6768,7 +7217,7 @@
       <c r="G34" s="67"/>
       <c r="H34" s="68"/>
       <c r="I34" s="69" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J34" s="97"/>
@@ -6839,7 +7288,7 @@
       <c r="G35" s="67"/>
       <c r="H35" s="68"/>
       <c r="I35" s="69" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="33"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J35" s="97"/>
@@ -7052,7 +7501,7 @@
       <c r="D38" s="79"/>
       <c r="E38" s="100"/>
       <c r="F38" s="101" t="str">
-        <f t="shared" ref="F38:F41" si="7">IF(ISBLANK(E38)," - ",IF(G38=0,E38,E38+G38-1))</f>
+        <f t="shared" ref="F38:F41" si="36">IF(ISBLANK(E38)," - ",IF(G38=0,E38,E38+G38-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G38" s="62"/>
@@ -7131,13 +7580,13 @@
       <c r="D39" s="79"/>
       <c r="E39" s="100"/>
       <c r="F39" s="101" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="36"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G39" s="62"/>
       <c r="H39" s="63"/>
       <c r="I39" s="80" t="str">
-        <f t="shared" ref="I39:I41" si="8">IF(OR(F39=0,E39=0)," - ",NETWORKDAYS(E39,F39))</f>
+        <f t="shared" ref="I39:I41" si="37">IF(OR(F39=0,E39=0)," - ",NETWORKDAYS(E39,F39))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J39" s="99"/>
@@ -7210,13 +7659,13 @@
       <c r="D40" s="79"/>
       <c r="E40" s="100"/>
       <c r="F40" s="101" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="36"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G40" s="62"/>
       <c r="H40" s="63"/>
       <c r="I40" s="80" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="37"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J40" s="99"/>
@@ -7289,13 +7738,13 @@
       <c r="D41" s="79"/>
       <c r="E41" s="100"/>
       <c r="F41" s="101" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="36"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G41" s="62"/>
       <c r="H41" s="63"/>
       <c r="I41" s="80" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="37"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J41" s="99"/>
@@ -7426,16 +7875,15 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
-  <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
+  <mergeCells count="27">
+    <mergeCell ref="CJ4:CP4"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BO4:BU4"/>
+    <mergeCell ref="BV4:CB4"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="CC5:CI5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -7446,10 +7894,19 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8:H41">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7463,24 +7920,64 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN7">
-    <cfRule type="expression" dxfId="3" priority="45">
+    <cfRule type="expression" dxfId="11" priority="53">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:BN41">
-    <cfRule type="expression" dxfId="2" priority="48">
+    <cfRule type="expression" dxfId="10" priority="56">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="49">
+    <cfRule type="expression" dxfId="9" priority="57">
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN41">
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="8" priority="16">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <conditionalFormatting sqref="BO6:BU7">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>BO$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BO6:BU7">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>BO$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BV6:CB7">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>BV$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BV6:CB7">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>BV$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CC6:CI7">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>CC$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CC6:CI7">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>CC$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CJ6:CP7">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>CJ$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CJ6:CP7">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>CJ$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Enter the week number to display first in the Gantt Chart. The weeks are numbered starting from the week containing the Project Start Date." sqref="H4"/>
   </dataValidations>
   <hyperlinks>
@@ -7490,7 +7987,7 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 A34:B35 B29 B30:B32 B23:B26 A37:B37 B36 E16 E22 E28 E34:H37 G14 G11 G16:H16 G22:H22 G28:H32 G38 G39:G40 G41 H23:H26" unlockedFormula="1"/>
+    <ignoredError sqref="H9 A34:B35 B29 B30:B32 A37:B37 B36 E16 E22 E28 E34:H37 G14 G11 G16:H16 G22:H22 G28:H32 G38 G39:G40 G41 H23:H26" unlockedFormula="1"/>
     <ignoredError sqref="A28 A22 A16" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>

</xml_diff>

<commit_message>
Gantt updated for servo control and ultrasonic detection
</commit_message>
<xml_diff>
--- a/Gantt_Diagram_Robot_Project_2018.xlsx
+++ b/Gantt_Diagram_Robot_Project_2018.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolle\Documents\Robot_Project_IFX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Robot_Project_IFX\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27075" windowHeight="11370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27080" windowHeight="11370"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="0">GanttChart!$A1048576</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">GanttChartPro!$A$1:$C$47</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">GanttChart!$4:$7</definedName>
     <definedName name="valuevx">42.314159</definedName>
@@ -442,7 +442,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="169">
   <si>
     <t>WBS</t>
   </si>
@@ -466,9 +466,6 @@
   </si>
   <si>
     <t>Creating Task Dependencies</t>
-  </si>
-  <si>
-    <t>[Task Category]</t>
   </si>
   <si>
     <t>[Task]</t>
@@ -1592,6 +1589,24 @@
   </si>
   <si>
     <t>M,Guillaume Nicolle</t>
+  </si>
+  <si>
+    <t>[Ultrasonic Detection]</t>
+  </si>
+  <si>
+    <t>Marlon BOURGOGNE</t>
+  </si>
+  <si>
+    <t>[Comments]</t>
+  </si>
+  <si>
+    <t>[Wiki page]</t>
+  </si>
+  <si>
+    <t>[Servomotors]</t>
+  </si>
+  <si>
+    <t>[Servomotors control]</t>
   </si>
 </sst>
 </file>
@@ -2945,6 +2960,24 @@
     </xf>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2952,27 +2985,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3024,7 +3039,57 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="17">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -3308,11 +3373,11 @@
           <xdr:col>9</xdr:col>
           <xdr:colOff>95250</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>127000</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:to>
@@ -3893,55 +3958,55 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CP42"/>
+  <dimension ref="A1:CP46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BO23" sqref="BO23"/>
+      <pane ySplit="7" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="6.81640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" style="6" customWidth="1"/>
     <col min="5" max="6" width="12" style="1" customWidth="1"/>
     <col min="7" max="7" width="6" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="1.85546875" style="1" customWidth="1"/>
-    <col min="11" max="66" width="2.42578125" style="1" customWidth="1"/>
-    <col min="67" max="67" width="2.7109375" style="3" customWidth="1"/>
-    <col min="68" max="68" width="2.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.7265625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="1.81640625" style="1" customWidth="1"/>
+    <col min="11" max="66" width="2.453125" style="1" customWidth="1"/>
+    <col min="67" max="67" width="2.7265625" style="3" customWidth="1"/>
+    <col min="68" max="68" width="2.54296875" style="3" customWidth="1"/>
     <col min="69" max="70" width="3" style="3" customWidth="1"/>
-    <col min="71" max="71" width="3.28515625" style="3" customWidth="1"/>
-    <col min="72" max="72" width="2.7109375" style="3" customWidth="1"/>
-    <col min="73" max="73" width="2.5703125" style="3" customWidth="1"/>
-    <col min="74" max="74" width="2.7109375" style="3" customWidth="1"/>
-    <col min="75" max="76" width="2.85546875" style="3" customWidth="1"/>
+    <col min="71" max="71" width="3.26953125" style="3" customWidth="1"/>
+    <col min="72" max="72" width="2.7265625" style="3" customWidth="1"/>
+    <col min="73" max="73" width="2.54296875" style="3" customWidth="1"/>
+    <col min="74" max="74" width="2.7265625" style="3" customWidth="1"/>
+    <col min="75" max="76" width="2.81640625" style="3" customWidth="1"/>
     <col min="77" max="77" width="3" style="3" customWidth="1"/>
-    <col min="78" max="78" width="2.5703125" style="3" customWidth="1"/>
-    <col min="79" max="79" width="2.42578125" style="3" customWidth="1"/>
-    <col min="80" max="80" width="2.7109375" style="3" customWidth="1"/>
-    <col min="81" max="81" width="2.42578125" style="3" customWidth="1"/>
+    <col min="78" max="78" width="2.54296875" style="3" customWidth="1"/>
+    <col min="79" max="79" width="2.453125" style="3" customWidth="1"/>
+    <col min="80" max="80" width="2.7265625" style="3" customWidth="1"/>
+    <col min="81" max="81" width="2.453125" style="3" customWidth="1"/>
     <col min="82" max="82" width="3" style="3" customWidth="1"/>
-    <col min="83" max="83" width="2.42578125" style="3" customWidth="1"/>
-    <col min="84" max="84" width="2.7109375" style="3" customWidth="1"/>
-    <col min="85" max="85" width="2.85546875" style="3" customWidth="1"/>
-    <col min="86" max="86" width="2.42578125" style="3" customWidth="1"/>
-    <col min="87" max="88" width="2.5703125" style="3" customWidth="1"/>
+    <col min="83" max="83" width="2.453125" style="3" customWidth="1"/>
+    <col min="84" max="84" width="2.7265625" style="3" customWidth="1"/>
+    <col min="85" max="85" width="2.81640625" style="3" customWidth="1"/>
+    <col min="86" max="86" width="2.453125" style="3" customWidth="1"/>
+    <col min="87" max="88" width="2.54296875" style="3" customWidth="1"/>
     <col min="89" max="89" width="3" style="3" customWidth="1"/>
-    <col min="90" max="90" width="2.5703125" style="3" customWidth="1"/>
-    <col min="91" max="92" width="3.140625" style="3" customWidth="1"/>
-    <col min="93" max="93" width="2.7109375" style="3" customWidth="1"/>
-    <col min="94" max="94" width="2.85546875" style="3" customWidth="1"/>
-    <col min="95" max="16384" width="9.140625" style="3"/>
+    <col min="90" max="90" width="2.54296875" style="3" customWidth="1"/>
+    <col min="91" max="92" width="3.1796875" style="3" customWidth="1"/>
+    <col min="93" max="93" width="2.7265625" style="3" customWidth="1"/>
+    <col min="94" max="94" width="2.81640625" style="3" customWidth="1"/>
+    <col min="95" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:94" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="125" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B1" s="47"/>
       <c r="C1" s="47"/>
@@ -3949,33 +4014,33 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
       <c r="I1" s="132"/>
-      <c r="K1" s="163" t="s">
-        <v>79</v>
-      </c>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
-      <c r="P1" s="163"/>
-      <c r="Q1" s="163"/>
-      <c r="R1" s="163"/>
-      <c r="S1" s="163"/>
-      <c r="T1" s="163"/>
-      <c r="U1" s="163"/>
-      <c r="V1" s="163"/>
-      <c r="W1" s="163"/>
-      <c r="X1" s="163"/>
-      <c r="Y1" s="163"/>
-      <c r="Z1" s="163"/>
-      <c r="AA1" s="163"/>
-      <c r="AB1" s="163"/>
-      <c r="AC1" s="163"/>
-      <c r="AD1" s="163"/>
-      <c r="AE1" s="163"/>
-    </row>
-    <row r="2" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K1" s="169" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="169"/>
+      <c r="M1" s="169"/>
+      <c r="N1" s="169"/>
+      <c r="O1" s="169"/>
+      <c r="P1" s="169"/>
+      <c r="Q1" s="169"/>
+      <c r="R1" s="169"/>
+      <c r="S1" s="169"/>
+      <c r="T1" s="169"/>
+      <c r="U1" s="169"/>
+      <c r="V1" s="169"/>
+      <c r="W1" s="169"/>
+      <c r="X1" s="169"/>
+      <c r="Y1" s="169"/>
+      <c r="Z1" s="169"/>
+      <c r="AA1" s="169"/>
+      <c r="AB1" s="169"/>
+      <c r="AC1" s="169"/>
+      <c r="AD1" s="169"/>
+      <c r="AE1" s="169"/>
+    </row>
+    <row r="2" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -3984,7 +4049,7 @@
       <c r="F2" s="160"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:94" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:94" ht="14" x14ac:dyDescent="0.25">
       <c r="A3" s="52"/>
       <c r="B3" s="48"/>
       <c r="C3" s="4"/>
@@ -4011,283 +4076,283 @@
       <c r="Z3" s="29"/>
       <c r="AA3" s="29"/>
     </row>
-    <row r="4" spans="1:94" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:94" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="110"/>
       <c r="B4" s="114" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="168">
+        <v>75</v>
+      </c>
+      <c r="C4" s="171">
         <v>43340</v>
       </c>
-      <c r="D4" s="168"/>
-      <c r="E4" s="168"/>
+      <c r="D4" s="171"/>
+      <c r="E4" s="171"/>
       <c r="F4" s="111"/>
       <c r="G4" s="114" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" s="129">
         <v>1</v>
       </c>
       <c r="I4" s="112"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="165" t="str">
+      <c r="K4" s="163" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="166"/>
-      <c r="M4" s="166"/>
-      <c r="N4" s="166"/>
-      <c r="O4" s="166"/>
-      <c r="P4" s="166"/>
-      <c r="Q4" s="167"/>
-      <c r="R4" s="165" t="str">
+      <c r="L4" s="164"/>
+      <c r="M4" s="164"/>
+      <c r="N4" s="164"/>
+      <c r="O4" s="164"/>
+      <c r="P4" s="164"/>
+      <c r="Q4" s="165"/>
+      <c r="R4" s="163" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="166"/>
-      <c r="T4" s="166"/>
-      <c r="U4" s="166"/>
-      <c r="V4" s="166"/>
-      <c r="W4" s="166"/>
-      <c r="X4" s="167"/>
-      <c r="Y4" s="165" t="str">
+      <c r="S4" s="164"/>
+      <c r="T4" s="164"/>
+      <c r="U4" s="164"/>
+      <c r="V4" s="164"/>
+      <c r="W4" s="164"/>
+      <c r="X4" s="165"/>
+      <c r="Y4" s="163" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="166"/>
-      <c r="AA4" s="166"/>
-      <c r="AB4" s="166"/>
-      <c r="AC4" s="166"/>
-      <c r="AD4" s="166"/>
-      <c r="AE4" s="167"/>
-      <c r="AF4" s="165" t="str">
+      <c r="Z4" s="164"/>
+      <c r="AA4" s="164"/>
+      <c r="AB4" s="164"/>
+      <c r="AC4" s="164"/>
+      <c r="AD4" s="164"/>
+      <c r="AE4" s="165"/>
+      <c r="AF4" s="163" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="166"/>
-      <c r="AH4" s="166"/>
-      <c r="AI4" s="166"/>
-      <c r="AJ4" s="166"/>
-      <c r="AK4" s="166"/>
-      <c r="AL4" s="167"/>
-      <c r="AM4" s="165" t="str">
+      <c r="AG4" s="164"/>
+      <c r="AH4" s="164"/>
+      <c r="AI4" s="164"/>
+      <c r="AJ4" s="164"/>
+      <c r="AK4" s="164"/>
+      <c r="AL4" s="165"/>
+      <c r="AM4" s="163" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="166"/>
-      <c r="AO4" s="166"/>
-      <c r="AP4" s="166"/>
-      <c r="AQ4" s="166"/>
-      <c r="AR4" s="166"/>
-      <c r="AS4" s="167"/>
-      <c r="AT4" s="165" t="str">
+      <c r="AN4" s="164"/>
+      <c r="AO4" s="164"/>
+      <c r="AP4" s="164"/>
+      <c r="AQ4" s="164"/>
+      <c r="AR4" s="164"/>
+      <c r="AS4" s="165"/>
+      <c r="AT4" s="163" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="166"/>
-      <c r="AV4" s="166"/>
-      <c r="AW4" s="166"/>
-      <c r="AX4" s="166"/>
-      <c r="AY4" s="166"/>
-      <c r="AZ4" s="167"/>
-      <c r="BA4" s="165" t="str">
+      <c r="AU4" s="164"/>
+      <c r="AV4" s="164"/>
+      <c r="AW4" s="164"/>
+      <c r="AX4" s="164"/>
+      <c r="AY4" s="164"/>
+      <c r="AZ4" s="165"/>
+      <c r="BA4" s="163" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="166"/>
-      <c r="BC4" s="166"/>
-      <c r="BD4" s="166"/>
-      <c r="BE4" s="166"/>
-      <c r="BF4" s="166"/>
-      <c r="BG4" s="167"/>
-      <c r="BH4" s="165" t="str">
+      <c r="BB4" s="164"/>
+      <c r="BC4" s="164"/>
+      <c r="BD4" s="164"/>
+      <c r="BE4" s="164"/>
+      <c r="BF4" s="164"/>
+      <c r="BG4" s="165"/>
+      <c r="BH4" s="163" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="166"/>
-      <c r="BJ4" s="166"/>
-      <c r="BK4" s="166"/>
-      <c r="BL4" s="166"/>
-      <c r="BM4" s="166"/>
-      <c r="BN4" s="167"/>
-      <c r="BO4" s="165" t="str">
+      <c r="BI4" s="164"/>
+      <c r="BJ4" s="164"/>
+      <c r="BK4" s="164"/>
+      <c r="BL4" s="164"/>
+      <c r="BM4" s="164"/>
+      <c r="BN4" s="165"/>
+      <c r="BO4" s="163" t="str">
         <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="BP4" s="166"/>
-      <c r="BQ4" s="166"/>
-      <c r="BR4" s="166"/>
-      <c r="BS4" s="166"/>
-      <c r="BT4" s="166"/>
-      <c r="BU4" s="167"/>
-      <c r="BV4" s="165" t="str">
+      <c r="BP4" s="164"/>
+      <c r="BQ4" s="164"/>
+      <c r="BR4" s="164"/>
+      <c r="BS4" s="164"/>
+      <c r="BT4" s="164"/>
+      <c r="BU4" s="165"/>
+      <c r="BV4" s="163" t="str">
         <f>"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="BW4" s="166"/>
-      <c r="BX4" s="166"/>
-      <c r="BY4" s="166"/>
-      <c r="BZ4" s="166"/>
-      <c r="CA4" s="166"/>
-      <c r="CB4" s="167"/>
-      <c r="CC4" s="165" t="str">
+      <c r="BW4" s="164"/>
+      <c r="BX4" s="164"/>
+      <c r="BY4" s="164"/>
+      <c r="BZ4" s="164"/>
+      <c r="CA4" s="164"/>
+      <c r="CB4" s="165"/>
+      <c r="CC4" s="163" t="str">
         <f>"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="CD4" s="166"/>
-      <c r="CE4" s="166"/>
-      <c r="CF4" s="166"/>
-      <c r="CG4" s="166"/>
-      <c r="CH4" s="166"/>
-      <c r="CI4" s="167"/>
-      <c r="CJ4" s="165" t="str">
+      <c r="CD4" s="164"/>
+      <c r="CE4" s="164"/>
+      <c r="CF4" s="164"/>
+      <c r="CG4" s="164"/>
+      <c r="CH4" s="164"/>
+      <c r="CI4" s="165"/>
+      <c r="CJ4" s="163" t="str">
         <f>"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="CK4" s="166"/>
-      <c r="CL4" s="166"/>
-      <c r="CM4" s="166"/>
-      <c r="CN4" s="166"/>
-      <c r="CO4" s="166"/>
-      <c r="CP4" s="167"/>
-    </row>
-    <row r="5" spans="1:94" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="CK4" s="164"/>
+      <c r="CL4" s="164"/>
+      <c r="CM4" s="164"/>
+      <c r="CN4" s="164"/>
+      <c r="CO4" s="164"/>
+      <c r="CP4" s="165"/>
+    </row>
+    <row r="5" spans="1:94" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="110"/>
       <c r="B5" s="114" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="164" t="s">
-        <v>140</v>
-      </c>
-      <c r="D5" s="164"/>
-      <c r="E5" s="164"/>
+        <v>76</v>
+      </c>
+      <c r="C5" s="170" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
       <c r="F5" s="113"/>
       <c r="G5" s="113"/>
       <c r="H5" s="113"/>
       <c r="I5" s="113"/>
       <c r="J5" s="50"/>
-      <c r="K5" s="169">
+      <c r="K5" s="166">
         <f>K6</f>
         <v>43339</v>
       </c>
-      <c r="L5" s="170"/>
-      <c r="M5" s="170"/>
-      <c r="N5" s="170"/>
-      <c r="O5" s="170"/>
-      <c r="P5" s="170"/>
-      <c r="Q5" s="171"/>
-      <c r="R5" s="169">
+      <c r="L5" s="167"/>
+      <c r="M5" s="167"/>
+      <c r="N5" s="167"/>
+      <c r="O5" s="167"/>
+      <c r="P5" s="167"/>
+      <c r="Q5" s="168"/>
+      <c r="R5" s="166">
         <f>R6</f>
         <v>43346</v>
       </c>
-      <c r="S5" s="170"/>
-      <c r="T5" s="170"/>
-      <c r="U5" s="170"/>
-      <c r="V5" s="170"/>
-      <c r="W5" s="170"/>
-      <c r="X5" s="171"/>
-      <c r="Y5" s="169">
+      <c r="S5" s="167"/>
+      <c r="T5" s="167"/>
+      <c r="U5" s="167"/>
+      <c r="V5" s="167"/>
+      <c r="W5" s="167"/>
+      <c r="X5" s="168"/>
+      <c r="Y5" s="166">
         <f>Y6</f>
         <v>43353</v>
       </c>
-      <c r="Z5" s="170"/>
-      <c r="AA5" s="170"/>
-      <c r="AB5" s="170"/>
-      <c r="AC5" s="170"/>
-      <c r="AD5" s="170"/>
-      <c r="AE5" s="171"/>
-      <c r="AF5" s="169">
+      <c r="Z5" s="167"/>
+      <c r="AA5" s="167"/>
+      <c r="AB5" s="167"/>
+      <c r="AC5" s="167"/>
+      <c r="AD5" s="167"/>
+      <c r="AE5" s="168"/>
+      <c r="AF5" s="166">
         <f>AF6</f>
         <v>43360</v>
       </c>
-      <c r="AG5" s="170"/>
-      <c r="AH5" s="170"/>
-      <c r="AI5" s="170"/>
-      <c r="AJ5" s="170"/>
-      <c r="AK5" s="170"/>
-      <c r="AL5" s="171"/>
-      <c r="AM5" s="169">
+      <c r="AG5" s="167"/>
+      <c r="AH5" s="167"/>
+      <c r="AI5" s="167"/>
+      <c r="AJ5" s="167"/>
+      <c r="AK5" s="167"/>
+      <c r="AL5" s="168"/>
+      <c r="AM5" s="166">
         <f>AM6</f>
         <v>43367</v>
       </c>
-      <c r="AN5" s="170"/>
-      <c r="AO5" s="170"/>
-      <c r="AP5" s="170"/>
-      <c r="AQ5" s="170"/>
-      <c r="AR5" s="170"/>
-      <c r="AS5" s="171"/>
-      <c r="AT5" s="169">
+      <c r="AN5" s="167"/>
+      <c r="AO5" s="167"/>
+      <c r="AP5" s="167"/>
+      <c r="AQ5" s="167"/>
+      <c r="AR5" s="167"/>
+      <c r="AS5" s="168"/>
+      <c r="AT5" s="166">
         <f>AT6</f>
         <v>43374</v>
       </c>
-      <c r="AU5" s="170"/>
-      <c r="AV5" s="170"/>
-      <c r="AW5" s="170"/>
-      <c r="AX5" s="170"/>
-      <c r="AY5" s="170"/>
-      <c r="AZ5" s="171"/>
-      <c r="BA5" s="169">
+      <c r="AU5" s="167"/>
+      <c r="AV5" s="167"/>
+      <c r="AW5" s="167"/>
+      <c r="AX5" s="167"/>
+      <c r="AY5" s="167"/>
+      <c r="AZ5" s="168"/>
+      <c r="BA5" s="166">
         <f>BA6</f>
         <v>43381</v>
       </c>
-      <c r="BB5" s="170"/>
-      <c r="BC5" s="170"/>
-      <c r="BD5" s="170"/>
-      <c r="BE5" s="170"/>
-      <c r="BF5" s="170"/>
-      <c r="BG5" s="171"/>
-      <c r="BH5" s="169">
+      <c r="BB5" s="167"/>
+      <c r="BC5" s="167"/>
+      <c r="BD5" s="167"/>
+      <c r="BE5" s="167"/>
+      <c r="BF5" s="167"/>
+      <c r="BG5" s="168"/>
+      <c r="BH5" s="166">
         <f>BH6</f>
         <v>43388</v>
       </c>
-      <c r="BI5" s="170"/>
-      <c r="BJ5" s="170"/>
-      <c r="BK5" s="170"/>
-      <c r="BL5" s="170"/>
-      <c r="BM5" s="170"/>
-      <c r="BN5" s="171"/>
-      <c r="BO5" s="169">
+      <c r="BI5" s="167"/>
+      <c r="BJ5" s="167"/>
+      <c r="BK5" s="167"/>
+      <c r="BL5" s="167"/>
+      <c r="BM5" s="167"/>
+      <c r="BN5" s="168"/>
+      <c r="BO5" s="166">
         <f>BO6</f>
         <v>43395</v>
       </c>
-      <c r="BP5" s="170"/>
-      <c r="BQ5" s="170"/>
-      <c r="BR5" s="170"/>
-      <c r="BS5" s="170"/>
-      <c r="BT5" s="170"/>
-      <c r="BU5" s="171"/>
-      <c r="BV5" s="169">
+      <c r="BP5" s="167"/>
+      <c r="BQ5" s="167"/>
+      <c r="BR5" s="167"/>
+      <c r="BS5" s="167"/>
+      <c r="BT5" s="167"/>
+      <c r="BU5" s="168"/>
+      <c r="BV5" s="166">
         <f>BV6</f>
         <v>43402</v>
       </c>
-      <c r="BW5" s="170"/>
-      <c r="BX5" s="170"/>
-      <c r="BY5" s="170"/>
-      <c r="BZ5" s="170"/>
-      <c r="CA5" s="170"/>
-      <c r="CB5" s="171"/>
-      <c r="CC5" s="169">
+      <c r="BW5" s="167"/>
+      <c r="BX5" s="167"/>
+      <c r="BY5" s="167"/>
+      <c r="BZ5" s="167"/>
+      <c r="CA5" s="167"/>
+      <c r="CB5" s="168"/>
+      <c r="CC5" s="166">
         <f>CC6</f>
         <v>43409</v>
       </c>
-      <c r="CD5" s="170"/>
-      <c r="CE5" s="170"/>
-      <c r="CF5" s="170"/>
-      <c r="CG5" s="170"/>
-      <c r="CH5" s="170"/>
-      <c r="CI5" s="171"/>
-      <c r="CJ5" s="169">
+      <c r="CD5" s="167"/>
+      <c r="CE5" s="167"/>
+      <c r="CF5" s="167"/>
+      <c r="CG5" s="167"/>
+      <c r="CH5" s="167"/>
+      <c r="CI5" s="168"/>
+      <c r="CJ5" s="166">
         <f>CJ6</f>
         <v>43416</v>
       </c>
-      <c r="CK5" s="170"/>
-      <c r="CL5" s="170"/>
-      <c r="CM5" s="170"/>
-      <c r="CN5" s="170"/>
-      <c r="CO5" s="170"/>
-      <c r="CP5" s="171"/>
-    </row>
-    <row r="6" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="CK5" s="167"/>
+      <c r="CL5" s="167"/>
+      <c r="CM5" s="167"/>
+      <c r="CN5" s="167"/>
+      <c r="CO5" s="167"/>
+      <c r="CP5" s="168"/>
+    </row>
+    <row r="6" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A6" s="49"/>
       <c r="B6" s="50"/>
       <c r="C6" s="50"/>
@@ -4635,33 +4700,33 @@
         <v>43422</v>
       </c>
     </row>
-    <row r="7" spans="1:94" s="124" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:94" s="124" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="116" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="117" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="118" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="118" t="s">
+      <c r="D7" s="119" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="120" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="119" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="120" t="s">
+      <c r="F7" s="120" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="120" t="s">
+      <c r="G7" s="118" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="118" t="s">
+      <c r="H7" s="118" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="118" t="s">
+      <c r="I7" s="118" t="s">
         <v>72</v>
-      </c>
-      <c r="I7" s="118" t="s">
-        <v>73</v>
       </c>
       <c r="J7" s="118"/>
       <c r="K7" s="121" t="str">
@@ -5001,13 +5066,13 @@
         <v>S</v>
       </c>
     </row>
-    <row r="8" spans="1:94" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:94" s="55" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A8" s="84" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
       </c>
       <c r="B8" s="85" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C8" s="86"/>
       <c r="D8" s="87"/>
@@ -5019,7 +5084,7 @@
       <c r="G8" s="89"/>
       <c r="H8" s="90"/>
       <c r="I8" s="91" t="str">
-        <f t="shared" ref="I8:I35" si="33">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
+        <f t="shared" ref="I8:I39" si="33">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J8" s="94"/>
@@ -5080,19 +5145,19 @@
       <c r="BM8" s="106"/>
       <c r="BN8" s="106"/>
     </row>
-    <row r="9" spans="1:94" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="str">
         <f t="shared" ref="A9:A15" si="34">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
       </c>
       <c r="B9" s="126" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="61" t="s">
         <v>142</v>
       </c>
-      <c r="C9" s="61" t="s">
-        <v>143</v>
-      </c>
       <c r="D9" s="127" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E9" s="100">
         <v>43340</v>
@@ -5169,16 +5234,16 @@
       <c r="BM9" s="107"/>
       <c r="BN9" s="107"/>
     </row>
-    <row r="10" spans="1:94" s="61" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="str">
         <f t="shared" si="34"/>
         <v>1.2</v>
       </c>
       <c r="B10" s="126" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C10" s="61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D10" s="127"/>
       <c r="E10" s="100">
@@ -5256,23 +5321,23 @@
       <c r="BM10" s="107"/>
       <c r="BN10" s="107"/>
     </row>
-    <row r="11" spans="1:94" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="str">
         <f t="shared" si="34"/>
         <v>1.3</v>
       </c>
       <c r="B11" s="126" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" s="61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D11" s="127"/>
       <c r="E11" s="100">
         <v>43139</v>
       </c>
       <c r="F11" s="101">
-        <f t="shared" ref="F11:F33" si="35">IF(ISBLANK(E11)," - ",IF(G11=0,E11,E11+G11-1))</f>
+        <f t="shared" ref="F11:F30" si="35">IF(ISBLANK(E11)," - ",IF(G11=0,E11,E11+G11-1))</f>
         <v>43142</v>
       </c>
       <c r="G11" s="62">
@@ -5343,13 +5408,13 @@
       <c r="BM11" s="107"/>
       <c r="BN11" s="107"/>
     </row>
-    <row r="12" spans="1:94" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.3.1</v>
       </c>
       <c r="B12" s="128" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D12" s="127"/>
       <c r="E12" s="100">
@@ -5427,13 +5492,13 @@
       <c r="BM12" s="107"/>
       <c r="BN12" s="107"/>
     </row>
-    <row r="13" spans="1:94" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.3.2</v>
       </c>
       <c r="B13" s="128" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D13" s="127"/>
       <c r="E13" s="100">
@@ -5511,16 +5576,16 @@
       <c r="BM13" s="107"/>
       <c r="BN13" s="107"/>
     </row>
-    <row r="14" spans="1:94" s="61" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:94" s="61" customFormat="1" ht="23" x14ac:dyDescent="0.25">
       <c r="A14" s="60" t="str">
         <f t="shared" si="34"/>
         <v>1.4</v>
       </c>
       <c r="B14" s="126" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C14" s="61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D14" s="127"/>
       <c r="E14" s="100">
@@ -5598,16 +5663,16 @@
       <c r="BM14" s="107"/>
       <c r="BN14" s="107"/>
     </row>
-    <row r="15" spans="1:94" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A15" s="60" t="str">
         <f t="shared" si="34"/>
         <v>1.5</v>
       </c>
       <c r="B15" s="126" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C15" s="61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D15" s="127"/>
       <c r="E15" s="100">
@@ -5685,13 +5750,13 @@
       <c r="BM15" s="107"/>
       <c r="BN15" s="107"/>
     </row>
-    <row r="16" spans="1:94" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:94" s="55" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A16" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>2</v>
       </c>
       <c r="B16" s="54" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D16" s="56"/>
       <c r="E16" s="102"/>
@@ -5763,19 +5828,19 @@
       <c r="BM16" s="109"/>
       <c r="BN16" s="109"/>
     </row>
-    <row r="17" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A17" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.1</v>
       </c>
       <c r="B17" s="126" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C17" s="61" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="127" t="s">
         <v>152</v>
-      </c>
-      <c r="D17" s="127" t="s">
-        <v>153</v>
       </c>
       <c r="E17" s="100">
         <v>43329</v>
@@ -5851,16 +5916,16 @@
       <c r="BM17" s="107"/>
       <c r="BN17" s="107"/>
     </row>
-    <row r="18" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A18" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.2</v>
       </c>
       <c r="B18" s="126" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C18" s="61" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D18" s="127"/>
       <c r="E18" s="100">
@@ -5938,16 +6003,16 @@
       <c r="BM18" s="107"/>
       <c r="BN18" s="107"/>
     </row>
-    <row r="19" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A19" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.3</v>
       </c>
       <c r="B19" s="126" t="s">
+        <v>155</v>
+      </c>
+      <c r="C19" s="61" t="s">
         <v>156</v>
-      </c>
-      <c r="C19" s="61" t="s">
-        <v>157</v>
       </c>
       <c r="D19" s="127"/>
       <c r="E19" s="100">
@@ -6025,16 +6090,16 @@
       <c r="BM19" s="107"/>
       <c r="BN19" s="107"/>
     </row>
-    <row r="20" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.4</v>
       </c>
       <c r="B20" s="126" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C20" s="61" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D20" s="127"/>
       <c r="E20" s="100">
@@ -6112,13 +6177,13 @@
       <c r="BM20" s="107"/>
       <c r="BN20" s="107"/>
     </row>
-    <row r="21" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A21" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.5</v>
       </c>
       <c r="B21" s="126" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="127"/>
       <c r="E21" s="100">
@@ -6196,13 +6261,13 @@
       <c r="BM21" s="107"/>
       <c r="BN21" s="107"/>
     </row>
-    <row r="22" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:66" s="55" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A22" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>3</v>
       </c>
       <c r="B22" s="54" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D22" s="56"/>
       <c r="E22" s="102"/>
@@ -6274,16 +6339,16 @@
       <c r="BM22" s="109"/>
       <c r="BN22" s="109"/>
     </row>
-    <row r="23" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A23" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.1</v>
       </c>
       <c r="B23" s="126" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C23" s="61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D23" s="127"/>
       <c r="E23" s="100">
@@ -6361,16 +6426,16 @@
       <c r="BM23" s="107"/>
       <c r="BN23" s="107"/>
     </row>
-    <row r="24" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A24" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.2</v>
       </c>
       <c r="B24" s="126" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C24" s="61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D24" s="127"/>
       <c r="E24" s="100">
@@ -6448,16 +6513,16 @@
       <c r="BM24" s="107"/>
       <c r="BN24" s="107"/>
     </row>
-    <row r="25" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.3</v>
       </c>
       <c r="B25" s="126" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C25" s="61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D25" s="127"/>
       <c r="E25" s="100">
@@ -6535,16 +6600,16 @@
       <c r="BM25" s="107"/>
       <c r="BN25" s="107"/>
     </row>
-    <row r="26" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A26" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.4</v>
       </c>
       <c r="B26" s="126" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" s="61" t="s">
         <v>162</v>
-      </c>
-      <c r="C26" s="61" t="s">
-        <v>163</v>
       </c>
       <c r="D26" s="127"/>
       <c r="E26" s="100">
@@ -6622,16 +6687,16 @@
       <c r="BM26" s="107"/>
       <c r="BN26" s="107"/>
     </row>
-    <row r="27" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A27" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.5</v>
       </c>
       <c r="B27" s="126" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C27" s="61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D27" s="127"/>
       <c r="E27" s="100">
@@ -6709,13 +6774,13 @@
       <c r="BM27" s="107"/>
       <c r="BN27" s="107"/>
     </row>
-    <row r="28" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:66" s="55" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A28" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>4</v>
       </c>
       <c r="B28" s="54" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="D28" s="56"/>
       <c r="E28" s="102"/>
@@ -6787,31 +6852,34 @@
       <c r="BM28" s="109"/>
       <c r="BN28" s="109"/>
     </row>
-    <row r="29" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A29" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.1</v>
       </c>
       <c r="B29" s="126" t="s">
-        <v>9</v>
+        <v>163</v>
+      </c>
+      <c r="C29" s="61" t="s">
+        <v>164</v>
       </c>
       <c r="D29" s="127"/>
       <c r="E29" s="100">
-        <v>43129</v>
+        <v>43353</v>
       </c>
       <c r="F29" s="101">
-        <f t="shared" si="35"/>
-        <v>43129</v>
+        <f>IF(ISBLANK(E29)," - ",IF(G29=0,E29,E29+G29-1))</f>
+        <v>43355</v>
       </c>
       <c r="G29" s="62">
+        <v>3</v>
+      </c>
+      <c r="H29" s="63">
         <v>1</v>
-      </c>
-      <c r="H29" s="63">
-        <v>0</v>
       </c>
       <c r="I29" s="64">
         <f t="shared" si="33"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J29" s="95"/>
       <c r="K29" s="107"/>
@@ -6871,27 +6939,30 @@
       <c r="BM29" s="107"/>
       <c r="BN29" s="107"/>
     </row>
-    <row r="30" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A30" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.2</v>
       </c>
       <c r="B30" s="126" t="s">
-        <v>9</v>
+        <v>165</v>
+      </c>
+      <c r="C30" s="61" t="s">
+        <v>164</v>
       </c>
       <c r="D30" s="127"/>
       <c r="E30" s="100">
-        <v>43130</v>
+        <v>43354</v>
       </c>
       <c r="F30" s="101">
         <f t="shared" si="35"/>
-        <v>43130</v>
+        <v>43354</v>
       </c>
       <c r="G30" s="62">
         <v>1</v>
       </c>
       <c r="H30" s="63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" s="64">
         <f t="shared" si="33"/>
@@ -6955,27 +7026,30 @@
       <c r="BM30" s="107"/>
       <c r="BN30" s="107"/>
     </row>
-    <row r="31" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A31" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.3</v>
       </c>
       <c r="B31" s="126" t="s">
-        <v>9</v>
+        <v>166</v>
+      </c>
+      <c r="C31" s="61" t="s">
+        <v>164</v>
       </c>
       <c r="D31" s="127"/>
       <c r="E31" s="100">
-        <v>43131</v>
+        <v>43357</v>
       </c>
       <c r="F31" s="101">
-        <f t="shared" si="35"/>
-        <v>43131</v>
+        <f>IF(ISBLANK(E31)," - ",IF(G31=0,E31,E31+G31-1))</f>
+        <v>43357</v>
       </c>
       <c r="G31" s="62">
         <v>1</v>
       </c>
       <c r="H31" s="63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="64">
         <f t="shared" si="33"/>
@@ -7039,115 +7113,112 @@
       <c r="BM31" s="107"/>
       <c r="BN31" s="107"/>
     </row>
-    <row r="32" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.4</v>
-      </c>
-      <c r="B32" s="126" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="127"/>
-      <c r="E32" s="100">
-        <v>43132</v>
-      </c>
-      <c r="F32" s="101">
-        <f t="shared" si="35"/>
-        <v>43132</v>
-      </c>
-      <c r="G32" s="62">
-        <v>1</v>
-      </c>
-      <c r="H32" s="63">
-        <v>0</v>
-      </c>
-      <c r="I32" s="64">
-        <f t="shared" si="33"/>
-        <v>1</v>
-      </c>
-      <c r="J32" s="95"/>
-      <c r="K32" s="107"/>
-      <c r="L32" s="107"/>
-      <c r="M32" s="107"/>
-      <c r="N32" s="107"/>
-      <c r="O32" s="107"/>
-      <c r="P32" s="107"/>
-      <c r="Q32" s="107"/>
-      <c r="R32" s="107"/>
-      <c r="S32" s="107"/>
-      <c r="T32" s="107"/>
-      <c r="U32" s="107"/>
-      <c r="V32" s="107"/>
-      <c r="W32" s="107"/>
-      <c r="X32" s="107"/>
-      <c r="Y32" s="107"/>
-      <c r="Z32" s="107"/>
-      <c r="AA32" s="107"/>
-      <c r="AB32" s="107"/>
-      <c r="AC32" s="107"/>
-      <c r="AD32" s="107"/>
-      <c r="AE32" s="107"/>
-      <c r="AF32" s="107"/>
-      <c r="AG32" s="107"/>
-      <c r="AH32" s="107"/>
-      <c r="AI32" s="107"/>
-      <c r="AJ32" s="107"/>
-      <c r="AK32" s="107"/>
-      <c r="AL32" s="107"/>
-      <c r="AM32" s="107"/>
-      <c r="AN32" s="107"/>
-      <c r="AO32" s="107"/>
-      <c r="AP32" s="107"/>
-      <c r="AQ32" s="107"/>
-      <c r="AR32" s="107"/>
-      <c r="AS32" s="107"/>
-      <c r="AT32" s="107"/>
-      <c r="AU32" s="107"/>
-      <c r="AV32" s="107"/>
-      <c r="AW32" s="107"/>
-      <c r="AX32" s="107"/>
-      <c r="AY32" s="107"/>
-      <c r="AZ32" s="107"/>
-      <c r="BA32" s="107"/>
-      <c r="BB32" s="107"/>
-      <c r="BC32" s="107"/>
-      <c r="BD32" s="107"/>
-      <c r="BE32" s="107"/>
-      <c r="BF32" s="107"/>
-      <c r="BG32" s="107"/>
-      <c r="BH32" s="107"/>
-      <c r="BI32" s="107"/>
-      <c r="BJ32" s="107"/>
-      <c r="BK32" s="107"/>
-      <c r="BL32" s="107"/>
-      <c r="BM32" s="107"/>
-      <c r="BN32" s="107"/>
-    </row>
-    <row r="33" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:66" s="55" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="53" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>5</v>
+      </c>
+      <c r="B32" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="D32" s="56"/>
+      <c r="E32" s="102"/>
+      <c r="F32" s="102" t="str">
+        <f t="shared" ref="F32:F37" si="36">IF(ISBLANK(E32)," - ",IF(G32=0,E32,E32+G32-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G32" s="57"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="59" t="str">
+        <f t="shared" ref="I32:I37" si="37">IF(OR(F32=0,E32=0)," - ",NETWORKDAYS(E32,F32))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J32" s="96"/>
+      <c r="K32" s="109"/>
+      <c r="L32" s="109"/>
+      <c r="M32" s="109"/>
+      <c r="N32" s="109"/>
+      <c r="O32" s="109"/>
+      <c r="P32" s="109"/>
+      <c r="Q32" s="109"/>
+      <c r="R32" s="109"/>
+      <c r="S32" s="109"/>
+      <c r="T32" s="109"/>
+      <c r="U32" s="109"/>
+      <c r="V32" s="109"/>
+      <c r="W32" s="109"/>
+      <c r="X32" s="109"/>
+      <c r="Y32" s="109"/>
+      <c r="Z32" s="109"/>
+      <c r="AA32" s="109"/>
+      <c r="AB32" s="109"/>
+      <c r="AC32" s="109"/>
+      <c r="AD32" s="109"/>
+      <c r="AE32" s="109"/>
+      <c r="AF32" s="109"/>
+      <c r="AG32" s="109"/>
+      <c r="AH32" s="109"/>
+      <c r="AI32" s="109"/>
+      <c r="AJ32" s="109"/>
+      <c r="AK32" s="109"/>
+      <c r="AL32" s="109"/>
+      <c r="AM32" s="109"/>
+      <c r="AN32" s="109"/>
+      <c r="AO32" s="109"/>
+      <c r="AP32" s="109"/>
+      <c r="AQ32" s="109"/>
+      <c r="AR32" s="109"/>
+      <c r="AS32" s="109"/>
+      <c r="AT32" s="109"/>
+      <c r="AU32" s="109"/>
+      <c r="AV32" s="109"/>
+      <c r="AW32" s="109"/>
+      <c r="AX32" s="109"/>
+      <c r="AY32" s="109"/>
+      <c r="AZ32" s="109"/>
+      <c r="BA32" s="109"/>
+      <c r="BB32" s="109"/>
+      <c r="BC32" s="109"/>
+      <c r="BD32" s="109"/>
+      <c r="BE32" s="109"/>
+      <c r="BF32" s="109"/>
+      <c r="BG32" s="109"/>
+      <c r="BH32" s="109"/>
+      <c r="BI32" s="109"/>
+      <c r="BJ32" s="109"/>
+      <c r="BK32" s="109"/>
+      <c r="BL32" s="109"/>
+      <c r="BM32" s="109"/>
+      <c r="BN32" s="109"/>
+    </row>
+    <row r="33" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A33" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.5</v>
+        <v>5.1</v>
       </c>
       <c r="B33" s="126" t="s">
-        <v>9</v>
+        <v>168</v>
+      </c>
+      <c r="C33" s="61" t="s">
+        <v>164</v>
       </c>
       <c r="D33" s="127"/>
       <c r="E33" s="100">
-        <v>43133</v>
+        <v>43391</v>
       </c>
       <c r="F33" s="101">
-        <f t="shared" si="35"/>
-        <v>43133</v>
+        <f>IF(ISBLANK(E33)," - ",IF(G33=0,E33,E33+G33-1))</f>
+        <v>43397</v>
       </c>
       <c r="G33" s="62">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H33" s="63">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="I33" s="64">
-        <f t="shared" si="33"/>
-        <v>1</v>
+        <f t="shared" si="37"/>
+        <v>5</v>
       </c>
       <c r="J33" s="95"/>
       <c r="K33" s="107"/>
@@ -7207,20 +7278,36 @@
       <c r="BM33" s="107"/>
       <c r="BN33" s="107"/>
     </row>
-    <row r="34" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A34" s="60"/>
-      <c r="B34" s="65"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="66"/>
-      <c r="E34" s="103"/>
-      <c r="F34" s="103"/>
-      <c r="G34" s="67"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="69" t="str">
-        <f t="shared" si="33"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J34" s="97"/>
+    <row r="34" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>5.2</v>
+      </c>
+      <c r="B34" s="126" t="s">
+        <v>165</v>
+      </c>
+      <c r="C34" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="D34" s="127"/>
+      <c r="E34" s="100">
+        <v>43391</v>
+      </c>
+      <c r="F34" s="101">
+        <f t="shared" ref="F34:F37" si="38">IF(ISBLANK(E34)," - ",IF(G34=0,E34,E34+G34-1))</f>
+        <v>43391</v>
+      </c>
+      <c r="G34" s="62">
+        <v>1</v>
+      </c>
+      <c r="H34" s="63">
+        <v>0</v>
+      </c>
+      <c r="I34" s="64">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="J34" s="95"/>
       <c r="K34" s="107"/>
       <c r="L34" s="107"/>
       <c r="M34" s="107"/>
@@ -7278,20 +7365,36 @@
       <c r="BM34" s="107"/>
       <c r="BN34" s="107"/>
     </row>
-    <row r="35" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A35" s="60"/>
-      <c r="B35" s="65"/>
-      <c r="C35" s="65"/>
-      <c r="D35" s="66"/>
-      <c r="E35" s="103"/>
-      <c r="F35" s="103"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="68"/>
-      <c r="I35" s="69" t="str">
-        <f t="shared" si="33"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J35" s="97"/>
+    <row r="35" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>5.3</v>
+      </c>
+      <c r="B35" s="126" t="s">
+        <v>166</v>
+      </c>
+      <c r="C35" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="D35" s="127"/>
+      <c r="E35" s="100">
+        <v>43391</v>
+      </c>
+      <c r="F35" s="101">
+        <f>IF(ISBLANK(E35)," - ",IF(G35=0,E35,E35+G35-1))</f>
+        <v>43391</v>
+      </c>
+      <c r="G35" s="62">
+        <v>1</v>
+      </c>
+      <c r="H35" s="63">
+        <v>0</v>
+      </c>
+      <c r="I35" s="64">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="J35" s="95"/>
       <c r="K35" s="107"/>
       <c r="L35" s="107"/>
       <c r="M35" s="107"/>
@@ -7349,19 +7452,33 @@
       <c r="BM35" s="107"/>
       <c r="BN35" s="107"/>
     </row>
-    <row r="36" spans="1:66" s="75" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="71" t="s">
+    <row r="36" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>5.4</v>
+      </c>
+      <c r="B36" s="126" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="127"/>
+      <c r="E36" s="100">
+        <v>43132</v>
+      </c>
+      <c r="F36" s="101">
+        <f t="shared" ref="F36:F37" si="39">IF(ISBLANK(E36)," - ",IF(G36=0,E36,E36+G36-1))</f>
+        <v>43132</v>
+      </c>
+      <c r="G36" s="62">
         <v>1</v>
       </c>
-      <c r="B36" s="72"/>
-      <c r="C36" s="73"/>
-      <c r="D36" s="73"/>
-      <c r="E36" s="104"/>
-      <c r="F36" s="104"/>
-      <c r="G36" s="74"/>
-      <c r="H36" s="74"/>
-      <c r="I36" s="74"/>
-      <c r="J36" s="98"/>
+      <c r="H36" s="63">
+        <v>0</v>
+      </c>
+      <c r="I36" s="64">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="J36" s="95"/>
       <c r="K36" s="107"/>
       <c r="L36" s="107"/>
       <c r="M36" s="107"/>
@@ -7419,19 +7536,33 @@
       <c r="BM36" s="107"/>
       <c r="BN36" s="107"/>
     </row>
-    <row r="37" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" s="76" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="77"/>
-      <c r="C37" s="77"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="105"/>
-      <c r="F37" s="105"/>
-      <c r="G37" s="77"/>
-      <c r="H37" s="77"/>
-      <c r="I37" s="77"/>
-      <c r="J37" s="98"/>
+    <row r="37" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>5.5</v>
+      </c>
+      <c r="B37" s="126" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="127"/>
+      <c r="E37" s="100">
+        <v>43133</v>
+      </c>
+      <c r="F37" s="101">
+        <f t="shared" si="39"/>
+        <v>43133</v>
+      </c>
+      <c r="G37" s="62">
+        <v>1</v>
+      </c>
+      <c r="H37" s="63">
+        <v>0</v>
+      </c>
+      <c r="I37" s="64">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="J37" s="95"/>
       <c r="K37" s="107"/>
       <c r="L37" s="107"/>
       <c r="M37" s="107"/>
@@ -7489,28 +7620,20 @@
       <c r="BM37" s="107"/>
       <c r="BN37" s="107"/>
     </row>
-    <row r="38" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A38" s="130" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>1</v>
-      </c>
-      <c r="B38" s="131" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="78"/>
-      <c r="D38" s="79"/>
-      <c r="E38" s="100"/>
-      <c r="F38" s="101" t="str">
-        <f t="shared" ref="F38:F41" si="36">IF(ISBLANK(E38)," - ",IF(G38=0,E38,E38+G38-1))</f>
+    <row r="38" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="60"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="103"/>
+      <c r="F38" s="103"/>
+      <c r="G38" s="67"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="69" t="str">
+        <f t="shared" si="33"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G38" s="62"/>
-      <c r="H38" s="63"/>
-      <c r="I38" s="80" t="str">
-        <f>IF(OR(F38=0,E38=0)," - ",NETWORKDAYS(E38,F38))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J38" s="99"/>
+      <c r="J38" s="97"/>
       <c r="K38" s="107"/>
       <c r="L38" s="107"/>
       <c r="M38" s="107"/>
@@ -7568,28 +7691,20 @@
       <c r="BM38" s="107"/>
       <c r="BN38" s="107"/>
     </row>
-    <row r="39" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A39" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>1.1</v>
-      </c>
-      <c r="B39" s="81" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" s="81"/>
-      <c r="D39" s="79"/>
-      <c r="E39" s="100"/>
-      <c r="F39" s="101" t="str">
-        <f t="shared" si="36"/>
+    <row r="39" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="60"/>
+      <c r="B39" s="65"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="103"/>
+      <c r="F39" s="103"/>
+      <c r="G39" s="67"/>
+      <c r="H39" s="68"/>
+      <c r="I39" s="69" t="str">
+        <f t="shared" si="33"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G39" s="62"/>
-      <c r="H39" s="63"/>
-      <c r="I39" s="80" t="str">
-        <f t="shared" ref="I39:I41" si="37">IF(OR(F39=0,E39=0)," - ",NETWORKDAYS(E39,F39))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J39" s="99"/>
+      <c r="J39" s="97"/>
       <c r="K39" s="107"/>
       <c r="L39" s="107"/>
       <c r="M39" s="107"/>
@@ -7647,28 +7762,19 @@
       <c r="BM39" s="107"/>
       <c r="BN39" s="107"/>
     </row>
-    <row r="40" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A40" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
-        <v>1.1.1</v>
-      </c>
-      <c r="B40" s="82" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="81"/>
-      <c r="D40" s="79"/>
-      <c r="E40" s="100"/>
-      <c r="F40" s="101" t="str">
-        <f t="shared" si="36"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G40" s="62"/>
-      <c r="H40" s="63"/>
-      <c r="I40" s="80" t="str">
-        <f t="shared" si="37"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J40" s="99"/>
+    <row r="40" spans="1:66" s="75" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="72"/>
+      <c r="C40" s="73"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="104"/>
+      <c r="F40" s="104"/>
+      <c r="G40" s="74"/>
+      <c r="H40" s="74"/>
+      <c r="I40" s="74"/>
+      <c r="J40" s="98"/>
       <c r="K40" s="107"/>
       <c r="L40" s="107"/>
       <c r="M40" s="107"/>
@@ -7726,28 +7832,19 @@
       <c r="BM40" s="107"/>
       <c r="BN40" s="107"/>
     </row>
-    <row r="41" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A41" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
-        <v>1.1.1.1</v>
-      </c>
-      <c r="B41" s="82" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" s="81"/>
-      <c r="D41" s="79"/>
-      <c r="E41" s="100"/>
-      <c r="F41" s="101" t="str">
-        <f t="shared" si="36"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G41" s="62"/>
-      <c r="H41" s="63"/>
-      <c r="I41" s="80" t="str">
-        <f t="shared" si="37"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J41" s="99"/>
+    <row r="41" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="77"/>
+      <c r="C41" s="77"/>
+      <c r="D41" s="77"/>
+      <c r="E41" s="105"/>
+      <c r="F41" s="105"/>
+      <c r="G41" s="77"/>
+      <c r="H41" s="77"/>
+      <c r="I41" s="77"/>
+      <c r="J41" s="98"/>
       <c r="K41" s="107"/>
       <c r="L41" s="107"/>
       <c r="M41" s="107"/>
@@ -7805,85 +7902,402 @@
       <c r="BM41" s="107"/>
       <c r="BN41" s="107"/>
     </row>
-    <row r="42" spans="1:66" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="30"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="31"/>
-      <c r="I42" s="31"/>
-      <c r="J42" s="31"/>
-      <c r="K42" s="31"/>
-      <c r="L42" s="31"/>
-      <c r="M42" s="31"/>
-      <c r="N42" s="31"/>
-      <c r="O42" s="31"/>
-      <c r="P42" s="31"/>
-      <c r="Q42" s="31"/>
-      <c r="R42" s="31"/>
-      <c r="S42" s="31"/>
-      <c r="T42" s="31"/>
-      <c r="U42" s="31"/>
-      <c r="V42" s="31"/>
-      <c r="W42" s="31"/>
-      <c r="X42" s="31"/>
-      <c r="Y42" s="31"/>
-      <c r="Z42" s="31"/>
-      <c r="AA42" s="31"/>
-      <c r="AB42" s="31"/>
-      <c r="AC42" s="31"/>
-      <c r="AD42" s="31"/>
-      <c r="AE42" s="31"/>
-      <c r="AF42" s="31"/>
-      <c r="AG42" s="31"/>
-      <c r="AH42" s="31"/>
-      <c r="AI42" s="31"/>
-      <c r="AJ42" s="31"/>
-      <c r="AK42" s="31"/>
-      <c r="AL42" s="31"/>
-      <c r="AM42" s="31"/>
-      <c r="AN42" s="31"/>
-      <c r="AO42" s="31"/>
-      <c r="AP42" s="31"/>
-      <c r="AQ42" s="31"/>
-      <c r="AR42" s="31"/>
-      <c r="AS42" s="31"/>
-      <c r="AT42" s="31"/>
-      <c r="AU42" s="31"/>
-      <c r="AV42" s="31"/>
-      <c r="AW42" s="31"/>
-      <c r="AX42" s="31"/>
-      <c r="AY42" s="31"/>
-      <c r="AZ42" s="31"/>
-      <c r="BA42" s="31"/>
-      <c r="BB42" s="31"/>
-      <c r="BC42" s="31"/>
-      <c r="BD42" s="31"/>
-      <c r="BE42" s="31"/>
-      <c r="BF42" s="31"/>
-      <c r="BG42" s="31"/>
-      <c r="BH42" s="31"/>
-      <c r="BI42" s="31"/>
-      <c r="BJ42" s="31"/>
-      <c r="BK42" s="31"/>
-      <c r="BL42" s="31"/>
-      <c r="BM42" s="31"/>
-      <c r="BN42" s="31"/>
+    <row r="42" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="130" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>1</v>
+      </c>
+      <c r="B42" s="131" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="78"/>
+      <c r="D42" s="79"/>
+      <c r="E42" s="100"/>
+      <c r="F42" s="101" t="str">
+        <f t="shared" ref="F42:F45" si="40">IF(ISBLANK(E42)," - ",IF(G42=0,E42,E42+G42-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G42" s="62"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="80" t="str">
+        <f>IF(OR(F42=0,E42=0)," - ",NETWORKDAYS(E42,F42))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J42" s="99"/>
+      <c r="K42" s="107"/>
+      <c r="L42" s="107"/>
+      <c r="M42" s="107"/>
+      <c r="N42" s="107"/>
+      <c r="O42" s="107"/>
+      <c r="P42" s="107"/>
+      <c r="Q42" s="107"/>
+      <c r="R42" s="107"/>
+      <c r="S42" s="107"/>
+      <c r="T42" s="107"/>
+      <c r="U42" s="107"/>
+      <c r="V42" s="107"/>
+      <c r="W42" s="107"/>
+      <c r="X42" s="107"/>
+      <c r="Y42" s="107"/>
+      <c r="Z42" s="107"/>
+      <c r="AA42" s="107"/>
+      <c r="AB42" s="107"/>
+      <c r="AC42" s="107"/>
+      <c r="AD42" s="107"/>
+      <c r="AE42" s="107"/>
+      <c r="AF42" s="107"/>
+      <c r="AG42" s="107"/>
+      <c r="AH42" s="107"/>
+      <c r="AI42" s="107"/>
+      <c r="AJ42" s="107"/>
+      <c r="AK42" s="107"/>
+      <c r="AL42" s="107"/>
+      <c r="AM42" s="107"/>
+      <c r="AN42" s="107"/>
+      <c r="AO42" s="107"/>
+      <c r="AP42" s="107"/>
+      <c r="AQ42" s="107"/>
+      <c r="AR42" s="107"/>
+      <c r="AS42" s="107"/>
+      <c r="AT42" s="107"/>
+      <c r="AU42" s="107"/>
+      <c r="AV42" s="107"/>
+      <c r="AW42" s="107"/>
+      <c r="AX42" s="107"/>
+      <c r="AY42" s="107"/>
+      <c r="AZ42" s="107"/>
+      <c r="BA42" s="107"/>
+      <c r="BB42" s="107"/>
+      <c r="BC42" s="107"/>
+      <c r="BD42" s="107"/>
+      <c r="BE42" s="107"/>
+      <c r="BF42" s="107"/>
+      <c r="BG42" s="107"/>
+      <c r="BH42" s="107"/>
+      <c r="BI42" s="107"/>
+      <c r="BJ42" s="107"/>
+      <c r="BK42" s="107"/>
+      <c r="BL42" s="107"/>
+      <c r="BM42" s="107"/>
+      <c r="BN42" s="107"/>
+    </row>
+    <row r="43" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>1.1</v>
+      </c>
+      <c r="B43" s="81" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="81"/>
+      <c r="D43" s="79"/>
+      <c r="E43" s="100"/>
+      <c r="F43" s="101" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G43" s="62"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="80" t="str">
+        <f t="shared" ref="I43:I45" si="41">IF(OR(F43=0,E43=0)," - ",NETWORKDAYS(E43,F43))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J43" s="99"/>
+      <c r="K43" s="107"/>
+      <c r="L43" s="107"/>
+      <c r="M43" s="107"/>
+      <c r="N43" s="107"/>
+      <c r="O43" s="107"/>
+      <c r="P43" s="107"/>
+      <c r="Q43" s="107"/>
+      <c r="R43" s="107"/>
+      <c r="S43" s="107"/>
+      <c r="T43" s="107"/>
+      <c r="U43" s="107"/>
+      <c r="V43" s="107"/>
+      <c r="W43" s="107"/>
+      <c r="X43" s="107"/>
+      <c r="Y43" s="107"/>
+      <c r="Z43" s="107"/>
+      <c r="AA43" s="107"/>
+      <c r="AB43" s="107"/>
+      <c r="AC43" s="107"/>
+      <c r="AD43" s="107"/>
+      <c r="AE43" s="107"/>
+      <c r="AF43" s="107"/>
+      <c r="AG43" s="107"/>
+      <c r="AH43" s="107"/>
+      <c r="AI43" s="107"/>
+      <c r="AJ43" s="107"/>
+      <c r="AK43" s="107"/>
+      <c r="AL43" s="107"/>
+      <c r="AM43" s="107"/>
+      <c r="AN43" s="107"/>
+      <c r="AO43" s="107"/>
+      <c r="AP43" s="107"/>
+      <c r="AQ43" s="107"/>
+      <c r="AR43" s="107"/>
+      <c r="AS43" s="107"/>
+      <c r="AT43" s="107"/>
+      <c r="AU43" s="107"/>
+      <c r="AV43" s="107"/>
+      <c r="AW43" s="107"/>
+      <c r="AX43" s="107"/>
+      <c r="AY43" s="107"/>
+      <c r="AZ43" s="107"/>
+      <c r="BA43" s="107"/>
+      <c r="BB43" s="107"/>
+      <c r="BC43" s="107"/>
+      <c r="BD43" s="107"/>
+      <c r="BE43" s="107"/>
+      <c r="BF43" s="107"/>
+      <c r="BG43" s="107"/>
+      <c r="BH43" s="107"/>
+      <c r="BI43" s="107"/>
+      <c r="BJ43" s="107"/>
+      <c r="BK43" s="107"/>
+      <c r="BL43" s="107"/>
+      <c r="BM43" s="107"/>
+      <c r="BN43" s="107"/>
+    </row>
+    <row r="44" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <v>1.1.1</v>
+      </c>
+      <c r="B44" s="82" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="81"/>
+      <c r="D44" s="79"/>
+      <c r="E44" s="100"/>
+      <c r="F44" s="101" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G44" s="62"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="80" t="str">
+        <f t="shared" si="41"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J44" s="99"/>
+      <c r="K44" s="107"/>
+      <c r="L44" s="107"/>
+      <c r="M44" s="107"/>
+      <c r="N44" s="107"/>
+      <c r="O44" s="107"/>
+      <c r="P44" s="107"/>
+      <c r="Q44" s="107"/>
+      <c r="R44" s="107"/>
+      <c r="S44" s="107"/>
+      <c r="T44" s="107"/>
+      <c r="U44" s="107"/>
+      <c r="V44" s="107"/>
+      <c r="W44" s="107"/>
+      <c r="X44" s="107"/>
+      <c r="Y44" s="107"/>
+      <c r="Z44" s="107"/>
+      <c r="AA44" s="107"/>
+      <c r="AB44" s="107"/>
+      <c r="AC44" s="107"/>
+      <c r="AD44" s="107"/>
+      <c r="AE44" s="107"/>
+      <c r="AF44" s="107"/>
+      <c r="AG44" s="107"/>
+      <c r="AH44" s="107"/>
+      <c r="AI44" s="107"/>
+      <c r="AJ44" s="107"/>
+      <c r="AK44" s="107"/>
+      <c r="AL44" s="107"/>
+      <c r="AM44" s="107"/>
+      <c r="AN44" s="107"/>
+      <c r="AO44" s="107"/>
+      <c r="AP44" s="107"/>
+      <c r="AQ44" s="107"/>
+      <c r="AR44" s="107"/>
+      <c r="AS44" s="107"/>
+      <c r="AT44" s="107"/>
+      <c r="AU44" s="107"/>
+      <c r="AV44" s="107"/>
+      <c r="AW44" s="107"/>
+      <c r="AX44" s="107"/>
+      <c r="AY44" s="107"/>
+      <c r="AZ44" s="107"/>
+      <c r="BA44" s="107"/>
+      <c r="BB44" s="107"/>
+      <c r="BC44" s="107"/>
+      <c r="BD44" s="107"/>
+      <c r="BE44" s="107"/>
+      <c r="BF44" s="107"/>
+      <c r="BG44" s="107"/>
+      <c r="BH44" s="107"/>
+      <c r="BI44" s="107"/>
+      <c r="BJ44" s="107"/>
+      <c r="BK44" s="107"/>
+      <c r="BL44" s="107"/>
+      <c r="BM44" s="107"/>
+      <c r="BN44" s="107"/>
+    </row>
+    <row r="45" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
+        <v>1.1.1.1</v>
+      </c>
+      <c r="B45" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" s="81"/>
+      <c r="D45" s="79"/>
+      <c r="E45" s="100"/>
+      <c r="F45" s="101" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G45" s="62"/>
+      <c r="H45" s="63"/>
+      <c r="I45" s="80" t="str">
+        <f t="shared" si="41"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J45" s="99"/>
+      <c r="K45" s="107"/>
+      <c r="L45" s="107"/>
+      <c r="M45" s="107"/>
+      <c r="N45" s="107"/>
+      <c r="O45" s="107"/>
+      <c r="P45" s="107"/>
+      <c r="Q45" s="107"/>
+      <c r="R45" s="107"/>
+      <c r="S45" s="107"/>
+      <c r="T45" s="107"/>
+      <c r="U45" s="107"/>
+      <c r="V45" s="107"/>
+      <c r="W45" s="107"/>
+      <c r="X45" s="107"/>
+      <c r="Y45" s="107"/>
+      <c r="Z45" s="107"/>
+      <c r="AA45" s="107"/>
+      <c r="AB45" s="107"/>
+      <c r="AC45" s="107"/>
+      <c r="AD45" s="107"/>
+      <c r="AE45" s="107"/>
+      <c r="AF45" s="107"/>
+      <c r="AG45" s="107"/>
+      <c r="AH45" s="107"/>
+      <c r="AI45" s="107"/>
+      <c r="AJ45" s="107"/>
+      <c r="AK45" s="107"/>
+      <c r="AL45" s="107"/>
+      <c r="AM45" s="107"/>
+      <c r="AN45" s="107"/>
+      <c r="AO45" s="107"/>
+      <c r="AP45" s="107"/>
+      <c r="AQ45" s="107"/>
+      <c r="AR45" s="107"/>
+      <c r="AS45" s="107"/>
+      <c r="AT45" s="107"/>
+      <c r="AU45" s="107"/>
+      <c r="AV45" s="107"/>
+      <c r="AW45" s="107"/>
+      <c r="AX45" s="107"/>
+      <c r="AY45" s="107"/>
+      <c r="AZ45" s="107"/>
+      <c r="BA45" s="107"/>
+      <c r="BB45" s="107"/>
+      <c r="BC45" s="107"/>
+      <c r="BD45" s="107"/>
+      <c r="BE45" s="107"/>
+      <c r="BF45" s="107"/>
+      <c r="BG45" s="107"/>
+      <c r="BH45" s="107"/>
+      <c r="BI45" s="107"/>
+      <c r="BJ45" s="107"/>
+      <c r="BK45" s="107"/>
+      <c r="BL45" s="107"/>
+      <c r="BM45" s="107"/>
+      <c r="BN45" s="107"/>
+    </row>
+    <row r="46" spans="1:66" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="30"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="31"/>
+      <c r="H46" s="31"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
+      <c r="K46" s="31"/>
+      <c r="L46" s="31"/>
+      <c r="M46" s="31"/>
+      <c r="N46" s="31"/>
+      <c r="O46" s="31"/>
+      <c r="P46" s="31"/>
+      <c r="Q46" s="31"/>
+      <c r="R46" s="31"/>
+      <c r="S46" s="31"/>
+      <c r="T46" s="31"/>
+      <c r="U46" s="31"/>
+      <c r="V46" s="31"/>
+      <c r="W46" s="31"/>
+      <c r="X46" s="31"/>
+      <c r="Y46" s="31"/>
+      <c r="Z46" s="31"/>
+      <c r="AA46" s="31"/>
+      <c r="AB46" s="31"/>
+      <c r="AC46" s="31"/>
+      <c r="AD46" s="31"/>
+      <c r="AE46" s="31"/>
+      <c r="AF46" s="31"/>
+      <c r="AG46" s="31"/>
+      <c r="AH46" s="31"/>
+      <c r="AI46" s="31"/>
+      <c r="AJ46" s="31"/>
+      <c r="AK46" s="31"/>
+      <c r="AL46" s="31"/>
+      <c r="AM46" s="31"/>
+      <c r="AN46" s="31"/>
+      <c r="AO46" s="31"/>
+      <c r="AP46" s="31"/>
+      <c r="AQ46" s="31"/>
+      <c r="AR46" s="31"/>
+      <c r="AS46" s="31"/>
+      <c r="AT46" s="31"/>
+      <c r="AU46" s="31"/>
+      <c r="AV46" s="31"/>
+      <c r="AW46" s="31"/>
+      <c r="AX46" s="31"/>
+      <c r="AY46" s="31"/>
+      <c r="AZ46" s="31"/>
+      <c r="BA46" s="31"/>
+      <c r="BB46" s="31"/>
+      <c r="BC46" s="31"/>
+      <c r="BD46" s="31"/>
+      <c r="BE46" s="31"/>
+      <c r="BF46" s="31"/>
+      <c r="BG46" s="31"/>
+      <c r="BH46" s="31"/>
+      <c r="BI46" s="31"/>
+      <c r="BJ46" s="31"/>
+      <c r="BK46" s="31"/>
+      <c r="BL46" s="31"/>
+      <c r="BM46" s="31"/>
+      <c r="BN46" s="31"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="27">
-    <mergeCell ref="CJ4:CP4"/>
-    <mergeCell ref="CJ5:CP5"/>
-    <mergeCell ref="BO5:BU5"/>
-    <mergeCell ref="BO4:BU4"/>
-    <mergeCell ref="BV4:CB4"/>
-    <mergeCell ref="BV5:CB5"/>
-    <mergeCell ref="CC4:CI4"/>
-    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -7894,19 +8308,18 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="CJ4:CP4"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BO4:BU4"/>
+    <mergeCell ref="BV4:CB4"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="CC5:CI5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H8:H41">
-    <cfRule type="dataBar" priority="10">
+  <conditionalFormatting sqref="H8:H27 H38:H45">
+    <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7920,61 +8333,126 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN7">
-    <cfRule type="expression" dxfId="11" priority="53">
+    <cfRule type="expression" dxfId="16" priority="65">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BN41">
-    <cfRule type="expression" dxfId="10" priority="56">
+  <conditionalFormatting sqref="K8:BN27 K32:BN45">
+    <cfRule type="expression" dxfId="15" priority="68">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="57">
+    <cfRule type="expression" dxfId="14" priority="69">
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:BN41">
-    <cfRule type="expression" dxfId="8" priority="16">
+  <conditionalFormatting sqref="K6:BN27 K38:BN45">
+    <cfRule type="expression" dxfId="13" priority="28">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO6:BU7">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="12" priority="20">
       <formula>BO$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO6:BU7">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="11" priority="19">
       <formula>BO$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV6:CB7">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="10" priority="18">
       <formula>BV$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV6:CB7">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="9" priority="17">
       <formula>BV$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC6:CI7">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="8" priority="16">
       <formula>CC$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC6:CI7">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="7" priority="15">
       <formula>CC$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ6:CP7">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="6" priority="14">
       <formula>CJ$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ6:CP7">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="5" priority="13">
       <formula>CJ$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28:H31">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{39DD3482-289E-4C59-8060-F014DFA1AD27}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K28:BN31">
+    <cfRule type="expression" dxfId="4" priority="11">
+      <formula>AND($E28&lt;=K$6,ROUNDDOWN(($F28-$E28+1)*$H28,0)+$E28-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="12">
+      <formula>AND(NOT(ISBLANK($E28)),$E28&lt;=K$6,$F28&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K28:BN31">
+    <cfRule type="expression" dxfId="2" priority="10">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32:H35">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{77E327D2-3825-42D2-A5BB-1041E338E7F5}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36:H37">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C53DBB2B-7B66-4016-AEA3-0CABB39E0149}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K36:BN37">
+    <cfRule type="expression" dxfId="1" priority="6">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K32:BN35">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
@@ -7987,8 +8465,8 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 A34:B35 B29 B30:B32 A37:B37 B36 E16 E22 E28 E34:H37 G14 G11 G16:H16 G22:H22 G28:H32 G38 G39:G40 G41 H23:H26" unlockedFormula="1"/>
-    <ignoredError sqref="A28 A22 A16" formula="1"/>
+    <ignoredError sqref="H9 A38:B39 A41:B41 B40 E16 E22 E38:H41 G14 G11 G16:H16 G22:H22 G42 G43:G44 G45 H23:H26" unlockedFormula="1"/>
+    <ignoredError sqref="A22 A16" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
@@ -8004,11 +8482,11 @@
                     <xdr:col>9</xdr:col>
                     <xdr:colOff>95250</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>127000</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>27</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>114300</xdr:rowOff>
                   </to>
@@ -8036,7 +8514,52 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H8:H41</xm:sqref>
+          <xm:sqref>H8:H27 H38:H45</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{39DD3482-289E-4C59-8060-F014DFA1AD27}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H28:H31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{77E327D2-3825-42D2-A5BB-1041E338E7F5}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H32:H35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C53DBB2B-7B66-4016-AEA3-0CABB39E0149}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H36:H37</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -8055,177 +8578,177 @@
       <selection activeCell="A16" sqref="A16:C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" style="16" customWidth="1"/>
-    <col min="3" max="3" width="55.140625" style="16" customWidth="1"/>
-    <col min="4" max="7" width="8.85546875" style="16"/>
+    <col min="1" max="1" width="5.54296875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="37.7265625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="55.1796875" style="16" customWidth="1"/>
+    <col min="4" max="7" width="8.81640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="C4" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="20"/>
+    </row>
+    <row r="7" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="C7" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="C13" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="B18" s="26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B22" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B26" s="26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="B34" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="B39" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B42" s="26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:2" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="B46" s="24" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C4" s="23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C5" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C6" s="20"/>
-    </row>
-    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="C7" s="24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C8" s="25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C10" s="20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C11" s="20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="C13" s="24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B18" s="26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B22" s="26" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B26" s="26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B29" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B30" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B31" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B32" s="16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B34" s="26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" s="20" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" s="20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B39" s="26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B42" s="26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="20" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="2:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="B46" s="24" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -8249,511 +8772,511 @@
       <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="90.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="7"/>
+    <col min="1" max="1" width="5.54296875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="90.453125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="42"/>
     </row>
-    <row r="2" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="138" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="8"/>
     </row>
-    <row r="3" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="9"/>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A4" s="133" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="39"/>
+    </row>
+    <row r="5" spans="1:3" s="8" customFormat="1" ht="56" x14ac:dyDescent="0.3">
+      <c r="B5" s="139" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28" x14ac:dyDescent="0.3">
+      <c r="B7" s="139" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="39"/>
-    </row>
-    <row r="5" spans="1:3" s="8" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="B5" s="139" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B7" s="139" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.3">
       <c r="B9" s="138" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28" x14ac:dyDescent="0.3">
+      <c r="B11" s="137" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B11" s="137" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A13" s="172" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="172"/>
     </row>
-    <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:3" s="134" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:3" s="134" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A15" s="142"/>
       <c r="B15" s="140" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="134" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="134" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A16" s="142"/>
       <c r="B16" s="141" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="136" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A17" s="143"/>
       <c r="B17" s="141" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="20" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A18" s="143"/>
       <c r="B18" s="141" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="42" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A19" s="146"/>
       <c r="B19" s="141" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="134" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="134" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A20" s="142"/>
       <c r="B20" s="140" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" s="135" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A21" s="143"/>
       <c r="B21" s="141" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A22" s="144"/>
       <c r="B22" s="145" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A23" s="144"/>
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A24" s="172" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24" s="172"/>
     </row>
-    <row r="25" spans="1:3" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" s="8" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A25" s="144"/>
       <c r="B25" s="141" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A26" s="144"/>
       <c r="B26" s="141"/>
     </row>
-    <row r="27" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A27" s="144"/>
       <c r="B27" s="162" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A28" s="144"/>
       <c r="B28" s="141" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A29" s="144"/>
       <c r="B29" s="141" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A30" s="144"/>
       <c r="B30" s="141"/>
     </row>
-    <row r="31" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A31" s="144"/>
       <c r="B31" s="162" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A32" s="144"/>
       <c r="B32" s="141" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A33" s="144"/>
       <c r="B33" s="141" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A34" s="144"/>
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A35" s="144"/>
       <c r="B35" s="141" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A36" s="144"/>
       <c r="B36" s="147" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A37" s="144"/>
       <c r="B37" s="10"/>
     </row>
-    <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A38" s="172" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B38" s="172"/>
     </row>
-    <row r="39" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" ht="28" x14ac:dyDescent="0.25">
       <c r="B39" s="141" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:2" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.25">
+      <c r="B41" s="141" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:2" s="20" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B41" s="141" t="s">
+    <row r="42" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:2" s="20" customFormat="1" ht="28" x14ac:dyDescent="0.25">
+      <c r="B43" s="141" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:2" ht="28" x14ac:dyDescent="0.25">
+      <c r="B45" s="141" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:2" s="20" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B43" s="141" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B45" s="141" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="21"/>
+    </row>
+    <row r="47" spans="1:2" ht="28" x14ac:dyDescent="0.25">
+      <c r="B47" s="141" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="21"/>
-    </row>
-    <row r="47" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B47" s="141" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" s="11"/>
     </row>
-    <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A49" s="172" t="s">
         <v>7</v>
       </c>
       <c r="B49" s="172"/>
     </row>
-    <row r="50" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" ht="28" x14ac:dyDescent="0.25">
       <c r="B50" s="141" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B51" s="11"/>
     </row>
-    <row r="52" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A52" s="148" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="B52" s="141" t="s">
+    </row>
+    <row r="53" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="A53" s="148" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A53" s="148" t="s">
+      <c r="B53" s="141" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="141" t="s">
+    </row>
+    <row r="54" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="A54" s="148" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A54" s="148" t="s">
+      <c r="B54" s="141" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="141" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:2" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A55" s="137"/>
       <c r="B55" s="141" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A56" s="137"/>
       <c r="B56" s="141" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A57" s="148" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="B57" s="141" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A58" s="137"/>
       <c r="B58" s="141" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A59" s="137"/>
       <c r="B59" s="141" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A60" s="148" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="B60" s="141" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:2" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A61" s="137"/>
       <c r="B61" s="141" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="A62" s="148" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A62" s="148" t="s">
+      <c r="B62" s="141" t="s">
         <v>110</v>
       </c>
-      <c r="B62" s="141" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A63" s="149"/>
       <c r="B63" s="141" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="12"/>
+    </row>
+    <row r="65" spans="1:2" s="20" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A65" s="172" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65" s="172"/>
+    </row>
+    <row r="66" spans="1:2" s="20" customFormat="1" ht="42" x14ac:dyDescent="0.25">
+      <c r="B66" s="141" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="12"/>
-    </row>
-    <row r="65" spans="1:2" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A65" s="172" t="s">
-        <v>10</v>
-      </c>
-      <c r="B65" s="172"/>
-    </row>
-    <row r="66" spans="1:2" s="20" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="B66" s="141" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="13"/>
     </row>
-    <row r="68" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A68" s="172" t="s">
         <v>5</v>
       </c>
       <c r="B68" s="172"/>
     </row>
-    <row r="69" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A69" s="156" t="s">
         <v>6</v>
       </c>
       <c r="B69" s="157" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A70" s="150"/>
       <c r="B70" s="155" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A71" s="150"/>
       <c r="B71" s="151"/>
     </row>
-    <row r="72" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A72" s="156" t="s">
         <v>6</v>
       </c>
       <c r="B72" s="157" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A73" s="150"/>
       <c r="B73" s="155" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A74" s="150"/>
       <c r="B74" s="151"/>
     </row>
-    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A75" s="156" t="s">
         <v>6</v>
       </c>
       <c r="B75" s="159" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" s="8" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A76" s="150"/>
       <c r="B76" s="139" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A77" s="149"/>
       <c r="B77" s="149"/>
     </row>
-    <row r="78" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A78" s="156" t="s">
         <v>6</v>
       </c>
       <c r="B78" s="159" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A79" s="150"/>
       <c r="B79" s="139" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" s="20" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A80" s="149"/>
       <c r="B80" s="149"/>
     </row>
-    <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A81" s="156" t="s">
         <v>6</v>
       </c>
       <c r="B81" s="159" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A82" s="150"/>
       <c r="B82" s="154" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A83" s="150"/>
       <c r="B83" s="154" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A84" s="150"/>
       <c r="B84" s="154" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A85" s="149"/>
       <c r="B85" s="153"/>
     </row>
-    <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A86" s="156" t="s">
         <v>6</v>
       </c>
       <c r="B86" s="159" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" s="8" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A87" s="150"/>
       <c r="B87" s="139" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A88" s="150"/>
       <c r="B88" s="152" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" s="8" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" s="8" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A89" s="150"/>
       <c r="B89" s="158" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A90" s="149"/>
       <c r="B90" s="149"/>
     </row>
-    <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A91" s="156" t="s">
         <v>6</v>
       </c>
       <c r="B91" s="161" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="28" x14ac:dyDescent="0.3">
       <c r="A92" s="137"/>
       <c r="B92" s="154" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -8787,178 +9310,178 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="20" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="16"/>
+    <col min="1" max="1" width="5.54296875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="20" customWidth="1"/>
+    <col min="3" max="16384" width="8.81640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="45"/>
       <c r="D1" s="45"/>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="42"/>
       <c r="B2" s="46"/>
       <c r="C2" s="45"/>
       <c r="D2" s="45"/>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="43"/>
       <c r="B3" s="36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="44"/>
     </row>
-    <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="15"/>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="14"/>
       <c r="B5" s="17"/>
       <c r="C5" s="15"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="15"/>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="14"/>
       <c r="B7" s="17"/>
       <c r="C7" s="15"/>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="14"/>
       <c r="B8" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="14"/>
       <c r="B9" s="17"/>
       <c r="C9" s="15"/>
     </row>
-    <row r="10" spans="1:4" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A10" s="14"/>
       <c r="B10" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="15"/>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="14"/>
       <c r="B11" s="17"/>
       <c r="C11" s="15"/>
     </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A12" s="14"/>
       <c r="B12" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="15"/>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="14"/>
       <c r="B13" s="17"/>
       <c r="C13" s="15"/>
     </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="62" x14ac:dyDescent="0.35">
       <c r="A14" s="14"/>
       <c r="B14" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="14"/>
       <c r="B15" s="17"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:4" ht="30.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="14"/>
       <c r="B16" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="14"/>
       <c r="B17" s="17"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="14"/>
       <c r="B18" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="14"/>
       <c r="B19" s="37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="14"/>
       <c r="B20" s="19"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>

</xml_diff>

<commit_message>
Pins Update for I2C Protocol
</commit_message>
<xml_diff>
--- a/Gantt_Diagram_Robot_Project_2018.xlsx
+++ b/Gantt_Diagram_Robot_Project_2018.xlsx
@@ -442,7 +442,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="163">
   <si>
     <t>WBS</t>
   </si>
@@ -1571,9 +1571,6 @@
   </si>
   <si>
     <t>Proportional correction</t>
-  </si>
-  <si>
-    <t>M.Amine Gaizi</t>
   </si>
   <si>
     <t>Gyroscope/Accelerometer</t>
@@ -2945,6 +2942,24 @@
     </xf>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2952,27 +2967,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3896,8 +3893,8 @@
   <dimension ref="A1:CP42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BO23" sqref="BO23"/>
+      <pane ySplit="7" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3949,29 +3946,29 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
       <c r="I1" s="132"/>
-      <c r="K1" s="163" t="s">
+      <c r="K1" s="169" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
-      <c r="P1" s="163"/>
-      <c r="Q1" s="163"/>
-      <c r="R1" s="163"/>
-      <c r="S1" s="163"/>
-      <c r="T1" s="163"/>
-      <c r="U1" s="163"/>
-      <c r="V1" s="163"/>
-      <c r="W1" s="163"/>
-      <c r="X1" s="163"/>
-      <c r="Y1" s="163"/>
-      <c r="Z1" s="163"/>
-      <c r="AA1" s="163"/>
-      <c r="AB1" s="163"/>
-      <c r="AC1" s="163"/>
-      <c r="AD1" s="163"/>
-      <c r="AE1" s="163"/>
+      <c r="L1" s="169"/>
+      <c r="M1" s="169"/>
+      <c r="N1" s="169"/>
+      <c r="O1" s="169"/>
+      <c r="P1" s="169"/>
+      <c r="Q1" s="169"/>
+      <c r="R1" s="169"/>
+      <c r="S1" s="169"/>
+      <c r="T1" s="169"/>
+      <c r="U1" s="169"/>
+      <c r="V1" s="169"/>
+      <c r="W1" s="169"/>
+      <c r="X1" s="169"/>
+      <c r="Y1" s="169"/>
+      <c r="Z1" s="169"/>
+      <c r="AA1" s="169"/>
+      <c r="AB1" s="169"/>
+      <c r="AC1" s="169"/>
+      <c r="AD1" s="169"/>
+      <c r="AE1" s="169"/>
     </row>
     <row r="2" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
@@ -4016,11 +4013,11 @@
       <c r="B4" s="114" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="168">
+      <c r="C4" s="171">
         <v>43340</v>
       </c>
-      <c r="D4" s="168"/>
-      <c r="E4" s="168"/>
+      <c r="D4" s="171"/>
+      <c r="E4" s="171"/>
       <c r="F4" s="111"/>
       <c r="G4" s="114" t="s">
         <v>75</v>
@@ -4030,262 +4027,262 @@
       </c>
       <c r="I4" s="112"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="165" t="str">
+      <c r="K4" s="163" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="166"/>
-      <c r="M4" s="166"/>
-      <c r="N4" s="166"/>
-      <c r="O4" s="166"/>
-      <c r="P4" s="166"/>
-      <c r="Q4" s="167"/>
-      <c r="R4" s="165" t="str">
+      <c r="L4" s="164"/>
+      <c r="M4" s="164"/>
+      <c r="N4" s="164"/>
+      <c r="O4" s="164"/>
+      <c r="P4" s="164"/>
+      <c r="Q4" s="165"/>
+      <c r="R4" s="163" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="166"/>
-      <c r="T4" s="166"/>
-      <c r="U4" s="166"/>
-      <c r="V4" s="166"/>
-      <c r="W4" s="166"/>
-      <c r="X4" s="167"/>
-      <c r="Y4" s="165" t="str">
+      <c r="S4" s="164"/>
+      <c r="T4" s="164"/>
+      <c r="U4" s="164"/>
+      <c r="V4" s="164"/>
+      <c r="W4" s="164"/>
+      <c r="X4" s="165"/>
+      <c r="Y4" s="163" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="166"/>
-      <c r="AA4" s="166"/>
-      <c r="AB4" s="166"/>
-      <c r="AC4" s="166"/>
-      <c r="AD4" s="166"/>
-      <c r="AE4" s="167"/>
-      <c r="AF4" s="165" t="str">
+      <c r="Z4" s="164"/>
+      <c r="AA4" s="164"/>
+      <c r="AB4" s="164"/>
+      <c r="AC4" s="164"/>
+      <c r="AD4" s="164"/>
+      <c r="AE4" s="165"/>
+      <c r="AF4" s="163" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="166"/>
-      <c r="AH4" s="166"/>
-      <c r="AI4" s="166"/>
-      <c r="AJ4" s="166"/>
-      <c r="AK4" s="166"/>
-      <c r="AL4" s="167"/>
-      <c r="AM4" s="165" t="str">
+      <c r="AG4" s="164"/>
+      <c r="AH4" s="164"/>
+      <c r="AI4" s="164"/>
+      <c r="AJ4" s="164"/>
+      <c r="AK4" s="164"/>
+      <c r="AL4" s="165"/>
+      <c r="AM4" s="163" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="166"/>
-      <c r="AO4" s="166"/>
-      <c r="AP4" s="166"/>
-      <c r="AQ4" s="166"/>
-      <c r="AR4" s="166"/>
-      <c r="AS4" s="167"/>
-      <c r="AT4" s="165" t="str">
+      <c r="AN4" s="164"/>
+      <c r="AO4" s="164"/>
+      <c r="AP4" s="164"/>
+      <c r="AQ4" s="164"/>
+      <c r="AR4" s="164"/>
+      <c r="AS4" s="165"/>
+      <c r="AT4" s="163" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="166"/>
-      <c r="AV4" s="166"/>
-      <c r="AW4" s="166"/>
-      <c r="AX4" s="166"/>
-      <c r="AY4" s="166"/>
-      <c r="AZ4" s="167"/>
-      <c r="BA4" s="165" t="str">
+      <c r="AU4" s="164"/>
+      <c r="AV4" s="164"/>
+      <c r="AW4" s="164"/>
+      <c r="AX4" s="164"/>
+      <c r="AY4" s="164"/>
+      <c r="AZ4" s="165"/>
+      <c r="BA4" s="163" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="166"/>
-      <c r="BC4" s="166"/>
-      <c r="BD4" s="166"/>
-      <c r="BE4" s="166"/>
-      <c r="BF4" s="166"/>
-      <c r="BG4" s="167"/>
-      <c r="BH4" s="165" t="str">
+      <c r="BB4" s="164"/>
+      <c r="BC4" s="164"/>
+      <c r="BD4" s="164"/>
+      <c r="BE4" s="164"/>
+      <c r="BF4" s="164"/>
+      <c r="BG4" s="165"/>
+      <c r="BH4" s="163" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="166"/>
-      <c r="BJ4" s="166"/>
-      <c r="BK4" s="166"/>
-      <c r="BL4" s="166"/>
-      <c r="BM4" s="166"/>
-      <c r="BN4" s="167"/>
-      <c r="BO4" s="165" t="str">
+      <c r="BI4" s="164"/>
+      <c r="BJ4" s="164"/>
+      <c r="BK4" s="164"/>
+      <c r="BL4" s="164"/>
+      <c r="BM4" s="164"/>
+      <c r="BN4" s="165"/>
+      <c r="BO4" s="163" t="str">
         <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="BP4" s="166"/>
-      <c r="BQ4" s="166"/>
-      <c r="BR4" s="166"/>
-      <c r="BS4" s="166"/>
-      <c r="BT4" s="166"/>
-      <c r="BU4" s="167"/>
-      <c r="BV4" s="165" t="str">
+      <c r="BP4" s="164"/>
+      <c r="BQ4" s="164"/>
+      <c r="BR4" s="164"/>
+      <c r="BS4" s="164"/>
+      <c r="BT4" s="164"/>
+      <c r="BU4" s="165"/>
+      <c r="BV4" s="163" t="str">
         <f>"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="BW4" s="166"/>
-      <c r="BX4" s="166"/>
-      <c r="BY4" s="166"/>
-      <c r="BZ4" s="166"/>
-      <c r="CA4" s="166"/>
-      <c r="CB4" s="167"/>
-      <c r="CC4" s="165" t="str">
+      <c r="BW4" s="164"/>
+      <c r="BX4" s="164"/>
+      <c r="BY4" s="164"/>
+      <c r="BZ4" s="164"/>
+      <c r="CA4" s="164"/>
+      <c r="CB4" s="165"/>
+      <c r="CC4" s="163" t="str">
         <f>"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="CD4" s="166"/>
-      <c r="CE4" s="166"/>
-      <c r="CF4" s="166"/>
-      <c r="CG4" s="166"/>
-      <c r="CH4" s="166"/>
-      <c r="CI4" s="167"/>
-      <c r="CJ4" s="165" t="str">
+      <c r="CD4" s="164"/>
+      <c r="CE4" s="164"/>
+      <c r="CF4" s="164"/>
+      <c r="CG4" s="164"/>
+      <c r="CH4" s="164"/>
+      <c r="CI4" s="165"/>
+      <c r="CJ4" s="163" t="str">
         <f>"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="CK4" s="166"/>
-      <c r="CL4" s="166"/>
-      <c r="CM4" s="166"/>
-      <c r="CN4" s="166"/>
-      <c r="CO4" s="166"/>
-      <c r="CP4" s="167"/>
+      <c r="CK4" s="164"/>
+      <c r="CL4" s="164"/>
+      <c r="CM4" s="164"/>
+      <c r="CN4" s="164"/>
+      <c r="CO4" s="164"/>
+      <c r="CP4" s="165"/>
     </row>
     <row r="5" spans="1:94" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="110"/>
       <c r="B5" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="164" t="s">
+      <c r="C5" s="170" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="164"/>
-      <c r="E5" s="164"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
       <c r="F5" s="113"/>
       <c r="G5" s="113"/>
       <c r="H5" s="113"/>
       <c r="I5" s="113"/>
       <c r="J5" s="50"/>
-      <c r="K5" s="169">
+      <c r="K5" s="166">
         <f>K6</f>
         <v>43339</v>
       </c>
-      <c r="L5" s="170"/>
-      <c r="M5" s="170"/>
-      <c r="N5" s="170"/>
-      <c r="O5" s="170"/>
-      <c r="P5" s="170"/>
-      <c r="Q5" s="171"/>
-      <c r="R5" s="169">
+      <c r="L5" s="167"/>
+      <c r="M5" s="167"/>
+      <c r="N5" s="167"/>
+      <c r="O5" s="167"/>
+      <c r="P5" s="167"/>
+      <c r="Q5" s="168"/>
+      <c r="R5" s="166">
         <f>R6</f>
         <v>43346</v>
       </c>
-      <c r="S5" s="170"/>
-      <c r="T5" s="170"/>
-      <c r="U5" s="170"/>
-      <c r="V5" s="170"/>
-      <c r="W5" s="170"/>
-      <c r="X5" s="171"/>
-      <c r="Y5" s="169">
+      <c r="S5" s="167"/>
+      <c r="T5" s="167"/>
+      <c r="U5" s="167"/>
+      <c r="V5" s="167"/>
+      <c r="W5" s="167"/>
+      <c r="X5" s="168"/>
+      <c r="Y5" s="166">
         <f>Y6</f>
         <v>43353</v>
       </c>
-      <c r="Z5" s="170"/>
-      <c r="AA5" s="170"/>
-      <c r="AB5" s="170"/>
-      <c r="AC5" s="170"/>
-      <c r="AD5" s="170"/>
-      <c r="AE5" s="171"/>
-      <c r="AF5" s="169">
+      <c r="Z5" s="167"/>
+      <c r="AA5" s="167"/>
+      <c r="AB5" s="167"/>
+      <c r="AC5" s="167"/>
+      <c r="AD5" s="167"/>
+      <c r="AE5" s="168"/>
+      <c r="AF5" s="166">
         <f>AF6</f>
         <v>43360</v>
       </c>
-      <c r="AG5" s="170"/>
-      <c r="AH5" s="170"/>
-      <c r="AI5" s="170"/>
-      <c r="AJ5" s="170"/>
-      <c r="AK5" s="170"/>
-      <c r="AL5" s="171"/>
-      <c r="AM5" s="169">
+      <c r="AG5" s="167"/>
+      <c r="AH5" s="167"/>
+      <c r="AI5" s="167"/>
+      <c r="AJ5" s="167"/>
+      <c r="AK5" s="167"/>
+      <c r="AL5" s="168"/>
+      <c r="AM5" s="166">
         <f>AM6</f>
         <v>43367</v>
       </c>
-      <c r="AN5" s="170"/>
-      <c r="AO5" s="170"/>
-      <c r="AP5" s="170"/>
-      <c r="AQ5" s="170"/>
-      <c r="AR5" s="170"/>
-      <c r="AS5" s="171"/>
-      <c r="AT5" s="169">
+      <c r="AN5" s="167"/>
+      <c r="AO5" s="167"/>
+      <c r="AP5" s="167"/>
+      <c r="AQ5" s="167"/>
+      <c r="AR5" s="167"/>
+      <c r="AS5" s="168"/>
+      <c r="AT5" s="166">
         <f>AT6</f>
         <v>43374</v>
       </c>
-      <c r="AU5" s="170"/>
-      <c r="AV5" s="170"/>
-      <c r="AW5" s="170"/>
-      <c r="AX5" s="170"/>
-      <c r="AY5" s="170"/>
-      <c r="AZ5" s="171"/>
-      <c r="BA5" s="169">
+      <c r="AU5" s="167"/>
+      <c r="AV5" s="167"/>
+      <c r="AW5" s="167"/>
+      <c r="AX5" s="167"/>
+      <c r="AY5" s="167"/>
+      <c r="AZ5" s="168"/>
+      <c r="BA5" s="166">
         <f>BA6</f>
         <v>43381</v>
       </c>
-      <c r="BB5" s="170"/>
-      <c r="BC5" s="170"/>
-      <c r="BD5" s="170"/>
-      <c r="BE5" s="170"/>
-      <c r="BF5" s="170"/>
-      <c r="BG5" s="171"/>
-      <c r="BH5" s="169">
+      <c r="BB5" s="167"/>
+      <c r="BC5" s="167"/>
+      <c r="BD5" s="167"/>
+      <c r="BE5" s="167"/>
+      <c r="BF5" s="167"/>
+      <c r="BG5" s="168"/>
+      <c r="BH5" s="166">
         <f>BH6</f>
         <v>43388</v>
       </c>
-      <c r="BI5" s="170"/>
-      <c r="BJ5" s="170"/>
-      <c r="BK5" s="170"/>
-      <c r="BL5" s="170"/>
-      <c r="BM5" s="170"/>
-      <c r="BN5" s="171"/>
-      <c r="BO5" s="169">
+      <c r="BI5" s="167"/>
+      <c r="BJ5" s="167"/>
+      <c r="BK5" s="167"/>
+      <c r="BL5" s="167"/>
+      <c r="BM5" s="167"/>
+      <c r="BN5" s="168"/>
+      <c r="BO5" s="166">
         <f>BO6</f>
         <v>43395</v>
       </c>
-      <c r="BP5" s="170"/>
-      <c r="BQ5" s="170"/>
-      <c r="BR5" s="170"/>
-      <c r="BS5" s="170"/>
-      <c r="BT5" s="170"/>
-      <c r="BU5" s="171"/>
-      <c r="BV5" s="169">
+      <c r="BP5" s="167"/>
+      <c r="BQ5" s="167"/>
+      <c r="BR5" s="167"/>
+      <c r="BS5" s="167"/>
+      <c r="BT5" s="167"/>
+      <c r="BU5" s="168"/>
+      <c r="BV5" s="166">
         <f>BV6</f>
         <v>43402</v>
       </c>
-      <c r="BW5" s="170"/>
-      <c r="BX5" s="170"/>
-      <c r="BY5" s="170"/>
-      <c r="BZ5" s="170"/>
-      <c r="CA5" s="170"/>
-      <c r="CB5" s="171"/>
-      <c r="CC5" s="169">
+      <c r="BW5" s="167"/>
+      <c r="BX5" s="167"/>
+      <c r="BY5" s="167"/>
+      <c r="BZ5" s="167"/>
+      <c r="CA5" s="167"/>
+      <c r="CB5" s="168"/>
+      <c r="CC5" s="166">
         <f>CC6</f>
         <v>43409</v>
       </c>
-      <c r="CD5" s="170"/>
-      <c r="CE5" s="170"/>
-      <c r="CF5" s="170"/>
-      <c r="CG5" s="170"/>
-      <c r="CH5" s="170"/>
-      <c r="CI5" s="171"/>
-      <c r="CJ5" s="169">
+      <c r="CD5" s="167"/>
+      <c r="CE5" s="167"/>
+      <c r="CF5" s="167"/>
+      <c r="CG5" s="167"/>
+      <c r="CH5" s="167"/>
+      <c r="CI5" s="168"/>
+      <c r="CJ5" s="166">
         <f>CJ6</f>
         <v>43416</v>
       </c>
-      <c r="CK5" s="170"/>
-      <c r="CL5" s="170"/>
-      <c r="CM5" s="170"/>
-      <c r="CN5" s="170"/>
-      <c r="CO5" s="170"/>
-      <c r="CP5" s="171"/>
+      <c r="CK5" s="167"/>
+      <c r="CL5" s="167"/>
+      <c r="CM5" s="167"/>
+      <c r="CN5" s="167"/>
+      <c r="CO5" s="167"/>
+      <c r="CP5" s="168"/>
     </row>
     <row r="6" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A6" s="49"/>
@@ -5947,7 +5944,7 @@
         <v>156</v>
       </c>
       <c r="C19" s="61" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D19" s="127"/>
       <c r="E19" s="100">
@@ -6202,7 +6199,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="54" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D22" s="56"/>
       <c r="E22" s="102"/>
@@ -6280,10 +6277,10 @@
         <v>3.1</v>
       </c>
       <c r="B23" s="126" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C23" s="61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D23" s="127"/>
       <c r="E23" s="100">
@@ -6367,10 +6364,10 @@
         <v>3.2</v>
       </c>
       <c r="B24" s="126" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C24" s="61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D24" s="127"/>
       <c r="E24" s="100">
@@ -6454,10 +6451,10 @@
         <v>3.3</v>
       </c>
       <c r="B25" s="126" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C25" s="61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D25" s="127"/>
       <c r="E25" s="100">
@@ -6541,10 +6538,10 @@
         <v>3.4</v>
       </c>
       <c r="B26" s="126" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" s="61" t="s">
         <v>162</v>
-      </c>
-      <c r="C26" s="61" t="s">
-        <v>163</v>
       </c>
       <c r="D26" s="127"/>
       <c r="E26" s="100">
@@ -6631,7 +6628,7 @@
         <v>149</v>
       </c>
       <c r="C27" s="61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D27" s="127"/>
       <c r="E27" s="100">
@@ -7876,14 +7873,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="27">
-    <mergeCell ref="CJ4:CP4"/>
-    <mergeCell ref="CJ5:CP5"/>
-    <mergeCell ref="BO5:BU5"/>
-    <mergeCell ref="BO4:BU4"/>
-    <mergeCell ref="BV4:CB4"/>
-    <mergeCell ref="BV5:CB5"/>
-    <mergeCell ref="CC4:CI4"/>
-    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -7894,15 +7892,14 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="CJ4:CP4"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BO4:BU4"/>
+    <mergeCell ref="BV4:CB4"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="CC5:CI5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8:H41">

</xml_diff>

<commit_message>
updated Gantt try 2, for ultrasonic detection and servo
</commit_message>
<xml_diff>
--- a/Gantt_Diagram_Robot_Project_2018.xlsx
+++ b/Gantt_Diagram_Robot_Project_2018.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolle\Documents\Robot_Project_IFX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Robot_Project_IFX\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27075" windowHeight="11370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27080" windowHeight="11370"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="0">GanttChart!$A1048576</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$45</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">GanttChartPro!$A$1:$C$47</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">GanttChart!$4:$7</definedName>
     <definedName name="valuevx">42.314159</definedName>
@@ -442,7 +442,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="169">
   <si>
     <t>WBS</t>
   </si>
@@ -1589,6 +1589,24 @@
   </si>
   <si>
     <t>M,Guillaume Nicolle</t>
+  </si>
+  <si>
+    <t>[Ultrasonic Detection]</t>
+  </si>
+  <si>
+    <t>Marlon BOURGOGNE</t>
+  </si>
+  <si>
+    <t>[Comments]</t>
+  </si>
+  <si>
+    <t>[Wiki page]</t>
+  </si>
+  <si>
+    <t>[Servomotors]</t>
+  </si>
+  <si>
+    <t>[Servomotors control]</t>
   </si>
 </sst>
 </file>
@@ -2942,24 +2960,6 @@
     </xf>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2967,9 +2967,27 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3021,7 +3039,71 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="19">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -3305,11 +3387,11 @@
           <xdr:col>9</xdr:col>
           <xdr:colOff>95250</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>127000</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>107950</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:to>
@@ -3890,53 +3972,53 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CP42"/>
+  <dimension ref="A1:CP52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <pane ySplit="7" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="6.81640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" style="6" customWidth="1"/>
     <col min="5" max="6" width="12" style="1" customWidth="1"/>
     <col min="7" max="7" width="6" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="1.85546875" style="1" customWidth="1"/>
-    <col min="11" max="66" width="2.42578125" style="1" customWidth="1"/>
-    <col min="67" max="67" width="2.7109375" style="3" customWidth="1"/>
-    <col min="68" max="68" width="2.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.7265625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="1.81640625" style="1" customWidth="1"/>
+    <col min="11" max="66" width="2.453125" style="1" customWidth="1"/>
+    <col min="67" max="67" width="2.7265625" style="3" customWidth="1"/>
+    <col min="68" max="68" width="2.54296875" style="3" customWidth="1"/>
     <col min="69" max="70" width="3" style="3" customWidth="1"/>
-    <col min="71" max="71" width="3.28515625" style="3" customWidth="1"/>
-    <col min="72" max="72" width="2.7109375" style="3" customWidth="1"/>
-    <col min="73" max="73" width="2.5703125" style="3" customWidth="1"/>
-    <col min="74" max="74" width="2.7109375" style="3" customWidth="1"/>
-    <col min="75" max="76" width="2.85546875" style="3" customWidth="1"/>
+    <col min="71" max="71" width="3.26953125" style="3" customWidth="1"/>
+    <col min="72" max="72" width="2.7265625" style="3" customWidth="1"/>
+    <col min="73" max="73" width="2.54296875" style="3" customWidth="1"/>
+    <col min="74" max="74" width="2.7265625" style="3" customWidth="1"/>
+    <col min="75" max="76" width="2.81640625" style="3" customWidth="1"/>
     <col min="77" max="77" width="3" style="3" customWidth="1"/>
-    <col min="78" max="78" width="2.5703125" style="3" customWidth="1"/>
-    <col min="79" max="79" width="2.42578125" style="3" customWidth="1"/>
-    <col min="80" max="80" width="2.7109375" style="3" customWidth="1"/>
-    <col min="81" max="81" width="2.42578125" style="3" customWidth="1"/>
+    <col min="78" max="78" width="2.54296875" style="3" customWidth="1"/>
+    <col min="79" max="79" width="2.453125" style="3" customWidth="1"/>
+    <col min="80" max="80" width="2.7265625" style="3" customWidth="1"/>
+    <col min="81" max="81" width="2.453125" style="3" customWidth="1"/>
     <col min="82" max="82" width="3" style="3" customWidth="1"/>
-    <col min="83" max="83" width="2.42578125" style="3" customWidth="1"/>
-    <col min="84" max="84" width="2.7109375" style="3" customWidth="1"/>
-    <col min="85" max="85" width="2.85546875" style="3" customWidth="1"/>
-    <col min="86" max="86" width="2.42578125" style="3" customWidth="1"/>
-    <col min="87" max="88" width="2.5703125" style="3" customWidth="1"/>
+    <col min="83" max="83" width="2.453125" style="3" customWidth="1"/>
+    <col min="84" max="84" width="2.7265625" style="3" customWidth="1"/>
+    <col min="85" max="85" width="2.81640625" style="3" customWidth="1"/>
+    <col min="86" max="86" width="2.453125" style="3" customWidth="1"/>
+    <col min="87" max="88" width="2.54296875" style="3" customWidth="1"/>
     <col min="89" max="89" width="3" style="3" customWidth="1"/>
-    <col min="90" max="90" width="2.5703125" style="3" customWidth="1"/>
-    <col min="91" max="92" width="3.140625" style="3" customWidth="1"/>
-    <col min="93" max="93" width="2.7109375" style="3" customWidth="1"/>
-    <col min="94" max="94" width="2.85546875" style="3" customWidth="1"/>
-    <col min="95" max="16384" width="9.140625" style="3"/>
+    <col min="90" max="90" width="2.54296875" style="3" customWidth="1"/>
+    <col min="91" max="92" width="3.1796875" style="3" customWidth="1"/>
+    <col min="93" max="93" width="2.7265625" style="3" customWidth="1"/>
+    <col min="94" max="94" width="2.81640625" style="3" customWidth="1"/>
+    <col min="95" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:94" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="125" t="s">
         <v>138</v>
       </c>
@@ -3946,31 +4028,31 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
       <c r="I1" s="132"/>
-      <c r="K1" s="169" t="s">
+      <c r="K1" s="163" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="169"/>
-      <c r="M1" s="169"/>
-      <c r="N1" s="169"/>
-      <c r="O1" s="169"/>
-      <c r="P1" s="169"/>
-      <c r="Q1" s="169"/>
-      <c r="R1" s="169"/>
-      <c r="S1" s="169"/>
-      <c r="T1" s="169"/>
-      <c r="U1" s="169"/>
-      <c r="V1" s="169"/>
-      <c r="W1" s="169"/>
-      <c r="X1" s="169"/>
-      <c r="Y1" s="169"/>
-      <c r="Z1" s="169"/>
-      <c r="AA1" s="169"/>
-      <c r="AB1" s="169"/>
-      <c r="AC1" s="169"/>
-      <c r="AD1" s="169"/>
-      <c r="AE1" s="169"/>
-    </row>
-    <row r="2" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L1" s="163"/>
+      <c r="M1" s="163"/>
+      <c r="N1" s="163"/>
+      <c r="O1" s="163"/>
+      <c r="P1" s="163"/>
+      <c r="Q1" s="163"/>
+      <c r="R1" s="163"/>
+      <c r="S1" s="163"/>
+      <c r="T1" s="163"/>
+      <c r="U1" s="163"/>
+      <c r="V1" s="163"/>
+      <c r="W1" s="163"/>
+      <c r="X1" s="163"/>
+      <c r="Y1" s="163"/>
+      <c r="Z1" s="163"/>
+      <c r="AA1" s="163"/>
+      <c r="AB1" s="163"/>
+      <c r="AC1" s="163"/>
+      <c r="AD1" s="163"/>
+      <c r="AE1" s="163"/>
+    </row>
+    <row r="2" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
         <v>139</v>
       </c>
@@ -3981,7 +4063,7 @@
       <c r="F2" s="160"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:94" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:94" ht="14" x14ac:dyDescent="0.25">
       <c r="A3" s="52"/>
       <c r="B3" s="48"/>
       <c r="C3" s="4"/>
@@ -4008,16 +4090,16 @@
       <c r="Z3" s="29"/>
       <c r="AA3" s="29"/>
     </row>
-    <row r="4" spans="1:94" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:94" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="110"/>
       <c r="B4" s="114" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="171">
+      <c r="C4" s="168">
         <v>43340</v>
       </c>
-      <c r="D4" s="171"/>
-      <c r="E4" s="171"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="168"/>
       <c r="F4" s="111"/>
       <c r="G4" s="114" t="s">
         <v>75</v>
@@ -4027,264 +4109,264 @@
       </c>
       <c r="I4" s="112"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="163" t="str">
+      <c r="K4" s="165" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="164"/>
-      <c r="M4" s="164"/>
-      <c r="N4" s="164"/>
-      <c r="O4" s="164"/>
-      <c r="P4" s="164"/>
-      <c r="Q4" s="165"/>
-      <c r="R4" s="163" t="str">
+      <c r="L4" s="166"/>
+      <c r="M4" s="166"/>
+      <c r="N4" s="166"/>
+      <c r="O4" s="166"/>
+      <c r="P4" s="166"/>
+      <c r="Q4" s="167"/>
+      <c r="R4" s="165" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="164"/>
-      <c r="T4" s="164"/>
-      <c r="U4" s="164"/>
-      <c r="V4" s="164"/>
-      <c r="W4" s="164"/>
-      <c r="X4" s="165"/>
-      <c r="Y4" s="163" t="str">
+      <c r="S4" s="166"/>
+      <c r="T4" s="166"/>
+      <c r="U4" s="166"/>
+      <c r="V4" s="166"/>
+      <c r="W4" s="166"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="165" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="164"/>
-      <c r="AA4" s="164"/>
-      <c r="AB4" s="164"/>
-      <c r="AC4" s="164"/>
-      <c r="AD4" s="164"/>
-      <c r="AE4" s="165"/>
-      <c r="AF4" s="163" t="str">
+      <c r="Z4" s="166"/>
+      <c r="AA4" s="166"/>
+      <c r="AB4" s="166"/>
+      <c r="AC4" s="166"/>
+      <c r="AD4" s="166"/>
+      <c r="AE4" s="167"/>
+      <c r="AF4" s="165" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="164"/>
-      <c r="AH4" s="164"/>
-      <c r="AI4" s="164"/>
-      <c r="AJ4" s="164"/>
-      <c r="AK4" s="164"/>
-      <c r="AL4" s="165"/>
-      <c r="AM4" s="163" t="str">
+      <c r="AG4" s="166"/>
+      <c r="AH4" s="166"/>
+      <c r="AI4" s="166"/>
+      <c r="AJ4" s="166"/>
+      <c r="AK4" s="166"/>
+      <c r="AL4" s="167"/>
+      <c r="AM4" s="165" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="164"/>
-      <c r="AO4" s="164"/>
-      <c r="AP4" s="164"/>
-      <c r="AQ4" s="164"/>
-      <c r="AR4" s="164"/>
-      <c r="AS4" s="165"/>
-      <c r="AT4" s="163" t="str">
+      <c r="AN4" s="166"/>
+      <c r="AO4" s="166"/>
+      <c r="AP4" s="166"/>
+      <c r="AQ4" s="166"/>
+      <c r="AR4" s="166"/>
+      <c r="AS4" s="167"/>
+      <c r="AT4" s="165" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="164"/>
-      <c r="AV4" s="164"/>
-      <c r="AW4" s="164"/>
-      <c r="AX4" s="164"/>
-      <c r="AY4" s="164"/>
-      <c r="AZ4" s="165"/>
-      <c r="BA4" s="163" t="str">
+      <c r="AU4" s="166"/>
+      <c r="AV4" s="166"/>
+      <c r="AW4" s="166"/>
+      <c r="AX4" s="166"/>
+      <c r="AY4" s="166"/>
+      <c r="AZ4" s="167"/>
+      <c r="BA4" s="165" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="164"/>
-      <c r="BC4" s="164"/>
-      <c r="BD4" s="164"/>
-      <c r="BE4" s="164"/>
-      <c r="BF4" s="164"/>
-      <c r="BG4" s="165"/>
-      <c r="BH4" s="163" t="str">
+      <c r="BB4" s="166"/>
+      <c r="BC4" s="166"/>
+      <c r="BD4" s="166"/>
+      <c r="BE4" s="166"/>
+      <c r="BF4" s="166"/>
+      <c r="BG4" s="167"/>
+      <c r="BH4" s="165" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="164"/>
-      <c r="BJ4" s="164"/>
-      <c r="BK4" s="164"/>
-      <c r="BL4" s="164"/>
-      <c r="BM4" s="164"/>
-      <c r="BN4" s="165"/>
-      <c r="BO4" s="163" t="str">
+      <c r="BI4" s="166"/>
+      <c r="BJ4" s="166"/>
+      <c r="BK4" s="166"/>
+      <c r="BL4" s="166"/>
+      <c r="BM4" s="166"/>
+      <c r="BN4" s="167"/>
+      <c r="BO4" s="165" t="str">
         <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="BP4" s="164"/>
-      <c r="BQ4" s="164"/>
-      <c r="BR4" s="164"/>
-      <c r="BS4" s="164"/>
-      <c r="BT4" s="164"/>
-      <c r="BU4" s="165"/>
-      <c r="BV4" s="163" t="str">
+      <c r="BP4" s="166"/>
+      <c r="BQ4" s="166"/>
+      <c r="BR4" s="166"/>
+      <c r="BS4" s="166"/>
+      <c r="BT4" s="166"/>
+      <c r="BU4" s="167"/>
+      <c r="BV4" s="165" t="str">
         <f>"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="BW4" s="164"/>
-      <c r="BX4" s="164"/>
-      <c r="BY4" s="164"/>
-      <c r="BZ4" s="164"/>
-      <c r="CA4" s="164"/>
-      <c r="CB4" s="165"/>
-      <c r="CC4" s="163" t="str">
+      <c r="BW4" s="166"/>
+      <c r="BX4" s="166"/>
+      <c r="BY4" s="166"/>
+      <c r="BZ4" s="166"/>
+      <c r="CA4" s="166"/>
+      <c r="CB4" s="167"/>
+      <c r="CC4" s="165" t="str">
         <f>"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="CD4" s="164"/>
-      <c r="CE4" s="164"/>
-      <c r="CF4" s="164"/>
-      <c r="CG4" s="164"/>
-      <c r="CH4" s="164"/>
-      <c r="CI4" s="165"/>
-      <c r="CJ4" s="163" t="str">
+      <c r="CD4" s="166"/>
+      <c r="CE4" s="166"/>
+      <c r="CF4" s="166"/>
+      <c r="CG4" s="166"/>
+      <c r="CH4" s="166"/>
+      <c r="CI4" s="167"/>
+      <c r="CJ4" s="165" t="str">
         <f>"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="CK4" s="164"/>
-      <c r="CL4" s="164"/>
-      <c r="CM4" s="164"/>
-      <c r="CN4" s="164"/>
-      <c r="CO4" s="164"/>
-      <c r="CP4" s="165"/>
-    </row>
-    <row r="5" spans="1:94" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="CK4" s="166"/>
+      <c r="CL4" s="166"/>
+      <c r="CM4" s="166"/>
+      <c r="CN4" s="166"/>
+      <c r="CO4" s="166"/>
+      <c r="CP4" s="167"/>
+    </row>
+    <row r="5" spans="1:94" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="110"/>
       <c r="B5" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="170" t="s">
+      <c r="C5" s="164" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
+      <c r="D5" s="164"/>
+      <c r="E5" s="164"/>
       <c r="F5" s="113"/>
       <c r="G5" s="113"/>
       <c r="H5" s="113"/>
       <c r="I5" s="113"/>
       <c r="J5" s="50"/>
-      <c r="K5" s="166">
+      <c r="K5" s="169">
         <f>K6</f>
         <v>43339</v>
       </c>
-      <c r="L5" s="167"/>
-      <c r="M5" s="167"/>
-      <c r="N5" s="167"/>
-      <c r="O5" s="167"/>
-      <c r="P5" s="167"/>
-      <c r="Q5" s="168"/>
-      <c r="R5" s="166">
+      <c r="L5" s="170"/>
+      <c r="M5" s="170"/>
+      <c r="N5" s="170"/>
+      <c r="O5" s="170"/>
+      <c r="P5" s="170"/>
+      <c r="Q5" s="171"/>
+      <c r="R5" s="169">
         <f>R6</f>
         <v>43346</v>
       </c>
-      <c r="S5" s="167"/>
-      <c r="T5" s="167"/>
-      <c r="U5" s="167"/>
-      <c r="V5" s="167"/>
-      <c r="W5" s="167"/>
-      <c r="X5" s="168"/>
-      <c r="Y5" s="166">
+      <c r="S5" s="170"/>
+      <c r="T5" s="170"/>
+      <c r="U5" s="170"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
+      <c r="X5" s="171"/>
+      <c r="Y5" s="169">
         <f>Y6</f>
         <v>43353</v>
       </c>
-      <c r="Z5" s="167"/>
-      <c r="AA5" s="167"/>
-      <c r="AB5" s="167"/>
-      <c r="AC5" s="167"/>
-      <c r="AD5" s="167"/>
-      <c r="AE5" s="168"/>
-      <c r="AF5" s="166">
+      <c r="Z5" s="170"/>
+      <c r="AA5" s="170"/>
+      <c r="AB5" s="170"/>
+      <c r="AC5" s="170"/>
+      <c r="AD5" s="170"/>
+      <c r="AE5" s="171"/>
+      <c r="AF5" s="169">
         <f>AF6</f>
         <v>43360</v>
       </c>
-      <c r="AG5" s="167"/>
-      <c r="AH5" s="167"/>
-      <c r="AI5" s="167"/>
-      <c r="AJ5" s="167"/>
-      <c r="AK5" s="167"/>
-      <c r="AL5" s="168"/>
-      <c r="AM5" s="166">
+      <c r="AG5" s="170"/>
+      <c r="AH5" s="170"/>
+      <c r="AI5" s="170"/>
+      <c r="AJ5" s="170"/>
+      <c r="AK5" s="170"/>
+      <c r="AL5" s="171"/>
+      <c r="AM5" s="169">
         <f>AM6</f>
         <v>43367</v>
       </c>
-      <c r="AN5" s="167"/>
-      <c r="AO5" s="167"/>
-      <c r="AP5" s="167"/>
-      <c r="AQ5" s="167"/>
-      <c r="AR5" s="167"/>
-      <c r="AS5" s="168"/>
-      <c r="AT5" s="166">
+      <c r="AN5" s="170"/>
+      <c r="AO5" s="170"/>
+      <c r="AP5" s="170"/>
+      <c r="AQ5" s="170"/>
+      <c r="AR5" s="170"/>
+      <c r="AS5" s="171"/>
+      <c r="AT5" s="169">
         <f>AT6</f>
         <v>43374</v>
       </c>
-      <c r="AU5" s="167"/>
-      <c r="AV5" s="167"/>
-      <c r="AW5" s="167"/>
-      <c r="AX5" s="167"/>
-      <c r="AY5" s="167"/>
-      <c r="AZ5" s="168"/>
-      <c r="BA5" s="166">
+      <c r="AU5" s="170"/>
+      <c r="AV5" s="170"/>
+      <c r="AW5" s="170"/>
+      <c r="AX5" s="170"/>
+      <c r="AY5" s="170"/>
+      <c r="AZ5" s="171"/>
+      <c r="BA5" s="169">
         <f>BA6</f>
         <v>43381</v>
       </c>
-      <c r="BB5" s="167"/>
-      <c r="BC5" s="167"/>
-      <c r="BD5" s="167"/>
-      <c r="BE5" s="167"/>
-      <c r="BF5" s="167"/>
-      <c r="BG5" s="168"/>
-      <c r="BH5" s="166">
+      <c r="BB5" s="170"/>
+      <c r="BC5" s="170"/>
+      <c r="BD5" s="170"/>
+      <c r="BE5" s="170"/>
+      <c r="BF5" s="170"/>
+      <c r="BG5" s="171"/>
+      <c r="BH5" s="169">
         <f>BH6</f>
         <v>43388</v>
       </c>
-      <c r="BI5" s="167"/>
-      <c r="BJ5" s="167"/>
-      <c r="BK5" s="167"/>
-      <c r="BL5" s="167"/>
-      <c r="BM5" s="167"/>
-      <c r="BN5" s="168"/>
-      <c r="BO5" s="166">
+      <c r="BI5" s="170"/>
+      <c r="BJ5" s="170"/>
+      <c r="BK5" s="170"/>
+      <c r="BL5" s="170"/>
+      <c r="BM5" s="170"/>
+      <c r="BN5" s="171"/>
+      <c r="BO5" s="169">
         <f>BO6</f>
         <v>43395</v>
       </c>
-      <c r="BP5" s="167"/>
-      <c r="BQ5" s="167"/>
-      <c r="BR5" s="167"/>
-      <c r="BS5" s="167"/>
-      <c r="BT5" s="167"/>
-      <c r="BU5" s="168"/>
-      <c r="BV5" s="166">
+      <c r="BP5" s="170"/>
+      <c r="BQ5" s="170"/>
+      <c r="BR5" s="170"/>
+      <c r="BS5" s="170"/>
+      <c r="BT5" s="170"/>
+      <c r="BU5" s="171"/>
+      <c r="BV5" s="169">
         <f>BV6</f>
         <v>43402</v>
       </c>
-      <c r="BW5" s="167"/>
-      <c r="BX5" s="167"/>
-      <c r="BY5" s="167"/>
-      <c r="BZ5" s="167"/>
-      <c r="CA5" s="167"/>
-      <c r="CB5" s="168"/>
-      <c r="CC5" s="166">
+      <c r="BW5" s="170"/>
+      <c r="BX5" s="170"/>
+      <c r="BY5" s="170"/>
+      <c r="BZ5" s="170"/>
+      <c r="CA5" s="170"/>
+      <c r="CB5" s="171"/>
+      <c r="CC5" s="169">
         <f>CC6</f>
         <v>43409</v>
       </c>
-      <c r="CD5" s="167"/>
-      <c r="CE5" s="167"/>
-      <c r="CF5" s="167"/>
-      <c r="CG5" s="167"/>
-      <c r="CH5" s="167"/>
-      <c r="CI5" s="168"/>
-      <c r="CJ5" s="166">
+      <c r="CD5" s="170"/>
+      <c r="CE5" s="170"/>
+      <c r="CF5" s="170"/>
+      <c r="CG5" s="170"/>
+      <c r="CH5" s="170"/>
+      <c r="CI5" s="171"/>
+      <c r="CJ5" s="169">
         <f>CJ6</f>
         <v>43416</v>
       </c>
-      <c r="CK5" s="167"/>
-      <c r="CL5" s="167"/>
-      <c r="CM5" s="167"/>
-      <c r="CN5" s="167"/>
-      <c r="CO5" s="167"/>
-      <c r="CP5" s="168"/>
-    </row>
-    <row r="6" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="CK5" s="170"/>
+      <c r="CL5" s="170"/>
+      <c r="CM5" s="170"/>
+      <c r="CN5" s="170"/>
+      <c r="CO5" s="170"/>
+      <c r="CP5" s="171"/>
+    </row>
+    <row r="6" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A6" s="49"/>
       <c r="B6" s="50"/>
       <c r="C6" s="50"/>
@@ -4632,7 +4714,7 @@
         <v>43422</v>
       </c>
     </row>
-    <row r="7" spans="1:94" s="124" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:94" s="124" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="116" t="s">
         <v>0</v>
       </c>
@@ -4998,7 +5080,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="8" spans="1:94" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:94" s="55" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A8" s="84" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -5016,7 +5098,7 @@
       <c r="G8" s="89"/>
       <c r="H8" s="90"/>
       <c r="I8" s="91" t="str">
-        <f t="shared" ref="I8:I35" si="33">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
+        <f t="shared" ref="I8:I45" si="33">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J8" s="94"/>
@@ -5077,7 +5159,7 @@
       <c r="BM8" s="106"/>
       <c r="BN8" s="106"/>
     </row>
-    <row r="9" spans="1:94" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="str">
         <f t="shared" ref="A9:A15" si="34">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -5166,7 +5248,7 @@
       <c r="BM9" s="107"/>
       <c r="BN9" s="107"/>
     </row>
-    <row r="10" spans="1:94" s="61" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="str">
         <f t="shared" si="34"/>
         <v>1.2</v>
@@ -5253,7 +5335,7 @@
       <c r="BM10" s="107"/>
       <c r="BN10" s="107"/>
     </row>
-    <row r="11" spans="1:94" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="str">
         <f t="shared" si="34"/>
         <v>1.3</v>
@@ -5269,7 +5351,7 @@
         <v>43139</v>
       </c>
       <c r="F11" s="101">
-        <f t="shared" ref="F11:F33" si="35">IF(ISBLANK(E11)," - ",IF(G11=0,E11,E11+G11-1))</f>
+        <f t="shared" ref="F11:F43" si="35">IF(ISBLANK(E11)," - ",IF(G11=0,E11,E11+G11-1))</f>
         <v>43142</v>
       </c>
       <c r="G11" s="62">
@@ -5340,7 +5422,7 @@
       <c r="BM11" s="107"/>
       <c r="BN11" s="107"/>
     </row>
-    <row r="12" spans="1:94" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.3.1</v>
@@ -5424,7 +5506,7 @@
       <c r="BM12" s="107"/>
       <c r="BN12" s="107"/>
     </row>
-    <row r="13" spans="1:94" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.3.2</v>
@@ -5508,7 +5590,7 @@
       <c r="BM13" s="107"/>
       <c r="BN13" s="107"/>
     </row>
-    <row r="14" spans="1:94" s="61" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:94" s="61" customFormat="1" ht="23" x14ac:dyDescent="0.25">
       <c r="A14" s="60" t="str">
         <f t="shared" si="34"/>
         <v>1.4</v>
@@ -5595,7 +5677,7 @@
       <c r="BM14" s="107"/>
       <c r="BN14" s="107"/>
     </row>
-    <row r="15" spans="1:94" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A15" s="60" t="str">
         <f t="shared" si="34"/>
         <v>1.5</v>
@@ -5682,7 +5764,7 @@
       <c r="BM15" s="107"/>
       <c r="BN15" s="107"/>
     </row>
-    <row r="16" spans="1:94" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:94" s="55" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A16" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>2</v>
@@ -5760,7 +5842,7 @@
       <c r="BM16" s="109"/>
       <c r="BN16" s="109"/>
     </row>
-    <row r="17" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A17" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.1</v>
@@ -5848,7 +5930,7 @@
       <c r="BM17" s="107"/>
       <c r="BN17" s="107"/>
     </row>
-    <row r="18" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A18" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.2</v>
@@ -5935,7 +6017,7 @@
       <c r="BM18" s="107"/>
       <c r="BN18" s="107"/>
     </row>
-    <row r="19" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A19" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.3</v>
@@ -6022,7 +6104,7 @@
       <c r="BM19" s="107"/>
       <c r="BN19" s="107"/>
     </row>
-    <row r="20" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.4</v>
@@ -6109,7 +6191,7 @@
       <c r="BM20" s="107"/>
       <c r="BN20" s="107"/>
     </row>
-    <row r="21" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A21" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.5</v>
@@ -6193,7 +6275,7 @@
       <c r="BM21" s="107"/>
       <c r="BN21" s="107"/>
     </row>
-    <row r="22" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:66" s="55" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A22" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>3</v>
@@ -6271,7 +6353,7 @@
       <c r="BM22" s="109"/>
       <c r="BN22" s="109"/>
     </row>
-    <row r="23" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A23" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.1</v>
@@ -6358,7 +6440,7 @@
       <c r="BM23" s="107"/>
       <c r="BN23" s="107"/>
     </row>
-    <row r="24" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A24" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.2</v>
@@ -6445,7 +6527,7 @@
       <c r="BM24" s="107"/>
       <c r="BN24" s="107"/>
     </row>
-    <row r="25" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.3</v>
@@ -6532,7 +6614,7 @@
       <c r="BM25" s="107"/>
       <c r="BN25" s="107"/>
     </row>
-    <row r="26" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A26" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.4</v>
@@ -6619,7 +6701,7 @@
       <c r="BM26" s="107"/>
       <c r="BN26" s="107"/>
     </row>
-    <row r="27" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A27" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.5</v>
@@ -6706,13 +6788,13 @@
       <c r="BM27" s="107"/>
       <c r="BN27" s="107"/>
     </row>
-    <row r="28" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:66" s="55" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A28" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>4</v>
       </c>
       <c r="B28" s="54" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="D28" s="56"/>
       <c r="E28" s="102"/>
@@ -6784,31 +6866,34 @@
       <c r="BM28" s="109"/>
       <c r="BN28" s="109"/>
     </row>
-    <row r="29" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A29" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.1</v>
       </c>
       <c r="B29" s="126" t="s">
-        <v>9</v>
+        <v>163</v>
+      </c>
+      <c r="C29" s="61" t="s">
+        <v>164</v>
       </c>
       <c r="D29" s="127"/>
       <c r="E29" s="100">
-        <v>43129</v>
+        <v>43353</v>
       </c>
       <c r="F29" s="101">
-        <f t="shared" si="35"/>
-        <v>43129</v>
+        <f>IF(ISBLANK(E29)," - ",IF(G29=0,E29,E29+G29-1))</f>
+        <v>43355</v>
       </c>
       <c r="G29" s="62">
+        <v>3</v>
+      </c>
+      <c r="H29" s="63">
         <v>1</v>
-      </c>
-      <c r="H29" s="63">
-        <v>0</v>
       </c>
       <c r="I29" s="64">
         <f t="shared" si="33"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J29" s="95"/>
       <c r="K29" s="107"/>
@@ -6868,27 +6953,30 @@
       <c r="BM29" s="107"/>
       <c r="BN29" s="107"/>
     </row>
-    <row r="30" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A30" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.2</v>
       </c>
       <c r="B30" s="126" t="s">
-        <v>9</v>
+        <v>165</v>
+      </c>
+      <c r="C30" s="61" t="s">
+        <v>164</v>
       </c>
       <c r="D30" s="127"/>
       <c r="E30" s="100">
-        <v>43130</v>
+        <v>43354</v>
       </c>
       <c r="F30" s="101">
         <f t="shared" si="35"/>
-        <v>43130</v>
+        <v>43354</v>
       </c>
       <c r="G30" s="62">
         <v>1</v>
       </c>
       <c r="H30" s="63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" s="64">
         <f t="shared" si="33"/>
@@ -6952,27 +7040,30 @@
       <c r="BM30" s="107"/>
       <c r="BN30" s="107"/>
     </row>
-    <row r="31" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A31" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.3</v>
       </c>
       <c r="B31" s="126" t="s">
-        <v>9</v>
+        <v>166</v>
+      </c>
+      <c r="C31" s="61" t="s">
+        <v>164</v>
       </c>
       <c r="D31" s="127"/>
       <c r="E31" s="100">
-        <v>43131</v>
+        <v>43357</v>
       </c>
       <c r="F31" s="101">
-        <f t="shared" si="35"/>
-        <v>43131</v>
+        <f>IF(ISBLANK(E31)," - ",IF(G31=0,E31,E31+G31-1))</f>
+        <v>43357</v>
       </c>
       <c r="G31" s="62">
         <v>1</v>
       </c>
       <c r="H31" s="63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="64">
         <f t="shared" si="33"/>
@@ -7036,115 +7127,112 @@
       <c r="BM31" s="107"/>
       <c r="BN31" s="107"/>
     </row>
-    <row r="32" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.4</v>
-      </c>
-      <c r="B32" s="126" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="127"/>
-      <c r="E32" s="100">
-        <v>43132</v>
-      </c>
-      <c r="F32" s="101">
-        <f t="shared" si="35"/>
-        <v>43132</v>
-      </c>
-      <c r="G32" s="62">
-        <v>1</v>
-      </c>
-      <c r="H32" s="63">
-        <v>0</v>
-      </c>
-      <c r="I32" s="64">
+    <row r="32" spans="1:66" s="55" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="53" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>5</v>
+      </c>
+      <c r="B32" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="D32" s="56"/>
+      <c r="E32" s="102"/>
+      <c r="F32" s="102" t="str">
+        <f t="shared" ref="F32" si="36">IF(ISBLANK(E32)," - ",IF(G32=0,E32,E32+G32-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G32" s="57"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="59" t="str">
         <f t="shared" si="33"/>
-        <v>1</v>
-      </c>
-      <c r="J32" s="95"/>
-      <c r="K32" s="107"/>
-      <c r="L32" s="107"/>
-      <c r="M32" s="107"/>
-      <c r="N32" s="107"/>
-      <c r="O32" s="107"/>
-      <c r="P32" s="107"/>
-      <c r="Q32" s="107"/>
-      <c r="R32" s="107"/>
-      <c r="S32" s="107"/>
-      <c r="T32" s="107"/>
-      <c r="U32" s="107"/>
-      <c r="V32" s="107"/>
-      <c r="W32" s="107"/>
-      <c r="X32" s="107"/>
-      <c r="Y32" s="107"/>
-      <c r="Z32" s="107"/>
-      <c r="AA32" s="107"/>
-      <c r="AB32" s="107"/>
-      <c r="AC32" s="107"/>
-      <c r="AD32" s="107"/>
-      <c r="AE32" s="107"/>
-      <c r="AF32" s="107"/>
-      <c r="AG32" s="107"/>
-      <c r="AH32" s="107"/>
-      <c r="AI32" s="107"/>
-      <c r="AJ32" s="107"/>
-      <c r="AK32" s="107"/>
-      <c r="AL32" s="107"/>
-      <c r="AM32" s="107"/>
-      <c r="AN32" s="107"/>
-      <c r="AO32" s="107"/>
-      <c r="AP32" s="107"/>
-      <c r="AQ32" s="107"/>
-      <c r="AR32" s="107"/>
-      <c r="AS32" s="107"/>
-      <c r="AT32" s="107"/>
-      <c r="AU32" s="107"/>
-      <c r="AV32" s="107"/>
-      <c r="AW32" s="107"/>
-      <c r="AX32" s="107"/>
-      <c r="AY32" s="107"/>
-      <c r="AZ32" s="107"/>
-      <c r="BA32" s="107"/>
-      <c r="BB32" s="107"/>
-      <c r="BC32" s="107"/>
-      <c r="BD32" s="107"/>
-      <c r="BE32" s="107"/>
-      <c r="BF32" s="107"/>
-      <c r="BG32" s="107"/>
-      <c r="BH32" s="107"/>
-      <c r="BI32" s="107"/>
-      <c r="BJ32" s="107"/>
-      <c r="BK32" s="107"/>
-      <c r="BL32" s="107"/>
-      <c r="BM32" s="107"/>
-      <c r="BN32" s="107"/>
-    </row>
-    <row r="33" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J32" s="96"/>
+      <c r="K32" s="109"/>
+      <c r="L32" s="109"/>
+      <c r="M32" s="109"/>
+      <c r="N32" s="109"/>
+      <c r="O32" s="109"/>
+      <c r="P32" s="109"/>
+      <c r="Q32" s="109"/>
+      <c r="R32" s="109"/>
+      <c r="S32" s="109"/>
+      <c r="T32" s="109"/>
+      <c r="U32" s="109"/>
+      <c r="V32" s="109"/>
+      <c r="W32" s="109"/>
+      <c r="X32" s="109"/>
+      <c r="Y32" s="109"/>
+      <c r="Z32" s="109"/>
+      <c r="AA32" s="109"/>
+      <c r="AB32" s="109"/>
+      <c r="AC32" s="109"/>
+      <c r="AD32" s="109"/>
+      <c r="AE32" s="109"/>
+      <c r="AF32" s="109"/>
+      <c r="AG32" s="109"/>
+      <c r="AH32" s="109"/>
+      <c r="AI32" s="109"/>
+      <c r="AJ32" s="109"/>
+      <c r="AK32" s="109"/>
+      <c r="AL32" s="109"/>
+      <c r="AM32" s="109"/>
+      <c r="AN32" s="109"/>
+      <c r="AO32" s="109"/>
+      <c r="AP32" s="109"/>
+      <c r="AQ32" s="109"/>
+      <c r="AR32" s="109"/>
+      <c r="AS32" s="109"/>
+      <c r="AT32" s="109"/>
+      <c r="AU32" s="109"/>
+      <c r="AV32" s="109"/>
+      <c r="AW32" s="109"/>
+      <c r="AX32" s="109"/>
+      <c r="AY32" s="109"/>
+      <c r="AZ32" s="109"/>
+      <c r="BA32" s="109"/>
+      <c r="BB32" s="109"/>
+      <c r="BC32" s="109"/>
+      <c r="BD32" s="109"/>
+      <c r="BE32" s="109"/>
+      <c r="BF32" s="109"/>
+      <c r="BG32" s="109"/>
+      <c r="BH32" s="109"/>
+      <c r="BI32" s="109"/>
+      <c r="BJ32" s="109"/>
+      <c r="BK32" s="109"/>
+      <c r="BL32" s="109"/>
+      <c r="BM32" s="109"/>
+      <c r="BN32" s="109"/>
+    </row>
+    <row r="33" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A33" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.5</v>
+        <v>5.1</v>
       </c>
       <c r="B33" s="126" t="s">
-        <v>9</v>
+        <v>168</v>
+      </c>
+      <c r="C33" s="61" t="s">
+        <v>164</v>
       </c>
       <c r="D33" s="127"/>
       <c r="E33" s="100">
-        <v>43133</v>
+        <v>43391</v>
       </c>
       <c r="F33" s="101">
-        <f t="shared" si="35"/>
-        <v>43133</v>
+        <f>IF(ISBLANK(E33)," - ",IF(G33=0,E33,E33+G33-1))</f>
+        <v>43397</v>
       </c>
       <c r="G33" s="62">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H33" s="63">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="I33" s="64">
         <f t="shared" si="33"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J33" s="95"/>
       <c r="K33" s="107"/>
@@ -7204,20 +7292,36 @@
       <c r="BM33" s="107"/>
       <c r="BN33" s="107"/>
     </row>
-    <row r="34" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A34" s="60"/>
-      <c r="B34" s="65"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="66"/>
-      <c r="E34" s="103"/>
-      <c r="F34" s="103"/>
-      <c r="G34" s="67"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="69" t="str">
+    <row r="34" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>5.2</v>
+      </c>
+      <c r="B34" s="126" t="s">
+        <v>165</v>
+      </c>
+      <c r="C34" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="D34" s="127"/>
+      <c r="E34" s="100">
+        <v>43391</v>
+      </c>
+      <c r="F34" s="101">
+        <f t="shared" ref="F34" si="37">IF(ISBLANK(E34)," - ",IF(G34=0,E34,E34+G34-1))</f>
+        <v>43391</v>
+      </c>
+      <c r="G34" s="62">
+        <v>1</v>
+      </c>
+      <c r="H34" s="63">
+        <v>0</v>
+      </c>
+      <c r="I34" s="64">
         <f t="shared" si="33"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J34" s="97"/>
+        <v>1</v>
+      </c>
+      <c r="J34" s="95"/>
       <c r="K34" s="107"/>
       <c r="L34" s="107"/>
       <c r="M34" s="107"/>
@@ -7275,20 +7379,36 @@
       <c r="BM34" s="107"/>
       <c r="BN34" s="107"/>
     </row>
-    <row r="35" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A35" s="60"/>
-      <c r="B35" s="65"/>
-      <c r="C35" s="65"/>
-      <c r="D35" s="66"/>
-      <c r="E35" s="103"/>
-      <c r="F35" s="103"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="68"/>
-      <c r="I35" s="69" t="str">
+    <row r="35" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>5.3</v>
+      </c>
+      <c r="B35" s="126" t="s">
+        <v>166</v>
+      </c>
+      <c r="C35" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="D35" s="127"/>
+      <c r="E35" s="100">
+        <v>43391</v>
+      </c>
+      <c r="F35" s="101">
+        <f>IF(ISBLANK(E35)," - ",IF(G35=0,E35,E35+G35-1))</f>
+        <v>43391</v>
+      </c>
+      <c r="G35" s="62">
+        <v>1</v>
+      </c>
+      <c r="H35" s="63">
+        <v>0</v>
+      </c>
+      <c r="I35" s="64">
         <f t="shared" si="33"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J35" s="97"/>
+        <v>1</v>
+      </c>
+      <c r="J35" s="95"/>
       <c r="K35" s="107"/>
       <c r="L35" s="107"/>
       <c r="M35" s="107"/>
@@ -7346,19 +7466,33 @@
       <c r="BM35" s="107"/>
       <c r="BN35" s="107"/>
     </row>
-    <row r="36" spans="1:66" s="75" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="71" t="s">
+    <row r="36" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>5.4</v>
+      </c>
+      <c r="B36" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="127"/>
+      <c r="E36" s="100">
+        <v>43132</v>
+      </c>
+      <c r="F36" s="101">
+        <f t="shared" ref="F36:F37" si="38">IF(ISBLANK(E36)," - ",IF(G36=0,E36,E36+G36-1))</f>
+        <v>43132</v>
+      </c>
+      <c r="G36" s="62">
         <v>1</v>
       </c>
-      <c r="B36" s="72"/>
-      <c r="C36" s="73"/>
-      <c r="D36" s="73"/>
-      <c r="E36" s="104"/>
-      <c r="F36" s="104"/>
-      <c r="G36" s="74"/>
-      <c r="H36" s="74"/>
-      <c r="I36" s="74"/>
-      <c r="J36" s="98"/>
+      <c r="H36" s="63">
+        <v>0</v>
+      </c>
+      <c r="I36" s="64">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="J36" s="95"/>
       <c r="K36" s="107"/>
       <c r="L36" s="107"/>
       <c r="M36" s="107"/>
@@ -7416,19 +7550,33 @@
       <c r="BM36" s="107"/>
       <c r="BN36" s="107"/>
     </row>
-    <row r="37" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" s="76" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="77"/>
-      <c r="C37" s="77"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="105"/>
-      <c r="F37" s="105"/>
-      <c r="G37" s="77"/>
-      <c r="H37" s="77"/>
-      <c r="I37" s="77"/>
-      <c r="J37" s="98"/>
+    <row r="37" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>5.5</v>
+      </c>
+      <c r="B37" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="127"/>
+      <c r="E37" s="100">
+        <v>43133</v>
+      </c>
+      <c r="F37" s="101">
+        <f t="shared" si="38"/>
+        <v>43133</v>
+      </c>
+      <c r="G37" s="62">
+        <v>1</v>
+      </c>
+      <c r="H37" s="63">
+        <v>0</v>
+      </c>
+      <c r="I37" s="64">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="J37" s="95"/>
       <c r="K37" s="107"/>
       <c r="L37" s="107"/>
       <c r="M37" s="107"/>
@@ -7486,107 +7634,111 @@
       <c r="BM37" s="107"/>
       <c r="BN37" s="107"/>
     </row>
-    <row r="38" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A38" s="130" t="str">
+    <row r="38" spans="1:66" s="55" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>1</v>
-      </c>
-      <c r="B38" s="131" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="78"/>
-      <c r="D38" s="79"/>
-      <c r="E38" s="100"/>
-      <c r="F38" s="101" t="str">
-        <f t="shared" ref="F38:F41" si="36">IF(ISBLANK(E38)," - ",IF(G38=0,E38,E38+G38-1))</f>
+        <v>6</v>
+      </c>
+      <c r="B38" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="56"/>
+      <c r="E38" s="102"/>
+      <c r="F38" s="102" t="str">
+        <f t="shared" si="35"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G38" s="62"/>
-      <c r="H38" s="63"/>
-      <c r="I38" s="80" t="str">
-        <f>IF(OR(F38=0,E38=0)," - ",NETWORKDAYS(E38,F38))</f>
+      <c r="G38" s="57"/>
+      <c r="H38" s="58"/>
+      <c r="I38" s="59" t="str">
+        <f t="shared" si="33"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J38" s="99"/>
-      <c r="K38" s="107"/>
-      <c r="L38" s="107"/>
-      <c r="M38" s="107"/>
-      <c r="N38" s="107"/>
-      <c r="O38" s="107"/>
-      <c r="P38" s="107"/>
-      <c r="Q38" s="107"/>
-      <c r="R38" s="107"/>
-      <c r="S38" s="107"/>
-      <c r="T38" s="107"/>
-      <c r="U38" s="107"/>
-      <c r="V38" s="107"/>
-      <c r="W38" s="107"/>
-      <c r="X38" s="107"/>
-      <c r="Y38" s="107"/>
-      <c r="Z38" s="107"/>
-      <c r="AA38" s="107"/>
-      <c r="AB38" s="107"/>
-      <c r="AC38" s="107"/>
-      <c r="AD38" s="107"/>
-      <c r="AE38" s="107"/>
-      <c r="AF38" s="107"/>
-      <c r="AG38" s="107"/>
-      <c r="AH38" s="107"/>
-      <c r="AI38" s="107"/>
-      <c r="AJ38" s="107"/>
-      <c r="AK38" s="107"/>
-      <c r="AL38" s="107"/>
-      <c r="AM38" s="107"/>
-      <c r="AN38" s="107"/>
-      <c r="AO38" s="107"/>
-      <c r="AP38" s="107"/>
-      <c r="AQ38" s="107"/>
-      <c r="AR38" s="107"/>
-      <c r="AS38" s="107"/>
-      <c r="AT38" s="107"/>
-      <c r="AU38" s="107"/>
-      <c r="AV38" s="107"/>
-      <c r="AW38" s="107"/>
-      <c r="AX38" s="107"/>
-      <c r="AY38" s="107"/>
-      <c r="AZ38" s="107"/>
-      <c r="BA38" s="107"/>
-      <c r="BB38" s="107"/>
-      <c r="BC38" s="107"/>
-      <c r="BD38" s="107"/>
-      <c r="BE38" s="107"/>
-      <c r="BF38" s="107"/>
-      <c r="BG38" s="107"/>
-      <c r="BH38" s="107"/>
-      <c r="BI38" s="107"/>
-      <c r="BJ38" s="107"/>
-      <c r="BK38" s="107"/>
-      <c r="BL38" s="107"/>
-      <c r="BM38" s="107"/>
-      <c r="BN38" s="107"/>
-    </row>
-    <row r="39" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="J38" s="96"/>
+      <c r="K38" s="109"/>
+      <c r="L38" s="109"/>
+      <c r="M38" s="109"/>
+      <c r="N38" s="109"/>
+      <c r="O38" s="109"/>
+      <c r="P38" s="109"/>
+      <c r="Q38" s="109"/>
+      <c r="R38" s="109"/>
+      <c r="S38" s="109"/>
+      <c r="T38" s="109"/>
+      <c r="U38" s="109"/>
+      <c r="V38" s="109"/>
+      <c r="W38" s="109"/>
+      <c r="X38" s="109"/>
+      <c r="Y38" s="109"/>
+      <c r="Z38" s="109"/>
+      <c r="AA38" s="109"/>
+      <c r="AB38" s="109"/>
+      <c r="AC38" s="109"/>
+      <c r="AD38" s="109"/>
+      <c r="AE38" s="109"/>
+      <c r="AF38" s="109"/>
+      <c r="AG38" s="109"/>
+      <c r="AH38" s="109"/>
+      <c r="AI38" s="109"/>
+      <c r="AJ38" s="109"/>
+      <c r="AK38" s="109"/>
+      <c r="AL38" s="109"/>
+      <c r="AM38" s="109"/>
+      <c r="AN38" s="109"/>
+      <c r="AO38" s="109"/>
+      <c r="AP38" s="109"/>
+      <c r="AQ38" s="109"/>
+      <c r="AR38" s="109"/>
+      <c r="AS38" s="109"/>
+      <c r="AT38" s="109"/>
+      <c r="AU38" s="109"/>
+      <c r="AV38" s="109"/>
+      <c r="AW38" s="109"/>
+      <c r="AX38" s="109"/>
+      <c r="AY38" s="109"/>
+      <c r="AZ38" s="109"/>
+      <c r="BA38" s="109"/>
+      <c r="BB38" s="109"/>
+      <c r="BC38" s="109"/>
+      <c r="BD38" s="109"/>
+      <c r="BE38" s="109"/>
+      <c r="BF38" s="109"/>
+      <c r="BG38" s="109"/>
+      <c r="BH38" s="109"/>
+      <c r="BI38" s="109"/>
+      <c r="BJ38" s="109"/>
+      <c r="BK38" s="109"/>
+      <c r="BL38" s="109"/>
+      <c r="BM38" s="109"/>
+      <c r="BN38" s="109"/>
+    </row>
+    <row r="39" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A39" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>1.1</v>
-      </c>
-      <c r="B39" s="81" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" s="81"/>
-      <c r="D39" s="79"/>
-      <c r="E39" s="100"/>
-      <c r="F39" s="101" t="str">
-        <f t="shared" si="36"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G39" s="62"/>
-      <c r="H39" s="63"/>
-      <c r="I39" s="80" t="str">
-        <f t="shared" ref="I39:I41" si="37">IF(OR(F39=0,E39=0)," - ",NETWORKDAYS(E39,F39))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J39" s="99"/>
+        <v>6.1</v>
+      </c>
+      <c r="B39" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="127"/>
+      <c r="E39" s="100">
+        <v>43129</v>
+      </c>
+      <c r="F39" s="101">
+        <f t="shared" si="35"/>
+        <v>43129</v>
+      </c>
+      <c r="G39" s="62">
+        <v>1</v>
+      </c>
+      <c r="H39" s="63">
+        <v>0</v>
+      </c>
+      <c r="I39" s="64">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="J39" s="95"/>
       <c r="K39" s="107"/>
       <c r="L39" s="107"/>
       <c r="M39" s="107"/>
@@ -7644,28 +7796,33 @@
       <c r="BM39" s="107"/>
       <c r="BN39" s="107"/>
     </row>
-    <row r="40" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A40" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
-        <v>1.1.1</v>
-      </c>
-      <c r="B40" s="82" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="81"/>
-      <c r="D40" s="79"/>
-      <c r="E40" s="100"/>
-      <c r="F40" s="101" t="str">
-        <f t="shared" si="36"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G40" s="62"/>
-      <c r="H40" s="63"/>
-      <c r="I40" s="80" t="str">
-        <f t="shared" si="37"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J40" s="99"/>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>6.2</v>
+      </c>
+      <c r="B40" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="127"/>
+      <c r="E40" s="100">
+        <v>43130</v>
+      </c>
+      <c r="F40" s="101">
+        <f t="shared" si="35"/>
+        <v>43130</v>
+      </c>
+      <c r="G40" s="62">
+        <v>1</v>
+      </c>
+      <c r="H40" s="63">
+        <v>0</v>
+      </c>
+      <c r="I40" s="64">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="J40" s="95"/>
       <c r="K40" s="107"/>
       <c r="L40" s="107"/>
       <c r="M40" s="107"/>
@@ -7723,28 +7880,33 @@
       <c r="BM40" s="107"/>
       <c r="BN40" s="107"/>
     </row>
-    <row r="41" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A41" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
-        <v>1.1.1.1</v>
-      </c>
-      <c r="B41" s="82" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" s="81"/>
-      <c r="D41" s="79"/>
-      <c r="E41" s="100"/>
-      <c r="F41" s="101" t="str">
-        <f t="shared" si="36"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G41" s="62"/>
-      <c r="H41" s="63"/>
-      <c r="I41" s="80" t="str">
-        <f t="shared" si="37"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J41" s="99"/>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>6.3</v>
+      </c>
+      <c r="B41" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="127"/>
+      <c r="E41" s="100">
+        <v>43131</v>
+      </c>
+      <c r="F41" s="101">
+        <f t="shared" si="35"/>
+        <v>43131</v>
+      </c>
+      <c r="G41" s="62">
+        <v>1</v>
+      </c>
+      <c r="H41" s="63">
+        <v>0</v>
+      </c>
+      <c r="I41" s="64">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="J41" s="95"/>
       <c r="K41" s="107"/>
       <c r="L41" s="107"/>
       <c r="M41" s="107"/>
@@ -7802,86 +7964,851 @@
       <c r="BM41" s="107"/>
       <c r="BN41" s="107"/>
     </row>
-    <row r="42" spans="1:66" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="30"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="31"/>
-      <c r="I42" s="31"/>
-      <c r="J42" s="31"/>
-      <c r="K42" s="31"/>
-      <c r="L42" s="31"/>
-      <c r="M42" s="31"/>
-      <c r="N42" s="31"/>
-      <c r="O42" s="31"/>
-      <c r="P42" s="31"/>
-      <c r="Q42" s="31"/>
-      <c r="R42" s="31"/>
-      <c r="S42" s="31"/>
-      <c r="T42" s="31"/>
-      <c r="U42" s="31"/>
-      <c r="V42" s="31"/>
-      <c r="W42" s="31"/>
-      <c r="X42" s="31"/>
-      <c r="Y42" s="31"/>
-      <c r="Z42" s="31"/>
-      <c r="AA42" s="31"/>
-      <c r="AB42" s="31"/>
-      <c r="AC42" s="31"/>
-      <c r="AD42" s="31"/>
-      <c r="AE42" s="31"/>
-      <c r="AF42" s="31"/>
-      <c r="AG42" s="31"/>
-      <c r="AH42" s="31"/>
-      <c r="AI42" s="31"/>
-      <c r="AJ42" s="31"/>
-      <c r="AK42" s="31"/>
-      <c r="AL42" s="31"/>
-      <c r="AM42" s="31"/>
-      <c r="AN42" s="31"/>
-      <c r="AO42" s="31"/>
-      <c r="AP42" s="31"/>
-      <c r="AQ42" s="31"/>
-      <c r="AR42" s="31"/>
-      <c r="AS42" s="31"/>
-      <c r="AT42" s="31"/>
-      <c r="AU42" s="31"/>
-      <c r="AV42" s="31"/>
-      <c r="AW42" s="31"/>
-      <c r="AX42" s="31"/>
-      <c r="AY42" s="31"/>
-      <c r="AZ42" s="31"/>
-      <c r="BA42" s="31"/>
-      <c r="BB42" s="31"/>
-      <c r="BC42" s="31"/>
-      <c r="BD42" s="31"/>
-      <c r="BE42" s="31"/>
-      <c r="BF42" s="31"/>
-      <c r="BG42" s="31"/>
-      <c r="BH42" s="31"/>
-      <c r="BI42" s="31"/>
-      <c r="BJ42" s="31"/>
-      <c r="BK42" s="31"/>
-      <c r="BL42" s="31"/>
-      <c r="BM42" s="31"/>
-      <c r="BN42" s="31"/>
+    <row r="42" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>6.4</v>
+      </c>
+      <c r="B42" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="127"/>
+      <c r="E42" s="100">
+        <v>43132</v>
+      </c>
+      <c r="F42" s="101">
+        <f t="shared" si="35"/>
+        <v>43132</v>
+      </c>
+      <c r="G42" s="62">
+        <v>1</v>
+      </c>
+      <c r="H42" s="63">
+        <v>0</v>
+      </c>
+      <c r="I42" s="64">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="J42" s="95"/>
+      <c r="K42" s="107"/>
+      <c r="L42" s="107"/>
+      <c r="M42" s="107"/>
+      <c r="N42" s="107"/>
+      <c r="O42" s="107"/>
+      <c r="P42" s="107"/>
+      <c r="Q42" s="107"/>
+      <c r="R42" s="107"/>
+      <c r="S42" s="107"/>
+      <c r="T42" s="107"/>
+      <c r="U42" s="107"/>
+      <c r="V42" s="107"/>
+      <c r="W42" s="107"/>
+      <c r="X42" s="107"/>
+      <c r="Y42" s="107"/>
+      <c r="Z42" s="107"/>
+      <c r="AA42" s="107"/>
+      <c r="AB42" s="107"/>
+      <c r="AC42" s="107"/>
+      <c r="AD42" s="107"/>
+      <c r="AE42" s="107"/>
+      <c r="AF42" s="107"/>
+      <c r="AG42" s="107"/>
+      <c r="AH42" s="107"/>
+      <c r="AI42" s="107"/>
+      <c r="AJ42" s="107"/>
+      <c r="AK42" s="107"/>
+      <c r="AL42" s="107"/>
+      <c r="AM42" s="107"/>
+      <c r="AN42" s="107"/>
+      <c r="AO42" s="107"/>
+      <c r="AP42" s="107"/>
+      <c r="AQ42" s="107"/>
+      <c r="AR42" s="107"/>
+      <c r="AS42" s="107"/>
+      <c r="AT42" s="107"/>
+      <c r="AU42" s="107"/>
+      <c r="AV42" s="107"/>
+      <c r="AW42" s="107"/>
+      <c r="AX42" s="107"/>
+      <c r="AY42" s="107"/>
+      <c r="AZ42" s="107"/>
+      <c r="BA42" s="107"/>
+      <c r="BB42" s="107"/>
+      <c r="BC42" s="107"/>
+      <c r="BD42" s="107"/>
+      <c r="BE42" s="107"/>
+      <c r="BF42" s="107"/>
+      <c r="BG42" s="107"/>
+      <c r="BH42" s="107"/>
+      <c r="BI42" s="107"/>
+      <c r="BJ42" s="107"/>
+      <c r="BK42" s="107"/>
+      <c r="BL42" s="107"/>
+      <c r="BM42" s="107"/>
+      <c r="BN42" s="107"/>
+    </row>
+    <row r="43" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>6.5</v>
+      </c>
+      <c r="B43" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="127"/>
+      <c r="E43" s="100">
+        <v>43133</v>
+      </c>
+      <c r="F43" s="101">
+        <f t="shared" si="35"/>
+        <v>43133</v>
+      </c>
+      <c r="G43" s="62">
+        <v>1</v>
+      </c>
+      <c r="H43" s="63">
+        <v>0</v>
+      </c>
+      <c r="I43" s="64">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="J43" s="95"/>
+      <c r="K43" s="107"/>
+      <c r="L43" s="107"/>
+      <c r="M43" s="107"/>
+      <c r="N43" s="107"/>
+      <c r="O43" s="107"/>
+      <c r="P43" s="107"/>
+      <c r="Q43" s="107"/>
+      <c r="R43" s="107"/>
+      <c r="S43" s="107"/>
+      <c r="T43" s="107"/>
+      <c r="U43" s="107"/>
+      <c r="V43" s="107"/>
+      <c r="W43" s="107"/>
+      <c r="X43" s="107"/>
+      <c r="Y43" s="107"/>
+      <c r="Z43" s="107"/>
+      <c r="AA43" s="107"/>
+      <c r="AB43" s="107"/>
+      <c r="AC43" s="107"/>
+      <c r="AD43" s="107"/>
+      <c r="AE43" s="107"/>
+      <c r="AF43" s="107"/>
+      <c r="AG43" s="107"/>
+      <c r="AH43" s="107"/>
+      <c r="AI43" s="107"/>
+      <c r="AJ43" s="107"/>
+      <c r="AK43" s="107"/>
+      <c r="AL43" s="107"/>
+      <c r="AM43" s="107"/>
+      <c r="AN43" s="107"/>
+      <c r="AO43" s="107"/>
+      <c r="AP43" s="107"/>
+      <c r="AQ43" s="107"/>
+      <c r="AR43" s="107"/>
+      <c r="AS43" s="107"/>
+      <c r="AT43" s="107"/>
+      <c r="AU43" s="107"/>
+      <c r="AV43" s="107"/>
+      <c r="AW43" s="107"/>
+      <c r="AX43" s="107"/>
+      <c r="AY43" s="107"/>
+      <c r="AZ43" s="107"/>
+      <c r="BA43" s="107"/>
+      <c r="BB43" s="107"/>
+      <c r="BC43" s="107"/>
+      <c r="BD43" s="107"/>
+      <c r="BE43" s="107"/>
+      <c r="BF43" s="107"/>
+      <c r="BG43" s="107"/>
+      <c r="BH43" s="107"/>
+      <c r="BI43" s="107"/>
+      <c r="BJ43" s="107"/>
+      <c r="BK43" s="107"/>
+      <c r="BL43" s="107"/>
+      <c r="BM43" s="107"/>
+      <c r="BN43" s="107"/>
+    </row>
+    <row r="44" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="60"/>
+      <c r="B44" s="65"/>
+      <c r="C44" s="65"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="103"/>
+      <c r="F44" s="103"/>
+      <c r="G44" s="67"/>
+      <c r="H44" s="68"/>
+      <c r="I44" s="69" t="str">
+        <f t="shared" si="33"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J44" s="97"/>
+      <c r="K44" s="107"/>
+      <c r="L44" s="107"/>
+      <c r="M44" s="107"/>
+      <c r="N44" s="107"/>
+      <c r="O44" s="107"/>
+      <c r="P44" s="107"/>
+      <c r="Q44" s="107"/>
+      <c r="R44" s="107"/>
+      <c r="S44" s="107"/>
+      <c r="T44" s="107"/>
+      <c r="U44" s="107"/>
+      <c r="V44" s="107"/>
+      <c r="W44" s="107"/>
+      <c r="X44" s="107"/>
+      <c r="Y44" s="107"/>
+      <c r="Z44" s="107"/>
+      <c r="AA44" s="107"/>
+      <c r="AB44" s="107"/>
+      <c r="AC44" s="107"/>
+      <c r="AD44" s="107"/>
+      <c r="AE44" s="107"/>
+      <c r="AF44" s="107"/>
+      <c r="AG44" s="107"/>
+      <c r="AH44" s="107"/>
+      <c r="AI44" s="107"/>
+      <c r="AJ44" s="107"/>
+      <c r="AK44" s="107"/>
+      <c r="AL44" s="107"/>
+      <c r="AM44" s="107"/>
+      <c r="AN44" s="107"/>
+      <c r="AO44" s="107"/>
+      <c r="AP44" s="107"/>
+      <c r="AQ44" s="107"/>
+      <c r="AR44" s="107"/>
+      <c r="AS44" s="107"/>
+      <c r="AT44" s="107"/>
+      <c r="AU44" s="107"/>
+      <c r="AV44" s="107"/>
+      <c r="AW44" s="107"/>
+      <c r="AX44" s="107"/>
+      <c r="AY44" s="107"/>
+      <c r="AZ44" s="107"/>
+      <c r="BA44" s="107"/>
+      <c r="BB44" s="107"/>
+      <c r="BC44" s="107"/>
+      <c r="BD44" s="107"/>
+      <c r="BE44" s="107"/>
+      <c r="BF44" s="107"/>
+      <c r="BG44" s="107"/>
+      <c r="BH44" s="107"/>
+      <c r="BI44" s="107"/>
+      <c r="BJ44" s="107"/>
+      <c r="BK44" s="107"/>
+      <c r="BL44" s="107"/>
+      <c r="BM44" s="107"/>
+      <c r="BN44" s="107"/>
+    </row>
+    <row r="45" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="60"/>
+      <c r="B45" s="65"/>
+      <c r="C45" s="65"/>
+      <c r="D45" s="66"/>
+      <c r="E45" s="103"/>
+      <c r="F45" s="103"/>
+      <c r="G45" s="67"/>
+      <c r="H45" s="68"/>
+      <c r="I45" s="69" t="str">
+        <f t="shared" si="33"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J45" s="97"/>
+      <c r="K45" s="107"/>
+      <c r="L45" s="107"/>
+      <c r="M45" s="107"/>
+      <c r="N45" s="107"/>
+      <c r="O45" s="107"/>
+      <c r="P45" s="107"/>
+      <c r="Q45" s="107"/>
+      <c r="R45" s="107"/>
+      <c r="S45" s="107"/>
+      <c r="T45" s="107"/>
+      <c r="U45" s="107"/>
+      <c r="V45" s="107"/>
+      <c r="W45" s="107"/>
+      <c r="X45" s="107"/>
+      <c r="Y45" s="107"/>
+      <c r="Z45" s="107"/>
+      <c r="AA45" s="107"/>
+      <c r="AB45" s="107"/>
+      <c r="AC45" s="107"/>
+      <c r="AD45" s="107"/>
+      <c r="AE45" s="107"/>
+      <c r="AF45" s="107"/>
+      <c r="AG45" s="107"/>
+      <c r="AH45" s="107"/>
+      <c r="AI45" s="107"/>
+      <c r="AJ45" s="107"/>
+      <c r="AK45" s="107"/>
+      <c r="AL45" s="107"/>
+      <c r="AM45" s="107"/>
+      <c r="AN45" s="107"/>
+      <c r="AO45" s="107"/>
+      <c r="AP45" s="107"/>
+      <c r="AQ45" s="107"/>
+      <c r="AR45" s="107"/>
+      <c r="AS45" s="107"/>
+      <c r="AT45" s="107"/>
+      <c r="AU45" s="107"/>
+      <c r="AV45" s="107"/>
+      <c r="AW45" s="107"/>
+      <c r="AX45" s="107"/>
+      <c r="AY45" s="107"/>
+      <c r="AZ45" s="107"/>
+      <c r="BA45" s="107"/>
+      <c r="BB45" s="107"/>
+      <c r="BC45" s="107"/>
+      <c r="BD45" s="107"/>
+      <c r="BE45" s="107"/>
+      <c r="BF45" s="107"/>
+      <c r="BG45" s="107"/>
+      <c r="BH45" s="107"/>
+      <c r="BI45" s="107"/>
+      <c r="BJ45" s="107"/>
+      <c r="BK45" s="107"/>
+      <c r="BL45" s="107"/>
+      <c r="BM45" s="107"/>
+      <c r="BN45" s="107"/>
+    </row>
+    <row r="46" spans="1:66" s="75" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="72"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="73"/>
+      <c r="E46" s="104"/>
+      <c r="F46" s="104"/>
+      <c r="G46" s="74"/>
+      <c r="H46" s="74"/>
+      <c r="I46" s="74"/>
+      <c r="J46" s="98"/>
+      <c r="K46" s="107"/>
+      <c r="L46" s="107"/>
+      <c r="M46" s="107"/>
+      <c r="N46" s="107"/>
+      <c r="O46" s="107"/>
+      <c r="P46" s="107"/>
+      <c r="Q46" s="107"/>
+      <c r="R46" s="107"/>
+      <c r="S46" s="107"/>
+      <c r="T46" s="107"/>
+      <c r="U46" s="107"/>
+      <c r="V46" s="107"/>
+      <c r="W46" s="107"/>
+      <c r="X46" s="107"/>
+      <c r="Y46" s="107"/>
+      <c r="Z46" s="107"/>
+      <c r="AA46" s="107"/>
+      <c r="AB46" s="107"/>
+      <c r="AC46" s="107"/>
+      <c r="AD46" s="107"/>
+      <c r="AE46" s="107"/>
+      <c r="AF46" s="107"/>
+      <c r="AG46" s="107"/>
+      <c r="AH46" s="107"/>
+      <c r="AI46" s="107"/>
+      <c r="AJ46" s="107"/>
+      <c r="AK46" s="107"/>
+      <c r="AL46" s="107"/>
+      <c r="AM46" s="107"/>
+      <c r="AN46" s="107"/>
+      <c r="AO46" s="107"/>
+      <c r="AP46" s="107"/>
+      <c r="AQ46" s="107"/>
+      <c r="AR46" s="107"/>
+      <c r="AS46" s="107"/>
+      <c r="AT46" s="107"/>
+      <c r="AU46" s="107"/>
+      <c r="AV46" s="107"/>
+      <c r="AW46" s="107"/>
+      <c r="AX46" s="107"/>
+      <c r="AY46" s="107"/>
+      <c r="AZ46" s="107"/>
+      <c r="BA46" s="107"/>
+      <c r="BB46" s="107"/>
+      <c r="BC46" s="107"/>
+      <c r="BD46" s="107"/>
+      <c r="BE46" s="107"/>
+      <c r="BF46" s="107"/>
+      <c r="BG46" s="107"/>
+      <c r="BH46" s="107"/>
+      <c r="BI46" s="107"/>
+      <c r="BJ46" s="107"/>
+      <c r="BK46" s="107"/>
+      <c r="BL46" s="107"/>
+      <c r="BM46" s="107"/>
+      <c r="BN46" s="107"/>
+    </row>
+    <row r="47" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="B47" s="77"/>
+      <c r="C47" s="77"/>
+      <c r="D47" s="77"/>
+      <c r="E47" s="105"/>
+      <c r="F47" s="105"/>
+      <c r="G47" s="77"/>
+      <c r="H47" s="77"/>
+      <c r="I47" s="77"/>
+      <c r="J47" s="98"/>
+      <c r="K47" s="107"/>
+      <c r="L47" s="107"/>
+      <c r="M47" s="107"/>
+      <c r="N47" s="107"/>
+      <c r="O47" s="107"/>
+      <c r="P47" s="107"/>
+      <c r="Q47" s="107"/>
+      <c r="R47" s="107"/>
+      <c r="S47" s="107"/>
+      <c r="T47" s="107"/>
+      <c r="U47" s="107"/>
+      <c r="V47" s="107"/>
+      <c r="W47" s="107"/>
+      <c r="X47" s="107"/>
+      <c r="Y47" s="107"/>
+      <c r="Z47" s="107"/>
+      <c r="AA47" s="107"/>
+      <c r="AB47" s="107"/>
+      <c r="AC47" s="107"/>
+      <c r="AD47" s="107"/>
+      <c r="AE47" s="107"/>
+      <c r="AF47" s="107"/>
+      <c r="AG47" s="107"/>
+      <c r="AH47" s="107"/>
+      <c r="AI47" s="107"/>
+      <c r="AJ47" s="107"/>
+      <c r="AK47" s="107"/>
+      <c r="AL47" s="107"/>
+      <c r="AM47" s="107"/>
+      <c r="AN47" s="107"/>
+      <c r="AO47" s="107"/>
+      <c r="AP47" s="107"/>
+      <c r="AQ47" s="107"/>
+      <c r="AR47" s="107"/>
+      <c r="AS47" s="107"/>
+      <c r="AT47" s="107"/>
+      <c r="AU47" s="107"/>
+      <c r="AV47" s="107"/>
+      <c r="AW47" s="107"/>
+      <c r="AX47" s="107"/>
+      <c r="AY47" s="107"/>
+      <c r="AZ47" s="107"/>
+      <c r="BA47" s="107"/>
+      <c r="BB47" s="107"/>
+      <c r="BC47" s="107"/>
+      <c r="BD47" s="107"/>
+      <c r="BE47" s="107"/>
+      <c r="BF47" s="107"/>
+      <c r="BG47" s="107"/>
+      <c r="BH47" s="107"/>
+      <c r="BI47" s="107"/>
+      <c r="BJ47" s="107"/>
+      <c r="BK47" s="107"/>
+      <c r="BL47" s="107"/>
+      <c r="BM47" s="107"/>
+      <c r="BN47" s="107"/>
+    </row>
+    <row r="48" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="130" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>1</v>
+      </c>
+      <c r="B48" s="131" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" s="78"/>
+      <c r="D48" s="79"/>
+      <c r="E48" s="100"/>
+      <c r="F48" s="101" t="str">
+        <f t="shared" ref="F48:F51" si="39">IF(ISBLANK(E48)," - ",IF(G48=0,E48,E48+G48-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G48" s="62"/>
+      <c r="H48" s="63"/>
+      <c r="I48" s="80" t="str">
+        <f>IF(OR(F48=0,E48=0)," - ",NETWORKDAYS(E48,F48))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J48" s="99"/>
+      <c r="K48" s="107"/>
+      <c r="L48" s="107"/>
+      <c r="M48" s="107"/>
+      <c r="N48" s="107"/>
+      <c r="O48" s="107"/>
+      <c r="P48" s="107"/>
+      <c r="Q48" s="107"/>
+      <c r="R48" s="107"/>
+      <c r="S48" s="107"/>
+      <c r="T48" s="107"/>
+      <c r="U48" s="107"/>
+      <c r="V48" s="107"/>
+      <c r="W48" s="107"/>
+      <c r="X48" s="107"/>
+      <c r="Y48" s="107"/>
+      <c r="Z48" s="107"/>
+      <c r="AA48" s="107"/>
+      <c r="AB48" s="107"/>
+      <c r="AC48" s="107"/>
+      <c r="AD48" s="107"/>
+      <c r="AE48" s="107"/>
+      <c r="AF48" s="107"/>
+      <c r="AG48" s="107"/>
+      <c r="AH48" s="107"/>
+      <c r="AI48" s="107"/>
+      <c r="AJ48" s="107"/>
+      <c r="AK48" s="107"/>
+      <c r="AL48" s="107"/>
+      <c r="AM48" s="107"/>
+      <c r="AN48" s="107"/>
+      <c r="AO48" s="107"/>
+      <c r="AP48" s="107"/>
+      <c r="AQ48" s="107"/>
+      <c r="AR48" s="107"/>
+      <c r="AS48" s="107"/>
+      <c r="AT48" s="107"/>
+      <c r="AU48" s="107"/>
+      <c r="AV48" s="107"/>
+      <c r="AW48" s="107"/>
+      <c r="AX48" s="107"/>
+      <c r="AY48" s="107"/>
+      <c r="AZ48" s="107"/>
+      <c r="BA48" s="107"/>
+      <c r="BB48" s="107"/>
+      <c r="BC48" s="107"/>
+      <c r="BD48" s="107"/>
+      <c r="BE48" s="107"/>
+      <c r="BF48" s="107"/>
+      <c r="BG48" s="107"/>
+      <c r="BH48" s="107"/>
+      <c r="BI48" s="107"/>
+      <c r="BJ48" s="107"/>
+      <c r="BK48" s="107"/>
+      <c r="BL48" s="107"/>
+      <c r="BM48" s="107"/>
+      <c r="BN48" s="107"/>
+    </row>
+    <row r="49" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>1.1</v>
+      </c>
+      <c r="B49" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="81"/>
+      <c r="D49" s="79"/>
+      <c r="E49" s="100"/>
+      <c r="F49" s="101" t="str">
+        <f t="shared" si="39"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G49" s="62"/>
+      <c r="H49" s="63"/>
+      <c r="I49" s="80" t="str">
+        <f t="shared" ref="I49:I51" si="40">IF(OR(F49=0,E49=0)," - ",NETWORKDAYS(E49,F49))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J49" s="99"/>
+      <c r="K49" s="107"/>
+      <c r="L49" s="107"/>
+      <c r="M49" s="107"/>
+      <c r="N49" s="107"/>
+      <c r="O49" s="107"/>
+      <c r="P49" s="107"/>
+      <c r="Q49" s="107"/>
+      <c r="R49" s="107"/>
+      <c r="S49" s="107"/>
+      <c r="T49" s="107"/>
+      <c r="U49" s="107"/>
+      <c r="V49" s="107"/>
+      <c r="W49" s="107"/>
+      <c r="X49" s="107"/>
+      <c r="Y49" s="107"/>
+      <c r="Z49" s="107"/>
+      <c r="AA49" s="107"/>
+      <c r="AB49" s="107"/>
+      <c r="AC49" s="107"/>
+      <c r="AD49" s="107"/>
+      <c r="AE49" s="107"/>
+      <c r="AF49" s="107"/>
+      <c r="AG49" s="107"/>
+      <c r="AH49" s="107"/>
+      <c r="AI49" s="107"/>
+      <c r="AJ49" s="107"/>
+      <c r="AK49" s="107"/>
+      <c r="AL49" s="107"/>
+      <c r="AM49" s="107"/>
+      <c r="AN49" s="107"/>
+      <c r="AO49" s="107"/>
+      <c r="AP49" s="107"/>
+      <c r="AQ49" s="107"/>
+      <c r="AR49" s="107"/>
+      <c r="AS49" s="107"/>
+      <c r="AT49" s="107"/>
+      <c r="AU49" s="107"/>
+      <c r="AV49" s="107"/>
+      <c r="AW49" s="107"/>
+      <c r="AX49" s="107"/>
+      <c r="AY49" s="107"/>
+      <c r="AZ49" s="107"/>
+      <c r="BA49" s="107"/>
+      <c r="BB49" s="107"/>
+      <c r="BC49" s="107"/>
+      <c r="BD49" s="107"/>
+      <c r="BE49" s="107"/>
+      <c r="BF49" s="107"/>
+      <c r="BG49" s="107"/>
+      <c r="BH49" s="107"/>
+      <c r="BI49" s="107"/>
+      <c r="BJ49" s="107"/>
+      <c r="BK49" s="107"/>
+      <c r="BL49" s="107"/>
+      <c r="BM49" s="107"/>
+      <c r="BN49" s="107"/>
+    </row>
+    <row r="50" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <v>1.1.1</v>
+      </c>
+      <c r="B50" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="81"/>
+      <c r="D50" s="79"/>
+      <c r="E50" s="100"/>
+      <c r="F50" s="101" t="str">
+        <f t="shared" si="39"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G50" s="62"/>
+      <c r="H50" s="63"/>
+      <c r="I50" s="80" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J50" s="99"/>
+      <c r="K50" s="107"/>
+      <c r="L50" s="107"/>
+      <c r="M50" s="107"/>
+      <c r="N50" s="107"/>
+      <c r="O50" s="107"/>
+      <c r="P50" s="107"/>
+      <c r="Q50" s="107"/>
+      <c r="R50" s="107"/>
+      <c r="S50" s="107"/>
+      <c r="T50" s="107"/>
+      <c r="U50" s="107"/>
+      <c r="V50" s="107"/>
+      <c r="W50" s="107"/>
+      <c r="X50" s="107"/>
+      <c r="Y50" s="107"/>
+      <c r="Z50" s="107"/>
+      <c r="AA50" s="107"/>
+      <c r="AB50" s="107"/>
+      <c r="AC50" s="107"/>
+      <c r="AD50" s="107"/>
+      <c r="AE50" s="107"/>
+      <c r="AF50" s="107"/>
+      <c r="AG50" s="107"/>
+      <c r="AH50" s="107"/>
+      <c r="AI50" s="107"/>
+      <c r="AJ50" s="107"/>
+      <c r="AK50" s="107"/>
+      <c r="AL50" s="107"/>
+      <c r="AM50" s="107"/>
+      <c r="AN50" s="107"/>
+      <c r="AO50" s="107"/>
+      <c r="AP50" s="107"/>
+      <c r="AQ50" s="107"/>
+      <c r="AR50" s="107"/>
+      <c r="AS50" s="107"/>
+      <c r="AT50" s="107"/>
+      <c r="AU50" s="107"/>
+      <c r="AV50" s="107"/>
+      <c r="AW50" s="107"/>
+      <c r="AX50" s="107"/>
+      <c r="AY50" s="107"/>
+      <c r="AZ50" s="107"/>
+      <c r="BA50" s="107"/>
+      <c r="BB50" s="107"/>
+      <c r="BC50" s="107"/>
+      <c r="BD50" s="107"/>
+      <c r="BE50" s="107"/>
+      <c r="BF50" s="107"/>
+      <c r="BG50" s="107"/>
+      <c r="BH50" s="107"/>
+      <c r="BI50" s="107"/>
+      <c r="BJ50" s="107"/>
+      <c r="BK50" s="107"/>
+      <c r="BL50" s="107"/>
+      <c r="BM50" s="107"/>
+      <c r="BN50" s="107"/>
+    </row>
+    <row r="51" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
+        <v>1.1.1.1</v>
+      </c>
+      <c r="B51" s="82" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" s="81"/>
+      <c r="D51" s="79"/>
+      <c r="E51" s="100"/>
+      <c r="F51" s="101" t="str">
+        <f t="shared" si="39"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G51" s="62"/>
+      <c r="H51" s="63"/>
+      <c r="I51" s="80" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J51" s="99"/>
+      <c r="K51" s="107"/>
+      <c r="L51" s="107"/>
+      <c r="M51" s="107"/>
+      <c r="N51" s="107"/>
+      <c r="O51" s="107"/>
+      <c r="P51" s="107"/>
+      <c r="Q51" s="107"/>
+      <c r="R51" s="107"/>
+      <c r="S51" s="107"/>
+      <c r="T51" s="107"/>
+      <c r="U51" s="107"/>
+      <c r="V51" s="107"/>
+      <c r="W51" s="107"/>
+      <c r="X51" s="107"/>
+      <c r="Y51" s="107"/>
+      <c r="Z51" s="107"/>
+      <c r="AA51" s="107"/>
+      <c r="AB51" s="107"/>
+      <c r="AC51" s="107"/>
+      <c r="AD51" s="107"/>
+      <c r="AE51" s="107"/>
+      <c r="AF51" s="107"/>
+      <c r="AG51" s="107"/>
+      <c r="AH51" s="107"/>
+      <c r="AI51" s="107"/>
+      <c r="AJ51" s="107"/>
+      <c r="AK51" s="107"/>
+      <c r="AL51" s="107"/>
+      <c r="AM51" s="107"/>
+      <c r="AN51" s="107"/>
+      <c r="AO51" s="107"/>
+      <c r="AP51" s="107"/>
+      <c r="AQ51" s="107"/>
+      <c r="AR51" s="107"/>
+      <c r="AS51" s="107"/>
+      <c r="AT51" s="107"/>
+      <c r="AU51" s="107"/>
+      <c r="AV51" s="107"/>
+      <c r="AW51" s="107"/>
+      <c r="AX51" s="107"/>
+      <c r="AY51" s="107"/>
+      <c r="AZ51" s="107"/>
+      <c r="BA51" s="107"/>
+      <c r="BB51" s="107"/>
+      <c r="BC51" s="107"/>
+      <c r="BD51" s="107"/>
+      <c r="BE51" s="107"/>
+      <c r="BF51" s="107"/>
+      <c r="BG51" s="107"/>
+      <c r="BH51" s="107"/>
+      <c r="BI51" s="107"/>
+      <c r="BJ51" s="107"/>
+      <c r="BK51" s="107"/>
+      <c r="BL51" s="107"/>
+      <c r="BM51" s="107"/>
+      <c r="BN51" s="107"/>
+    </row>
+    <row r="52" spans="1:66" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="30"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
+      <c r="H52" s="31"/>
+      <c r="I52" s="31"/>
+      <c r="J52" s="31"/>
+      <c r="K52" s="31"/>
+      <c r="L52" s="31"/>
+      <c r="M52" s="31"/>
+      <c r="N52" s="31"/>
+      <c r="O52" s="31"/>
+      <c r="P52" s="31"/>
+      <c r="Q52" s="31"/>
+      <c r="R52" s="31"/>
+      <c r="S52" s="31"/>
+      <c r="T52" s="31"/>
+      <c r="U52" s="31"/>
+      <c r="V52" s="31"/>
+      <c r="W52" s="31"/>
+      <c r="X52" s="31"/>
+      <c r="Y52" s="31"/>
+      <c r="Z52" s="31"/>
+      <c r="AA52" s="31"/>
+      <c r="AB52" s="31"/>
+      <c r="AC52" s="31"/>
+      <c r="AD52" s="31"/>
+      <c r="AE52" s="31"/>
+      <c r="AF52" s="31"/>
+      <c r="AG52" s="31"/>
+      <c r="AH52" s="31"/>
+      <c r="AI52" s="31"/>
+      <c r="AJ52" s="31"/>
+      <c r="AK52" s="31"/>
+      <c r="AL52" s="31"/>
+      <c r="AM52" s="31"/>
+      <c r="AN52" s="31"/>
+      <c r="AO52" s="31"/>
+      <c r="AP52" s="31"/>
+      <c r="AQ52" s="31"/>
+      <c r="AR52" s="31"/>
+      <c r="AS52" s="31"/>
+      <c r="AT52" s="31"/>
+      <c r="AU52" s="31"/>
+      <c r="AV52" s="31"/>
+      <c r="AW52" s="31"/>
+      <c r="AX52" s="31"/>
+      <c r="AY52" s="31"/>
+      <c r="AZ52" s="31"/>
+      <c r="BA52" s="31"/>
+      <c r="BB52" s="31"/>
+      <c r="BC52" s="31"/>
+      <c r="BD52" s="31"/>
+      <c r="BE52" s="31"/>
+      <c r="BF52" s="31"/>
+      <c r="BG52" s="31"/>
+      <c r="BH52" s="31"/>
+      <c r="BI52" s="31"/>
+      <c r="BJ52" s="31"/>
+      <c r="BK52" s="31"/>
+      <c r="BL52" s="31"/>
+      <c r="BM52" s="31"/>
+      <c r="BN52" s="31"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="27">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="CJ4:CP4"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BO4:BU4"/>
+    <mergeCell ref="BV4:CB4"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="CC5:CI5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -7892,18 +8819,19 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="CJ4:CP4"/>
-    <mergeCell ref="CJ5:CP5"/>
-    <mergeCell ref="BO5:BU5"/>
-    <mergeCell ref="BO4:BU4"/>
-    <mergeCell ref="BV4:CB4"/>
-    <mergeCell ref="BV5:CB5"/>
-    <mergeCell ref="CC4:CI4"/>
-    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H8:H41">
-    <cfRule type="dataBar" priority="10">
+  <conditionalFormatting sqref="H8:H27 H38:H51">
+    <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7917,61 +8845,134 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN7">
-    <cfRule type="expression" dxfId="11" priority="53">
+    <cfRule type="expression" dxfId="18" priority="63">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BN41">
-    <cfRule type="expression" dxfId="10" priority="56">
+  <conditionalFormatting sqref="K8:BN27 K38:BN51">
+    <cfRule type="expression" dxfId="17" priority="66">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="57">
+    <cfRule type="expression" dxfId="16" priority="67">
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:BN41">
-    <cfRule type="expression" dxfId="8" priority="16">
+  <conditionalFormatting sqref="K6:BN27 K38:BN51">
+    <cfRule type="expression" dxfId="15" priority="26">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO6:BU7">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="14" priority="18">
       <formula>BO$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO6:BU7">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="13" priority="17">
       <formula>BO$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV6:CB7">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="12" priority="16">
       <formula>BV$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV6:CB7">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="11" priority="15">
       <formula>BV$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC6:CI7">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="10" priority="14">
       <formula>CC$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC6:CI7">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="9" priority="13">
       <formula>CC$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ6:CP7">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="8" priority="12">
       <formula>CJ$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ6:CP7">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="7" priority="11">
       <formula>CJ$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K32:BN37">
+    <cfRule type="expression" dxfId="6" priority="9">
+      <formula>AND($E32&lt;=K$6,ROUNDDOWN(($F32-$E32+1)*$H32,0)+$E32-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="10">
+      <formula>AND(NOT(ISBLANK($E32)),$E32&lt;=K$6,$F32&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28:H31">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{FE744373-948F-4DF4-9B3E-95C2E34DC4FE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K28:BN31">
+    <cfRule type="expression" dxfId="4" priority="7">
+      <formula>AND($E28&lt;=K$6,ROUNDDOWN(($F28-$E28+1)*$H28,0)+$E28-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="8">
+      <formula>AND(NOT(ISBLANK($E28)),$E28&lt;=K$6,$F28&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K28:BN31">
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32:H35">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D1031EA8-9A20-464F-8924-40F8769CD1E1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36:H37">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5DB45CD5-8AFF-4405-9C9C-03F0C97B1A7F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K36:BN37">
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K32:BN35">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
@@ -7984,8 +8985,8 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 A34:B35 B29 B30:B32 A37:B37 B36 E16 E22 E28 E34:H37 G14 G11 G16:H16 G22:H22 G28:H32 G38 G39:G40 G41 H23:H26" unlockedFormula="1"/>
-    <ignoredError sqref="A28 A22 A16" formula="1"/>
+    <ignoredError sqref="H9 A44:B45 B39 B40:B42 A47:B47 B46 E16 E22 E38 E44:H47 G14 G11 G16:H16 G22:H22 G38:H42 G48 G49:G50 G51 H23:H26" unlockedFormula="1"/>
+    <ignoredError sqref="A38 A22 A16" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
@@ -8001,11 +9002,11 @@
                     <xdr:col>9</xdr:col>
                     <xdr:colOff>95250</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>127000</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>27</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>107950</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>114300</xdr:rowOff>
                   </to>
@@ -8033,7 +9034,52 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H8:H41</xm:sqref>
+          <xm:sqref>H8:H27 H38:H51</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{FE744373-948F-4DF4-9B3E-95C2E34DC4FE}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H28:H31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D1031EA8-9A20-464F-8924-40F8769CD1E1}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H32:H35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5DB45CD5-8AFF-4405-9C9C-03F0C97B1A7F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H36:H37</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -8052,175 +9098,175 @@
       <selection activeCell="A16" sqref="A16:C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" style="16" customWidth="1"/>
-    <col min="3" max="3" width="55.140625" style="16" customWidth="1"/>
-    <col min="4" max="7" width="8.85546875" style="16"/>
+    <col min="1" max="1" width="5.54296875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="37.7265625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="55.1796875" style="16" customWidth="1"/>
+    <col min="4" max="7" width="8.81640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="C4" s="23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" s="20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" s="20"/>
     </row>
-    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
       <c r="C7" s="24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" s="25" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" s="20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" s="20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
       <c r="C13" s="24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.3">
       <c r="B18" s="26" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B22" s="26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B26" s="26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" ht="14" x14ac:dyDescent="0.3">
       <c r="B34" s="26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="20" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="20" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="20" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" ht="14" x14ac:dyDescent="0.3">
       <c r="B39" s="26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B42" s="26" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="20" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="2:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:2" ht="17.5" x14ac:dyDescent="0.35">
       <c r="B46" s="24" t="s">
         <v>24</v>
       </c>
@@ -8246,74 +9292,74 @@
       <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="90.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="7"/>
+    <col min="1" max="1" width="5.54296875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="90.453125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>124</v>
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="42"/>
     </row>
-    <row r="2" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="138" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="8"/>
     </row>
-    <row r="3" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="9"/>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A4" s="133" t="s">
         <v>91</v>
       </c>
       <c r="B4" s="39"/>
     </row>
-    <row r="5" spans="1:3" s="8" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="8" customFormat="1" ht="56" x14ac:dyDescent="0.3">
       <c r="B5" s="139" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="B7" s="139" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.3">
       <c r="B9" s="138" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="B11" s="137" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A13" s="172" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="172"/>
     </row>
-    <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:3" s="134" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:3" s="134" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A15" s="142"/>
       <c r="B15" s="140" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="134" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" s="134" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A16" s="142"/>
       <c r="B16" s="141" t="s">
         <v>81</v>
@@ -8322,25 +9368,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A17" s="143"/>
       <c r="B17" s="141" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" s="20" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A18" s="143"/>
       <c r="B18" s="141" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" s="42" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A19" s="146"/>
       <c r="B19" s="141" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="134" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" s="134" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
       <c r="A20" s="142"/>
       <c r="B20" s="140" t="s">
         <v>82</v>
@@ -8349,153 +9395,153 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A21" s="143"/>
       <c r="B21" s="141" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A22" s="144"/>
       <c r="B22" s="145" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A23" s="144"/>
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A24" s="172" t="s">
         <v>87</v>
       </c>
       <c r="B24" s="172"/>
     </row>
-    <row r="25" spans="1:3" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" s="8" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A25" s="144"/>
       <c r="B25" s="141" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A26" s="144"/>
       <c r="B26" s="141"/>
     </row>
-    <row r="27" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A27" s="144"/>
       <c r="B27" s="162" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A28" s="144"/>
       <c r="B28" s="141" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A29" s="144"/>
       <c r="B29" s="141" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A30" s="144"/>
       <c r="B30" s="141"/>
     </row>
-    <row r="31" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A31" s="144"/>
       <c r="B31" s="162" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A32" s="144"/>
       <c r="B32" s="141" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A33" s="144"/>
       <c r="B33" s="141" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A34" s="144"/>
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A35" s="144"/>
       <c r="B35" s="141" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A36" s="144"/>
       <c r="B36" s="147" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A37" s="144"/>
       <c r="B37" s="10"/>
     </row>
-    <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A38" s="172" t="s">
         <v>11</v>
       </c>
       <c r="B38" s="172"/>
     </row>
-    <row r="39" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" ht="28" x14ac:dyDescent="0.25">
       <c r="B39" s="141" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:2" s="20" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:2" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.25">
       <c r="B41" s="141" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:2" s="20" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:2" s="20" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="B43" s="141" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:2" ht="28" x14ac:dyDescent="0.25">
       <c r="B45" s="141" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B46" s="21"/>
     </row>
-    <row r="47" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" ht="28" x14ac:dyDescent="0.25">
       <c r="B47" s="141" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" s="11"/>
     </row>
-    <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A49" s="172" t="s">
         <v>7</v>
       </c>
       <c r="B49" s="172"/>
     </row>
-    <row r="50" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" ht="28" x14ac:dyDescent="0.25">
       <c r="B50" s="141" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B51" s="11"/>
     </row>
-    <row r="52" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A52" s="148" t="s">
         <v>12</v>
       </c>
@@ -8503,7 +9549,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A53" s="148" t="s">
         <v>14</v>
       </c>
@@ -8511,7 +9557,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A54" s="148" t="s">
         <v>16</v>
       </c>
@@ -8519,19 +9565,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A55" s="137"/>
       <c r="B55" s="141" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A56" s="137"/>
       <c r="B56" s="141" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A57" s="148" t="s">
         <v>18</v>
       </c>
@@ -8539,19 +9585,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A58" s="137"/>
       <c r="B58" s="141" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A59" s="137"/>
       <c r="B59" s="141" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A60" s="148" t="s">
         <v>20</v>
       </c>
@@ -8559,13 +9605,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A61" s="137"/>
       <c r="B61" s="141" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A62" s="148" t="s">
         <v>110</v>
       </c>
@@ -8573,36 +9619,36 @@
         <v>111</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A63" s="149"/>
       <c r="B63" s="141" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="12"/>
     </row>
-    <row r="65" spans="1:2" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" s="20" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A65" s="172" t="s">
         <v>10</v>
       </c>
       <c r="B65" s="172"/>
     </row>
-    <row r="66" spans="1:2" s="20" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" s="20" customFormat="1" ht="42" x14ac:dyDescent="0.25">
       <c r="B66" s="141" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="13"/>
     </row>
-    <row r="68" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A68" s="172" t="s">
         <v>5</v>
       </c>
       <c r="B68" s="172"/>
     </row>
-    <row r="69" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A69" s="156" t="s">
         <v>6</v>
       </c>
@@ -8610,17 +9656,17 @@
         <v>114</v>
       </c>
     </row>
-    <row r="70" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A70" s="150"/>
       <c r="B70" s="155" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A71" s="150"/>
       <c r="B71" s="151"/>
     </row>
-    <row r="72" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A72" s="156" t="s">
         <v>6</v>
       </c>
@@ -8628,17 +9674,17 @@
         <v>133</v>
       </c>
     </row>
-    <row r="73" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A73" s="150"/>
       <c r="B73" s="155" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="74" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A74" s="150"/>
       <c r="B74" s="151"/>
     </row>
-    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A75" s="156" t="s">
         <v>6</v>
       </c>
@@ -8646,17 +9692,17 @@
         <v>119</v>
       </c>
     </row>
-    <row r="76" spans="1:2" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" s="8" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A76" s="150"/>
       <c r="B76" s="139" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A77" s="149"/>
       <c r="B77" s="149"/>
     </row>
-    <row r="78" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A78" s="156" t="s">
         <v>6</v>
       </c>
@@ -8664,17 +9710,17 @@
         <v>125</v>
       </c>
     </row>
-    <row r="79" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A79" s="150"/>
       <c r="B79" s="139" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="80" spans="1:2" s="20" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A80" s="149"/>
       <c r="B80" s="149"/>
     </row>
-    <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A81" s="156" t="s">
         <v>6</v>
       </c>
@@ -8682,29 +9728,29 @@
         <v>126</v>
       </c>
     </row>
-    <row r="82" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A82" s="150"/>
       <c r="B82" s="154" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="83" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A83" s="150"/>
       <c r="B83" s="154" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="84" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A84" s="150"/>
       <c r="B84" s="154" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A85" s="149"/>
       <c r="B85" s="153"/>
     </row>
-    <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A86" s="156" t="s">
         <v>6</v>
       </c>
@@ -8712,29 +9758,29 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:2" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" s="8" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A87" s="150"/>
       <c r="B87" s="139" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="88" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A88" s="150"/>
       <c r="B88" s="152" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="89" spans="1:2" s="8" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" s="8" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A89" s="150"/>
       <c r="B89" s="158" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A90" s="149"/>
       <c r="B90" s="149"/>
     </row>
-    <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A91" s="156" t="s">
         <v>6</v>
       </c>
@@ -8742,13 +9788,13 @@
         <v>128</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" ht="28" x14ac:dyDescent="0.3">
       <c r="A92" s="137"/>
       <c r="B92" s="154" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="28" t="s">
         <v>55</v>
       </c>
@@ -8784,14 +9830,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="20" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="16"/>
+    <col min="1" max="1" width="5.54296875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="20" customWidth="1"/>
+    <col min="3" max="16384" width="8.81640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>53</v>
       </c>
@@ -8799,163 +9845,163 @@
       <c r="C1" s="45"/>
       <c r="D1" s="45"/>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="42"/>
       <c r="B2" s="46"/>
       <c r="C2" s="45"/>
       <c r="D2" s="45"/>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="43"/>
       <c r="B3" s="36" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="44"/>
     </row>
-    <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="38" t="s">
         <v>50</v>
       </c>
       <c r="C4" s="15"/>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="14"/>
       <c r="B5" s="17"/>
       <c r="C5" s="15"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="18" t="s">
         <v>55</v>
       </c>
       <c r="C6" s="15"/>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="14"/>
       <c r="B7" s="17"/>
       <c r="C7" s="15"/>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="14"/>
       <c r="B8" s="17" t="s">
         <v>56</v>
       </c>
       <c r="C8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="14"/>
       <c r="B9" s="17"/>
       <c r="C9" s="15"/>
     </row>
-    <row r="10" spans="1:4" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A10" s="14"/>
       <c r="B10" s="17" t="s">
         <v>57</v>
       </c>
       <c r="C10" s="15"/>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="14"/>
       <c r="B11" s="17"/>
       <c r="C11" s="15"/>
     </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A12" s="14"/>
       <c r="B12" s="17" t="s">
         <v>58</v>
       </c>
       <c r="C12" s="15"/>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="14"/>
       <c r="B13" s="17"/>
       <c r="C13" s="15"/>
     </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="62" x14ac:dyDescent="0.35">
       <c r="A14" s="14"/>
       <c r="B14" s="17" t="s">
         <v>59</v>
       </c>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="14"/>
       <c r="B15" s="17"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:4" ht="30.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="14"/>
       <c r="B16" s="17" t="s">
         <v>60</v>
       </c>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="14"/>
       <c r="B17" s="17"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="14"/>
       <c r="B18" s="18" t="s">
         <v>61</v>
       </c>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="14"/>
       <c r="B19" s="37" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="14"/>
       <c r="B20" s="19"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>

</xml_diff>

<commit_message>
Gannt updated for servomotor
</commit_message>
<xml_diff>
--- a/Gantt_Diagram_Robot_Project_2018.xlsx
+++ b/Gantt_Diagram_Robot_Project_2018.xlsx
@@ -2960,6 +2960,24 @@
     </xf>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2967,27 +2985,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3975,8 +3975,8 @@
   <dimension ref="A1:CP52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
+      <pane ySplit="7" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4028,29 +4028,29 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
       <c r="I1" s="132"/>
-      <c r="K1" s="163" t="s">
+      <c r="K1" s="169" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
-      <c r="P1" s="163"/>
-      <c r="Q1" s="163"/>
-      <c r="R1" s="163"/>
-      <c r="S1" s="163"/>
-      <c r="T1" s="163"/>
-      <c r="U1" s="163"/>
-      <c r="V1" s="163"/>
-      <c r="W1" s="163"/>
-      <c r="X1" s="163"/>
-      <c r="Y1" s="163"/>
-      <c r="Z1" s="163"/>
-      <c r="AA1" s="163"/>
-      <c r="AB1" s="163"/>
-      <c r="AC1" s="163"/>
-      <c r="AD1" s="163"/>
-      <c r="AE1" s="163"/>
+      <c r="L1" s="169"/>
+      <c r="M1" s="169"/>
+      <c r="N1" s="169"/>
+      <c r="O1" s="169"/>
+      <c r="P1" s="169"/>
+      <c r="Q1" s="169"/>
+      <c r="R1" s="169"/>
+      <c r="S1" s="169"/>
+      <c r="T1" s="169"/>
+      <c r="U1" s="169"/>
+      <c r="V1" s="169"/>
+      <c r="W1" s="169"/>
+      <c r="X1" s="169"/>
+      <c r="Y1" s="169"/>
+      <c r="Z1" s="169"/>
+      <c r="AA1" s="169"/>
+      <c r="AB1" s="169"/>
+      <c r="AC1" s="169"/>
+      <c r="AD1" s="169"/>
+      <c r="AE1" s="169"/>
     </row>
     <row r="2" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
@@ -4095,11 +4095,11 @@
       <c r="B4" s="114" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="168">
+      <c r="C4" s="171">
         <v>43340</v>
       </c>
-      <c r="D4" s="168"/>
-      <c r="E4" s="168"/>
+      <c r="D4" s="171"/>
+      <c r="E4" s="171"/>
       <c r="F4" s="111"/>
       <c r="G4" s="114" t="s">
         <v>75</v>
@@ -4109,262 +4109,262 @@
       </c>
       <c r="I4" s="112"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="165" t="str">
+      <c r="K4" s="163" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="166"/>
-      <c r="M4" s="166"/>
-      <c r="N4" s="166"/>
-      <c r="O4" s="166"/>
-      <c r="P4" s="166"/>
-      <c r="Q4" s="167"/>
-      <c r="R4" s="165" t="str">
+      <c r="L4" s="164"/>
+      <c r="M4" s="164"/>
+      <c r="N4" s="164"/>
+      <c r="O4" s="164"/>
+      <c r="P4" s="164"/>
+      <c r="Q4" s="165"/>
+      <c r="R4" s="163" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="166"/>
-      <c r="T4" s="166"/>
-      <c r="U4" s="166"/>
-      <c r="V4" s="166"/>
-      <c r="W4" s="166"/>
-      <c r="X4" s="167"/>
-      <c r="Y4" s="165" t="str">
+      <c r="S4" s="164"/>
+      <c r="T4" s="164"/>
+      <c r="U4" s="164"/>
+      <c r="V4" s="164"/>
+      <c r="W4" s="164"/>
+      <c r="X4" s="165"/>
+      <c r="Y4" s="163" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="166"/>
-      <c r="AA4" s="166"/>
-      <c r="AB4" s="166"/>
-      <c r="AC4" s="166"/>
-      <c r="AD4" s="166"/>
-      <c r="AE4" s="167"/>
-      <c r="AF4" s="165" t="str">
+      <c r="Z4" s="164"/>
+      <c r="AA4" s="164"/>
+      <c r="AB4" s="164"/>
+      <c r="AC4" s="164"/>
+      <c r="AD4" s="164"/>
+      <c r="AE4" s="165"/>
+      <c r="AF4" s="163" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="166"/>
-      <c r="AH4" s="166"/>
-      <c r="AI4" s="166"/>
-      <c r="AJ4" s="166"/>
-      <c r="AK4" s="166"/>
-      <c r="AL4" s="167"/>
-      <c r="AM4" s="165" t="str">
+      <c r="AG4" s="164"/>
+      <c r="AH4" s="164"/>
+      <c r="AI4" s="164"/>
+      <c r="AJ4" s="164"/>
+      <c r="AK4" s="164"/>
+      <c r="AL4" s="165"/>
+      <c r="AM4" s="163" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="166"/>
-      <c r="AO4" s="166"/>
-      <c r="AP4" s="166"/>
-      <c r="AQ4" s="166"/>
-      <c r="AR4" s="166"/>
-      <c r="AS4" s="167"/>
-      <c r="AT4" s="165" t="str">
+      <c r="AN4" s="164"/>
+      <c r="AO4" s="164"/>
+      <c r="AP4" s="164"/>
+      <c r="AQ4" s="164"/>
+      <c r="AR4" s="164"/>
+      <c r="AS4" s="165"/>
+      <c r="AT4" s="163" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="166"/>
-      <c r="AV4" s="166"/>
-      <c r="AW4" s="166"/>
-      <c r="AX4" s="166"/>
-      <c r="AY4" s="166"/>
-      <c r="AZ4" s="167"/>
-      <c r="BA4" s="165" t="str">
+      <c r="AU4" s="164"/>
+      <c r="AV4" s="164"/>
+      <c r="AW4" s="164"/>
+      <c r="AX4" s="164"/>
+      <c r="AY4" s="164"/>
+      <c r="AZ4" s="165"/>
+      <c r="BA4" s="163" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="166"/>
-      <c r="BC4" s="166"/>
-      <c r="BD4" s="166"/>
-      <c r="BE4" s="166"/>
-      <c r="BF4" s="166"/>
-      <c r="BG4" s="167"/>
-      <c r="BH4" s="165" t="str">
+      <c r="BB4" s="164"/>
+      <c r="BC4" s="164"/>
+      <c r="BD4" s="164"/>
+      <c r="BE4" s="164"/>
+      <c r="BF4" s="164"/>
+      <c r="BG4" s="165"/>
+      <c r="BH4" s="163" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="166"/>
-      <c r="BJ4" s="166"/>
-      <c r="BK4" s="166"/>
-      <c r="BL4" s="166"/>
-      <c r="BM4" s="166"/>
-      <c r="BN4" s="167"/>
-      <c r="BO4" s="165" t="str">
+      <c r="BI4" s="164"/>
+      <c r="BJ4" s="164"/>
+      <c r="BK4" s="164"/>
+      <c r="BL4" s="164"/>
+      <c r="BM4" s="164"/>
+      <c r="BN4" s="165"/>
+      <c r="BO4" s="163" t="str">
         <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="BP4" s="166"/>
-      <c r="BQ4" s="166"/>
-      <c r="BR4" s="166"/>
-      <c r="BS4" s="166"/>
-      <c r="BT4" s="166"/>
-      <c r="BU4" s="167"/>
-      <c r="BV4" s="165" t="str">
+      <c r="BP4" s="164"/>
+      <c r="BQ4" s="164"/>
+      <c r="BR4" s="164"/>
+      <c r="BS4" s="164"/>
+      <c r="BT4" s="164"/>
+      <c r="BU4" s="165"/>
+      <c r="BV4" s="163" t="str">
         <f>"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="BW4" s="166"/>
-      <c r="BX4" s="166"/>
-      <c r="BY4" s="166"/>
-      <c r="BZ4" s="166"/>
-      <c r="CA4" s="166"/>
-      <c r="CB4" s="167"/>
-      <c r="CC4" s="165" t="str">
+      <c r="BW4" s="164"/>
+      <c r="BX4" s="164"/>
+      <c r="BY4" s="164"/>
+      <c r="BZ4" s="164"/>
+      <c r="CA4" s="164"/>
+      <c r="CB4" s="165"/>
+      <c r="CC4" s="163" t="str">
         <f>"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="CD4" s="166"/>
-      <c r="CE4" s="166"/>
-      <c r="CF4" s="166"/>
-      <c r="CG4" s="166"/>
-      <c r="CH4" s="166"/>
-      <c r="CI4" s="167"/>
-      <c r="CJ4" s="165" t="str">
+      <c r="CD4" s="164"/>
+      <c r="CE4" s="164"/>
+      <c r="CF4" s="164"/>
+      <c r="CG4" s="164"/>
+      <c r="CH4" s="164"/>
+      <c r="CI4" s="165"/>
+      <c r="CJ4" s="163" t="str">
         <f>"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="CK4" s="166"/>
-      <c r="CL4" s="166"/>
-      <c r="CM4" s="166"/>
-      <c r="CN4" s="166"/>
-      <c r="CO4" s="166"/>
-      <c r="CP4" s="167"/>
+      <c r="CK4" s="164"/>
+      <c r="CL4" s="164"/>
+      <c r="CM4" s="164"/>
+      <c r="CN4" s="164"/>
+      <c r="CO4" s="164"/>
+      <c r="CP4" s="165"/>
     </row>
     <row r="5" spans="1:94" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="110"/>
       <c r="B5" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="164" t="s">
+      <c r="C5" s="170" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="164"/>
-      <c r="E5" s="164"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
       <c r="F5" s="113"/>
       <c r="G5" s="113"/>
       <c r="H5" s="113"/>
       <c r="I5" s="113"/>
       <c r="J5" s="50"/>
-      <c r="K5" s="169">
+      <c r="K5" s="166">
         <f>K6</f>
         <v>43339</v>
       </c>
-      <c r="L5" s="170"/>
-      <c r="M5" s="170"/>
-      <c r="N5" s="170"/>
-      <c r="O5" s="170"/>
-      <c r="P5" s="170"/>
-      <c r="Q5" s="171"/>
-      <c r="R5" s="169">
+      <c r="L5" s="167"/>
+      <c r="M5" s="167"/>
+      <c r="N5" s="167"/>
+      <c r="O5" s="167"/>
+      <c r="P5" s="167"/>
+      <c r="Q5" s="168"/>
+      <c r="R5" s="166">
         <f>R6</f>
         <v>43346</v>
       </c>
-      <c r="S5" s="170"/>
-      <c r="T5" s="170"/>
-      <c r="U5" s="170"/>
-      <c r="V5" s="170"/>
-      <c r="W5" s="170"/>
-      <c r="X5" s="171"/>
-      <c r="Y5" s="169">
+      <c r="S5" s="167"/>
+      <c r="T5" s="167"/>
+      <c r="U5" s="167"/>
+      <c r="V5" s="167"/>
+      <c r="W5" s="167"/>
+      <c r="X5" s="168"/>
+      <c r="Y5" s="166">
         <f>Y6</f>
         <v>43353</v>
       </c>
-      <c r="Z5" s="170"/>
-      <c r="AA5" s="170"/>
-      <c r="AB5" s="170"/>
-      <c r="AC5" s="170"/>
-      <c r="AD5" s="170"/>
-      <c r="AE5" s="171"/>
-      <c r="AF5" s="169">
+      <c r="Z5" s="167"/>
+      <c r="AA5" s="167"/>
+      <c r="AB5" s="167"/>
+      <c r="AC5" s="167"/>
+      <c r="AD5" s="167"/>
+      <c r="AE5" s="168"/>
+      <c r="AF5" s="166">
         <f>AF6</f>
         <v>43360</v>
       </c>
-      <c r="AG5" s="170"/>
-      <c r="AH5" s="170"/>
-      <c r="AI5" s="170"/>
-      <c r="AJ5" s="170"/>
-      <c r="AK5" s="170"/>
-      <c r="AL5" s="171"/>
-      <c r="AM5" s="169">
+      <c r="AG5" s="167"/>
+      <c r="AH5" s="167"/>
+      <c r="AI5" s="167"/>
+      <c r="AJ5" s="167"/>
+      <c r="AK5" s="167"/>
+      <c r="AL5" s="168"/>
+      <c r="AM5" s="166">
         <f>AM6</f>
         <v>43367</v>
       </c>
-      <c r="AN5" s="170"/>
-      <c r="AO5" s="170"/>
-      <c r="AP5" s="170"/>
-      <c r="AQ5" s="170"/>
-      <c r="AR5" s="170"/>
-      <c r="AS5" s="171"/>
-      <c r="AT5" s="169">
+      <c r="AN5" s="167"/>
+      <c r="AO5" s="167"/>
+      <c r="AP5" s="167"/>
+      <c r="AQ5" s="167"/>
+      <c r="AR5" s="167"/>
+      <c r="AS5" s="168"/>
+      <c r="AT5" s="166">
         <f>AT6</f>
         <v>43374</v>
       </c>
-      <c r="AU5" s="170"/>
-      <c r="AV5" s="170"/>
-      <c r="AW5" s="170"/>
-      <c r="AX5" s="170"/>
-      <c r="AY5" s="170"/>
-      <c r="AZ5" s="171"/>
-      <c r="BA5" s="169">
+      <c r="AU5" s="167"/>
+      <c r="AV5" s="167"/>
+      <c r="AW5" s="167"/>
+      <c r="AX5" s="167"/>
+      <c r="AY5" s="167"/>
+      <c r="AZ5" s="168"/>
+      <c r="BA5" s="166">
         <f>BA6</f>
         <v>43381</v>
       </c>
-      <c r="BB5" s="170"/>
-      <c r="BC5" s="170"/>
-      <c r="BD5" s="170"/>
-      <c r="BE5" s="170"/>
-      <c r="BF5" s="170"/>
-      <c r="BG5" s="171"/>
-      <c r="BH5" s="169">
+      <c r="BB5" s="167"/>
+      <c r="BC5" s="167"/>
+      <c r="BD5" s="167"/>
+      <c r="BE5" s="167"/>
+      <c r="BF5" s="167"/>
+      <c r="BG5" s="168"/>
+      <c r="BH5" s="166">
         <f>BH6</f>
         <v>43388</v>
       </c>
-      <c r="BI5" s="170"/>
-      <c r="BJ5" s="170"/>
-      <c r="BK5" s="170"/>
-      <c r="BL5" s="170"/>
-      <c r="BM5" s="170"/>
-      <c r="BN5" s="171"/>
-      <c r="BO5" s="169">
+      <c r="BI5" s="167"/>
+      <c r="BJ5" s="167"/>
+      <c r="BK5" s="167"/>
+      <c r="BL5" s="167"/>
+      <c r="BM5" s="167"/>
+      <c r="BN5" s="168"/>
+      <c r="BO5" s="166">
         <f>BO6</f>
         <v>43395</v>
       </c>
-      <c r="BP5" s="170"/>
-      <c r="BQ5" s="170"/>
-      <c r="BR5" s="170"/>
-      <c r="BS5" s="170"/>
-      <c r="BT5" s="170"/>
-      <c r="BU5" s="171"/>
-      <c r="BV5" s="169">
+      <c r="BP5" s="167"/>
+      <c r="BQ5" s="167"/>
+      <c r="BR5" s="167"/>
+      <c r="BS5" s="167"/>
+      <c r="BT5" s="167"/>
+      <c r="BU5" s="168"/>
+      <c r="BV5" s="166">
         <f>BV6</f>
         <v>43402</v>
       </c>
-      <c r="BW5" s="170"/>
-      <c r="BX5" s="170"/>
-      <c r="BY5" s="170"/>
-      <c r="BZ5" s="170"/>
-      <c r="CA5" s="170"/>
-      <c r="CB5" s="171"/>
-      <c r="CC5" s="169">
+      <c r="BW5" s="167"/>
+      <c r="BX5" s="167"/>
+      <c r="BY5" s="167"/>
+      <c r="BZ5" s="167"/>
+      <c r="CA5" s="167"/>
+      <c r="CB5" s="168"/>
+      <c r="CC5" s="166">
         <f>CC6</f>
         <v>43409</v>
       </c>
-      <c r="CD5" s="170"/>
-      <c r="CE5" s="170"/>
-      <c r="CF5" s="170"/>
-      <c r="CG5" s="170"/>
-      <c r="CH5" s="170"/>
-      <c r="CI5" s="171"/>
-      <c r="CJ5" s="169">
+      <c r="CD5" s="167"/>
+      <c r="CE5" s="167"/>
+      <c r="CF5" s="167"/>
+      <c r="CG5" s="167"/>
+      <c r="CH5" s="167"/>
+      <c r="CI5" s="168"/>
+      <c r="CJ5" s="166">
         <f>CJ6</f>
         <v>43416</v>
       </c>
-      <c r="CK5" s="170"/>
-      <c r="CL5" s="170"/>
-      <c r="CM5" s="170"/>
-      <c r="CN5" s="170"/>
-      <c r="CO5" s="170"/>
-      <c r="CP5" s="171"/>
+      <c r="CK5" s="167"/>
+      <c r="CL5" s="167"/>
+      <c r="CM5" s="167"/>
+      <c r="CN5" s="167"/>
+      <c r="CO5" s="167"/>
+      <c r="CP5" s="168"/>
     </row>
     <row r="6" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A6" s="49"/>
@@ -7222,17 +7222,16 @@
       </c>
       <c r="F33" s="101">
         <f>IF(ISBLANK(E33)," - ",IF(G33=0,E33,E33+G33-1))</f>
-        <v>43397</v>
+        <v>43413</v>
       </c>
       <c r="G33" s="62">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="H33" s="63">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I33" s="64">
-        <f t="shared" si="33"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J33" s="95"/>
       <c r="K33" s="107"/>
@@ -7309,17 +7308,16 @@
       </c>
       <c r="F34" s="101">
         <f t="shared" ref="F34" si="37">IF(ISBLANK(E34)," - ",IF(G34=0,E34,E34+G34-1))</f>
-        <v>43391</v>
+        <v>43413</v>
       </c>
       <c r="G34" s="62">
+        <v>23</v>
+      </c>
+      <c r="H34" s="63">
         <v>1</v>
       </c>
-      <c r="H34" s="63">
-        <v>0</v>
-      </c>
       <c r="I34" s="64">
-        <f t="shared" si="33"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J34" s="95"/>
       <c r="K34" s="107"/>
@@ -7392,17 +7390,17 @@
       </c>
       <c r="D35" s="127"/>
       <c r="E35" s="100">
-        <v>43391</v>
+        <v>43445</v>
       </c>
       <c r="F35" s="101">
         <f>IF(ISBLANK(E35)," - ",IF(G35=0,E35,E35+G35-1))</f>
-        <v>43391</v>
+        <v>43445</v>
       </c>
       <c r="G35" s="62">
         <v>1</v>
       </c>
       <c r="H35" s="63">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="I35" s="64">
         <f t="shared" si="33"/>
@@ -8801,14 +8799,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="27">
-    <mergeCell ref="CJ4:CP4"/>
-    <mergeCell ref="CJ5:CP5"/>
-    <mergeCell ref="BO5:BU5"/>
-    <mergeCell ref="BO4:BU4"/>
-    <mergeCell ref="BV4:CB4"/>
-    <mergeCell ref="BV5:CB5"/>
-    <mergeCell ref="CC4:CI4"/>
-    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -8819,15 +8818,14 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="CJ4:CP4"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BO4:BU4"/>
+    <mergeCell ref="BV4:CB4"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="CC5:CI5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8:H27 H38:H51">

</xml_diff>

<commit_message>
Gant and Pin Map update
</commit_message>
<xml_diff>
--- a/Gantt_Diagram_Robot_Project_2018.xlsx
+++ b/Gantt_Diagram_Robot_Project_2018.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Robot_Project_IFX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolle\Documents\Robot_Project_IFX\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27080" windowHeight="11370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27075" windowHeight="11370"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -2960,24 +2960,6 @@
     </xf>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2985,9 +2967,27 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3039,7 +3039,95 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="27">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -3387,11 +3475,11 @@
           <xdr:col>9</xdr:col>
           <xdr:colOff>95250</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>127000</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>107950</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:to>
@@ -3972,53 +4060,78 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CP52"/>
+  <dimension ref="A1:DR52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T34" sqref="T34"/>
+      <pane ySplit="7" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB26" sqref="AB26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.81640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="26.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="6" customWidth="1"/>
     <col min="5" max="6" width="12" style="1" customWidth="1"/>
     <col min="7" max="7" width="6" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7265625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="1.81640625" style="1" customWidth="1"/>
-    <col min="11" max="66" width="2.453125" style="1" customWidth="1"/>
-    <col min="67" max="67" width="2.7265625" style="3" customWidth="1"/>
-    <col min="68" max="68" width="2.54296875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="1.85546875" style="1" customWidth="1"/>
+    <col min="11" max="66" width="2.42578125" style="1" customWidth="1"/>
+    <col min="67" max="67" width="2.7109375" style="3" customWidth="1"/>
+    <col min="68" max="68" width="2.5703125" style="3" customWidth="1"/>
     <col min="69" max="70" width="3" style="3" customWidth="1"/>
-    <col min="71" max="71" width="3.26953125" style="3" customWidth="1"/>
-    <col min="72" max="72" width="2.7265625" style="3" customWidth="1"/>
-    <col min="73" max="73" width="2.54296875" style="3" customWidth="1"/>
-    <col min="74" max="74" width="2.7265625" style="3" customWidth="1"/>
-    <col min="75" max="76" width="2.81640625" style="3" customWidth="1"/>
+    <col min="71" max="71" width="3.28515625" style="3" customWidth="1"/>
+    <col min="72" max="72" width="2.7109375" style="3" customWidth="1"/>
+    <col min="73" max="73" width="2.5703125" style="3" customWidth="1"/>
+    <col min="74" max="74" width="2.7109375" style="3" customWidth="1"/>
+    <col min="75" max="76" width="2.85546875" style="3" customWidth="1"/>
     <col min="77" max="77" width="3" style="3" customWidth="1"/>
-    <col min="78" max="78" width="2.54296875" style="3" customWidth="1"/>
-    <col min="79" max="79" width="2.453125" style="3" customWidth="1"/>
-    <col min="80" max="80" width="2.7265625" style="3" customWidth="1"/>
-    <col min="81" max="81" width="2.453125" style="3" customWidth="1"/>
+    <col min="78" max="78" width="2.5703125" style="3" customWidth="1"/>
+    <col min="79" max="79" width="2.42578125" style="3" customWidth="1"/>
+    <col min="80" max="80" width="2.7109375" style="3" customWidth="1"/>
+    <col min="81" max="81" width="2.42578125" style="3" customWidth="1"/>
     <col min="82" max="82" width="3" style="3" customWidth="1"/>
-    <col min="83" max="83" width="2.453125" style="3" customWidth="1"/>
-    <col min="84" max="84" width="2.7265625" style="3" customWidth="1"/>
-    <col min="85" max="85" width="2.81640625" style="3" customWidth="1"/>
-    <col min="86" max="86" width="2.453125" style="3" customWidth="1"/>
-    <col min="87" max="88" width="2.54296875" style="3" customWidth="1"/>
+    <col min="83" max="83" width="2.42578125" style="3" customWidth="1"/>
+    <col min="84" max="84" width="2.7109375" style="3" customWidth="1"/>
+    <col min="85" max="85" width="2.85546875" style="3" customWidth="1"/>
+    <col min="86" max="86" width="2.42578125" style="3" customWidth="1"/>
+    <col min="87" max="88" width="2.5703125" style="3" customWidth="1"/>
     <col min="89" max="89" width="3" style="3" customWidth="1"/>
-    <col min="90" max="90" width="2.54296875" style="3" customWidth="1"/>
-    <col min="91" max="92" width="3.1796875" style="3" customWidth="1"/>
-    <col min="93" max="93" width="2.7265625" style="3" customWidth="1"/>
-    <col min="94" max="94" width="2.81640625" style="3" customWidth="1"/>
-    <col min="95" max="16384" width="9.1796875" style="3"/>
+    <col min="90" max="90" width="2.5703125" style="3" customWidth="1"/>
+    <col min="91" max="92" width="3.140625" style="3" customWidth="1"/>
+    <col min="93" max="93" width="2.7109375" style="3" customWidth="1"/>
+    <col min="94" max="94" width="2.85546875" style="3" customWidth="1"/>
+    <col min="95" max="96" width="3.42578125" style="3" customWidth="1"/>
+    <col min="97" max="97" width="3.140625" style="3" customWidth="1"/>
+    <col min="98" max="98" width="2.7109375" style="3" customWidth="1"/>
+    <col min="99" max="99" width="2.85546875" style="3" customWidth="1"/>
+    <col min="100" max="101" width="2.7109375" style="3" customWidth="1"/>
+    <col min="102" max="102" width="3.140625" style="3" customWidth="1"/>
+    <col min="103" max="103" width="3.28515625" style="3" customWidth="1"/>
+    <col min="104" max="104" width="3.42578125" style="3" customWidth="1"/>
+    <col min="105" max="105" width="3" style="3" customWidth="1"/>
+    <col min="106" max="106" width="3.42578125" style="3" customWidth="1"/>
+    <col min="107" max="107" width="3" style="3" customWidth="1"/>
+    <col min="108" max="108" width="3.42578125" style="3" customWidth="1"/>
+    <col min="109" max="109" width="4" style="3" customWidth="1"/>
+    <col min="110" max="110" width="3.28515625" style="3" customWidth="1"/>
+    <col min="111" max="111" width="3.5703125" style="3" customWidth="1"/>
+    <col min="112" max="112" width="3.42578125" style="3" customWidth="1"/>
+    <col min="113" max="113" width="3.140625" style="3" customWidth="1"/>
+    <col min="114" max="114" width="2.85546875" style="3" customWidth="1"/>
+    <col min="115" max="115" width="2.28515625" style="3" customWidth="1"/>
+    <col min="116" max="116" width="3.85546875" style="3" customWidth="1"/>
+    <col min="117" max="118" width="3.28515625" style="3" customWidth="1"/>
+    <col min="119" max="119" width="3" style="3" customWidth="1"/>
+    <col min="120" max="120" width="2.85546875" style="3" customWidth="1"/>
+    <col min="121" max="121" width="3.28515625" style="3" customWidth="1"/>
+    <col min="122" max="122" width="3" style="3" customWidth="1"/>
+    <col min="123" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:122" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="125" t="s">
         <v>138</v>
       </c>
@@ -4028,31 +4141,31 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
       <c r="I1" s="132"/>
-      <c r="K1" s="169" t="s">
+      <c r="K1" s="163" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="169"/>
-      <c r="M1" s="169"/>
-      <c r="N1" s="169"/>
-      <c r="O1" s="169"/>
-      <c r="P1" s="169"/>
-      <c r="Q1" s="169"/>
-      <c r="R1" s="169"/>
-      <c r="S1" s="169"/>
-      <c r="T1" s="169"/>
-      <c r="U1" s="169"/>
-      <c r="V1" s="169"/>
-      <c r="W1" s="169"/>
-      <c r="X1" s="169"/>
-      <c r="Y1" s="169"/>
-      <c r="Z1" s="169"/>
-      <c r="AA1" s="169"/>
-      <c r="AB1" s="169"/>
-      <c r="AC1" s="169"/>
-      <c r="AD1" s="169"/>
-      <c r="AE1" s="169"/>
-    </row>
-    <row r="2" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L1" s="163"/>
+      <c r="M1" s="163"/>
+      <c r="N1" s="163"/>
+      <c r="O1" s="163"/>
+      <c r="P1" s="163"/>
+      <c r="Q1" s="163"/>
+      <c r="R1" s="163"/>
+      <c r="S1" s="163"/>
+      <c r="T1" s="163"/>
+      <c r="U1" s="163"/>
+      <c r="V1" s="163"/>
+      <c r="W1" s="163"/>
+      <c r="X1" s="163"/>
+      <c r="Y1" s="163"/>
+      <c r="Z1" s="163"/>
+      <c r="AA1" s="163"/>
+      <c r="AB1" s="163"/>
+      <c r="AC1" s="163"/>
+      <c r="AD1" s="163"/>
+      <c r="AE1" s="163"/>
+    </row>
+    <row r="2" spans="1:122" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
         <v>139</v>
       </c>
@@ -4063,7 +4176,7 @@
       <c r="F2" s="160"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:94" ht="14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:122" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="52"/>
       <c r="B3" s="48"/>
       <c r="C3" s="4"/>
@@ -4090,16 +4203,16 @@
       <c r="Z3" s="29"/>
       <c r="AA3" s="29"/>
     </row>
-    <row r="4" spans="1:94" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:122" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="110"/>
       <c r="B4" s="114" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="171">
+      <c r="C4" s="168">
         <v>43340</v>
       </c>
-      <c r="D4" s="171"/>
-      <c r="E4" s="171"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="168"/>
       <c r="F4" s="111"/>
       <c r="G4" s="114" t="s">
         <v>75</v>
@@ -4109,264 +4222,344 @@
       </c>
       <c r="I4" s="112"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="163" t="str">
+      <c r="K4" s="165" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="164"/>
-      <c r="M4" s="164"/>
-      <c r="N4" s="164"/>
-      <c r="O4" s="164"/>
-      <c r="P4" s="164"/>
-      <c r="Q4" s="165"/>
-      <c r="R4" s="163" t="str">
+      <c r="L4" s="166"/>
+      <c r="M4" s="166"/>
+      <c r="N4" s="166"/>
+      <c r="O4" s="166"/>
+      <c r="P4" s="166"/>
+      <c r="Q4" s="167"/>
+      <c r="R4" s="165" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="164"/>
-      <c r="T4" s="164"/>
-      <c r="U4" s="164"/>
-      <c r="V4" s="164"/>
-      <c r="W4" s="164"/>
-      <c r="X4" s="165"/>
-      <c r="Y4" s="163" t="str">
+      <c r="S4" s="166"/>
+      <c r="T4" s="166"/>
+      <c r="U4" s="166"/>
+      <c r="V4" s="166"/>
+      <c r="W4" s="166"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="165" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="164"/>
-      <c r="AA4" s="164"/>
-      <c r="AB4" s="164"/>
-      <c r="AC4" s="164"/>
-      <c r="AD4" s="164"/>
-      <c r="AE4" s="165"/>
-      <c r="AF4" s="163" t="str">
+      <c r="Z4" s="166"/>
+      <c r="AA4" s="166"/>
+      <c r="AB4" s="166"/>
+      <c r="AC4" s="166"/>
+      <c r="AD4" s="166"/>
+      <c r="AE4" s="167"/>
+      <c r="AF4" s="165" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="164"/>
-      <c r="AH4" s="164"/>
-      <c r="AI4" s="164"/>
-      <c r="AJ4" s="164"/>
-      <c r="AK4" s="164"/>
-      <c r="AL4" s="165"/>
-      <c r="AM4" s="163" t="str">
+      <c r="AG4" s="166"/>
+      <c r="AH4" s="166"/>
+      <c r="AI4" s="166"/>
+      <c r="AJ4" s="166"/>
+      <c r="AK4" s="166"/>
+      <c r="AL4" s="167"/>
+      <c r="AM4" s="165" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="164"/>
-      <c r="AO4" s="164"/>
-      <c r="AP4" s="164"/>
-      <c r="AQ4" s="164"/>
-      <c r="AR4" s="164"/>
-      <c r="AS4" s="165"/>
-      <c r="AT4" s="163" t="str">
+      <c r="AN4" s="166"/>
+      <c r="AO4" s="166"/>
+      <c r="AP4" s="166"/>
+      <c r="AQ4" s="166"/>
+      <c r="AR4" s="166"/>
+      <c r="AS4" s="167"/>
+      <c r="AT4" s="165" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="164"/>
-      <c r="AV4" s="164"/>
-      <c r="AW4" s="164"/>
-      <c r="AX4" s="164"/>
-      <c r="AY4" s="164"/>
-      <c r="AZ4" s="165"/>
-      <c r="BA4" s="163" t="str">
+      <c r="AU4" s="166"/>
+      <c r="AV4" s="166"/>
+      <c r="AW4" s="166"/>
+      <c r="AX4" s="166"/>
+      <c r="AY4" s="166"/>
+      <c r="AZ4" s="167"/>
+      <c r="BA4" s="165" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="164"/>
-      <c r="BC4" s="164"/>
-      <c r="BD4" s="164"/>
-      <c r="BE4" s="164"/>
-      <c r="BF4" s="164"/>
-      <c r="BG4" s="165"/>
-      <c r="BH4" s="163" t="str">
+      <c r="BB4" s="166"/>
+      <c r="BC4" s="166"/>
+      <c r="BD4" s="166"/>
+      <c r="BE4" s="166"/>
+      <c r="BF4" s="166"/>
+      <c r="BG4" s="167"/>
+      <c r="BH4" s="165" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="164"/>
-      <c r="BJ4" s="164"/>
-      <c r="BK4" s="164"/>
-      <c r="BL4" s="164"/>
-      <c r="BM4" s="164"/>
-      <c r="BN4" s="165"/>
-      <c r="BO4" s="163" t="str">
+      <c r="BI4" s="166"/>
+      <c r="BJ4" s="166"/>
+      <c r="BK4" s="166"/>
+      <c r="BL4" s="166"/>
+      <c r="BM4" s="166"/>
+      <c r="BN4" s="167"/>
+      <c r="BO4" s="165" t="str">
         <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="BP4" s="164"/>
-      <c r="BQ4" s="164"/>
-      <c r="BR4" s="164"/>
-      <c r="BS4" s="164"/>
-      <c r="BT4" s="164"/>
-      <c r="BU4" s="165"/>
-      <c r="BV4" s="163" t="str">
+      <c r="BP4" s="166"/>
+      <c r="BQ4" s="166"/>
+      <c r="BR4" s="166"/>
+      <c r="BS4" s="166"/>
+      <c r="BT4" s="166"/>
+      <c r="BU4" s="167"/>
+      <c r="BV4" s="165" t="str">
         <f>"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="BW4" s="164"/>
-      <c r="BX4" s="164"/>
-      <c r="BY4" s="164"/>
-      <c r="BZ4" s="164"/>
-      <c r="CA4" s="164"/>
-      <c r="CB4" s="165"/>
-      <c r="CC4" s="163" t="str">
+      <c r="BW4" s="166"/>
+      <c r="BX4" s="166"/>
+      <c r="BY4" s="166"/>
+      <c r="BZ4" s="166"/>
+      <c r="CA4" s="166"/>
+      <c r="CB4" s="167"/>
+      <c r="CC4" s="165" t="str">
         <f>"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="CD4" s="164"/>
-      <c r="CE4" s="164"/>
-      <c r="CF4" s="164"/>
-      <c r="CG4" s="164"/>
-      <c r="CH4" s="164"/>
-      <c r="CI4" s="165"/>
-      <c r="CJ4" s="163" t="str">
+      <c r="CD4" s="166"/>
+      <c r="CE4" s="166"/>
+      <c r="CF4" s="166"/>
+      <c r="CG4" s="166"/>
+      <c r="CH4" s="166"/>
+      <c r="CI4" s="167"/>
+      <c r="CJ4" s="165" t="str">
         <f>"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="CK4" s="164"/>
-      <c r="CL4" s="164"/>
-      <c r="CM4" s="164"/>
-      <c r="CN4" s="164"/>
-      <c r="CO4" s="164"/>
-      <c r="CP4" s="165"/>
-    </row>
-    <row r="5" spans="1:94" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CK4" s="166"/>
+      <c r="CL4" s="166"/>
+      <c r="CM4" s="166"/>
+      <c r="CN4" s="166"/>
+      <c r="CO4" s="166"/>
+      <c r="CP4" s="167"/>
+      <c r="CQ4" s="165" t="str">
+        <f>"Week "&amp;(CQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 13</v>
+      </c>
+      <c r="CR4" s="166"/>
+      <c r="CS4" s="166"/>
+      <c r="CT4" s="166"/>
+      <c r="CU4" s="166"/>
+      <c r="CV4" s="166"/>
+      <c r="CW4" s="167"/>
+      <c r="CX4" s="165" t="str">
+        <f>"Week "&amp;(CX6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 14</v>
+      </c>
+      <c r="CY4" s="166"/>
+      <c r="CZ4" s="166"/>
+      <c r="DA4" s="166"/>
+      <c r="DB4" s="166"/>
+      <c r="DC4" s="166"/>
+      <c r="DD4" s="167"/>
+      <c r="DE4" s="165" t="str">
+        <f>"Week "&amp;(DE6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 15</v>
+      </c>
+      <c r="DF4" s="166"/>
+      <c r="DG4" s="166"/>
+      <c r="DH4" s="166"/>
+      <c r="DI4" s="166"/>
+      <c r="DJ4" s="166"/>
+      <c r="DK4" s="167"/>
+      <c r="DL4" s="165" t="str">
+        <f>"Week "&amp;(DL6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 16</v>
+      </c>
+      <c r="DM4" s="166"/>
+      <c r="DN4" s="166"/>
+      <c r="DO4" s="166"/>
+      <c r="DP4" s="166"/>
+      <c r="DQ4" s="166"/>
+      <c r="DR4" s="167"/>
+    </row>
+    <row r="5" spans="1:122" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="110"/>
       <c r="B5" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="170" t="s">
+      <c r="C5" s="164" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
+      <c r="D5" s="164"/>
+      <c r="E5" s="164"/>
       <c r="F5" s="113"/>
       <c r="G5" s="113"/>
       <c r="H5" s="113"/>
       <c r="I5" s="113"/>
       <c r="J5" s="50"/>
-      <c r="K5" s="166">
+      <c r="K5" s="169">
         <f>K6</f>
         <v>43339</v>
       </c>
-      <c r="L5" s="167"/>
-      <c r="M5" s="167"/>
-      <c r="N5" s="167"/>
-      <c r="O5" s="167"/>
-      <c r="P5" s="167"/>
-      <c r="Q5" s="168"/>
-      <c r="R5" s="166">
+      <c r="L5" s="170"/>
+      <c r="M5" s="170"/>
+      <c r="N5" s="170"/>
+      <c r="O5" s="170"/>
+      <c r="P5" s="170"/>
+      <c r="Q5" s="171"/>
+      <c r="R5" s="169">
         <f>R6</f>
         <v>43346</v>
       </c>
-      <c r="S5" s="167"/>
-      <c r="T5" s="167"/>
-      <c r="U5" s="167"/>
-      <c r="V5" s="167"/>
-      <c r="W5" s="167"/>
-      <c r="X5" s="168"/>
-      <c r="Y5" s="166">
+      <c r="S5" s="170"/>
+      <c r="T5" s="170"/>
+      <c r="U5" s="170"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
+      <c r="X5" s="171"/>
+      <c r="Y5" s="169">
         <f>Y6</f>
         <v>43353</v>
       </c>
-      <c r="Z5" s="167"/>
-      <c r="AA5" s="167"/>
-      <c r="AB5" s="167"/>
-      <c r="AC5" s="167"/>
-      <c r="AD5" s="167"/>
-      <c r="AE5" s="168"/>
-      <c r="AF5" s="166">
+      <c r="Z5" s="170"/>
+      <c r="AA5" s="170"/>
+      <c r="AB5" s="170"/>
+      <c r="AC5" s="170"/>
+      <c r="AD5" s="170"/>
+      <c r="AE5" s="171"/>
+      <c r="AF5" s="169">
         <f>AF6</f>
         <v>43360</v>
       </c>
-      <c r="AG5" s="167"/>
-      <c r="AH5" s="167"/>
-      <c r="AI5" s="167"/>
-      <c r="AJ5" s="167"/>
-      <c r="AK5" s="167"/>
-      <c r="AL5" s="168"/>
-      <c r="AM5" s="166">
+      <c r="AG5" s="170"/>
+      <c r="AH5" s="170"/>
+      <c r="AI5" s="170"/>
+      <c r="AJ5" s="170"/>
+      <c r="AK5" s="170"/>
+      <c r="AL5" s="171"/>
+      <c r="AM5" s="169">
         <f>AM6</f>
         <v>43367</v>
       </c>
-      <c r="AN5" s="167"/>
-      <c r="AO5" s="167"/>
-      <c r="AP5" s="167"/>
-      <c r="AQ5" s="167"/>
-      <c r="AR5" s="167"/>
-      <c r="AS5" s="168"/>
-      <c r="AT5" s="166">
+      <c r="AN5" s="170"/>
+      <c r="AO5" s="170"/>
+      <c r="AP5" s="170"/>
+      <c r="AQ5" s="170"/>
+      <c r="AR5" s="170"/>
+      <c r="AS5" s="171"/>
+      <c r="AT5" s="169">
         <f>AT6</f>
         <v>43374</v>
       </c>
-      <c r="AU5" s="167"/>
-      <c r="AV5" s="167"/>
-      <c r="AW5" s="167"/>
-      <c r="AX5" s="167"/>
-      <c r="AY5" s="167"/>
-      <c r="AZ5" s="168"/>
-      <c r="BA5" s="166">
+      <c r="AU5" s="170"/>
+      <c r="AV5" s="170"/>
+      <c r="AW5" s="170"/>
+      <c r="AX5" s="170"/>
+      <c r="AY5" s="170"/>
+      <c r="AZ5" s="171"/>
+      <c r="BA5" s="169">
         <f>BA6</f>
         <v>43381</v>
       </c>
-      <c r="BB5" s="167"/>
-      <c r="BC5" s="167"/>
-      <c r="BD5" s="167"/>
-      <c r="BE5" s="167"/>
-      <c r="BF5" s="167"/>
-      <c r="BG5" s="168"/>
-      <c r="BH5" s="166">
+      <c r="BB5" s="170"/>
+      <c r="BC5" s="170"/>
+      <c r="BD5" s="170"/>
+      <c r="BE5" s="170"/>
+      <c r="BF5" s="170"/>
+      <c r="BG5" s="171"/>
+      <c r="BH5" s="169">
         <f>BH6</f>
         <v>43388</v>
       </c>
-      <c r="BI5" s="167"/>
-      <c r="BJ5" s="167"/>
-      <c r="BK5" s="167"/>
-      <c r="BL5" s="167"/>
-      <c r="BM5" s="167"/>
-      <c r="BN5" s="168"/>
-      <c r="BO5" s="166">
+      <c r="BI5" s="170"/>
+      <c r="BJ5" s="170"/>
+      <c r="BK5" s="170"/>
+      <c r="BL5" s="170"/>
+      <c r="BM5" s="170"/>
+      <c r="BN5" s="171"/>
+      <c r="BO5" s="169">
         <f>BO6</f>
         <v>43395</v>
       </c>
-      <c r="BP5" s="167"/>
-      <c r="BQ5" s="167"/>
-      <c r="BR5" s="167"/>
-      <c r="BS5" s="167"/>
-      <c r="BT5" s="167"/>
-      <c r="BU5" s="168"/>
-      <c r="BV5" s="166">
+      <c r="BP5" s="170"/>
+      <c r="BQ5" s="170"/>
+      <c r="BR5" s="170"/>
+      <c r="BS5" s="170"/>
+      <c r="BT5" s="170"/>
+      <c r="BU5" s="171"/>
+      <c r="BV5" s="169">
         <f>BV6</f>
         <v>43402</v>
       </c>
-      <c r="BW5" s="167"/>
-      <c r="BX5" s="167"/>
-      <c r="BY5" s="167"/>
-      <c r="BZ5" s="167"/>
-      <c r="CA5" s="167"/>
-      <c r="CB5" s="168"/>
-      <c r="CC5" s="166">
+      <c r="BW5" s="170"/>
+      <c r="BX5" s="170"/>
+      <c r="BY5" s="170"/>
+      <c r="BZ5" s="170"/>
+      <c r="CA5" s="170"/>
+      <c r="CB5" s="171"/>
+      <c r="CC5" s="169">
         <f>CC6</f>
         <v>43409</v>
       </c>
-      <c r="CD5" s="167"/>
-      <c r="CE5" s="167"/>
-      <c r="CF5" s="167"/>
-      <c r="CG5" s="167"/>
-      <c r="CH5" s="167"/>
-      <c r="CI5" s="168"/>
-      <c r="CJ5" s="166">
+      <c r="CD5" s="170"/>
+      <c r="CE5" s="170"/>
+      <c r="CF5" s="170"/>
+      <c r="CG5" s="170"/>
+      <c r="CH5" s="170"/>
+      <c r="CI5" s="171"/>
+      <c r="CJ5" s="169">
         <f>CJ6</f>
         <v>43416</v>
       </c>
-      <c r="CK5" s="167"/>
-      <c r="CL5" s="167"/>
-      <c r="CM5" s="167"/>
-      <c r="CN5" s="167"/>
-      <c r="CO5" s="167"/>
-      <c r="CP5" s="168"/>
-    </row>
-    <row r="6" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CK5" s="170"/>
+      <c r="CL5" s="170"/>
+      <c r="CM5" s="170"/>
+      <c r="CN5" s="170"/>
+      <c r="CO5" s="170"/>
+      <c r="CP5" s="171"/>
+      <c r="CQ5" s="169">
+        <f>CQ6</f>
+        <v>43423</v>
+      </c>
+      <c r="CR5" s="170"/>
+      <c r="CS5" s="170"/>
+      <c r="CT5" s="170"/>
+      <c r="CU5" s="170"/>
+      <c r="CV5" s="170"/>
+      <c r="CW5" s="171"/>
+      <c r="CX5" s="169">
+        <f>CX6</f>
+        <v>43430</v>
+      </c>
+      <c r="CY5" s="170"/>
+      <c r="CZ5" s="170"/>
+      <c r="DA5" s="170"/>
+      <c r="DB5" s="170"/>
+      <c r="DC5" s="170"/>
+      <c r="DD5" s="171"/>
+      <c r="DE5" s="169">
+        <f>DE6</f>
+        <v>43437</v>
+      </c>
+      <c r="DF5" s="170"/>
+      <c r="DG5" s="170"/>
+      <c r="DH5" s="170"/>
+      <c r="DI5" s="170"/>
+      <c r="DJ5" s="170"/>
+      <c r="DK5" s="171"/>
+      <c r="DL5" s="169">
+        <f>DL6</f>
+        <v>43444</v>
+      </c>
+      <c r="DM5" s="170"/>
+      <c r="DN5" s="170"/>
+      <c r="DO5" s="170"/>
+      <c r="DP5" s="170"/>
+      <c r="DQ5" s="170"/>
+      <c r="DR5" s="171"/>
+    </row>
+    <row r="6" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A6" s="49"/>
       <c r="B6" s="50"/>
       <c r="C6" s="50"/>
@@ -4713,8 +4906,120 @@
         <f t="shared" ref="CP6" si="29">CO6+1</f>
         <v>43422</v>
       </c>
-    </row>
-    <row r="7" spans="1:94" s="124" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="CQ6" s="92">
+        <f t="shared" ref="CQ6" si="30">CP6+1</f>
+        <v>43423</v>
+      </c>
+      <c r="CR6" s="83">
+        <f t="shared" ref="CR6" si="31">CQ6+1</f>
+        <v>43424</v>
+      </c>
+      <c r="CS6" s="83">
+        <f t="shared" ref="CS6" si="32">CR6+1</f>
+        <v>43425</v>
+      </c>
+      <c r="CT6" s="83">
+        <f t="shared" ref="CT6" si="33">CS6+1</f>
+        <v>43426</v>
+      </c>
+      <c r="CU6" s="83">
+        <f t="shared" ref="CU6" si="34">CT6+1</f>
+        <v>43427</v>
+      </c>
+      <c r="CV6" s="83">
+        <f t="shared" ref="CV6" si="35">CU6+1</f>
+        <v>43428</v>
+      </c>
+      <c r="CW6" s="93">
+        <f t="shared" ref="CW6" si="36">CV6+1</f>
+        <v>43429</v>
+      </c>
+      <c r="CX6" s="92">
+        <f t="shared" ref="CX6" si="37">CW6+1</f>
+        <v>43430</v>
+      </c>
+      <c r="CY6" s="83">
+        <f t="shared" ref="CY6" si="38">CX6+1</f>
+        <v>43431</v>
+      </c>
+      <c r="CZ6" s="83">
+        <f t="shared" ref="CZ6" si="39">CY6+1</f>
+        <v>43432</v>
+      </c>
+      <c r="DA6" s="83">
+        <f t="shared" ref="DA6" si="40">CZ6+1</f>
+        <v>43433</v>
+      </c>
+      <c r="DB6" s="83">
+        <f t="shared" ref="DB6" si="41">DA6+1</f>
+        <v>43434</v>
+      </c>
+      <c r="DC6" s="83">
+        <f t="shared" ref="DC6" si="42">DB6+1</f>
+        <v>43435</v>
+      </c>
+      <c r="DD6" s="93">
+        <f t="shared" ref="DD6" si="43">DC6+1</f>
+        <v>43436</v>
+      </c>
+      <c r="DE6" s="92">
+        <f t="shared" ref="DE6" si="44">DD6+1</f>
+        <v>43437</v>
+      </c>
+      <c r="DF6" s="83">
+        <f t="shared" ref="DF6" si="45">DE6+1</f>
+        <v>43438</v>
+      </c>
+      <c r="DG6" s="83">
+        <f t="shared" ref="DG6" si="46">DF6+1</f>
+        <v>43439</v>
+      </c>
+      <c r="DH6" s="83">
+        <f t="shared" ref="DH6" si="47">DG6+1</f>
+        <v>43440</v>
+      </c>
+      <c r="DI6" s="83">
+        <f t="shared" ref="DI6" si="48">DH6+1</f>
+        <v>43441</v>
+      </c>
+      <c r="DJ6" s="83">
+        <f t="shared" ref="DJ6" si="49">DI6+1</f>
+        <v>43442</v>
+      </c>
+      <c r="DK6" s="93">
+        <f t="shared" ref="DK6" si="50">DJ6+1</f>
+        <v>43443</v>
+      </c>
+      <c r="DL6" s="92">
+        <f t="shared" ref="DL6" si="51">DK6+1</f>
+        <v>43444</v>
+      </c>
+      <c r="DM6" s="83">
+        <f t="shared" ref="DM6" si="52">DL6+1</f>
+        <v>43445</v>
+      </c>
+      <c r="DN6" s="83">
+        <f t="shared" ref="DN6" si="53">DM6+1</f>
+        <v>43446</v>
+      </c>
+      <c r="DO6" s="83">
+        <f t="shared" ref="DO6" si="54">DN6+1</f>
+        <v>43447</v>
+      </c>
+      <c r="DP6" s="83">
+        <f t="shared" ref="DP6" si="55">DO6+1</f>
+        <v>43448</v>
+      </c>
+      <c r="DQ6" s="83">
+        <f t="shared" ref="DQ6" si="56">DP6+1</f>
+        <v>43449</v>
+      </c>
+      <c r="DR6" s="93">
+        <f t="shared" ref="DR6" si="57">DQ6+1</f>
+        <v>43450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:122" s="124" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="116" t="s">
         <v>0</v>
       </c>
@@ -4744,343 +5049,455 @@
       </c>
       <c r="J7" s="118"/>
       <c r="K7" s="121" t="str">
-        <f t="shared" ref="K7:AP7" si="30">CHOOSE(WEEKDAY(K6,1),"S","M","T","W","T","F","S")</f>
+        <f t="shared" ref="K7:AP7" si="58">CHOOSE(WEEKDAY(K6,1),"S","M","T","W","T","F","S")</f>
         <v>M</v>
       </c>
       <c r="L7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>T</v>
       </c>
       <c r="M7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>W</v>
       </c>
       <c r="N7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>T</v>
       </c>
       <c r="O7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>F</v>
       </c>
       <c r="P7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>S</v>
       </c>
       <c r="Q7" s="123" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>S</v>
       </c>
       <c r="R7" s="121" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>M</v>
       </c>
       <c r="S7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>T</v>
       </c>
       <c r="T7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>W</v>
       </c>
       <c r="U7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>T</v>
       </c>
       <c r="V7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>F</v>
       </c>
       <c r="W7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>S</v>
       </c>
       <c r="X7" s="123" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>S</v>
       </c>
       <c r="Y7" s="121" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>M</v>
       </c>
       <c r="Z7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>T</v>
       </c>
       <c r="AA7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>W</v>
       </c>
       <c r="AB7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>T</v>
       </c>
       <c r="AC7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>F</v>
       </c>
       <c r="AD7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>S</v>
       </c>
       <c r="AE7" s="123" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>S</v>
       </c>
       <c r="AF7" s="121" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>M</v>
       </c>
       <c r="AG7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>T</v>
       </c>
       <c r="AH7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>W</v>
       </c>
       <c r="AI7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>T</v>
       </c>
       <c r="AJ7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>F</v>
       </c>
       <c r="AK7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>S</v>
       </c>
       <c r="AL7" s="123" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>S</v>
       </c>
       <c r="AM7" s="121" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>M</v>
       </c>
       <c r="AN7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>T</v>
       </c>
       <c r="AO7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>W</v>
       </c>
       <c r="AP7" s="122" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>T</v>
       </c>
       <c r="AQ7" s="122" t="str">
-        <f t="shared" ref="AQ7:BN7" si="31">CHOOSE(WEEKDAY(AQ6,1),"S","M","T","W","T","F","S")</f>
+        <f t="shared" ref="AQ7:BN7" si="59">CHOOSE(WEEKDAY(AQ6,1),"S","M","T","W","T","F","S")</f>
         <v>F</v>
       </c>
       <c r="AR7" s="122" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>S</v>
       </c>
       <c r="AS7" s="123" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>S</v>
       </c>
       <c r="AT7" s="121" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>M</v>
       </c>
       <c r="AU7" s="122" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>T</v>
       </c>
       <c r="AV7" s="122" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>W</v>
       </c>
       <c r="AW7" s="122" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>T</v>
       </c>
       <c r="AX7" s="122" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>F</v>
       </c>
       <c r="AY7" s="122" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>S</v>
       </c>
       <c r="AZ7" s="123" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>S</v>
       </c>
       <c r="BA7" s="121" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>M</v>
       </c>
       <c r="BB7" s="122" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>T</v>
       </c>
       <c r="BC7" s="122" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>W</v>
       </c>
       <c r="BD7" s="122" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>T</v>
       </c>
       <c r="BE7" s="122" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>F</v>
       </c>
       <c r="BF7" s="122" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>S</v>
       </c>
       <c r="BG7" s="123" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>S</v>
       </c>
       <c r="BH7" s="121" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>M</v>
       </c>
       <c r="BI7" s="122" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>T</v>
       </c>
       <c r="BJ7" s="122" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>W</v>
       </c>
       <c r="BK7" s="122" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>T</v>
       </c>
       <c r="BL7" s="122" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>F</v>
       </c>
       <c r="BM7" s="122" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>S</v>
       </c>
       <c r="BN7" s="123" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="59"/>
         <v>S</v>
       </c>
       <c r="BO7" s="121" t="str">
-        <f t="shared" ref="BO7:CP7" si="32">CHOOSE(WEEKDAY(BO6,1),"S","M","T","W","T","F","S")</f>
+        <f t="shared" ref="BO7:CP7" si="60">CHOOSE(WEEKDAY(BO6,1),"S","M","T","W","T","F","S")</f>
         <v>M</v>
       </c>
       <c r="BP7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>T</v>
       </c>
       <c r="BQ7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>W</v>
       </c>
       <c r="BR7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>T</v>
       </c>
       <c r="BS7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>F</v>
       </c>
       <c r="BT7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>S</v>
       </c>
       <c r="BU7" s="123" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>S</v>
       </c>
       <c r="BV7" s="121" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>M</v>
       </c>
       <c r="BW7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>T</v>
       </c>
       <c r="BX7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>W</v>
       </c>
       <c r="BY7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>T</v>
       </c>
       <c r="BZ7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>F</v>
       </c>
       <c r="CA7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>S</v>
       </c>
       <c r="CB7" s="123" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>S</v>
       </c>
       <c r="CC7" s="121" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>M</v>
       </c>
       <c r="CD7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>T</v>
       </c>
       <c r="CE7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>W</v>
       </c>
       <c r="CF7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>T</v>
       </c>
       <c r="CG7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>F</v>
       </c>
       <c r="CH7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>S</v>
       </c>
       <c r="CI7" s="123" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>S</v>
       </c>
       <c r="CJ7" s="121" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>M</v>
       </c>
       <c r="CK7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>T</v>
       </c>
       <c r="CL7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>W</v>
       </c>
       <c r="CM7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>T</v>
       </c>
       <c r="CN7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>F</v>
       </c>
       <c r="CO7" s="122" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>S</v>
       </c>
       <c r="CP7" s="123" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="8" spans="1:94" s="55" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="CQ7" s="121" t="str">
+        <f t="shared" ref="CQ7:DR7" si="61">CHOOSE(WEEKDAY(CQ6,1),"S","M","T","W","T","F","S")</f>
+        <v>M</v>
+      </c>
+      <c r="CR7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>T</v>
+      </c>
+      <c r="CS7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>W</v>
+      </c>
+      <c r="CT7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>T</v>
+      </c>
+      <c r="CU7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>F</v>
+      </c>
+      <c r="CV7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>S</v>
+      </c>
+      <c r="CW7" s="123" t="str">
+        <f t="shared" si="61"/>
+        <v>S</v>
+      </c>
+      <c r="CX7" s="121" t="str">
+        <f t="shared" si="61"/>
+        <v>M</v>
+      </c>
+      <c r="CY7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>T</v>
+      </c>
+      <c r="CZ7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>W</v>
+      </c>
+      <c r="DA7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>T</v>
+      </c>
+      <c r="DB7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>F</v>
+      </c>
+      <c r="DC7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>S</v>
+      </c>
+      <c r="DD7" s="123" t="str">
+        <f t="shared" si="61"/>
+        <v>S</v>
+      </c>
+      <c r="DE7" s="121" t="str">
+        <f t="shared" si="61"/>
+        <v>M</v>
+      </c>
+      <c r="DF7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>T</v>
+      </c>
+      <c r="DG7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>W</v>
+      </c>
+      <c r="DH7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>T</v>
+      </c>
+      <c r="DI7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>F</v>
+      </c>
+      <c r="DJ7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>S</v>
+      </c>
+      <c r="DK7" s="123" t="str">
+        <f t="shared" si="61"/>
+        <v>S</v>
+      </c>
+      <c r="DL7" s="121" t="str">
+        <f t="shared" si="61"/>
+        <v>M</v>
+      </c>
+      <c r="DM7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>T</v>
+      </c>
+      <c r="DN7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>W</v>
+      </c>
+      <c r="DO7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>T</v>
+      </c>
+      <c r="DP7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>F</v>
+      </c>
+      <c r="DQ7" s="122" t="str">
+        <f t="shared" si="61"/>
+        <v>S</v>
+      </c>
+      <c r="DR7" s="123" t="str">
+        <f t="shared" si="61"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="8" spans="1:122" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="84" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -5098,7 +5515,7 @@
       <c r="G8" s="89"/>
       <c r="H8" s="90"/>
       <c r="I8" s="91" t="str">
-        <f t="shared" ref="I8:I45" si="33">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
+        <f t="shared" ref="I8:I45" si="62">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J8" s="94"/>
@@ -5159,9 +5576,9 @@
       <c r="BM8" s="106"/>
       <c r="BN8" s="106"/>
     </row>
-    <row r="9" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:122" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="60" t="str">
-        <f t="shared" ref="A9:A15" si="34">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A9:A15" si="63">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
       </c>
       <c r="B9" s="126" t="s">
@@ -5187,7 +5604,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>10</v>
       </c>
       <c r="J9" s="95"/>
@@ -5248,9 +5665,9 @@
       <c r="BM9" s="107"/>
       <c r="BN9" s="107"/>
     </row>
-    <row r="10" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:122" s="61" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A10" s="60" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="63"/>
         <v>1.2</v>
       </c>
       <c r="B10" s="126" t="s">
@@ -5274,7 +5691,7 @@
         <v>0.8</v>
       </c>
       <c r="I10" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>23</v>
       </c>
       <c r="J10" s="95"/>
@@ -5335,9 +5752,9 @@
       <c r="BM10" s="107"/>
       <c r="BN10" s="107"/>
     </row>
-    <row r="11" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:122" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="60" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="63"/>
         <v>1.3</v>
       </c>
       <c r="B11" s="126" t="s">
@@ -5351,7 +5768,7 @@
         <v>43139</v>
       </c>
       <c r="F11" s="101">
-        <f t="shared" ref="F11:F43" si="35">IF(ISBLANK(E11)," - ",IF(G11=0,E11,E11+G11-1))</f>
+        <f t="shared" ref="F11:F43" si="64">IF(ISBLANK(E11)," - ",IF(G11=0,E11,E11+G11-1))</f>
         <v>43142</v>
       </c>
       <c r="G11" s="62">
@@ -5361,7 +5778,7 @@
         <v>0.5</v>
       </c>
       <c r="I11" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>2</v>
       </c>
       <c r="J11" s="95"/>
@@ -5422,7 +5839,7 @@
       <c r="BM11" s="107"/>
       <c r="BN11" s="107"/>
     </row>
-    <row r="12" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:122" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.3.1</v>
@@ -5445,7 +5862,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>5</v>
       </c>
       <c r="J12" s="95"/>
@@ -5506,7 +5923,7 @@
       <c r="BM12" s="107"/>
       <c r="BN12" s="107"/>
     </row>
-    <row r="13" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:122" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.3.2</v>
@@ -5519,7 +5936,7 @@
         <v>43384</v>
       </c>
       <c r="F13" s="101">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v>43403</v>
       </c>
       <c r="G13" s="62">
@@ -5529,7 +5946,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>14</v>
       </c>
       <c r="J13" s="95"/>
@@ -5590,9 +6007,9 @@
       <c r="BM13" s="107"/>
       <c r="BN13" s="107"/>
     </row>
-    <row r="14" spans="1:94" s="61" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:122" s="61" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="60" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="63"/>
         <v>1.4</v>
       </c>
       <c r="B14" s="126" t="s">
@@ -5606,7 +6023,7 @@
         <v>43405</v>
       </c>
       <c r="F14" s="101">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v>43409</v>
       </c>
       <c r="G14" s="62">
@@ -5616,7 +6033,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>3</v>
       </c>
       <c r="J14" s="95"/>
@@ -5677,9 +6094,9 @@
       <c r="BM14" s="107"/>
       <c r="BN14" s="107"/>
     </row>
-    <row r="15" spans="1:94" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:122" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="60" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="63"/>
         <v>1.5</v>
       </c>
       <c r="B15" s="126" t="s">
@@ -5703,7 +6120,7 @@
         <v>0.95</v>
       </c>
       <c r="I15" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>22</v>
       </c>
       <c r="J15" s="95"/>
@@ -5764,7 +6181,7 @@
       <c r="BM15" s="107"/>
       <c r="BN15" s="107"/>
     </row>
-    <row r="16" spans="1:94" s="55" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:122" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>2</v>
@@ -5775,13 +6192,13 @@
       <c r="D16" s="56"/>
       <c r="E16" s="102"/>
       <c r="F16" s="102" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G16" s="57"/>
       <c r="H16" s="58"/>
       <c r="I16" s="59" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J16" s="96"/>
@@ -5842,7 +6259,7 @@
       <c r="BM16" s="109"/>
       <c r="BN16" s="109"/>
     </row>
-    <row r="17" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.1</v>
@@ -5930,7 +6347,7 @@
       <c r="BM17" s="107"/>
       <c r="BN17" s="107"/>
     </row>
-    <row r="18" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.2</v>
@@ -5946,7 +6363,7 @@
         <v>43354</v>
       </c>
       <c r="F18" s="101">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v>43367</v>
       </c>
       <c r="G18" s="62">
@@ -5956,7 +6373,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>10</v>
       </c>
       <c r="J18" s="95"/>
@@ -6017,7 +6434,7 @@
       <c r="BM18" s="107"/>
       <c r="BN18" s="107"/>
     </row>
-    <row r="19" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.3</v>
@@ -6033,7 +6450,7 @@
         <v>43374</v>
       </c>
       <c r="F19" s="101">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v>43392</v>
       </c>
       <c r="G19" s="62">
@@ -6043,7 +6460,7 @@
         <v>0.9</v>
       </c>
       <c r="I19" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>15</v>
       </c>
       <c r="J19" s="95"/>
@@ -6104,7 +6521,7 @@
       <c r="BM19" s="107"/>
       <c r="BN19" s="107"/>
     </row>
-    <row r="20" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.4</v>
@@ -6120,7 +6537,7 @@
         <v>43364</v>
       </c>
       <c r="F20" s="101">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v>43367</v>
       </c>
       <c r="G20" s="62">
@@ -6130,7 +6547,7 @@
         <v>0.6</v>
       </c>
       <c r="I20" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>2</v>
       </c>
       <c r="J20" s="95"/>
@@ -6191,7 +6608,7 @@
       <c r="BM20" s="107"/>
       <c r="BN20" s="107"/>
     </row>
-    <row r="21" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.5</v>
@@ -6204,7 +6621,7 @@
         <v>43154</v>
       </c>
       <c r="F21" s="101">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v>43156</v>
       </c>
       <c r="G21" s="62">
@@ -6214,7 +6631,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="J21" s="95"/>
@@ -6275,7 +6692,7 @@
       <c r="BM21" s="107"/>
       <c r="BN21" s="107"/>
     </row>
-    <row r="22" spans="1:66" s="55" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:90" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>3</v>
@@ -6286,13 +6703,13 @@
       <c r="D22" s="56"/>
       <c r="E22" s="102"/>
       <c r="F22" s="102" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G22" s="57"/>
       <c r="H22" s="58"/>
       <c r="I22" s="59" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J22" s="96"/>
@@ -6353,7 +6770,7 @@
       <c r="BM22" s="109"/>
       <c r="BN22" s="109"/>
     </row>
-    <row r="23" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.1</v>
@@ -6369,18 +6786,18 @@
         <v>43384</v>
       </c>
       <c r="F23" s="101">
-        <f t="shared" si="35"/>
-        <v>43408</v>
+        <f t="shared" si="64"/>
+        <v>43418</v>
       </c>
       <c r="G23" s="62">
+        <v>35</v>
+      </c>
+      <c r="H23" s="63">
+        <v>1</v>
+      </c>
+      <c r="I23" s="64">
+        <f t="shared" si="62"/>
         <v>25</v>
-      </c>
-      <c r="H23" s="63">
-        <v>0</v>
-      </c>
-      <c r="I23" s="64">
-        <f t="shared" si="33"/>
-        <v>17</v>
       </c>
       <c r="J23" s="95"/>
       <c r="K23" s="107"/>
@@ -6439,8 +6856,32 @@
       <c r="BL23" s="107"/>
       <c r="BM23" s="107"/>
       <c r="BN23" s="107"/>
-    </row>
-    <row r="24" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+      <c r="BO23" s="107"/>
+      <c r="BP23" s="107"/>
+      <c r="BQ23" s="107"/>
+      <c r="BR23" s="107"/>
+      <c r="BS23" s="107"/>
+      <c r="BT23" s="107"/>
+      <c r="BU23" s="107"/>
+      <c r="BV23" s="107"/>
+      <c r="BW23" s="107"/>
+      <c r="BX23" s="107"/>
+      <c r="BY23" s="107"/>
+      <c r="BZ23" s="107"/>
+      <c r="CA23" s="107"/>
+      <c r="CB23" s="107"/>
+      <c r="CC23" s="107"/>
+      <c r="CD23" s="107"/>
+      <c r="CE23" s="107"/>
+      <c r="CF23" s="107"/>
+      <c r="CG23" s="107"/>
+      <c r="CH23" s="107"/>
+      <c r="CI23" s="107"/>
+      <c r="CJ23" s="107"/>
+      <c r="CK23" s="107"/>
+      <c r="CL23" s="107"/>
+    </row>
+    <row r="24" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.2</v>
@@ -6453,11 +6894,11 @@
       </c>
       <c r="D24" s="127"/>
       <c r="E24" s="100">
-        <v>43384</v>
+        <v>43418</v>
       </c>
       <c r="F24" s="101">
-        <f t="shared" si="35"/>
-        <v>43385</v>
+        <f t="shared" si="64"/>
+        <v>43419</v>
       </c>
       <c r="G24" s="62">
         <v>2</v>
@@ -6466,7 +6907,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>2</v>
       </c>
       <c r="J24" s="95"/>
@@ -6527,7 +6968,7 @@
       <c r="BM24" s="107"/>
       <c r="BN24" s="107"/>
     </row>
-    <row r="25" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.3</v>
@@ -6543,7 +6984,7 @@
         <v>43384</v>
       </c>
       <c r="F25" s="101">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v>43390</v>
       </c>
       <c r="G25" s="62">
@@ -6553,7 +6994,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>5</v>
       </c>
       <c r="J25" s="95"/>
@@ -6614,7 +7055,7 @@
       <c r="BM25" s="107"/>
       <c r="BN25" s="107"/>
     </row>
-    <row r="26" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.4</v>
@@ -6630,7 +7071,7 @@
         <v>43384</v>
       </c>
       <c r="F26" s="101">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v>43397</v>
       </c>
       <c r="G26" s="62">
@@ -6640,7 +7081,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>10</v>
       </c>
       <c r="J26" s="95"/>
@@ -6701,7 +7142,7 @@
       <c r="BM26" s="107"/>
       <c r="BN26" s="107"/>
     </row>
-    <row r="27" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.5</v>
@@ -6717,7 +7158,7 @@
         <v>43384</v>
       </c>
       <c r="F27" s="101">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v>43384</v>
       </c>
       <c r="G27" s="62">
@@ -6727,7 +7168,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="J27" s="95"/>
@@ -6788,7 +7229,7 @@
       <c r="BM27" s="107"/>
       <c r="BN27" s="107"/>
     </row>
-    <row r="28" spans="1:66" s="55" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:90" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>4</v>
@@ -6799,13 +7240,13 @@
       <c r="D28" s="56"/>
       <c r="E28" s="102"/>
       <c r="F28" s="102" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G28" s="57"/>
       <c r="H28" s="58"/>
       <c r="I28" s="59" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J28" s="96"/>
@@ -6866,7 +7307,7 @@
       <c r="BM28" s="109"/>
       <c r="BN28" s="109"/>
     </row>
-    <row r="29" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.1</v>
@@ -6892,7 +7333,7 @@
         <v>1</v>
       </c>
       <c r="I29" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>3</v>
       </c>
       <c r="J29" s="95"/>
@@ -6953,7 +7394,7 @@
       <c r="BM29" s="107"/>
       <c r="BN29" s="107"/>
     </row>
-    <row r="30" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.2</v>
@@ -6969,7 +7410,7 @@
         <v>43354</v>
       </c>
       <c r="F30" s="101">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v>43354</v>
       </c>
       <c r="G30" s="62">
@@ -6979,7 +7420,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="J30" s="95"/>
@@ -7040,7 +7481,7 @@
       <c r="BM30" s="107"/>
       <c r="BN30" s="107"/>
     </row>
-    <row r="31" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.3</v>
@@ -7066,7 +7507,7 @@
         <v>1</v>
       </c>
       <c r="I31" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="J31" s="95"/>
@@ -7127,7 +7568,7 @@
       <c r="BM31" s="107"/>
       <c r="BN31" s="107"/>
     </row>
-    <row r="32" spans="1:66" s="55" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:90" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>5</v>
@@ -7138,13 +7579,13 @@
       <c r="D32" s="56"/>
       <c r="E32" s="102"/>
       <c r="F32" s="102" t="str">
-        <f t="shared" ref="F32" si="36">IF(ISBLANK(E32)," - ",IF(G32=0,E32,E32+G32-1))</f>
+        <f t="shared" ref="F32" si="65">IF(ISBLANK(E32)," - ",IF(G32=0,E32,E32+G32-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G32" s="57"/>
       <c r="H32" s="58"/>
       <c r="I32" s="59" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J32" s="96"/>
@@ -7205,7 +7646,7 @@
       <c r="BM32" s="109"/>
       <c r="BN32" s="109"/>
     </row>
-    <row r="33" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
@@ -7291,7 +7732,7 @@
       <c r="BM33" s="107"/>
       <c r="BN33" s="107"/>
     </row>
-    <row r="34" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.2</v>
@@ -7307,7 +7748,7 @@
         <v>43391</v>
       </c>
       <c r="F34" s="101">
-        <f t="shared" ref="F34" si="37">IF(ISBLANK(E34)," - ",IF(G34=0,E34,E34+G34-1))</f>
+        <f t="shared" ref="F34" si="66">IF(ISBLANK(E34)," - ",IF(G34=0,E34,E34+G34-1))</f>
         <v>43413</v>
       </c>
       <c r="G34" s="62">
@@ -7377,7 +7818,7 @@
       <c r="BM34" s="107"/>
       <c r="BN34" s="107"/>
     </row>
-    <row r="35" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.3</v>
@@ -7403,7 +7844,7 @@
         <v>0.9</v>
       </c>
       <c r="I35" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="J35" s="95"/>
@@ -7464,7 +7905,7 @@
       <c r="BM35" s="107"/>
       <c r="BN35" s="107"/>
     </row>
-    <row r="36" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.4</v>
@@ -7477,7 +7918,7 @@
         <v>43132</v>
       </c>
       <c r="F36" s="101">
-        <f t="shared" ref="F36:F37" si="38">IF(ISBLANK(E36)," - ",IF(G36=0,E36,E36+G36-1))</f>
+        <f t="shared" ref="F36:F37" si="67">IF(ISBLANK(E36)," - ",IF(G36=0,E36,E36+G36-1))</f>
         <v>43132</v>
       </c>
       <c r="G36" s="62">
@@ -7487,7 +7928,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="J36" s="95"/>
@@ -7548,7 +7989,7 @@
       <c r="BM36" s="107"/>
       <c r="BN36" s="107"/>
     </row>
-    <row r="37" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.5</v>
@@ -7561,7 +8002,7 @@
         <v>43133</v>
       </c>
       <c r="F37" s="101">
-        <f t="shared" si="38"/>
+        <f t="shared" si="67"/>
         <v>43133</v>
       </c>
       <c r="G37" s="62">
@@ -7571,7 +8012,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="J37" s="95"/>
@@ -7632,7 +8073,7 @@
       <c r="BM37" s="107"/>
       <c r="BN37" s="107"/>
     </row>
-    <row r="38" spans="1:66" s="55" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>6</v>
@@ -7643,13 +8084,13 @@
       <c r="D38" s="56"/>
       <c r="E38" s="102"/>
       <c r="F38" s="102" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G38" s="57"/>
       <c r="H38" s="58"/>
       <c r="I38" s="59" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J38" s="96"/>
@@ -7710,7 +8151,7 @@
       <c r="BM38" s="109"/>
       <c r="BN38" s="109"/>
     </row>
-    <row r="39" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>6.1</v>
@@ -7723,7 +8164,7 @@
         <v>43129</v>
       </c>
       <c r="F39" s="101">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v>43129</v>
       </c>
       <c r="G39" s="62">
@@ -7733,7 +8174,7 @@
         <v>0</v>
       </c>
       <c r="I39" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="J39" s="95"/>
@@ -7794,7 +8235,7 @@
       <c r="BM39" s="107"/>
       <c r="BN39" s="107"/>
     </row>
-    <row r="40" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>6.2</v>
@@ -7807,7 +8248,7 @@
         <v>43130</v>
       </c>
       <c r="F40" s="101">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v>43130</v>
       </c>
       <c r="G40" s="62">
@@ -7817,7 +8258,7 @@
         <v>0</v>
       </c>
       <c r="I40" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="J40" s="95"/>
@@ -7878,7 +8319,7 @@
       <c r="BM40" s="107"/>
       <c r="BN40" s="107"/>
     </row>
-    <row r="41" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>6.3</v>
@@ -7891,7 +8332,7 @@
         <v>43131</v>
       </c>
       <c r="F41" s="101">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v>43131</v>
       </c>
       <c r="G41" s="62">
@@ -7901,7 +8342,7 @@
         <v>0</v>
       </c>
       <c r="I41" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="J41" s="95"/>
@@ -7962,7 +8403,7 @@
       <c r="BM41" s="107"/>
       <c r="BN41" s="107"/>
     </row>
-    <row r="42" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>6.4</v>
@@ -7975,7 +8416,7 @@
         <v>43132</v>
       </c>
       <c r="F42" s="101">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v>43132</v>
       </c>
       <c r="G42" s="62">
@@ -7985,7 +8426,7 @@
         <v>0</v>
       </c>
       <c r="I42" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="J42" s="95"/>
@@ -8046,7 +8487,7 @@
       <c r="BM42" s="107"/>
       <c r="BN42" s="107"/>
     </row>
-    <row r="43" spans="1:66" s="61" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>6.5</v>
@@ -8059,7 +8500,7 @@
         <v>43133</v>
       </c>
       <c r="F43" s="101">
-        <f t="shared" si="35"/>
+        <f t="shared" si="64"/>
         <v>43133</v>
       </c>
       <c r="G43" s="62">
@@ -8069,7 +8510,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="J43" s="95"/>
@@ -8130,7 +8571,7 @@
       <c r="BM43" s="107"/>
       <c r="BN43" s="107"/>
     </row>
-    <row r="44" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="60"/>
       <c r="B44" s="65"/>
       <c r="C44" s="65"/>
@@ -8140,7 +8581,7 @@
       <c r="G44" s="67"/>
       <c r="H44" s="68"/>
       <c r="I44" s="69" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J44" s="97"/>
@@ -8201,7 +8642,7 @@
       <c r="BM44" s="107"/>
       <c r="BN44" s="107"/>
     </row>
-    <row r="45" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="60"/>
       <c r="B45" s="65"/>
       <c r="C45" s="65"/>
@@ -8211,7 +8652,7 @@
       <c r="G45" s="67"/>
       <c r="H45" s="68"/>
       <c r="I45" s="69" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="62"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J45" s="97"/>
@@ -8272,7 +8713,7 @@
       <c r="BM45" s="107"/>
       <c r="BN45" s="107"/>
     </row>
-    <row r="46" spans="1:66" s="75" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:66" s="75" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="71" t="s">
         <v>1</v>
       </c>
@@ -8342,7 +8783,7 @@
       <c r="BM46" s="107"/>
       <c r="BN46" s="107"/>
     </row>
-    <row r="47" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="76" t="s">
         <v>39</v>
       </c>
@@ -8412,7 +8853,7 @@
       <c r="BM47" s="107"/>
       <c r="BN47" s="107"/>
     </row>
-    <row r="48" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="130" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -8424,7 +8865,7 @@
       <c r="D48" s="79"/>
       <c r="E48" s="100"/>
       <c r="F48" s="101" t="str">
-        <f t="shared" ref="F48:F51" si="39">IF(ISBLANK(E48)," - ",IF(G48=0,E48,E48+G48-1))</f>
+        <f t="shared" ref="F48:F51" si="68">IF(ISBLANK(E48)," - ",IF(G48=0,E48,E48+G48-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G48" s="62"/>
@@ -8491,7 +8932,7 @@
       <c r="BM48" s="107"/>
       <c r="BN48" s="107"/>
     </row>
-    <row r="49" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -8503,13 +8944,13 @@
       <c r="D49" s="79"/>
       <c r="E49" s="100"/>
       <c r="F49" s="101" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="68"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G49" s="62"/>
       <c r="H49" s="63"/>
       <c r="I49" s="80" t="str">
-        <f t="shared" ref="I49:I51" si="40">IF(OR(F49=0,E49=0)," - ",NETWORKDAYS(E49,F49))</f>
+        <f t="shared" ref="I49:I51" si="69">IF(OR(F49=0,E49=0)," - ",NETWORKDAYS(E49,F49))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J49" s="99"/>
@@ -8570,7 +9011,7 @@
       <c r="BM49" s="107"/>
       <c r="BN49" s="107"/>
     </row>
-    <row r="50" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.1</v>
@@ -8582,13 +9023,13 @@
       <c r="D50" s="79"/>
       <c r="E50" s="100"/>
       <c r="F50" s="101" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="68"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G50" s="62"/>
       <c r="H50" s="63"/>
       <c r="I50" s="80" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="69"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J50" s="99"/>
@@ -8649,7 +9090,7 @@
       <c r="BM50" s="107"/>
       <c r="BN50" s="107"/>
     </row>
-    <row r="51" spans="1:66" s="70" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
         <v>1.1.1.1</v>
@@ -8661,13 +9102,13 @@
       <c r="D51" s="79"/>
       <c r="E51" s="100"/>
       <c r="F51" s="101" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="68"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G51" s="62"/>
       <c r="H51" s="63"/>
       <c r="I51" s="80" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="69"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J51" s="99"/>
@@ -8728,7 +9169,7 @@
       <c r="BM51" s="107"/>
       <c r="BN51" s="107"/>
     </row>
-    <row r="52" spans="1:66" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:66" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="30"/>
       <c r="B52" s="31"/>
       <c r="C52" s="31"/>
@@ -8798,16 +9239,23 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
-  <mergeCells count="27">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
+  <mergeCells count="35">
+    <mergeCell ref="DL4:DR4"/>
+    <mergeCell ref="DL5:DR5"/>
+    <mergeCell ref="CQ4:CW4"/>
+    <mergeCell ref="CQ5:CW5"/>
+    <mergeCell ref="CX4:DD4"/>
+    <mergeCell ref="CX5:DD5"/>
+    <mergeCell ref="DE4:DK4"/>
+    <mergeCell ref="DE5:DK5"/>
+    <mergeCell ref="CJ4:CP4"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BO4:BU4"/>
+    <mergeCell ref="BV4:CB4"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="CC5:CI5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -8818,18 +9266,19 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="CJ4:CP4"/>
-    <mergeCell ref="CJ5:CP5"/>
-    <mergeCell ref="BO5:BU5"/>
-    <mergeCell ref="BO4:BU4"/>
-    <mergeCell ref="BV4:CB4"/>
-    <mergeCell ref="BV5:CB5"/>
-    <mergeCell ref="CC4:CI4"/>
-    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8:H27 H38:H51">
-    <cfRule type="dataBar" priority="20">
+    <cfRule type="dataBar" priority="28">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8843,73 +9292,73 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN7">
-    <cfRule type="expression" dxfId="18" priority="63">
+    <cfRule type="expression" dxfId="26" priority="71">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BN27 K38:BN51">
-    <cfRule type="expression" dxfId="17" priority="66">
+  <conditionalFormatting sqref="K8:BN27 K38:BN51 BO23:CL23">
+    <cfRule type="expression" dxfId="25" priority="74">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="67">
+    <cfRule type="expression" dxfId="24" priority="75">
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:BN27 K38:BN51">
-    <cfRule type="expression" dxfId="15" priority="26">
+  <conditionalFormatting sqref="K6:BN27 K38:BN51 BO23:CL23">
+    <cfRule type="expression" dxfId="23" priority="34">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO6:BU7">
-    <cfRule type="expression" dxfId="14" priority="18">
+    <cfRule type="expression" dxfId="22" priority="26">
       <formula>BO$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO6:BU7">
-    <cfRule type="expression" dxfId="13" priority="17">
+    <cfRule type="expression" dxfId="21" priority="25">
       <formula>BO$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV6:CB7">
-    <cfRule type="expression" dxfId="12" priority="16">
+    <cfRule type="expression" dxfId="20" priority="24">
       <formula>BV$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV6:CB7">
-    <cfRule type="expression" dxfId="11" priority="15">
+    <cfRule type="expression" dxfId="19" priority="23">
       <formula>BV$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC6:CI7">
-    <cfRule type="expression" dxfId="10" priority="14">
+    <cfRule type="expression" dxfId="18" priority="22">
       <formula>CC$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC6:CI7">
-    <cfRule type="expression" dxfId="9" priority="13">
+    <cfRule type="expression" dxfId="17" priority="21">
       <formula>CC$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ6:CP7">
-    <cfRule type="expression" dxfId="8" priority="12">
+    <cfRule type="expression" dxfId="16" priority="20">
       <formula>CJ$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ6:CP7">
-    <cfRule type="expression" dxfId="7" priority="11">
+    <cfRule type="expression" dxfId="15" priority="19">
       <formula>CJ$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:BN37">
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="14" priority="17">
       <formula>AND($E32&lt;=K$6,ROUNDDOWN(($F32-$E32+1)*$H32,0)+$E32-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="10">
+    <cfRule type="expression" dxfId="13" priority="18">
       <formula>AND(NOT(ISBLANK($E32)),$E32&lt;=K$6,$F32&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28:H31">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8923,20 +9372,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28:BN31">
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="12" priority="15">
       <formula>AND($E28&lt;=K$6,ROUNDDOWN(($F28-$E28+1)*$H28,0)+$E28-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="11" priority="16">
       <formula>AND(NOT(ISBLANK($E28)),$E28&lt;=K$6,$F28&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28:BN31">
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="10" priority="14">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32:H35">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8950,7 +9399,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36:H37">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8964,13 +9413,53 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36:BN37">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="9" priority="12">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:BN35">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CQ6:CW7">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>CQ$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CQ6:CW7">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>CQ$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CX6:DD7">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>CX$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CX6:DD7">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>CX$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="DE6:DK7">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>DE$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="DE6:DK7">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>DE$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="DL6:DR7">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>DL$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="DL6:DR7">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>DL$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
@@ -8983,7 +9472,7 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 A44:B45 B39 B40:B42 A47:B47 B46 E16 E22 E38 E44:H47 G14 G11 G16:H16 G22:H22 G38:H42 G48 G49:G50 G51 H23:H26" unlockedFormula="1"/>
+    <ignoredError sqref="H9 A44:B45 B39 B40:B42 A47:B47 B46 E16 E22 E38 E44:H47 G14 G11 G16:H16 G22:H22 G38:H42 G48 G49:G50 G51 H24:H26" unlockedFormula="1"/>
     <ignoredError sqref="A38 A22 A16" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
@@ -9000,11 +9489,11 @@
                     <xdr:col>9</xdr:col>
                     <xdr:colOff>95250</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>127000</xdr:rowOff>
+                    <xdr:rowOff>123825</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>27</xdr:col>
-                    <xdr:colOff>107950</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>114300</xdr:rowOff>
                   </to>
@@ -9096,175 +9585,175 @@
       <selection activeCell="A16" sqref="A16:C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.54296875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="37.7265625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="55.1796875" style="16" customWidth="1"/>
-    <col min="4" max="7" width="8.81640625" style="16"/>
+    <col min="1" max="1" width="5.5703125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" style="16" customWidth="1"/>
+    <col min="3" max="3" width="55.140625" style="16" customWidth="1"/>
+    <col min="4" max="7" width="8.85546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C4" s="23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C5" s="20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C6" s="20"/>
     </row>
-    <row r="7" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="C7" s="24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C8" s="25" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C10" s="20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C11" s="20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="C13" s="24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:2" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="2:2" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B29" s="20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B30" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B31" s="16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B32" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B34" s="26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="20" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="20" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" s="20" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="2:2" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B42" s="26" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B43" s="20" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B44" s="20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:2" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="2:2" ht="18" x14ac:dyDescent="0.25">
       <c r="B46" s="24" t="s">
         <v>24</v>
       </c>
@@ -9290,74 +9779,74 @@
       <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.54296875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="90.453125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.81640625" style="7"/>
+    <col min="1" max="1" width="5.5703125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="90.42578125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
         <v>124</v>
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="42"/>
     </row>
-    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="138" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="8"/>
     </row>
-    <row r="3" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
       <c r="B3" s="9"/>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="133" t="s">
         <v>91</v>
       </c>
       <c r="B4" s="39"/>
     </row>
-    <row r="5" spans="1:3" s="8" customFormat="1" ht="56" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" s="8" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="B5" s="139" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B7" s="139" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B9" s="138" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B11" s="137" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="172" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="172"/>
     </row>
-    <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:3" s="134" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:3" s="134" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="142"/>
       <c r="B15" s="140" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="134" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="134" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="142"/>
       <c r="B16" s="141" t="s">
         <v>81</v>
@@ -9366,25 +9855,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="143"/>
       <c r="B17" s="141" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="20" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="143"/>
       <c r="B18" s="141" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="42" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="146"/>
       <c r="B19" s="141" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="134" customFormat="1" ht="17.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" s="134" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="142"/>
       <c r="B20" s="140" t="s">
         <v>82</v>
@@ -9393,153 +9882,153 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="143"/>
       <c r="B21" s="141" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="144"/>
       <c r="B22" s="145" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="144"/>
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="172" t="s">
         <v>87</v>
       </c>
       <c r="B24" s="172"/>
     </row>
-    <row r="25" spans="1:3" s="8" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A25" s="144"/>
       <c r="B25" s="141" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="144"/>
       <c r="B26" s="141"/>
     </row>
-    <row r="27" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="144"/>
       <c r="B27" s="162" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="144"/>
       <c r="B28" s="141" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A29" s="144"/>
       <c r="B29" s="141" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="144"/>
       <c r="B30" s="141"/>
     </row>
-    <row r="31" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="144"/>
       <c r="B31" s="162" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="144"/>
       <c r="B32" s="141" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:2" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="144"/>
       <c r="B33" s="141" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="144"/>
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:2" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A35" s="144"/>
       <c r="B35" s="141" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="144"/>
       <c r="B36" s="147" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:2" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="144"/>
       <c r="B37" s="10"/>
     </row>
-    <row r="38" spans="1:2" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="172" t="s">
         <v>11</v>
       </c>
       <c r="B38" s="172"/>
     </row>
-    <row r="39" spans="1:2" ht="28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B39" s="141" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:2" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:2" s="20" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B41" s="141" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:2" s="20" customFormat="1" ht="28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:2" s="20" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B43" s="141" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:2" ht="28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B45" s="141" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="21"/>
     </row>
-    <row r="47" spans="1:2" ht="28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B47" s="141" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" s="11"/>
     </row>
-    <row r="49" spans="1:2" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="172" t="s">
         <v>7</v>
       </c>
       <c r="B49" s="172"/>
     </row>
-    <row r="50" spans="1:2" ht="28" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B50" s="141" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B51" s="11"/>
     </row>
-    <row r="52" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A52" s="148" t="s">
         <v>12</v>
       </c>
@@ -9547,7 +10036,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A53" s="148" t="s">
         <v>14</v>
       </c>
@@ -9555,7 +10044,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A54" s="148" t="s">
         <v>16</v>
       </c>
@@ -9563,19 +10052,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A55" s="137"/>
       <c r="B55" s="141" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A56" s="137"/>
       <c r="B56" s="141" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A57" s="148" t="s">
         <v>18</v>
       </c>
@@ -9583,19 +10072,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A58" s="137"/>
       <c r="B58" s="141" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A59" s="137"/>
       <c r="B59" s="141" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A60" s="148" t="s">
         <v>20</v>
       </c>
@@ -9603,13 +10092,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A61" s="137"/>
       <c r="B61" s="141" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A62" s="148" t="s">
         <v>110</v>
       </c>
@@ -9617,36 +10106,36 @@
         <v>111</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A63" s="149"/>
       <c r="B63" s="141" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B64" s="12"/>
     </row>
-    <row r="65" spans="1:2" s="20" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="172" t="s">
         <v>10</v>
       </c>
       <c r="B65" s="172"/>
     </row>
-    <row r="66" spans="1:2" s="20" customFormat="1" ht="42" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" s="20" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B66" s="141" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B67" s="13"/>
     </row>
-    <row r="68" spans="1:2" s="8" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="172" t="s">
         <v>5</v>
       </c>
       <c r="B68" s="172"/>
     </row>
-    <row r="69" spans="1:2" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="156" t="s">
         <v>6</v>
       </c>
@@ -9654,17 +10143,17 @@
         <v>114</v>
       </c>
     </row>
-    <row r="70" spans="1:2" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A70" s="150"/>
       <c r="B70" s="155" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:2" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A71" s="150"/>
       <c r="B71" s="151"/>
     </row>
-    <row r="72" spans="1:2" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="156" t="s">
         <v>6</v>
       </c>
@@ -9672,17 +10161,17 @@
         <v>133</v>
       </c>
     </row>
-    <row r="73" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A73" s="150"/>
       <c r="B73" s="155" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="74" spans="1:2" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A74" s="150"/>
       <c r="B74" s="151"/>
     </row>
-    <row r="75" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="156" t="s">
         <v>6</v>
       </c>
@@ -9690,17 +10179,17 @@
         <v>119</v>
       </c>
     </row>
-    <row r="76" spans="1:2" s="8" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A76" s="150"/>
       <c r="B76" s="139" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A77" s="149"/>
       <c r="B77" s="149"/>
     </row>
-    <row r="78" spans="1:2" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="156" t="s">
         <v>6</v>
       </c>
@@ -9708,17 +10197,17 @@
         <v>125</v>
       </c>
     </row>
-    <row r="79" spans="1:2" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A79" s="150"/>
       <c r="B79" s="139" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="80" spans="1:2" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" s="20" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A80" s="149"/>
       <c r="B80" s="149"/>
     </row>
-    <row r="81" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="156" t="s">
         <v>6</v>
       </c>
@@ -9726,29 +10215,29 @@
         <v>126</v>
       </c>
     </row>
-    <row r="82" spans="1:2" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A82" s="150"/>
       <c r="B82" s="154" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="83" spans="1:2" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A83" s="150"/>
       <c r="B83" s="154" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="84" spans="1:2" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A84" s="150"/>
       <c r="B84" s="154" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="149"/>
       <c r="B85" s="153"/>
     </row>
-    <row r="86" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="156" t="s">
         <v>6</v>
       </c>
@@ -9756,29 +10245,29 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:2" s="8" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A87" s="150"/>
       <c r="B87" s="139" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="88" spans="1:2" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A88" s="150"/>
       <c r="B88" s="152" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="89" spans="1:2" s="8" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" s="8" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A89" s="150"/>
       <c r="B89" s="158" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A90" s="149"/>
       <c r="B90" s="149"/>
     </row>
-    <row r="91" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="156" t="s">
         <v>6</v>
       </c>
@@ -9786,13 +10275,13 @@
         <v>128</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="28" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A92" s="137"/>
       <c r="B92" s="154" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="28" t="s">
         <v>55</v>
       </c>
@@ -9828,14 +10317,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.54296875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="20" customWidth="1"/>
-    <col min="3" max="16384" width="8.81640625" style="16"/>
+    <col min="1" max="1" width="5.5703125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="20" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
         <v>53</v>
       </c>
@@ -9843,163 +10332,163 @@
       <c r="C1" s="45"/>
       <c r="D1" s="45"/>
     </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="42"/>
       <c r="B2" s="46"/>
       <c r="C2" s="45"/>
       <c r="D2" s="45"/>
     </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="43"/>
       <c r="B3" s="36" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="44"/>
     </row>
-    <row r="4" spans="1:4" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
       <c r="B4" s="38" t="s">
         <v>50</v>
       </c>
       <c r="C4" s="15"/>
     </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="17"/>
       <c r="C5" s="15"/>
     </row>
-    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="18" t="s">
         <v>55</v>
       </c>
       <c r="C6" s="15"/>
     </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="17"/>
       <c r="C7" s="15"/>
     </row>
-    <row r="8" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="17" t="s">
         <v>56</v>
       </c>
       <c r="C8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
       <c r="B9" s="17"/>
       <c r="C9" s="15"/>
     </row>
-    <row r="10" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="17" t="s">
         <v>57</v>
       </c>
       <c r="C10" s="15"/>
     </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="B11" s="17"/>
       <c r="C11" s="15"/>
     </row>
-    <row r="12" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
       <c r="B12" s="17" t="s">
         <v>58</v>
       </c>
       <c r="C12" s="15"/>
     </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
       <c r="B13" s="17"/>
       <c r="C13" s="15"/>
     </row>
-    <row r="14" spans="1:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
       <c r="B14" s="17" t="s">
         <v>59</v>
       </c>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
       <c r="B15" s="17"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="30.75" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
       <c r="B16" s="17" t="s">
         <v>60</v>
       </c>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
       <c r="B17" s="17"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="18" t="s">
         <v>61</v>
       </c>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="B19" s="37" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
       <c r="B20" s="19"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>

</xml_diff>

<commit_message>
Amine - Gantt excel update + added the robot project meetings PP
</commit_message>
<xml_diff>
--- a/Gantt_Diagram_Robot_Project_2018.xlsx
+++ b/Gantt_Diagram_Robot_Project_2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evaux\Documents\Internship_Projects\4_Robot\Robot_Project_IFX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaizi\Desktop\Robot_Project_IFX\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="0">GanttChart!$A1048576</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$49</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">GanttChartPro!$A$1:$C$47</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">GanttChart!$4:$7</definedName>
     <definedName name="valuevx">42.314159</definedName>
@@ -442,7 +442,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="174">
   <si>
     <t>WBS</t>
   </si>
@@ -1564,9 +1564,6 @@
     <t>Soldered circuit</t>
   </si>
   <si>
-    <t>Proportional correction</t>
-  </si>
-  <si>
     <t>Gyroscope/Accelerometer</t>
   </si>
   <si>
@@ -1634,6 +1631,21 @@
   </si>
   <si>
     <t>Software processing (Raspberry and Aurix)</t>
+  </si>
+  <si>
+    <t>Proportional correction - Wheel Enslvement V1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wheel Enslvement V2 - in interrupts</t>
+  </si>
+  <si>
+    <t>Adapt code to make proper Remote control with bluetooth</t>
+  </si>
+  <si>
+    <t>Write on wiki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wiki Page (unfinished and modified because of new enslavement) </t>
   </si>
 </sst>
 </file>
@@ -2993,23 +3005,11 @@
     </xf>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="42" fillId="27" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3018,18 +3018,30 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="27" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3078,7 +3090,111 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="44">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -3493,7 +3609,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="8"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4149,11 +4265,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DR53"/>
+  <dimension ref="A1:DR56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4230,29 +4346,29 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
       <c r="I1" s="132"/>
-      <c r="K1" s="169" t="s">
+      <c r="K1" s="165" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="169"/>
-      <c r="M1" s="169"/>
-      <c r="N1" s="169"/>
-      <c r="O1" s="169"/>
-      <c r="P1" s="169"/>
-      <c r="Q1" s="169"/>
-      <c r="R1" s="169"/>
-      <c r="S1" s="169"/>
-      <c r="T1" s="169"/>
-      <c r="U1" s="169"/>
-      <c r="V1" s="169"/>
-      <c r="W1" s="169"/>
-      <c r="X1" s="169"/>
-      <c r="Y1" s="169"/>
-      <c r="Z1" s="169"/>
-      <c r="AA1" s="169"/>
-      <c r="AB1" s="169"/>
-      <c r="AC1" s="169"/>
-      <c r="AD1" s="169"/>
-      <c r="AE1" s="169"/>
+      <c r="L1" s="165"/>
+      <c r="M1" s="165"/>
+      <c r="N1" s="165"/>
+      <c r="O1" s="165"/>
+      <c r="P1" s="165"/>
+      <c r="Q1" s="165"/>
+      <c r="R1" s="165"/>
+      <c r="S1" s="165"/>
+      <c r="T1" s="165"/>
+      <c r="U1" s="165"/>
+      <c r="V1" s="165"/>
+      <c r="W1" s="165"/>
+      <c r="X1" s="165"/>
+      <c r="Y1" s="165"/>
+      <c r="Z1" s="165"/>
+      <c r="AA1" s="165"/>
+      <c r="AB1" s="165"/>
+      <c r="AC1" s="165"/>
+      <c r="AD1" s="165"/>
+      <c r="AE1" s="165"/>
     </row>
     <row r="2" spans="1:122" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
@@ -4297,356 +4413,356 @@
       <c r="B4" s="114" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="171">
+      <c r="C4" s="170">
         <v>43340</v>
       </c>
-      <c r="D4" s="171"/>
-      <c r="E4" s="171"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="170"/>
       <c r="F4" s="111"/>
       <c r="G4" s="114" t="s">
         <v>75</v>
       </c>
       <c r="H4" s="129">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I4" s="112"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="163" t="str">
+      <c r="K4" s="167" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 8</v>
+      </c>
+      <c r="L4" s="168"/>
+      <c r="M4" s="168"/>
+      <c r="N4" s="168"/>
+      <c r="O4" s="168"/>
+      <c r="P4" s="168"/>
+      <c r="Q4" s="169"/>
+      <c r="R4" s="167" t="str">
+        <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 9</v>
+      </c>
+      <c r="S4" s="168"/>
+      <c r="T4" s="168"/>
+      <c r="U4" s="168"/>
+      <c r="V4" s="168"/>
+      <c r="W4" s="168"/>
+      <c r="X4" s="169"/>
+      <c r="Y4" s="167" t="str">
+        <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="L4" s="164"/>
-      <c r="M4" s="164"/>
-      <c r="N4" s="164"/>
-      <c r="O4" s="164"/>
-      <c r="P4" s="164"/>
-      <c r="Q4" s="165"/>
-      <c r="R4" s="163" t="str">
-        <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="Z4" s="168"/>
+      <c r="AA4" s="168"/>
+      <c r="AB4" s="168"/>
+      <c r="AC4" s="168"/>
+      <c r="AD4" s="168"/>
+      <c r="AE4" s="169"/>
+      <c r="AF4" s="167" t="str">
+        <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="S4" s="164"/>
-      <c r="T4" s="164"/>
-      <c r="U4" s="164"/>
-      <c r="V4" s="164"/>
-      <c r="W4" s="164"/>
-      <c r="X4" s="165"/>
-      <c r="Y4" s="163" t="str">
-        <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AG4" s="168"/>
+      <c r="AH4" s="168"/>
+      <c r="AI4" s="168"/>
+      <c r="AJ4" s="168"/>
+      <c r="AK4" s="168"/>
+      <c r="AL4" s="169"/>
+      <c r="AM4" s="167" t="str">
+        <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="Z4" s="164"/>
-      <c r="AA4" s="164"/>
-      <c r="AB4" s="164"/>
-      <c r="AC4" s="164"/>
-      <c r="AD4" s="164"/>
-      <c r="AE4" s="165"/>
-      <c r="AF4" s="163" t="str">
-        <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AN4" s="168"/>
+      <c r="AO4" s="168"/>
+      <c r="AP4" s="168"/>
+      <c r="AQ4" s="168"/>
+      <c r="AR4" s="168"/>
+      <c r="AS4" s="169"/>
+      <c r="AT4" s="167" t="str">
+        <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 13</v>
       </c>
-      <c r="AG4" s="164"/>
-      <c r="AH4" s="164"/>
-      <c r="AI4" s="164"/>
-      <c r="AJ4" s="164"/>
-      <c r="AK4" s="164"/>
-      <c r="AL4" s="165"/>
-      <c r="AM4" s="163" t="str">
-        <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AU4" s="168"/>
+      <c r="AV4" s="168"/>
+      <c r="AW4" s="168"/>
+      <c r="AX4" s="168"/>
+      <c r="AY4" s="168"/>
+      <c r="AZ4" s="169"/>
+      <c r="BA4" s="167" t="str">
+        <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 14</v>
       </c>
-      <c r="AN4" s="164"/>
-      <c r="AO4" s="164"/>
-      <c r="AP4" s="164"/>
-      <c r="AQ4" s="164"/>
-      <c r="AR4" s="164"/>
-      <c r="AS4" s="165"/>
-      <c r="AT4" s="163" t="str">
-        <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="BB4" s="168"/>
+      <c r="BC4" s="168"/>
+      <c r="BD4" s="168"/>
+      <c r="BE4" s="168"/>
+      <c r="BF4" s="168"/>
+      <c r="BG4" s="169"/>
+      <c r="BH4" s="167" t="str">
+        <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 15</v>
       </c>
-      <c r="AU4" s="164"/>
-      <c r="AV4" s="164"/>
-      <c r="AW4" s="164"/>
-      <c r="AX4" s="164"/>
-      <c r="AY4" s="164"/>
-      <c r="AZ4" s="165"/>
-      <c r="BA4" s="163" t="str">
-        <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="BI4" s="168"/>
+      <c r="BJ4" s="168"/>
+      <c r="BK4" s="168"/>
+      <c r="BL4" s="168"/>
+      <c r="BM4" s="168"/>
+      <c r="BN4" s="169"/>
+      <c r="BO4" s="167" t="str">
+        <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 16</v>
       </c>
-      <c r="BB4" s="164"/>
-      <c r="BC4" s="164"/>
-      <c r="BD4" s="164"/>
-      <c r="BE4" s="164"/>
-      <c r="BF4" s="164"/>
-      <c r="BG4" s="165"/>
-      <c r="BH4" s="163" t="str">
-        <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="BP4" s="168"/>
+      <c r="BQ4" s="168"/>
+      <c r="BR4" s="168"/>
+      <c r="BS4" s="168"/>
+      <c r="BT4" s="168"/>
+      <c r="BU4" s="169"/>
+      <c r="BV4" s="167" t="str">
+        <f>"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 17</v>
       </c>
-      <c r="BI4" s="164"/>
-      <c r="BJ4" s="164"/>
-      <c r="BK4" s="164"/>
-      <c r="BL4" s="164"/>
-      <c r="BM4" s="164"/>
-      <c r="BN4" s="165"/>
-      <c r="BO4" s="163" t="str">
-        <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="BW4" s="168"/>
+      <c r="BX4" s="168"/>
+      <c r="BY4" s="168"/>
+      <c r="BZ4" s="168"/>
+      <c r="CA4" s="168"/>
+      <c r="CB4" s="169"/>
+      <c r="CC4" s="167" t="str">
+        <f>"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 18</v>
       </c>
-      <c r="BP4" s="164"/>
-      <c r="BQ4" s="164"/>
-      <c r="BR4" s="164"/>
-      <c r="BS4" s="164"/>
-      <c r="BT4" s="164"/>
-      <c r="BU4" s="165"/>
-      <c r="BV4" s="163" t="str">
-        <f>"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="CD4" s="168"/>
+      <c r="CE4" s="168"/>
+      <c r="CF4" s="168"/>
+      <c r="CG4" s="168"/>
+      <c r="CH4" s="168"/>
+      <c r="CI4" s="169"/>
+      <c r="CJ4" s="167" t="str">
+        <f>"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 19</v>
       </c>
-      <c r="BW4" s="164"/>
-      <c r="BX4" s="164"/>
-      <c r="BY4" s="164"/>
-      <c r="BZ4" s="164"/>
-      <c r="CA4" s="164"/>
-      <c r="CB4" s="165"/>
-      <c r="CC4" s="163" t="str">
-        <f>"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="CK4" s="168"/>
+      <c r="CL4" s="168"/>
+      <c r="CM4" s="168"/>
+      <c r="CN4" s="168"/>
+      <c r="CO4" s="168"/>
+      <c r="CP4" s="169"/>
+      <c r="CQ4" s="167" t="str">
+        <f>"Week "&amp;(CQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="CD4" s="164"/>
-      <c r="CE4" s="164"/>
-      <c r="CF4" s="164"/>
-      <c r="CG4" s="164"/>
-      <c r="CH4" s="164"/>
-      <c r="CI4" s="165"/>
-      <c r="CJ4" s="163" t="str">
-        <f>"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="CR4" s="168"/>
+      <c r="CS4" s="168"/>
+      <c r="CT4" s="168"/>
+      <c r="CU4" s="168"/>
+      <c r="CV4" s="168"/>
+      <c r="CW4" s="169"/>
+      <c r="CX4" s="167" t="str">
+        <f>"Week "&amp;(CX6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="CK4" s="164"/>
-      <c r="CL4" s="164"/>
-      <c r="CM4" s="164"/>
-      <c r="CN4" s="164"/>
-      <c r="CO4" s="164"/>
-      <c r="CP4" s="165"/>
-      <c r="CQ4" s="163" t="str">
-        <f>"Week "&amp;(CQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="CY4" s="168"/>
+      <c r="CZ4" s="168"/>
+      <c r="DA4" s="168"/>
+      <c r="DB4" s="168"/>
+      <c r="DC4" s="168"/>
+      <c r="DD4" s="169"/>
+      <c r="DE4" s="167" t="str">
+        <f>"Week "&amp;(DE6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="CR4" s="164"/>
-      <c r="CS4" s="164"/>
-      <c r="CT4" s="164"/>
-      <c r="CU4" s="164"/>
-      <c r="CV4" s="164"/>
-      <c r="CW4" s="165"/>
-      <c r="CX4" s="163" t="str">
-        <f>"Week "&amp;(CX6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="DF4" s="168"/>
+      <c r="DG4" s="168"/>
+      <c r="DH4" s="168"/>
+      <c r="DI4" s="168"/>
+      <c r="DJ4" s="168"/>
+      <c r="DK4" s="169"/>
+      <c r="DL4" s="167" t="str">
+        <f>"Week "&amp;(DL6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="CY4" s="164"/>
-      <c r="CZ4" s="164"/>
-      <c r="DA4" s="164"/>
-      <c r="DB4" s="164"/>
-      <c r="DC4" s="164"/>
-      <c r="DD4" s="165"/>
-      <c r="DE4" s="163" t="str">
-        <f>"Week "&amp;(DE6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 24</v>
-      </c>
-      <c r="DF4" s="164"/>
-      <c r="DG4" s="164"/>
-      <c r="DH4" s="164"/>
-      <c r="DI4" s="164"/>
-      <c r="DJ4" s="164"/>
-      <c r="DK4" s="165"/>
-      <c r="DL4" s="163" t="str">
-        <f>"Week "&amp;(DL6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 25</v>
-      </c>
-      <c r="DM4" s="164"/>
-      <c r="DN4" s="164"/>
-      <c r="DO4" s="164"/>
-      <c r="DP4" s="164"/>
-      <c r="DQ4" s="164"/>
-      <c r="DR4" s="165"/>
+      <c r="DM4" s="168"/>
+      <c r="DN4" s="168"/>
+      <c r="DO4" s="168"/>
+      <c r="DP4" s="168"/>
+      <c r="DQ4" s="168"/>
+      <c r="DR4" s="169"/>
     </row>
     <row r="5" spans="1:122" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="110"/>
       <c r="B5" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="170" t="s">
+      <c r="C5" s="166" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
+      <c r="D5" s="166"/>
+      <c r="E5" s="166"/>
       <c r="F5" s="113"/>
       <c r="G5" s="113"/>
       <c r="H5" s="113"/>
       <c r="I5" s="113"/>
       <c r="J5" s="50"/>
-      <c r="K5" s="166">
+      <c r="K5" s="171">
         <f>K6</f>
+        <v>43388</v>
+      </c>
+      <c r="L5" s="172"/>
+      <c r="M5" s="172"/>
+      <c r="N5" s="172"/>
+      <c r="O5" s="172"/>
+      <c r="P5" s="172"/>
+      <c r="Q5" s="173"/>
+      <c r="R5" s="171">
+        <f>R6</f>
+        <v>43395</v>
+      </c>
+      <c r="S5" s="172"/>
+      <c r="T5" s="172"/>
+      <c r="U5" s="172"/>
+      <c r="V5" s="172"/>
+      <c r="W5" s="172"/>
+      <c r="X5" s="173"/>
+      <c r="Y5" s="171">
+        <f>Y6</f>
         <v>43402</v>
       </c>
-      <c r="L5" s="167"/>
-      <c r="M5" s="167"/>
-      <c r="N5" s="167"/>
-      <c r="O5" s="167"/>
-      <c r="P5" s="167"/>
-      <c r="Q5" s="168"/>
-      <c r="R5" s="166">
-        <f>R6</f>
+      <c r="Z5" s="172"/>
+      <c r="AA5" s="172"/>
+      <c r="AB5" s="172"/>
+      <c r="AC5" s="172"/>
+      <c r="AD5" s="172"/>
+      <c r="AE5" s="173"/>
+      <c r="AF5" s="171">
+        <f>AF6</f>
         <v>43409</v>
       </c>
-      <c r="S5" s="167"/>
-      <c r="T5" s="167"/>
-      <c r="U5" s="167"/>
-      <c r="V5" s="167"/>
-      <c r="W5" s="167"/>
-      <c r="X5" s="168"/>
-      <c r="Y5" s="166">
-        <f>Y6</f>
+      <c r="AG5" s="172"/>
+      <c r="AH5" s="172"/>
+      <c r="AI5" s="172"/>
+      <c r="AJ5" s="172"/>
+      <c r="AK5" s="172"/>
+      <c r="AL5" s="173"/>
+      <c r="AM5" s="171">
+        <f>AM6</f>
         <v>43416</v>
       </c>
-      <c r="Z5" s="167"/>
-      <c r="AA5" s="167"/>
-      <c r="AB5" s="167"/>
-      <c r="AC5" s="167"/>
-      <c r="AD5" s="167"/>
-      <c r="AE5" s="168"/>
-      <c r="AF5" s="166">
-        <f>AF6</f>
+      <c r="AN5" s="172"/>
+      <c r="AO5" s="172"/>
+      <c r="AP5" s="172"/>
+      <c r="AQ5" s="172"/>
+      <c r="AR5" s="172"/>
+      <c r="AS5" s="173"/>
+      <c r="AT5" s="171">
+        <f>AT6</f>
         <v>43423</v>
       </c>
-      <c r="AG5" s="167"/>
-      <c r="AH5" s="167"/>
-      <c r="AI5" s="167"/>
-      <c r="AJ5" s="167"/>
-      <c r="AK5" s="167"/>
-      <c r="AL5" s="168"/>
-      <c r="AM5" s="166">
-        <f>AM6</f>
+      <c r="AU5" s="172"/>
+      <c r="AV5" s="172"/>
+      <c r="AW5" s="172"/>
+      <c r="AX5" s="172"/>
+      <c r="AY5" s="172"/>
+      <c r="AZ5" s="173"/>
+      <c r="BA5" s="171">
+        <f>BA6</f>
         <v>43430</v>
       </c>
-      <c r="AN5" s="167"/>
-      <c r="AO5" s="167"/>
-      <c r="AP5" s="167"/>
-      <c r="AQ5" s="167"/>
-      <c r="AR5" s="167"/>
-      <c r="AS5" s="168"/>
-      <c r="AT5" s="166">
-        <f>AT6</f>
+      <c r="BB5" s="172"/>
+      <c r="BC5" s="172"/>
+      <c r="BD5" s="172"/>
+      <c r="BE5" s="172"/>
+      <c r="BF5" s="172"/>
+      <c r="BG5" s="173"/>
+      <c r="BH5" s="171">
+        <f>BH6</f>
         <v>43437</v>
       </c>
-      <c r="AU5" s="167"/>
-      <c r="AV5" s="167"/>
-      <c r="AW5" s="167"/>
-      <c r="AX5" s="167"/>
-      <c r="AY5" s="167"/>
-      <c r="AZ5" s="168"/>
-      <c r="BA5" s="166">
-        <f>BA6</f>
+      <c r="BI5" s="172"/>
+      <c r="BJ5" s="172"/>
+      <c r="BK5" s="172"/>
+      <c r="BL5" s="172"/>
+      <c r="BM5" s="172"/>
+      <c r="BN5" s="173"/>
+      <c r="BO5" s="171">
+        <f>BO6</f>
         <v>43444</v>
       </c>
-      <c r="BB5" s="167"/>
-      <c r="BC5" s="167"/>
-      <c r="BD5" s="167"/>
-      <c r="BE5" s="167"/>
-      <c r="BF5" s="167"/>
-      <c r="BG5" s="168"/>
-      <c r="BH5" s="166">
-        <f>BH6</f>
+      <c r="BP5" s="172"/>
+      <c r="BQ5" s="172"/>
+      <c r="BR5" s="172"/>
+      <c r="BS5" s="172"/>
+      <c r="BT5" s="172"/>
+      <c r="BU5" s="173"/>
+      <c r="BV5" s="171">
+        <f>BV6</f>
         <v>43451</v>
       </c>
-      <c r="BI5" s="167"/>
-      <c r="BJ5" s="167"/>
-      <c r="BK5" s="167"/>
-      <c r="BL5" s="167"/>
-      <c r="BM5" s="167"/>
-      <c r="BN5" s="168"/>
-      <c r="BO5" s="166">
-        <f>BO6</f>
+      <c r="BW5" s="172"/>
+      <c r="BX5" s="172"/>
+      <c r="BY5" s="172"/>
+      <c r="BZ5" s="172"/>
+      <c r="CA5" s="172"/>
+      <c r="CB5" s="173"/>
+      <c r="CC5" s="171">
+        <f>CC6</f>
         <v>43458</v>
       </c>
-      <c r="BP5" s="167"/>
-      <c r="BQ5" s="167"/>
-      <c r="BR5" s="167"/>
-      <c r="BS5" s="167"/>
-      <c r="BT5" s="167"/>
-      <c r="BU5" s="168"/>
-      <c r="BV5" s="166">
-        <f>BV6</f>
+      <c r="CD5" s="172"/>
+      <c r="CE5" s="172"/>
+      <c r="CF5" s="172"/>
+      <c r="CG5" s="172"/>
+      <c r="CH5" s="172"/>
+      <c r="CI5" s="173"/>
+      <c r="CJ5" s="171">
+        <f>CJ6</f>
         <v>43465</v>
       </c>
-      <c r="BW5" s="167"/>
-      <c r="BX5" s="167"/>
-      <c r="BY5" s="167"/>
-      <c r="BZ5" s="167"/>
-      <c r="CA5" s="167"/>
-      <c r="CB5" s="168"/>
-      <c r="CC5" s="166">
-        <f>CC6</f>
+      <c r="CK5" s="172"/>
+      <c r="CL5" s="172"/>
+      <c r="CM5" s="172"/>
+      <c r="CN5" s="172"/>
+      <c r="CO5" s="172"/>
+      <c r="CP5" s="173"/>
+      <c r="CQ5" s="171">
+        <f>CQ6</f>
         <v>43472</v>
       </c>
-      <c r="CD5" s="167"/>
-      <c r="CE5" s="167"/>
-      <c r="CF5" s="167"/>
-      <c r="CG5" s="167"/>
-      <c r="CH5" s="167"/>
-      <c r="CI5" s="168"/>
-      <c r="CJ5" s="166">
-        <f>CJ6</f>
+      <c r="CR5" s="172"/>
+      <c r="CS5" s="172"/>
+      <c r="CT5" s="172"/>
+      <c r="CU5" s="172"/>
+      <c r="CV5" s="172"/>
+      <c r="CW5" s="173"/>
+      <c r="CX5" s="171">
+        <f>CX6</f>
         <v>43479</v>
       </c>
-      <c r="CK5" s="167"/>
-      <c r="CL5" s="167"/>
-      <c r="CM5" s="167"/>
-      <c r="CN5" s="167"/>
-      <c r="CO5" s="167"/>
-      <c r="CP5" s="168"/>
-      <c r="CQ5" s="166">
-        <f>CQ6</f>
+      <c r="CY5" s="172"/>
+      <c r="CZ5" s="172"/>
+      <c r="DA5" s="172"/>
+      <c r="DB5" s="172"/>
+      <c r="DC5" s="172"/>
+      <c r="DD5" s="173"/>
+      <c r="DE5" s="171">
+        <f>DE6</f>
         <v>43486</v>
       </c>
-      <c r="CR5" s="167"/>
-      <c r="CS5" s="167"/>
-      <c r="CT5" s="167"/>
-      <c r="CU5" s="167"/>
-      <c r="CV5" s="167"/>
-      <c r="CW5" s="168"/>
-      <c r="CX5" s="166">
-        <f>CX6</f>
+      <c r="DF5" s="172"/>
+      <c r="DG5" s="172"/>
+      <c r="DH5" s="172"/>
+      <c r="DI5" s="172"/>
+      <c r="DJ5" s="172"/>
+      <c r="DK5" s="173"/>
+      <c r="DL5" s="171">
+        <f>DL6</f>
         <v>43493</v>
       </c>
-      <c r="CY5" s="167"/>
-      <c r="CZ5" s="167"/>
-      <c r="DA5" s="167"/>
-      <c r="DB5" s="167"/>
-      <c r="DC5" s="167"/>
-      <c r="DD5" s="168"/>
-      <c r="DE5" s="166">
-        <f>DE6</f>
-        <v>43500</v>
-      </c>
-      <c r="DF5" s="167"/>
-      <c r="DG5" s="167"/>
-      <c r="DH5" s="167"/>
-      <c r="DI5" s="167"/>
-      <c r="DJ5" s="167"/>
-      <c r="DK5" s="168"/>
-      <c r="DL5" s="166">
-        <f>DL6</f>
-        <v>43507</v>
-      </c>
-      <c r="DM5" s="167"/>
-      <c r="DN5" s="167"/>
-      <c r="DO5" s="167"/>
-      <c r="DP5" s="167"/>
-      <c r="DQ5" s="167"/>
-      <c r="DR5" s="168"/>
+      <c r="DM5" s="172"/>
+      <c r="DN5" s="172"/>
+      <c r="DO5" s="172"/>
+      <c r="DP5" s="172"/>
+      <c r="DQ5" s="172"/>
+      <c r="DR5" s="173"/>
     </row>
     <row r="6" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A6" s="49"/>
@@ -4661,451 +4777,451 @@
       <c r="J6" s="50"/>
       <c r="K6" s="92">
         <f>C4-WEEKDAY(C4,1)+2+7*(H4-1)</f>
-        <v>43402</v>
+        <v>43388</v>
       </c>
       <c r="L6" s="83">
         <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
-        <v>43403</v>
+        <v>43389</v>
       </c>
       <c r="M6" s="83">
         <f t="shared" si="0"/>
-        <v>43404</v>
+        <v>43390</v>
       </c>
       <c r="N6" s="83">
         <f t="shared" si="0"/>
-        <v>43405</v>
+        <v>43391</v>
       </c>
       <c r="O6" s="83">
         <f t="shared" si="0"/>
-        <v>43406</v>
+        <v>43392</v>
       </c>
       <c r="P6" s="83">
         <f t="shared" si="0"/>
-        <v>43407</v>
+        <v>43393</v>
       </c>
       <c r="Q6" s="93">
         <f t="shared" si="0"/>
-        <v>43408</v>
+        <v>43394</v>
       </c>
       <c r="R6" s="92">
         <f t="shared" si="0"/>
-        <v>43409</v>
+        <v>43395</v>
       </c>
       <c r="S6" s="83">
         <f t="shared" si="0"/>
-        <v>43410</v>
+        <v>43396</v>
       </c>
       <c r="T6" s="83">
         <f t="shared" si="0"/>
-        <v>43411</v>
+        <v>43397</v>
       </c>
       <c r="U6" s="83">
         <f t="shared" si="0"/>
-        <v>43412</v>
+        <v>43398</v>
       </c>
       <c r="V6" s="83">
         <f t="shared" si="0"/>
-        <v>43413</v>
+        <v>43399</v>
       </c>
       <c r="W6" s="83">
         <f t="shared" si="0"/>
-        <v>43414</v>
+        <v>43400</v>
       </c>
       <c r="X6" s="93">
         <f t="shared" si="0"/>
-        <v>43415</v>
+        <v>43401</v>
       </c>
       <c r="Y6" s="92">
         <f t="shared" si="0"/>
-        <v>43416</v>
+        <v>43402</v>
       </c>
       <c r="Z6" s="83">
         <f t="shared" si="0"/>
-        <v>43417</v>
+        <v>43403</v>
       </c>
       <c r="AA6" s="83">
         <f t="shared" si="0"/>
-        <v>43418</v>
+        <v>43404</v>
       </c>
       <c r="AB6" s="83">
         <f t="shared" si="0"/>
-        <v>43419</v>
+        <v>43405</v>
       </c>
       <c r="AC6" s="83">
         <f t="shared" si="0"/>
-        <v>43420</v>
+        <v>43406</v>
       </c>
       <c r="AD6" s="83">
         <f t="shared" si="0"/>
-        <v>43421</v>
+        <v>43407</v>
       </c>
       <c r="AE6" s="93">
         <f t="shared" si="0"/>
-        <v>43422</v>
+        <v>43408</v>
       </c>
       <c r="AF6" s="92">
         <f t="shared" si="0"/>
-        <v>43423</v>
+        <v>43409</v>
       </c>
       <c r="AG6" s="83">
         <f t="shared" si="0"/>
-        <v>43424</v>
+        <v>43410</v>
       </c>
       <c r="AH6" s="83">
         <f t="shared" si="0"/>
-        <v>43425</v>
+        <v>43411</v>
       </c>
       <c r="AI6" s="83">
         <f t="shared" si="0"/>
-        <v>43426</v>
+        <v>43412</v>
       </c>
       <c r="AJ6" s="83">
         <f t="shared" si="0"/>
-        <v>43427</v>
+        <v>43413</v>
       </c>
       <c r="AK6" s="83">
         <f t="shared" si="0"/>
-        <v>43428</v>
+        <v>43414</v>
       </c>
       <c r="AL6" s="93">
         <f t="shared" si="0"/>
-        <v>43429</v>
+        <v>43415</v>
       </c>
       <c r="AM6" s="92">
         <f t="shared" si="0"/>
-        <v>43430</v>
+        <v>43416</v>
       </c>
       <c r="AN6" s="83">
         <f t="shared" si="0"/>
-        <v>43431</v>
+        <v>43417</v>
       </c>
       <c r="AO6" s="83">
         <f t="shared" si="0"/>
-        <v>43432</v>
+        <v>43418</v>
       </c>
       <c r="AP6" s="83">
         <f t="shared" si="0"/>
-        <v>43433</v>
+        <v>43419</v>
       </c>
       <c r="AQ6" s="83">
         <f t="shared" si="0"/>
-        <v>43434</v>
+        <v>43420</v>
       </c>
       <c r="AR6" s="83">
         <f t="shared" ref="AR6:BN6" si="1">AQ6+1</f>
-        <v>43435</v>
+        <v>43421</v>
       </c>
       <c r="AS6" s="93">
         <f t="shared" si="1"/>
-        <v>43436</v>
+        <v>43422</v>
       </c>
       <c r="AT6" s="92">
         <f t="shared" si="1"/>
-        <v>43437</v>
+        <v>43423</v>
       </c>
       <c r="AU6" s="83">
         <f t="shared" si="1"/>
-        <v>43438</v>
+        <v>43424</v>
       </c>
       <c r="AV6" s="83">
         <f t="shared" si="1"/>
-        <v>43439</v>
+        <v>43425</v>
       </c>
       <c r="AW6" s="83">
         <f t="shared" si="1"/>
-        <v>43440</v>
+        <v>43426</v>
       </c>
       <c r="AX6" s="83">
         <f t="shared" si="1"/>
-        <v>43441</v>
+        <v>43427</v>
       </c>
       <c r="AY6" s="83">
         <f t="shared" si="1"/>
-        <v>43442</v>
+        <v>43428</v>
       </c>
       <c r="AZ6" s="93">
         <f t="shared" si="1"/>
-        <v>43443</v>
+        <v>43429</v>
       </c>
       <c r="BA6" s="92">
         <f t="shared" si="1"/>
-        <v>43444</v>
+        <v>43430</v>
       </c>
       <c r="BB6" s="83">
         <f t="shared" si="1"/>
-        <v>43445</v>
+        <v>43431</v>
       </c>
       <c r="BC6" s="83">
         <f t="shared" si="1"/>
-        <v>43446</v>
+        <v>43432</v>
       </c>
       <c r="BD6" s="83">
         <f t="shared" si="1"/>
-        <v>43447</v>
+        <v>43433</v>
       </c>
       <c r="BE6" s="83">
         <f t="shared" si="1"/>
-        <v>43448</v>
+        <v>43434</v>
       </c>
       <c r="BF6" s="83">
         <f t="shared" si="1"/>
-        <v>43449</v>
+        <v>43435</v>
       </c>
       <c r="BG6" s="93">
         <f t="shared" si="1"/>
-        <v>43450</v>
+        <v>43436</v>
       </c>
       <c r="BH6" s="92">
         <f t="shared" si="1"/>
-        <v>43451</v>
+        <v>43437</v>
       </c>
       <c r="BI6" s="83">
         <f t="shared" si="1"/>
-        <v>43452</v>
+        <v>43438</v>
       </c>
       <c r="BJ6" s="83">
         <f t="shared" si="1"/>
-        <v>43453</v>
+        <v>43439</v>
       </c>
       <c r="BK6" s="83">
         <f t="shared" si="1"/>
-        <v>43454</v>
+        <v>43440</v>
       </c>
       <c r="BL6" s="83">
         <f t="shared" si="1"/>
-        <v>43455</v>
+        <v>43441</v>
       </c>
       <c r="BM6" s="83">
         <f t="shared" si="1"/>
-        <v>43456</v>
+        <v>43442</v>
       </c>
       <c r="BN6" s="93">
         <f t="shared" si="1"/>
-        <v>43457</v>
+        <v>43443</v>
       </c>
       <c r="BO6" s="92">
         <f t="shared" ref="BO6" si="2">BN6+1</f>
-        <v>43458</v>
+        <v>43444</v>
       </c>
       <c r="BP6" s="83">
         <f t="shared" ref="BP6" si="3">BO6+1</f>
-        <v>43459</v>
+        <v>43445</v>
       </c>
       <c r="BQ6" s="83">
         <f t="shared" ref="BQ6" si="4">BP6+1</f>
-        <v>43460</v>
+        <v>43446</v>
       </c>
       <c r="BR6" s="83">
         <f t="shared" ref="BR6" si="5">BQ6+1</f>
-        <v>43461</v>
+        <v>43447</v>
       </c>
       <c r="BS6" s="83">
         <f t="shared" ref="BS6" si="6">BR6+1</f>
-        <v>43462</v>
+        <v>43448</v>
       </c>
       <c r="BT6" s="83">
         <f t="shared" ref="BT6" si="7">BS6+1</f>
-        <v>43463</v>
+        <v>43449</v>
       </c>
       <c r="BU6" s="93">
         <f t="shared" ref="BU6" si="8">BT6+1</f>
-        <v>43464</v>
+        <v>43450</v>
       </c>
       <c r="BV6" s="92">
         <f t="shared" ref="BV6" si="9">BU6+1</f>
-        <v>43465</v>
+        <v>43451</v>
       </c>
       <c r="BW6" s="83">
         <f t="shared" ref="BW6" si="10">BV6+1</f>
-        <v>43466</v>
+        <v>43452</v>
       </c>
       <c r="BX6" s="83">
         <f t="shared" ref="BX6" si="11">BW6+1</f>
-        <v>43467</v>
+        <v>43453</v>
       </c>
       <c r="BY6" s="83">
         <f t="shared" ref="BY6" si="12">BX6+1</f>
-        <v>43468</v>
+        <v>43454</v>
       </c>
       <c r="BZ6" s="83">
         <f t="shared" ref="BZ6" si="13">BY6+1</f>
-        <v>43469</v>
+        <v>43455</v>
       </c>
       <c r="CA6" s="83">
         <f t="shared" ref="CA6" si="14">BZ6+1</f>
-        <v>43470</v>
+        <v>43456</v>
       </c>
       <c r="CB6" s="93">
         <f t="shared" ref="CB6" si="15">CA6+1</f>
-        <v>43471</v>
+        <v>43457</v>
       </c>
       <c r="CC6" s="92">
         <f t="shared" ref="CC6" si="16">CB6+1</f>
-        <v>43472</v>
+        <v>43458</v>
       </c>
       <c r="CD6" s="83">
         <f t="shared" ref="CD6" si="17">CC6+1</f>
-        <v>43473</v>
+        <v>43459</v>
       </c>
       <c r="CE6" s="83">
         <f t="shared" ref="CE6" si="18">CD6+1</f>
-        <v>43474</v>
+        <v>43460</v>
       </c>
       <c r="CF6" s="83">
         <f t="shared" ref="CF6" si="19">CE6+1</f>
-        <v>43475</v>
+        <v>43461</v>
       </c>
       <c r="CG6" s="83">
         <f t="shared" ref="CG6" si="20">CF6+1</f>
-        <v>43476</v>
+        <v>43462</v>
       </c>
       <c r="CH6" s="83">
         <f t="shared" ref="CH6" si="21">CG6+1</f>
-        <v>43477</v>
+        <v>43463</v>
       </c>
       <c r="CI6" s="93">
         <f t="shared" ref="CI6" si="22">CH6+1</f>
-        <v>43478</v>
+        <v>43464</v>
       </c>
       <c r="CJ6" s="92">
         <f t="shared" ref="CJ6" si="23">CI6+1</f>
-        <v>43479</v>
+        <v>43465</v>
       </c>
       <c r="CK6" s="83">
         <f t="shared" ref="CK6" si="24">CJ6+1</f>
-        <v>43480</v>
+        <v>43466</v>
       </c>
       <c r="CL6" s="83">
         <f t="shared" ref="CL6" si="25">CK6+1</f>
-        <v>43481</v>
+        <v>43467</v>
       </c>
       <c r="CM6" s="83">
         <f t="shared" ref="CM6" si="26">CL6+1</f>
-        <v>43482</v>
+        <v>43468</v>
       </c>
       <c r="CN6" s="83">
         <f t="shared" ref="CN6" si="27">CM6+1</f>
-        <v>43483</v>
+        <v>43469</v>
       </c>
       <c r="CO6" s="83">
         <f t="shared" ref="CO6" si="28">CN6+1</f>
-        <v>43484</v>
+        <v>43470</v>
       </c>
       <c r="CP6" s="93">
         <f t="shared" ref="CP6" si="29">CO6+1</f>
-        <v>43485</v>
+        <v>43471</v>
       </c>
       <c r="CQ6" s="92">
         <f t="shared" ref="CQ6" si="30">CP6+1</f>
-        <v>43486</v>
+        <v>43472</v>
       </c>
       <c r="CR6" s="83">
         <f t="shared" ref="CR6" si="31">CQ6+1</f>
-        <v>43487</v>
+        <v>43473</v>
       </c>
       <c r="CS6" s="83">
         <f t="shared" ref="CS6" si="32">CR6+1</f>
-        <v>43488</v>
+        <v>43474</v>
       </c>
       <c r="CT6" s="83">
         <f t="shared" ref="CT6" si="33">CS6+1</f>
-        <v>43489</v>
+        <v>43475</v>
       </c>
       <c r="CU6" s="83">
         <f t="shared" ref="CU6" si="34">CT6+1</f>
-        <v>43490</v>
+        <v>43476</v>
       </c>
       <c r="CV6" s="83">
         <f t="shared" ref="CV6" si="35">CU6+1</f>
-        <v>43491</v>
+        <v>43477</v>
       </c>
       <c r="CW6" s="93">
         <f t="shared" ref="CW6" si="36">CV6+1</f>
-        <v>43492</v>
+        <v>43478</v>
       </c>
       <c r="CX6" s="92">
         <f t="shared" ref="CX6" si="37">CW6+1</f>
-        <v>43493</v>
+        <v>43479</v>
       </c>
       <c r="CY6" s="83">
         <f t="shared" ref="CY6" si="38">CX6+1</f>
-        <v>43494</v>
+        <v>43480</v>
       </c>
       <c r="CZ6" s="83">
         <f t="shared" ref="CZ6" si="39">CY6+1</f>
-        <v>43495</v>
+        <v>43481</v>
       </c>
       <c r="DA6" s="83">
         <f t="shared" ref="DA6" si="40">CZ6+1</f>
-        <v>43496</v>
+        <v>43482</v>
       </c>
       <c r="DB6" s="83">
         <f t="shared" ref="DB6" si="41">DA6+1</f>
-        <v>43497</v>
+        <v>43483</v>
       </c>
       <c r="DC6" s="83">
         <f t="shared" ref="DC6" si="42">DB6+1</f>
-        <v>43498</v>
+        <v>43484</v>
       </c>
       <c r="DD6" s="93">
         <f t="shared" ref="DD6" si="43">DC6+1</f>
-        <v>43499</v>
+        <v>43485</v>
       </c>
       <c r="DE6" s="92">
         <f t="shared" ref="DE6" si="44">DD6+1</f>
-        <v>43500</v>
+        <v>43486</v>
       </c>
       <c r="DF6" s="83">
         <f t="shared" ref="DF6" si="45">DE6+1</f>
-        <v>43501</v>
+        <v>43487</v>
       </c>
       <c r="DG6" s="83">
         <f t="shared" ref="DG6" si="46">DF6+1</f>
-        <v>43502</v>
+        <v>43488</v>
       </c>
       <c r="DH6" s="83">
         <f t="shared" ref="DH6" si="47">DG6+1</f>
-        <v>43503</v>
+        <v>43489</v>
       </c>
       <c r="DI6" s="83">
         <f t="shared" ref="DI6" si="48">DH6+1</f>
-        <v>43504</v>
+        <v>43490</v>
       </c>
       <c r="DJ6" s="83">
         <f t="shared" ref="DJ6" si="49">DI6+1</f>
-        <v>43505</v>
+        <v>43491</v>
       </c>
       <c r="DK6" s="93">
         <f t="shared" ref="DK6" si="50">DJ6+1</f>
-        <v>43506</v>
+        <v>43492</v>
       </c>
       <c r="DL6" s="92">
         <f t="shared" ref="DL6" si="51">DK6+1</f>
-        <v>43507</v>
+        <v>43493</v>
       </c>
       <c r="DM6" s="83">
         <f t="shared" ref="DM6" si="52">DL6+1</f>
-        <v>43508</v>
+        <v>43494</v>
       </c>
       <c r="DN6" s="83">
         <f t="shared" ref="DN6" si="53">DM6+1</f>
-        <v>43509</v>
+        <v>43495</v>
       </c>
       <c r="DO6" s="83">
         <f t="shared" ref="DO6" si="54">DN6+1</f>
-        <v>43510</v>
+        <v>43496</v>
       </c>
       <c r="DP6" s="83">
         <f t="shared" ref="DP6" si="55">DO6+1</f>
-        <v>43511</v>
+        <v>43497</v>
       </c>
       <c r="DQ6" s="83">
         <f t="shared" ref="DQ6" si="56">DP6+1</f>
-        <v>43512</v>
+        <v>43498</v>
       </c>
       <c r="DR6" s="93">
         <f t="shared" ref="DR6" si="57">DQ6+1</f>
-        <v>43513</v>
+        <v>43499</v>
       </c>
     </row>
     <row r="7" spans="1:122" s="124" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -5604,7 +5720,7 @@
       <c r="G8" s="89"/>
       <c r="H8" s="90"/>
       <c r="I8" s="91" t="str">
-        <f t="shared" ref="I8:I46" si="62">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
+        <f t="shared" ref="I8:I49" si="62">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J8" s="94"/>
@@ -5666,12 +5782,12 @@
       <c r="BN8" s="106"/>
     </row>
     <row r="9" spans="1:122" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="173" t="str">
+      <c r="A9" s="163" t="str">
         <f t="shared" ref="A9:A16" si="63">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
       </c>
-      <c r="B9" s="174" t="s">
-        <v>167</v>
+      <c r="B9" s="164" t="s">
+        <v>166</v>
       </c>
       <c r="C9" s="61" t="s">
         <v>142</v>
@@ -5755,12 +5871,12 @@
       <c r="BN9" s="107"/>
     </row>
     <row r="10" spans="1:122" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="173" t="str">
+      <c r="A10" s="163" t="str">
         <f t="shared" si="63"/>
         <v>1.2</v>
       </c>
-      <c r="B10" s="174" t="s">
-        <v>168</v>
+      <c r="B10" s="164" t="s">
+        <v>167</v>
       </c>
       <c r="C10" s="61" t="s">
         <v>142</v>
@@ -5859,7 +5975,7 @@
         <v>43388</v>
       </c>
       <c r="F11" s="101">
-        <f t="shared" ref="F11:F44" si="65">IF(ISBLANK(E11)," - ",IF(G11=0,E11,E11+G11-1))</f>
+        <f t="shared" ref="F11:F47" si="65">IF(ISBLANK(E11)," - ",IF(G11=0,E11,E11+G11-1))</f>
         <v>43453</v>
       </c>
       <c r="G11" s="62">
@@ -6191,7 +6307,7 @@
         <v>1.4.1</v>
       </c>
       <c r="B15" s="128" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D15" s="127"/>
       <c r="E15" s="100">
@@ -6609,13 +6725,13 @@
       <c r="BM19" s="107"/>
       <c r="BN19" s="107"/>
     </row>
-    <row r="20" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:90" s="61" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A20" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.3</v>
       </c>
       <c r="B20" s="126" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="C20" s="61" t="s">
         <v>150</v>
@@ -6696,33 +6812,30 @@
       <c r="BM20" s="107"/>
       <c r="BN20" s="107"/>
     </row>
-    <row r="21" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:90" s="61" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A21" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>2.4</v>
-      </c>
-      <c r="B21" s="126" t="s">
-        <v>147</v>
-      </c>
-      <c r="C21" s="61" t="s">
-        <v>150</v>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <v>2.3.1</v>
+      </c>
+      <c r="B21" s="128" t="s">
+        <v>173</v>
       </c>
       <c r="D21" s="127"/>
       <c r="E21" s="100">
         <v>43364</v>
       </c>
       <c r="F21" s="101">
-        <f t="shared" si="65"/>
+        <f>IF(ISBLANK(E21)," - ",IF(G21=0,E21,E21+G21-1))</f>
         <v>43367</v>
       </c>
       <c r="G21" s="62">
         <v>4</v>
       </c>
       <c r="H21" s="63">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="I21" s="64">
-        <f t="shared" si="62"/>
+        <f t="shared" ref="I21" si="68">IF(OR(F21=0,E21=0)," - ",NETWORKDAYS(E21,F21))</f>
         <v>2</v>
       </c>
       <c r="J21" s="95"/>
@@ -6786,28 +6899,31 @@
     <row r="22" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="B22" s="126" t="s">
-        <v>9</v>
+        <v>170</v>
+      </c>
+      <c r="C22" s="61" t="s">
+        <v>150</v>
       </c>
       <c r="D22" s="127"/>
       <c r="E22" s="100">
-        <v>43154</v>
+        <v>43416</v>
       </c>
       <c r="F22" s="101">
         <f t="shared" si="65"/>
-        <v>43156</v>
+        <v>43425</v>
       </c>
       <c r="G22" s="62">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H22" s="63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="64">
         <f t="shared" si="62"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J22" s="95"/>
       <c r="K22" s="107"/>
@@ -6867,112 +6983,115 @@
       <c r="BM22" s="107"/>
       <c r="BN22" s="107"/>
     </row>
-    <row r="23" spans="1:90" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A23" s="53" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+    <row r="23" spans="1:90" s="61" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A23" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <v>2.4.1</v>
+      </c>
+      <c r="B23" s="128" t="s">
+        <v>171</v>
+      </c>
+      <c r="D23" s="127"/>
+      <c r="E23" s="100">
+        <v>43425</v>
+      </c>
+      <c r="F23" s="101">
+        <f>IF(ISBLANK(E23)," - ",IF(G23=0,E23,E23+G23-1))</f>
+        <v>43427</v>
+      </c>
+      <c r="G23" s="62">
         <v>3</v>
       </c>
-      <c r="B23" s="54" t="s">
-        <v>155</v>
-      </c>
-      <c r="D23" s="56"/>
-      <c r="E23" s="102"/>
-      <c r="F23" s="102" t="str">
-        <f t="shared" si="65"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G23" s="57"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="59" t="str">
-        <f t="shared" si="62"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J23" s="96"/>
-      <c r="K23" s="109"/>
-      <c r="L23" s="109"/>
-      <c r="M23" s="109"/>
-      <c r="N23" s="109"/>
-      <c r="O23" s="109"/>
-      <c r="P23" s="109"/>
-      <c r="Q23" s="109"/>
-      <c r="R23" s="109"/>
-      <c r="S23" s="109"/>
-      <c r="T23" s="109"/>
-      <c r="U23" s="109"/>
-      <c r="V23" s="109"/>
-      <c r="W23" s="109"/>
-      <c r="X23" s="109"/>
-      <c r="Y23" s="109"/>
-      <c r="Z23" s="109"/>
-      <c r="AA23" s="109"/>
-      <c r="AB23" s="109"/>
-      <c r="AC23" s="109"/>
-      <c r="AD23" s="109"/>
-      <c r="AE23" s="109"/>
-      <c r="AF23" s="109"/>
-      <c r="AG23" s="109"/>
-      <c r="AH23" s="109"/>
-      <c r="AI23" s="109"/>
-      <c r="AJ23" s="109"/>
-      <c r="AK23" s="109"/>
-      <c r="AL23" s="109"/>
-      <c r="AM23" s="109"/>
-      <c r="AN23" s="109"/>
-      <c r="AO23" s="109"/>
-      <c r="AP23" s="109"/>
-      <c r="AQ23" s="109"/>
-      <c r="AR23" s="109"/>
-      <c r="AS23" s="109"/>
-      <c r="AT23" s="109"/>
-      <c r="AU23" s="109"/>
-      <c r="AV23" s="109"/>
-      <c r="AW23" s="109"/>
-      <c r="AX23" s="109"/>
-      <c r="AY23" s="109"/>
-      <c r="AZ23" s="109"/>
-      <c r="BA23" s="109"/>
-      <c r="BB23" s="109"/>
-      <c r="BC23" s="109"/>
-      <c r="BD23" s="109"/>
-      <c r="BE23" s="109"/>
-      <c r="BF23" s="109"/>
-      <c r="BG23" s="109"/>
-      <c r="BH23" s="109"/>
-      <c r="BI23" s="109"/>
-      <c r="BJ23" s="109"/>
-      <c r="BK23" s="109"/>
-      <c r="BL23" s="109"/>
-      <c r="BM23" s="109"/>
-      <c r="BN23" s="109"/>
+      <c r="H23" s="63">
+        <v>1</v>
+      </c>
+      <c r="I23" s="64">
+        <f t="shared" ref="I23:I24" si="69">IF(OR(F23=0,E23=0)," - ",NETWORKDAYS(E23,F23))</f>
+        <v>3</v>
+      </c>
+      <c r="J23" s="95"/>
+      <c r="K23" s="107"/>
+      <c r="L23" s="107"/>
+      <c r="M23" s="107"/>
+      <c r="N23" s="107"/>
+      <c r="O23" s="107"/>
+      <c r="P23" s="107"/>
+      <c r="Q23" s="107"/>
+      <c r="R23" s="107"/>
+      <c r="S23" s="107"/>
+      <c r="T23" s="107"/>
+      <c r="U23" s="107"/>
+      <c r="V23" s="107"/>
+      <c r="W23" s="107"/>
+      <c r="X23" s="107"/>
+      <c r="Y23" s="107"/>
+      <c r="Z23" s="107"/>
+      <c r="AA23" s="107"/>
+      <c r="AB23" s="107"/>
+      <c r="AC23" s="107"/>
+      <c r="AD23" s="107"/>
+      <c r="AE23" s="107"/>
+      <c r="AF23" s="107"/>
+      <c r="AG23" s="107"/>
+      <c r="AH23" s="107"/>
+      <c r="AI23" s="107"/>
+      <c r="AJ23" s="107"/>
+      <c r="AK23" s="107"/>
+      <c r="AL23" s="107"/>
+      <c r="AM23" s="107"/>
+      <c r="AN23" s="107"/>
+      <c r="AO23" s="107"/>
+      <c r="AP23" s="107"/>
+      <c r="AQ23" s="107"/>
+      <c r="AR23" s="107"/>
+      <c r="AS23" s="107"/>
+      <c r="AT23" s="107"/>
+      <c r="AU23" s="107"/>
+      <c r="AV23" s="107"/>
+      <c r="AW23" s="107"/>
+      <c r="AX23" s="107"/>
+      <c r="AY23" s="107"/>
+      <c r="AZ23" s="107"/>
+      <c r="BA23" s="107"/>
+      <c r="BB23" s="107"/>
+      <c r="BC23" s="107"/>
+      <c r="BD23" s="107"/>
+      <c r="BE23" s="107"/>
+      <c r="BF23" s="107"/>
+      <c r="BG23" s="107"/>
+      <c r="BH23" s="107"/>
+      <c r="BI23" s="107"/>
+      <c r="BJ23" s="107"/>
+      <c r="BK23" s="107"/>
+      <c r="BL23" s="107"/>
+      <c r="BM23" s="107"/>
+      <c r="BN23" s="107"/>
     </row>
     <row r="24" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.1</v>
-      </c>
-      <c r="B24" s="126" t="s">
-        <v>156</v>
-      </c>
-      <c r="C24" s="61" t="s">
-        <v>160</v>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <v>2.4.2</v>
+      </c>
+      <c r="B24" s="128" t="s">
+        <v>172</v>
       </c>
       <c r="D24" s="127"/>
       <c r="E24" s="100">
-        <v>43384</v>
+        <v>43437</v>
       </c>
       <c r="F24" s="101">
-        <f t="shared" si="65"/>
-        <v>43418</v>
+        <f>IF(ISBLANK(E24)," - ",IF(G24=0,E24,E24+G24-1))</f>
+        <v>43438</v>
       </c>
       <c r="G24" s="62">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="H24" s="63">
         <v>1</v>
       </c>
       <c r="I24" s="64">
-        <f t="shared" si="62"/>
-        <v>25</v>
+        <f t="shared" si="69"/>
+        <v>2</v>
       </c>
       <c r="J24" s="95"/>
       <c r="K24" s="107"/>
@@ -7031,59 +7150,32 @@
       <c r="BL24" s="107"/>
       <c r="BM24" s="107"/>
       <c r="BN24" s="107"/>
-      <c r="BO24" s="107"/>
-      <c r="BP24" s="107"/>
-      <c r="BQ24" s="107"/>
-      <c r="BR24" s="107"/>
-      <c r="BS24" s="107"/>
-      <c r="BT24" s="107"/>
-      <c r="BU24" s="107"/>
-      <c r="BV24" s="107"/>
-      <c r="BW24" s="107"/>
-      <c r="BX24" s="107"/>
-      <c r="BY24" s="107"/>
-      <c r="BZ24" s="107"/>
-      <c r="CA24" s="107"/>
-      <c r="CB24" s="107"/>
-      <c r="CC24" s="107"/>
-      <c r="CD24" s="107"/>
-      <c r="CE24" s="107"/>
-      <c r="CF24" s="107"/>
-      <c r="CG24" s="107"/>
-      <c r="CH24" s="107"/>
-      <c r="CI24" s="107"/>
-      <c r="CJ24" s="107"/>
-      <c r="CK24" s="107"/>
-      <c r="CL24" s="107"/>
     </row>
     <row r="25" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.2</v>
+        <v>2.5</v>
       </c>
       <c r="B25" s="126" t="s">
-        <v>157</v>
-      </c>
-      <c r="C25" s="61" t="s">
-        <v>160</v>
+        <v>9</v>
       </c>
       <c r="D25" s="127"/>
       <c r="E25" s="100">
-        <v>43418</v>
+        <v>43154</v>
       </c>
       <c r="F25" s="101">
         <f t="shared" si="65"/>
-        <v>43419</v>
+        <v>43156</v>
       </c>
       <c r="G25" s="62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H25" s="63">
         <v>0</v>
       </c>
       <c r="I25" s="64">
         <f t="shared" si="62"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J25" s="95"/>
       <c r="K25" s="107"/>
@@ -7143,103 +7235,94 @@
       <c r="BM25" s="107"/>
       <c r="BN25" s="107"/>
     </row>
-    <row r="26" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A26" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.3</v>
-      </c>
-      <c r="B26" s="126" t="s">
-        <v>158</v>
-      </c>
-      <c r="C26" s="61" t="s">
-        <v>160</v>
-      </c>
-      <c r="D26" s="127"/>
-      <c r="E26" s="100">
-        <v>43384</v>
-      </c>
-      <c r="F26" s="101">
+    <row r="26" spans="1:90" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="53" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>3</v>
+      </c>
+      <c r="B26" s="54" t="s">
+        <v>154</v>
+      </c>
+      <c r="D26" s="56"/>
+      <c r="E26" s="102"/>
+      <c r="F26" s="102" t="str">
         <f t="shared" si="65"/>
-        <v>43390</v>
-      </c>
-      <c r="G26" s="62">
-        <v>7</v>
-      </c>
-      <c r="H26" s="63">
-        <v>0</v>
-      </c>
-      <c r="I26" s="64">
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G26" s="57"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="59" t="str">
         <f t="shared" si="62"/>
-        <v>5</v>
-      </c>
-      <c r="J26" s="95"/>
-      <c r="K26" s="107"/>
-      <c r="L26" s="107"/>
-      <c r="M26" s="107"/>
-      <c r="N26" s="107"/>
-      <c r="O26" s="107"/>
-      <c r="P26" s="107"/>
-      <c r="Q26" s="107"/>
-      <c r="R26" s="107"/>
-      <c r="S26" s="107"/>
-      <c r="T26" s="107"/>
-      <c r="U26" s="107"/>
-      <c r="V26" s="107"/>
-      <c r="W26" s="107"/>
-      <c r="X26" s="107"/>
-      <c r="Y26" s="107"/>
-      <c r="Z26" s="107"/>
-      <c r="AA26" s="107"/>
-      <c r="AB26" s="107"/>
-      <c r="AC26" s="107"/>
-      <c r="AD26" s="107"/>
-      <c r="AE26" s="107"/>
-      <c r="AF26" s="107"/>
-      <c r="AG26" s="107"/>
-      <c r="AH26" s="107"/>
-      <c r="AI26" s="107"/>
-      <c r="AJ26" s="107"/>
-      <c r="AK26" s="107"/>
-      <c r="AL26" s="107"/>
-      <c r="AM26" s="107"/>
-      <c r="AN26" s="107"/>
-      <c r="AO26" s="107"/>
-      <c r="AP26" s="107"/>
-      <c r="AQ26" s="107"/>
-      <c r="AR26" s="107"/>
-      <c r="AS26" s="107"/>
-      <c r="AT26" s="107"/>
-      <c r="AU26" s="107"/>
-      <c r="AV26" s="107"/>
-      <c r="AW26" s="107"/>
-      <c r="AX26" s="107"/>
-      <c r="AY26" s="107"/>
-      <c r="AZ26" s="107"/>
-      <c r="BA26" s="107"/>
-      <c r="BB26" s="107"/>
-      <c r="BC26" s="107"/>
-      <c r="BD26" s="107"/>
-      <c r="BE26" s="107"/>
-      <c r="BF26" s="107"/>
-      <c r="BG26" s="107"/>
-      <c r="BH26" s="107"/>
-      <c r="BI26" s="107"/>
-      <c r="BJ26" s="107"/>
-      <c r="BK26" s="107"/>
-      <c r="BL26" s="107"/>
-      <c r="BM26" s="107"/>
-      <c r="BN26" s="107"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J26" s="96"/>
+      <c r="K26" s="109"/>
+      <c r="L26" s="109"/>
+      <c r="M26" s="109"/>
+      <c r="N26" s="109"/>
+      <c r="O26" s="109"/>
+      <c r="P26" s="109"/>
+      <c r="Q26" s="109"/>
+      <c r="R26" s="109"/>
+      <c r="S26" s="109"/>
+      <c r="T26" s="109"/>
+      <c r="U26" s="109"/>
+      <c r="V26" s="109"/>
+      <c r="W26" s="109"/>
+      <c r="X26" s="109"/>
+      <c r="Y26" s="109"/>
+      <c r="Z26" s="109"/>
+      <c r="AA26" s="109"/>
+      <c r="AB26" s="109"/>
+      <c r="AC26" s="109"/>
+      <c r="AD26" s="109"/>
+      <c r="AE26" s="109"/>
+      <c r="AF26" s="109"/>
+      <c r="AG26" s="109"/>
+      <c r="AH26" s="109"/>
+      <c r="AI26" s="109"/>
+      <c r="AJ26" s="109"/>
+      <c r="AK26" s="109"/>
+      <c r="AL26" s="109"/>
+      <c r="AM26" s="109"/>
+      <c r="AN26" s="109"/>
+      <c r="AO26" s="109"/>
+      <c r="AP26" s="109"/>
+      <c r="AQ26" s="109"/>
+      <c r="AR26" s="109"/>
+      <c r="AS26" s="109"/>
+      <c r="AT26" s="109"/>
+      <c r="AU26" s="109"/>
+      <c r="AV26" s="109"/>
+      <c r="AW26" s="109"/>
+      <c r="AX26" s="109"/>
+      <c r="AY26" s="109"/>
+      <c r="AZ26" s="109"/>
+      <c r="BA26" s="109"/>
+      <c r="BB26" s="109"/>
+      <c r="BC26" s="109"/>
+      <c r="BD26" s="109"/>
+      <c r="BE26" s="109"/>
+      <c r="BF26" s="109"/>
+      <c r="BG26" s="109"/>
+      <c r="BH26" s="109"/>
+      <c r="BI26" s="109"/>
+      <c r="BJ26" s="109"/>
+      <c r="BK26" s="109"/>
+      <c r="BL26" s="109"/>
+      <c r="BM26" s="109"/>
+      <c r="BN26" s="109"/>
     </row>
     <row r="27" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
       <c r="B27" s="126" t="s">
+        <v>155</v>
+      </c>
+      <c r="C27" s="61" t="s">
         <v>159</v>
-      </c>
-      <c r="C27" s="61" t="s">
-        <v>160</v>
       </c>
       <c r="D27" s="127"/>
       <c r="E27" s="100">
@@ -7247,17 +7330,17 @@
       </c>
       <c r="F27" s="101">
         <f t="shared" si="65"/>
-        <v>43397</v>
+        <v>43418</v>
       </c>
       <c r="G27" s="62">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="H27" s="63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="64">
         <f t="shared" si="62"/>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="J27" s="95"/>
       <c r="K27" s="107"/>
@@ -7316,35 +7399,59 @@
       <c r="BL27" s="107"/>
       <c r="BM27" s="107"/>
       <c r="BN27" s="107"/>
+      <c r="BO27" s="107"/>
+      <c r="BP27" s="107"/>
+      <c r="BQ27" s="107"/>
+      <c r="BR27" s="107"/>
+      <c r="BS27" s="107"/>
+      <c r="BT27" s="107"/>
+      <c r="BU27" s="107"/>
+      <c r="BV27" s="107"/>
+      <c r="BW27" s="107"/>
+      <c r="BX27" s="107"/>
+      <c r="BY27" s="107"/>
+      <c r="BZ27" s="107"/>
+      <c r="CA27" s="107"/>
+      <c r="CB27" s="107"/>
+      <c r="CC27" s="107"/>
+      <c r="CD27" s="107"/>
+      <c r="CE27" s="107"/>
+      <c r="CF27" s="107"/>
+      <c r="CG27" s="107"/>
+      <c r="CH27" s="107"/>
+      <c r="CI27" s="107"/>
+      <c r="CJ27" s="107"/>
+      <c r="CK27" s="107"/>
+      <c r="CL27" s="107"/>
     </row>
     <row r="28" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
       <c r="B28" s="126" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="C28" s="61" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D28" s="127"/>
       <c r="E28" s="100">
-        <v>43384</v>
+        <v>43418</v>
       </c>
       <c r="F28" s="101">
         <f t="shared" si="65"/>
-        <v>43384</v>
+        <v>43419</v>
       </c>
       <c r="G28" s="62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28" s="63">
         <v>0</v>
       </c>
       <c r="I28" s="64">
         <f t="shared" si="62"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J28" s="95"/>
       <c r="K28" s="107"/>
@@ -7404,112 +7511,121 @@
       <c r="BM28" s="107"/>
       <c r="BN28" s="107"/>
     </row>
-    <row r="29" spans="1:90" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A29" s="53" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>4</v>
-      </c>
-      <c r="B29" s="54" t="s">
-        <v>161</v>
-      </c>
-      <c r="D29" s="56"/>
-      <c r="E29" s="102"/>
-      <c r="F29" s="102" t="str">
+    <row r="29" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>3.3</v>
+      </c>
+      <c r="B29" s="126" t="s">
+        <v>157</v>
+      </c>
+      <c r="C29" s="61" t="s">
+        <v>159</v>
+      </c>
+      <c r="D29" s="127"/>
+      <c r="E29" s="100">
+        <v>43384</v>
+      </c>
+      <c r="F29" s="101">
         <f t="shared" si="65"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G29" s="57"/>
-      <c r="H29" s="58"/>
-      <c r="I29" s="59" t="str">
+        <v>43390</v>
+      </c>
+      <c r="G29" s="62">
+        <v>7</v>
+      </c>
+      <c r="H29" s="63">
+        <v>0</v>
+      </c>
+      <c r="I29" s="64">
         <f t="shared" si="62"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J29" s="96"/>
-      <c r="K29" s="109"/>
-      <c r="L29" s="109"/>
-      <c r="M29" s="109"/>
-      <c r="N29" s="109"/>
-      <c r="O29" s="109"/>
-      <c r="P29" s="109"/>
-      <c r="Q29" s="109"/>
-      <c r="R29" s="109"/>
-      <c r="S29" s="109"/>
-      <c r="T29" s="109"/>
-      <c r="U29" s="109"/>
-      <c r="V29" s="109"/>
-      <c r="W29" s="109"/>
-      <c r="X29" s="109"/>
-      <c r="Y29" s="109"/>
-      <c r="Z29" s="109"/>
-      <c r="AA29" s="109"/>
-      <c r="AB29" s="109"/>
-      <c r="AC29" s="109"/>
-      <c r="AD29" s="109"/>
-      <c r="AE29" s="109"/>
-      <c r="AF29" s="109"/>
-      <c r="AG29" s="109"/>
-      <c r="AH29" s="109"/>
-      <c r="AI29" s="109"/>
-      <c r="AJ29" s="109"/>
-      <c r="AK29" s="109"/>
-      <c r="AL29" s="109"/>
-      <c r="AM29" s="109"/>
-      <c r="AN29" s="109"/>
-      <c r="AO29" s="109"/>
-      <c r="AP29" s="109"/>
-      <c r="AQ29" s="109"/>
-      <c r="AR29" s="109"/>
-      <c r="AS29" s="109"/>
-      <c r="AT29" s="109"/>
-      <c r="AU29" s="109"/>
-      <c r="AV29" s="109"/>
-      <c r="AW29" s="109"/>
-      <c r="AX29" s="109"/>
-      <c r="AY29" s="109"/>
-      <c r="AZ29" s="109"/>
-      <c r="BA29" s="109"/>
-      <c r="BB29" s="109"/>
-      <c r="BC29" s="109"/>
-      <c r="BD29" s="109"/>
-      <c r="BE29" s="109"/>
-      <c r="BF29" s="109"/>
-      <c r="BG29" s="109"/>
-      <c r="BH29" s="109"/>
-      <c r="BI29" s="109"/>
-      <c r="BJ29" s="109"/>
-      <c r="BK29" s="109"/>
-      <c r="BL29" s="109"/>
-      <c r="BM29" s="109"/>
-      <c r="BN29" s="109"/>
+        <v>5</v>
+      </c>
+      <c r="J29" s="95"/>
+      <c r="K29" s="107"/>
+      <c r="L29" s="107"/>
+      <c r="M29" s="107"/>
+      <c r="N29" s="107"/>
+      <c r="O29" s="107"/>
+      <c r="P29" s="107"/>
+      <c r="Q29" s="107"/>
+      <c r="R29" s="107"/>
+      <c r="S29" s="107"/>
+      <c r="T29" s="107"/>
+      <c r="U29" s="107"/>
+      <c r="V29" s="107"/>
+      <c r="W29" s="107"/>
+      <c r="X29" s="107"/>
+      <c r="Y29" s="107"/>
+      <c r="Z29" s="107"/>
+      <c r="AA29" s="107"/>
+      <c r="AB29" s="107"/>
+      <c r="AC29" s="107"/>
+      <c r="AD29" s="107"/>
+      <c r="AE29" s="107"/>
+      <c r="AF29" s="107"/>
+      <c r="AG29" s="107"/>
+      <c r="AH29" s="107"/>
+      <c r="AI29" s="107"/>
+      <c r="AJ29" s="107"/>
+      <c r="AK29" s="107"/>
+      <c r="AL29" s="107"/>
+      <c r="AM29" s="107"/>
+      <c r="AN29" s="107"/>
+      <c r="AO29" s="107"/>
+      <c r="AP29" s="107"/>
+      <c r="AQ29" s="107"/>
+      <c r="AR29" s="107"/>
+      <c r="AS29" s="107"/>
+      <c r="AT29" s="107"/>
+      <c r="AU29" s="107"/>
+      <c r="AV29" s="107"/>
+      <c r="AW29" s="107"/>
+      <c r="AX29" s="107"/>
+      <c r="AY29" s="107"/>
+      <c r="AZ29" s="107"/>
+      <c r="BA29" s="107"/>
+      <c r="BB29" s="107"/>
+      <c r="BC29" s="107"/>
+      <c r="BD29" s="107"/>
+      <c r="BE29" s="107"/>
+      <c r="BF29" s="107"/>
+      <c r="BG29" s="107"/>
+      <c r="BH29" s="107"/>
+      <c r="BI29" s="107"/>
+      <c r="BJ29" s="107"/>
+      <c r="BK29" s="107"/>
+      <c r="BL29" s="107"/>
+      <c r="BM29" s="107"/>
+      <c r="BN29" s="107"/>
     </row>
     <row r="30" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.1</v>
+        <v>3.4</v>
       </c>
       <c r="B30" s="126" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C30" s="61" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D30" s="127"/>
       <c r="E30" s="100">
-        <v>43353</v>
+        <v>43384</v>
       </c>
       <c r="F30" s="101">
-        <f>IF(ISBLANK(E30)," - ",IF(G30=0,E30,E30+G30-1))</f>
-        <v>43355</v>
+        <f t="shared" si="65"/>
+        <v>43397</v>
       </c>
       <c r="G30" s="62">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="H30" s="63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" s="64">
         <f t="shared" si="62"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J30" s="95"/>
       <c r="K30" s="107"/>
@@ -7572,27 +7688,27 @@
     <row r="31" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="B31" s="126" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="C31" s="61" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D31" s="127"/>
       <c r="E31" s="100">
-        <v>43354</v>
+        <v>43384</v>
       </c>
       <c r="F31" s="101">
         <f t="shared" si="65"/>
-        <v>43354</v>
+        <v>43384</v>
       </c>
       <c r="G31" s="62">
         <v>1</v>
       </c>
       <c r="H31" s="63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" s="64">
         <f t="shared" si="62"/>
@@ -7656,198 +7772,199 @@
       <c r="BM31" s="107"/>
       <c r="BN31" s="107"/>
     </row>
-    <row r="32" spans="1:90" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.3</v>
-      </c>
-      <c r="B32" s="126" t="s">
-        <v>164</v>
-      </c>
-      <c r="C32" s="61" t="s">
-        <v>162</v>
-      </c>
-      <c r="D32" s="127"/>
-      <c r="E32" s="100">
-        <v>43357</v>
-      </c>
-      <c r="F32" s="101">
-        <f>IF(ISBLANK(E32)," - ",IF(G32=0,E32,E32+G32-1))</f>
-        <v>43357</v>
-      </c>
-      <c r="G32" s="62">
-        <v>1</v>
-      </c>
-      <c r="H32" s="63">
-        <v>1</v>
-      </c>
-      <c r="I32" s="64">
-        <f t="shared" si="62"/>
-        <v>1</v>
-      </c>
-      <c r="J32" s="95"/>
-      <c r="K32" s="107"/>
-      <c r="L32" s="107"/>
-      <c r="M32" s="107"/>
-      <c r="N32" s="107"/>
-      <c r="O32" s="107"/>
-      <c r="P32" s="107"/>
-      <c r="Q32" s="107"/>
-      <c r="R32" s="107"/>
-      <c r="S32" s="107"/>
-      <c r="T32" s="107"/>
-      <c r="U32" s="107"/>
-      <c r="V32" s="107"/>
-      <c r="W32" s="107"/>
-      <c r="X32" s="107"/>
-      <c r="Y32" s="107"/>
-      <c r="Z32" s="107"/>
-      <c r="AA32" s="107"/>
-      <c r="AB32" s="107"/>
-      <c r="AC32" s="107"/>
-      <c r="AD32" s="107"/>
-      <c r="AE32" s="107"/>
-      <c r="AF32" s="107"/>
-      <c r="AG32" s="107"/>
-      <c r="AH32" s="107"/>
-      <c r="AI32" s="107"/>
-      <c r="AJ32" s="107"/>
-      <c r="AK32" s="107"/>
-      <c r="AL32" s="107"/>
-      <c r="AM32" s="107"/>
-      <c r="AN32" s="107"/>
-      <c r="AO32" s="107"/>
-      <c r="AP32" s="107"/>
-      <c r="AQ32" s="107"/>
-      <c r="AR32" s="107"/>
-      <c r="AS32" s="107"/>
-      <c r="AT32" s="107"/>
-      <c r="AU32" s="107"/>
-      <c r="AV32" s="107"/>
-      <c r="AW32" s="107"/>
-      <c r="AX32" s="107"/>
-      <c r="AY32" s="107"/>
-      <c r="AZ32" s="107"/>
-      <c r="BA32" s="107"/>
-      <c r="BB32" s="107"/>
-      <c r="BC32" s="107"/>
-      <c r="BD32" s="107"/>
-      <c r="BE32" s="107"/>
-      <c r="BF32" s="107"/>
-      <c r="BG32" s="107"/>
-      <c r="BH32" s="107"/>
-      <c r="BI32" s="107"/>
-      <c r="BJ32" s="107"/>
-      <c r="BK32" s="107"/>
-      <c r="BL32" s="107"/>
-      <c r="BM32" s="107"/>
-      <c r="BN32" s="107"/>
-    </row>
-    <row r="33" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A33" s="53" t="str">
+    <row r="32" spans="1:90" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>5</v>
-      </c>
-      <c r="B33" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="D33" s="56"/>
-      <c r="E33" s="102"/>
-      <c r="F33" s="102" t="str">
-        <f t="shared" ref="F33" si="68">IF(ISBLANK(E33)," - ",IF(G33=0,E33,E33+G33-1))</f>
+        <v>4</v>
+      </c>
+      <c r="B32" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="D32" s="56"/>
+      <c r="E32" s="102"/>
+      <c r="F32" s="102" t="str">
+        <f t="shared" si="65"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G33" s="57"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="59" t="str">
+      <c r="G32" s="57"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="59" t="str">
         <f t="shared" si="62"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J33" s="96"/>
-      <c r="K33" s="109"/>
-      <c r="L33" s="109"/>
-      <c r="M33" s="109"/>
-      <c r="N33" s="109"/>
-      <c r="O33" s="109"/>
-      <c r="P33" s="109"/>
-      <c r="Q33" s="109"/>
-      <c r="R33" s="109"/>
-      <c r="S33" s="109"/>
-      <c r="T33" s="109"/>
-      <c r="U33" s="109"/>
-      <c r="V33" s="109"/>
-      <c r="W33" s="109"/>
-      <c r="X33" s="109"/>
-      <c r="Y33" s="109"/>
-      <c r="Z33" s="109"/>
-      <c r="AA33" s="109"/>
-      <c r="AB33" s="109"/>
-      <c r="AC33" s="109"/>
-      <c r="AD33" s="109"/>
-      <c r="AE33" s="109"/>
-      <c r="AF33" s="109"/>
-      <c r="AG33" s="109"/>
-      <c r="AH33" s="109"/>
-      <c r="AI33" s="109"/>
-      <c r="AJ33" s="109"/>
-      <c r="AK33" s="109"/>
-      <c r="AL33" s="109"/>
-      <c r="AM33" s="109"/>
-      <c r="AN33" s="109"/>
-      <c r="AO33" s="109"/>
-      <c r="AP33" s="109"/>
-      <c r="AQ33" s="109"/>
-      <c r="AR33" s="109"/>
-      <c r="AS33" s="109"/>
-      <c r="AT33" s="109"/>
-      <c r="AU33" s="109"/>
-      <c r="AV33" s="109"/>
-      <c r="AW33" s="109"/>
-      <c r="AX33" s="109"/>
-      <c r="AY33" s="109"/>
-      <c r="AZ33" s="109"/>
-      <c r="BA33" s="109"/>
-      <c r="BB33" s="109"/>
-      <c r="BC33" s="109"/>
-      <c r="BD33" s="109"/>
-      <c r="BE33" s="109"/>
-      <c r="BF33" s="109"/>
-      <c r="BG33" s="109"/>
-      <c r="BH33" s="109"/>
-      <c r="BI33" s="109"/>
-      <c r="BJ33" s="109"/>
-      <c r="BK33" s="109"/>
-      <c r="BL33" s="109"/>
-      <c r="BM33" s="109"/>
-      <c r="BN33" s="109"/>
+      <c r="J32" s="96"/>
+      <c r="K32" s="109"/>
+      <c r="L32" s="109"/>
+      <c r="M32" s="109"/>
+      <c r="N32" s="109"/>
+      <c r="O32" s="109"/>
+      <c r="P32" s="109"/>
+      <c r="Q32" s="109"/>
+      <c r="R32" s="109"/>
+      <c r="S32" s="109"/>
+      <c r="T32" s="109"/>
+      <c r="U32" s="109"/>
+      <c r="V32" s="109"/>
+      <c r="W32" s="109"/>
+      <c r="X32" s="109"/>
+      <c r="Y32" s="109"/>
+      <c r="Z32" s="109"/>
+      <c r="AA32" s="109"/>
+      <c r="AB32" s="109"/>
+      <c r="AC32" s="109"/>
+      <c r="AD32" s="109"/>
+      <c r="AE32" s="109"/>
+      <c r="AF32" s="109"/>
+      <c r="AG32" s="109"/>
+      <c r="AH32" s="109"/>
+      <c r="AI32" s="109"/>
+      <c r="AJ32" s="109"/>
+      <c r="AK32" s="109"/>
+      <c r="AL32" s="109"/>
+      <c r="AM32" s="109"/>
+      <c r="AN32" s="109"/>
+      <c r="AO32" s="109"/>
+      <c r="AP32" s="109"/>
+      <c r="AQ32" s="109"/>
+      <c r="AR32" s="109"/>
+      <c r="AS32" s="109"/>
+      <c r="AT32" s="109"/>
+      <c r="AU32" s="109"/>
+      <c r="AV32" s="109"/>
+      <c r="AW32" s="109"/>
+      <c r="AX32" s="109"/>
+      <c r="AY32" s="109"/>
+      <c r="AZ32" s="109"/>
+      <c r="BA32" s="109"/>
+      <c r="BB32" s="109"/>
+      <c r="BC32" s="109"/>
+      <c r="BD32" s="109"/>
+      <c r="BE32" s="109"/>
+      <c r="BF32" s="109"/>
+      <c r="BG32" s="109"/>
+      <c r="BH32" s="109"/>
+      <c r="BI32" s="109"/>
+      <c r="BJ32" s="109"/>
+      <c r="BK32" s="109"/>
+      <c r="BL32" s="109"/>
+      <c r="BM32" s="109"/>
+      <c r="BN32" s="109"/>
+    </row>
+    <row r="33" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>4.1</v>
+      </c>
+      <c r="B33" s="126" t="s">
+        <v>160</v>
+      </c>
+      <c r="C33" s="61" t="s">
+        <v>161</v>
+      </c>
+      <c r="D33" s="127"/>
+      <c r="E33" s="100">
+        <v>43353</v>
+      </c>
+      <c r="F33" s="101">
+        <f>IF(ISBLANK(E33)," - ",IF(G33=0,E33,E33+G33-1))</f>
+        <v>43355</v>
+      </c>
+      <c r="G33" s="62">
+        <v>3</v>
+      </c>
+      <c r="H33" s="63">
+        <v>1</v>
+      </c>
+      <c r="I33" s="64">
+        <f t="shared" si="62"/>
+        <v>3</v>
+      </c>
+      <c r="J33" s="95"/>
+      <c r="K33" s="107"/>
+      <c r="L33" s="107"/>
+      <c r="M33" s="107"/>
+      <c r="N33" s="107"/>
+      <c r="O33" s="107"/>
+      <c r="P33" s="107"/>
+      <c r="Q33" s="107"/>
+      <c r="R33" s="107"/>
+      <c r="S33" s="107"/>
+      <c r="T33" s="107"/>
+      <c r="U33" s="107"/>
+      <c r="V33" s="107"/>
+      <c r="W33" s="107"/>
+      <c r="X33" s="107"/>
+      <c r="Y33" s="107"/>
+      <c r="Z33" s="107"/>
+      <c r="AA33" s="107"/>
+      <c r="AB33" s="107"/>
+      <c r="AC33" s="107"/>
+      <c r="AD33" s="107"/>
+      <c r="AE33" s="107"/>
+      <c r="AF33" s="107"/>
+      <c r="AG33" s="107"/>
+      <c r="AH33" s="107"/>
+      <c r="AI33" s="107"/>
+      <c r="AJ33" s="107"/>
+      <c r="AK33" s="107"/>
+      <c r="AL33" s="107"/>
+      <c r="AM33" s="107"/>
+      <c r="AN33" s="107"/>
+      <c r="AO33" s="107"/>
+      <c r="AP33" s="107"/>
+      <c r="AQ33" s="107"/>
+      <c r="AR33" s="107"/>
+      <c r="AS33" s="107"/>
+      <c r="AT33" s="107"/>
+      <c r="AU33" s="107"/>
+      <c r="AV33" s="107"/>
+      <c r="AW33" s="107"/>
+      <c r="AX33" s="107"/>
+      <c r="AY33" s="107"/>
+      <c r="AZ33" s="107"/>
+      <c r="BA33" s="107"/>
+      <c r="BB33" s="107"/>
+      <c r="BC33" s="107"/>
+      <c r="BD33" s="107"/>
+      <c r="BE33" s="107"/>
+      <c r="BF33" s="107"/>
+      <c r="BG33" s="107"/>
+      <c r="BH33" s="107"/>
+      <c r="BI33" s="107"/>
+      <c r="BJ33" s="107"/>
+      <c r="BK33" s="107"/>
+      <c r="BL33" s="107"/>
+      <c r="BM33" s="107"/>
+      <c r="BN33" s="107"/>
     </row>
     <row r="34" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>5.1</v>
+        <v>4.2</v>
       </c>
       <c r="B34" s="126" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C34" s="61" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D34" s="127"/>
       <c r="E34" s="100">
-        <v>43391</v>
+        <v>43354</v>
       </c>
       <c r="F34" s="101">
-        <f>IF(ISBLANK(E34)," - ",IF(G34=0,E34,E34+G34-1))</f>
-        <v>43413</v>
+        <f t="shared" si="65"/>
+        <v>43354</v>
       </c>
       <c r="G34" s="62">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="H34" s="63">
         <v>1</v>
       </c>
       <c r="I34" s="64">
-        <v>10</v>
+        <f t="shared" si="62"/>
+        <v>1</v>
       </c>
       <c r="J34" s="95"/>
       <c r="K34" s="107"/>
@@ -7910,30 +8027,31 @@
     <row r="35" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>5.2</v>
+        <v>4.3</v>
       </c>
       <c r="B35" s="126" t="s">
         <v>163</v>
       </c>
       <c r="C35" s="61" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D35" s="127"/>
       <c r="E35" s="100">
-        <v>43391</v>
+        <v>43357</v>
       </c>
       <c r="F35" s="101">
-        <f t="shared" ref="F35" si="69">IF(ISBLANK(E35)," - ",IF(G35=0,E35,E35+G35-1))</f>
-        <v>43413</v>
+        <f>IF(ISBLANK(E35)," - ",IF(G35=0,E35,E35+G35-1))</f>
+        <v>43357</v>
       </c>
       <c r="G35" s="62">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="H35" s="63">
         <v>1</v>
       </c>
       <c r="I35" s="64">
-        <v>2</v>
+        <f t="shared" si="62"/>
+        <v>1</v>
       </c>
       <c r="J35" s="95"/>
       <c r="K35" s="107"/>
@@ -7993,118 +8111,111 @@
       <c r="BM35" s="107"/>
       <c r="BN35" s="107"/>
     </row>
-    <row r="36" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>5.3</v>
-      </c>
-      <c r="B36" s="126" t="s">
+    <row r="36" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="53" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>5</v>
+      </c>
+      <c r="B36" s="54" t="s">
         <v>164</v>
       </c>
-      <c r="C36" s="61" t="s">
-        <v>162</v>
-      </c>
-      <c r="D36" s="127"/>
-      <c r="E36" s="100">
-        <v>43445</v>
-      </c>
-      <c r="F36" s="101">
-        <f>IF(ISBLANK(E36)," - ",IF(G36=0,E36,E36+G36-1))</f>
-        <v>43445</v>
-      </c>
-      <c r="G36" s="62">
-        <v>1</v>
-      </c>
-      <c r="H36" s="63">
-        <v>0.9</v>
-      </c>
-      <c r="I36" s="64">
+      <c r="D36" s="56"/>
+      <c r="E36" s="102"/>
+      <c r="F36" s="102" t="str">
+        <f t="shared" ref="F36" si="70">IF(ISBLANK(E36)," - ",IF(G36=0,E36,E36+G36-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G36" s="57"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="59" t="str">
         <f t="shared" si="62"/>
-        <v>1</v>
-      </c>
-      <c r="J36" s="95"/>
-      <c r="K36" s="107"/>
-      <c r="L36" s="107"/>
-      <c r="M36" s="107"/>
-      <c r="N36" s="107"/>
-      <c r="O36" s="107"/>
-      <c r="P36" s="107"/>
-      <c r="Q36" s="107"/>
-      <c r="R36" s="107"/>
-      <c r="S36" s="107"/>
-      <c r="T36" s="107"/>
-      <c r="U36" s="107"/>
-      <c r="V36" s="107"/>
-      <c r="W36" s="107"/>
-      <c r="X36" s="107"/>
-      <c r="Y36" s="107"/>
-      <c r="Z36" s="107"/>
-      <c r="AA36" s="107"/>
-      <c r="AB36" s="107"/>
-      <c r="AC36" s="107"/>
-      <c r="AD36" s="107"/>
-      <c r="AE36" s="107"/>
-      <c r="AF36" s="107"/>
-      <c r="AG36" s="107"/>
-      <c r="AH36" s="107"/>
-      <c r="AI36" s="107"/>
-      <c r="AJ36" s="107"/>
-      <c r="AK36" s="107"/>
-      <c r="AL36" s="107"/>
-      <c r="AM36" s="107"/>
-      <c r="AN36" s="107"/>
-      <c r="AO36" s="107"/>
-      <c r="AP36" s="107"/>
-      <c r="AQ36" s="107"/>
-      <c r="AR36" s="107"/>
-      <c r="AS36" s="107"/>
-      <c r="AT36" s="107"/>
-      <c r="AU36" s="107"/>
-      <c r="AV36" s="107"/>
-      <c r="AW36" s="107"/>
-      <c r="AX36" s="107"/>
-      <c r="AY36" s="107"/>
-      <c r="AZ36" s="107"/>
-      <c r="BA36" s="107"/>
-      <c r="BB36" s="107"/>
-      <c r="BC36" s="107"/>
-      <c r="BD36" s="107"/>
-      <c r="BE36" s="107"/>
-      <c r="BF36" s="107"/>
-      <c r="BG36" s="107"/>
-      <c r="BH36" s="107"/>
-      <c r="BI36" s="107"/>
-      <c r="BJ36" s="107"/>
-      <c r="BK36" s="107"/>
-      <c r="BL36" s="107"/>
-      <c r="BM36" s="107"/>
-      <c r="BN36" s="107"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J36" s="96"/>
+      <c r="K36" s="109"/>
+      <c r="L36" s="109"/>
+      <c r="M36" s="109"/>
+      <c r="N36" s="109"/>
+      <c r="O36" s="109"/>
+      <c r="P36" s="109"/>
+      <c r="Q36" s="109"/>
+      <c r="R36" s="109"/>
+      <c r="S36" s="109"/>
+      <c r="T36" s="109"/>
+      <c r="U36" s="109"/>
+      <c r="V36" s="109"/>
+      <c r="W36" s="109"/>
+      <c r="X36" s="109"/>
+      <c r="Y36" s="109"/>
+      <c r="Z36" s="109"/>
+      <c r="AA36" s="109"/>
+      <c r="AB36" s="109"/>
+      <c r="AC36" s="109"/>
+      <c r="AD36" s="109"/>
+      <c r="AE36" s="109"/>
+      <c r="AF36" s="109"/>
+      <c r="AG36" s="109"/>
+      <c r="AH36" s="109"/>
+      <c r="AI36" s="109"/>
+      <c r="AJ36" s="109"/>
+      <c r="AK36" s="109"/>
+      <c r="AL36" s="109"/>
+      <c r="AM36" s="109"/>
+      <c r="AN36" s="109"/>
+      <c r="AO36" s="109"/>
+      <c r="AP36" s="109"/>
+      <c r="AQ36" s="109"/>
+      <c r="AR36" s="109"/>
+      <c r="AS36" s="109"/>
+      <c r="AT36" s="109"/>
+      <c r="AU36" s="109"/>
+      <c r="AV36" s="109"/>
+      <c r="AW36" s="109"/>
+      <c r="AX36" s="109"/>
+      <c r="AY36" s="109"/>
+      <c r="AZ36" s="109"/>
+      <c r="BA36" s="109"/>
+      <c r="BB36" s="109"/>
+      <c r="BC36" s="109"/>
+      <c r="BD36" s="109"/>
+      <c r="BE36" s="109"/>
+      <c r="BF36" s="109"/>
+      <c r="BG36" s="109"/>
+      <c r="BH36" s="109"/>
+      <c r="BI36" s="109"/>
+      <c r="BJ36" s="109"/>
+      <c r="BK36" s="109"/>
+      <c r="BL36" s="109"/>
+      <c r="BM36" s="109"/>
+      <c r="BN36" s="109"/>
     </row>
     <row r="37" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>5.4</v>
+        <v>5.1</v>
       </c>
       <c r="B37" s="126" t="s">
-        <v>9</v>
+        <v>165</v>
+      </c>
+      <c r="C37" s="61" t="s">
+        <v>161</v>
       </c>
       <c r="D37" s="127"/>
       <c r="E37" s="100">
-        <v>43132</v>
+        <v>43391</v>
       </c>
       <c r="F37" s="101">
-        <f t="shared" ref="F37:F38" si="70">IF(ISBLANK(E37)," - ",IF(G37=0,E37,E37+G37-1))</f>
-        <v>43132</v>
+        <f>IF(ISBLANK(E37)," - ",IF(G37=0,E37,E37+G37-1))</f>
+        <v>43413</v>
       </c>
       <c r="G37" s="62">
+        <v>23</v>
+      </c>
+      <c r="H37" s="63">
         <v>1</v>
       </c>
-      <c r="H37" s="63">
-        <v>0</v>
-      </c>
       <c r="I37" s="64">
-        <f t="shared" si="62"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J37" s="95"/>
       <c r="K37" s="107"/>
@@ -8167,28 +8278,30 @@
     <row r="38" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>5.5</v>
+        <v>5.2</v>
       </c>
       <c r="B38" s="126" t="s">
-        <v>9</v>
+        <v>162</v>
+      </c>
+      <c r="C38" s="61" t="s">
+        <v>161</v>
       </c>
       <c r="D38" s="127"/>
       <c r="E38" s="100">
-        <v>43133</v>
+        <v>43391</v>
       </c>
       <c r="F38" s="101">
-        <f t="shared" si="70"/>
-        <v>43133</v>
+        <f t="shared" ref="F38" si="71">IF(ISBLANK(E38)," - ",IF(G38=0,E38,E38+G38-1))</f>
+        <v>43413</v>
       </c>
       <c r="G38" s="62">
+        <v>23</v>
+      </c>
+      <c r="H38" s="63">
         <v>1</v>
       </c>
-      <c r="H38" s="63">
-        <v>0</v>
-      </c>
       <c r="I38" s="64">
-        <f t="shared" si="62"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J38" s="95"/>
       <c r="K38" s="107"/>
@@ -8248,99 +8361,108 @@
       <c r="BM38" s="107"/>
       <c r="BN38" s="107"/>
     </row>
-    <row r="39" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A39" s="53" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>6</v>
-      </c>
-      <c r="B39" s="54" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="56"/>
-      <c r="E39" s="102"/>
-      <c r="F39" s="102" t="str">
-        <f t="shared" si="65"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G39" s="57"/>
-      <c r="H39" s="58"/>
-      <c r="I39" s="59" t="str">
+    <row r="39" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A39" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>5.3</v>
+      </c>
+      <c r="B39" s="126" t="s">
+        <v>163</v>
+      </c>
+      <c r="C39" s="61" t="s">
+        <v>161</v>
+      </c>
+      <c r="D39" s="127"/>
+      <c r="E39" s="100">
+        <v>43445</v>
+      </c>
+      <c r="F39" s="101">
+        <f>IF(ISBLANK(E39)," - ",IF(G39=0,E39,E39+G39-1))</f>
+        <v>43445</v>
+      </c>
+      <c r="G39" s="62">
+        <v>1</v>
+      </c>
+      <c r="H39" s="63">
+        <v>0.9</v>
+      </c>
+      <c r="I39" s="64">
         <f t="shared" si="62"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J39" s="96"/>
-      <c r="K39" s="109"/>
-      <c r="L39" s="109"/>
-      <c r="M39" s="109"/>
-      <c r="N39" s="109"/>
-      <c r="O39" s="109"/>
-      <c r="P39" s="109"/>
-      <c r="Q39" s="109"/>
-      <c r="R39" s="109"/>
-      <c r="S39" s="109"/>
-      <c r="T39" s="109"/>
-      <c r="U39" s="109"/>
-      <c r="V39" s="109"/>
-      <c r="W39" s="109"/>
-      <c r="X39" s="109"/>
-      <c r="Y39" s="109"/>
-      <c r="Z39" s="109"/>
-      <c r="AA39" s="109"/>
-      <c r="AB39" s="109"/>
-      <c r="AC39" s="109"/>
-      <c r="AD39" s="109"/>
-      <c r="AE39" s="109"/>
-      <c r="AF39" s="109"/>
-      <c r="AG39" s="109"/>
-      <c r="AH39" s="109"/>
-      <c r="AI39" s="109"/>
-      <c r="AJ39" s="109"/>
-      <c r="AK39" s="109"/>
-      <c r="AL39" s="109"/>
-      <c r="AM39" s="109"/>
-      <c r="AN39" s="109"/>
-      <c r="AO39" s="109"/>
-      <c r="AP39" s="109"/>
-      <c r="AQ39" s="109"/>
-      <c r="AR39" s="109"/>
-      <c r="AS39" s="109"/>
-      <c r="AT39" s="109"/>
-      <c r="AU39" s="109"/>
-      <c r="AV39" s="109"/>
-      <c r="AW39" s="109"/>
-      <c r="AX39" s="109"/>
-      <c r="AY39" s="109"/>
-      <c r="AZ39" s="109"/>
-      <c r="BA39" s="109"/>
-      <c r="BB39" s="109"/>
-      <c r="BC39" s="109"/>
-      <c r="BD39" s="109"/>
-      <c r="BE39" s="109"/>
-      <c r="BF39" s="109"/>
-      <c r="BG39" s="109"/>
-      <c r="BH39" s="109"/>
-      <c r="BI39" s="109"/>
-      <c r="BJ39" s="109"/>
-      <c r="BK39" s="109"/>
-      <c r="BL39" s="109"/>
-      <c r="BM39" s="109"/>
-      <c r="BN39" s="109"/>
+        <v>1</v>
+      </c>
+      <c r="J39" s="95"/>
+      <c r="K39" s="107"/>
+      <c r="L39" s="107"/>
+      <c r="M39" s="107"/>
+      <c r="N39" s="107"/>
+      <c r="O39" s="107"/>
+      <c r="P39" s="107"/>
+      <c r="Q39" s="107"/>
+      <c r="R39" s="107"/>
+      <c r="S39" s="107"/>
+      <c r="T39" s="107"/>
+      <c r="U39" s="107"/>
+      <c r="V39" s="107"/>
+      <c r="W39" s="107"/>
+      <c r="X39" s="107"/>
+      <c r="Y39" s="107"/>
+      <c r="Z39" s="107"/>
+      <c r="AA39" s="107"/>
+      <c r="AB39" s="107"/>
+      <c r="AC39" s="107"/>
+      <c r="AD39" s="107"/>
+      <c r="AE39" s="107"/>
+      <c r="AF39" s="107"/>
+      <c r="AG39" s="107"/>
+      <c r="AH39" s="107"/>
+      <c r="AI39" s="107"/>
+      <c r="AJ39" s="107"/>
+      <c r="AK39" s="107"/>
+      <c r="AL39" s="107"/>
+      <c r="AM39" s="107"/>
+      <c r="AN39" s="107"/>
+      <c r="AO39" s="107"/>
+      <c r="AP39" s="107"/>
+      <c r="AQ39" s="107"/>
+      <c r="AR39" s="107"/>
+      <c r="AS39" s="107"/>
+      <c r="AT39" s="107"/>
+      <c r="AU39" s="107"/>
+      <c r="AV39" s="107"/>
+      <c r="AW39" s="107"/>
+      <c r="AX39" s="107"/>
+      <c r="AY39" s="107"/>
+      <c r="AZ39" s="107"/>
+      <c r="BA39" s="107"/>
+      <c r="BB39" s="107"/>
+      <c r="BC39" s="107"/>
+      <c r="BD39" s="107"/>
+      <c r="BE39" s="107"/>
+      <c r="BF39" s="107"/>
+      <c r="BG39" s="107"/>
+      <c r="BH39" s="107"/>
+      <c r="BI39" s="107"/>
+      <c r="BJ39" s="107"/>
+      <c r="BK39" s="107"/>
+      <c r="BL39" s="107"/>
+      <c r="BM39" s="107"/>
+      <c r="BN39" s="107"/>
     </row>
     <row r="40" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>6.1</v>
+        <v>5.4</v>
       </c>
       <c r="B40" s="126" t="s">
         <v>9</v>
       </c>
       <c r="D40" s="127"/>
       <c r="E40" s="100">
-        <v>43129</v>
+        <v>43132</v>
       </c>
       <c r="F40" s="101">
-        <f t="shared" si="65"/>
-        <v>43129</v>
+        <f t="shared" ref="F40:F41" si="72">IF(ISBLANK(E40)," - ",IF(G40=0,E40,E40+G40-1))</f>
+        <v>43132</v>
       </c>
       <c r="G40" s="62">
         <v>1</v>
@@ -8413,18 +8535,18 @@
     <row r="41" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>6.2</v>
+        <v>5.5</v>
       </c>
       <c r="B41" s="126" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="127"/>
       <c r="E41" s="100">
-        <v>43130</v>
+        <v>43133</v>
       </c>
       <c r="F41" s="101">
-        <f t="shared" si="65"/>
-        <v>43130</v>
+        <f t="shared" si="72"/>
+        <v>43133</v>
       </c>
       <c r="G41" s="62">
         <v>1</v>
@@ -8494,105 +8616,99 @@
       <c r="BM41" s="107"/>
       <c r="BN41" s="107"/>
     </row>
-    <row r="42" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A42" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>6.3</v>
-      </c>
-      <c r="B42" s="126" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" s="127"/>
-      <c r="E42" s="100">
-        <v>43131</v>
-      </c>
-      <c r="F42" s="101">
+    <row r="42" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A42" s="53" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>6</v>
+      </c>
+      <c r="B42" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="56"/>
+      <c r="E42" s="102"/>
+      <c r="F42" s="102" t="str">
         <f t="shared" si="65"/>
-        <v>43131</v>
-      </c>
-      <c r="G42" s="62">
-        <v>1</v>
-      </c>
-      <c r="H42" s="63">
-        <v>0</v>
-      </c>
-      <c r="I42" s="64">
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G42" s="57"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="59" t="str">
         <f t="shared" si="62"/>
-        <v>1</v>
-      </c>
-      <c r="J42" s="95"/>
-      <c r="K42" s="107"/>
-      <c r="L42" s="107"/>
-      <c r="M42" s="107"/>
-      <c r="N42" s="107"/>
-      <c r="O42" s="107"/>
-      <c r="P42" s="107"/>
-      <c r="Q42" s="107"/>
-      <c r="R42" s="107"/>
-      <c r="S42" s="107"/>
-      <c r="T42" s="107"/>
-      <c r="U42" s="107"/>
-      <c r="V42" s="107"/>
-      <c r="W42" s="107"/>
-      <c r="X42" s="107"/>
-      <c r="Y42" s="107"/>
-      <c r="Z42" s="107"/>
-      <c r="AA42" s="107"/>
-      <c r="AB42" s="107"/>
-      <c r="AC42" s="107"/>
-      <c r="AD42" s="107"/>
-      <c r="AE42" s="107"/>
-      <c r="AF42" s="107"/>
-      <c r="AG42" s="107"/>
-      <c r="AH42" s="107"/>
-      <c r="AI42" s="107"/>
-      <c r="AJ42" s="107"/>
-      <c r="AK42" s="107"/>
-      <c r="AL42" s="107"/>
-      <c r="AM42" s="107"/>
-      <c r="AN42" s="107"/>
-      <c r="AO42" s="107"/>
-      <c r="AP42" s="107"/>
-      <c r="AQ42" s="107"/>
-      <c r="AR42" s="107"/>
-      <c r="AS42" s="107"/>
-      <c r="AT42" s="107"/>
-      <c r="AU42" s="107"/>
-      <c r="AV42" s="107"/>
-      <c r="AW42" s="107"/>
-      <c r="AX42" s="107"/>
-      <c r="AY42" s="107"/>
-      <c r="AZ42" s="107"/>
-      <c r="BA42" s="107"/>
-      <c r="BB42" s="107"/>
-      <c r="BC42" s="107"/>
-      <c r="BD42" s="107"/>
-      <c r="BE42" s="107"/>
-      <c r="BF42" s="107"/>
-      <c r="BG42" s="107"/>
-      <c r="BH42" s="107"/>
-      <c r="BI42" s="107"/>
-      <c r="BJ42" s="107"/>
-      <c r="BK42" s="107"/>
-      <c r="BL42" s="107"/>
-      <c r="BM42" s="107"/>
-      <c r="BN42" s="107"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J42" s="96"/>
+      <c r="K42" s="109"/>
+      <c r="L42" s="109"/>
+      <c r="M42" s="109"/>
+      <c r="N42" s="109"/>
+      <c r="O42" s="109"/>
+      <c r="P42" s="109"/>
+      <c r="Q42" s="109"/>
+      <c r="R42" s="109"/>
+      <c r="S42" s="109"/>
+      <c r="T42" s="109"/>
+      <c r="U42" s="109"/>
+      <c r="V42" s="109"/>
+      <c r="W42" s="109"/>
+      <c r="X42" s="109"/>
+      <c r="Y42" s="109"/>
+      <c r="Z42" s="109"/>
+      <c r="AA42" s="109"/>
+      <c r="AB42" s="109"/>
+      <c r="AC42" s="109"/>
+      <c r="AD42" s="109"/>
+      <c r="AE42" s="109"/>
+      <c r="AF42" s="109"/>
+      <c r="AG42" s="109"/>
+      <c r="AH42" s="109"/>
+      <c r="AI42" s="109"/>
+      <c r="AJ42" s="109"/>
+      <c r="AK42" s="109"/>
+      <c r="AL42" s="109"/>
+      <c r="AM42" s="109"/>
+      <c r="AN42" s="109"/>
+      <c r="AO42" s="109"/>
+      <c r="AP42" s="109"/>
+      <c r="AQ42" s="109"/>
+      <c r="AR42" s="109"/>
+      <c r="AS42" s="109"/>
+      <c r="AT42" s="109"/>
+      <c r="AU42" s="109"/>
+      <c r="AV42" s="109"/>
+      <c r="AW42" s="109"/>
+      <c r="AX42" s="109"/>
+      <c r="AY42" s="109"/>
+      <c r="AZ42" s="109"/>
+      <c r="BA42" s="109"/>
+      <c r="BB42" s="109"/>
+      <c r="BC42" s="109"/>
+      <c r="BD42" s="109"/>
+      <c r="BE42" s="109"/>
+      <c r="BF42" s="109"/>
+      <c r="BG42" s="109"/>
+      <c r="BH42" s="109"/>
+      <c r="BI42" s="109"/>
+      <c r="BJ42" s="109"/>
+      <c r="BK42" s="109"/>
+      <c r="BL42" s="109"/>
+      <c r="BM42" s="109"/>
+      <c r="BN42" s="109"/>
     </row>
     <row r="43" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
       <c r="B43" s="126" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="127"/>
       <c r="E43" s="100">
-        <v>43132</v>
+        <v>43129</v>
       </c>
       <c r="F43" s="101">
         <f t="shared" si="65"/>
-        <v>43132</v>
+        <v>43129</v>
       </c>
       <c r="G43" s="62">
         <v>1</v>
@@ -8665,18 +8781,18 @@
     <row r="44" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>6.5</v>
+        <v>6.2</v>
       </c>
       <c r="B44" s="126" t="s">
         <v>9</v>
       </c>
       <c r="D44" s="127"/>
       <c r="E44" s="100">
-        <v>43133</v>
+        <v>43130</v>
       </c>
       <c r="F44" s="101">
         <f t="shared" si="65"/>
-        <v>43133</v>
+        <v>43130</v>
       </c>
       <c r="G44" s="62">
         <v>1</v>
@@ -8746,20 +8862,33 @@
       <c r="BM44" s="107"/>
       <c r="BN44" s="107"/>
     </row>
-    <row r="45" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A45" s="60"/>
-      <c r="B45" s="65"/>
-      <c r="C45" s="65"/>
-      <c r="D45" s="66"/>
-      <c r="E45" s="103"/>
-      <c r="F45" s="103"/>
-      <c r="G45" s="67"/>
-      <c r="H45" s="68"/>
-      <c r="I45" s="69" t="str">
+    <row r="45" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>6.3</v>
+      </c>
+      <c r="B45" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="127"/>
+      <c r="E45" s="100">
+        <v>43131</v>
+      </c>
+      <c r="F45" s="101">
+        <f t="shared" si="65"/>
+        <v>43131</v>
+      </c>
+      <c r="G45" s="62">
+        <v>1</v>
+      </c>
+      <c r="H45" s="63">
+        <v>0</v>
+      </c>
+      <c r="I45" s="64">
         <f t="shared" si="62"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J45" s="97"/>
+        <v>1</v>
+      </c>
+      <c r="J45" s="95"/>
       <c r="K45" s="107"/>
       <c r="L45" s="107"/>
       <c r="M45" s="107"/>
@@ -8817,20 +8946,33 @@
       <c r="BM45" s="107"/>
       <c r="BN45" s="107"/>
     </row>
-    <row r="46" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A46" s="60"/>
-      <c r="B46" s="65"/>
-      <c r="C46" s="65"/>
-      <c r="D46" s="66"/>
-      <c r="E46" s="103"/>
-      <c r="F46" s="103"/>
-      <c r="G46" s="67"/>
-      <c r="H46" s="68"/>
-      <c r="I46" s="69" t="str">
+    <row r="46" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A46" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>6.4</v>
+      </c>
+      <c r="B46" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="127"/>
+      <c r="E46" s="100">
+        <v>43132</v>
+      </c>
+      <c r="F46" s="101">
+        <f t="shared" si="65"/>
+        <v>43132</v>
+      </c>
+      <c r="G46" s="62">
+        <v>1</v>
+      </c>
+      <c r="H46" s="63">
+        <v>0</v>
+      </c>
+      <c r="I46" s="64">
         <f t="shared" si="62"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J46" s="97"/>
+        <v>1</v>
+      </c>
+      <c r="J46" s="95"/>
       <c r="K46" s="107"/>
       <c r="L46" s="107"/>
       <c r="M46" s="107"/>
@@ -8888,19 +9030,33 @@
       <c r="BM46" s="107"/>
       <c r="BN46" s="107"/>
     </row>
-    <row r="47" spans="1:66" s="75" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="71" t="s">
+    <row r="47" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A47" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>6.5</v>
+      </c>
+      <c r="B47" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="127"/>
+      <c r="E47" s="100">
+        <v>43133</v>
+      </c>
+      <c r="F47" s="101">
+        <f t="shared" si="65"/>
+        <v>43133</v>
+      </c>
+      <c r="G47" s="62">
         <v>1</v>
       </c>
-      <c r="B47" s="72"/>
-      <c r="C47" s="73"/>
-      <c r="D47" s="73"/>
-      <c r="E47" s="104"/>
-      <c r="F47" s="104"/>
-      <c r="G47" s="74"/>
-      <c r="H47" s="74"/>
-      <c r="I47" s="74"/>
-      <c r="J47" s="98"/>
+      <c r="H47" s="63">
+        <v>0</v>
+      </c>
+      <c r="I47" s="64">
+        <f t="shared" si="62"/>
+        <v>1</v>
+      </c>
+      <c r="J47" s="95"/>
       <c r="K47" s="107"/>
       <c r="L47" s="107"/>
       <c r="M47" s="107"/>
@@ -8959,18 +9115,19 @@
       <c r="BN47" s="107"/>
     </row>
     <row r="48" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A48" s="76" t="s">
-        <v>39</v>
-      </c>
-      <c r="B48" s="77"/>
-      <c r="C48" s="77"/>
-      <c r="D48" s="77"/>
-      <c r="E48" s="105"/>
-      <c r="F48" s="105"/>
-      <c r="G48" s="77"/>
-      <c r="H48" s="77"/>
-      <c r="I48" s="77"/>
-      <c r="J48" s="98"/>
+      <c r="A48" s="60"/>
+      <c r="B48" s="65"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="66"/>
+      <c r="E48" s="103"/>
+      <c r="F48" s="103"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="68"/>
+      <c r="I48" s="69" t="str">
+        <f t="shared" si="62"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J48" s="97"/>
       <c r="K48" s="107"/>
       <c r="L48" s="107"/>
       <c r="M48" s="107"/>
@@ -9029,27 +9186,19 @@
       <c r="BN48" s="107"/>
     </row>
     <row r="49" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A49" s="130" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>1</v>
-      </c>
-      <c r="B49" s="131" t="s">
-        <v>78</v>
-      </c>
-      <c r="C49" s="78"/>
-      <c r="D49" s="79"/>
-      <c r="E49" s="100"/>
-      <c r="F49" s="101" t="str">
-        <f t="shared" ref="F49:F52" si="71">IF(ISBLANK(E49)," - ",IF(G49=0,E49,E49+G49-1))</f>
+      <c r="A49" s="60"/>
+      <c r="B49" s="65"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="66"/>
+      <c r="E49" s="103"/>
+      <c r="F49" s="103"/>
+      <c r="G49" s="67"/>
+      <c r="H49" s="68"/>
+      <c r="I49" s="69" t="str">
+        <f t="shared" si="62"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G49" s="62"/>
-      <c r="H49" s="63"/>
-      <c r="I49" s="80" t="str">
-        <f>IF(OR(F49=0,E49=0)," - ",NETWORKDAYS(E49,F49))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J49" s="99"/>
+      <c r="J49" s="97"/>
       <c r="K49" s="107"/>
       <c r="L49" s="107"/>
       <c r="M49" s="107"/>
@@ -9107,28 +9256,19 @@
       <c r="BM49" s="107"/>
       <c r="BN49" s="107"/>
     </row>
-    <row r="50" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A50" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>1.1</v>
-      </c>
-      <c r="B50" s="81" t="s">
-        <v>64</v>
-      </c>
-      <c r="C50" s="81"/>
-      <c r="D50" s="79"/>
-      <c r="E50" s="100"/>
-      <c r="F50" s="101" t="str">
-        <f t="shared" si="71"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G50" s="62"/>
-      <c r="H50" s="63"/>
-      <c r="I50" s="80" t="str">
-        <f t="shared" ref="I50:I52" si="72">IF(OR(F50=0,E50=0)," - ",NETWORKDAYS(E50,F50))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J50" s="99"/>
+    <row r="50" spans="1:66" s="75" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A50" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="72"/>
+      <c r="C50" s="73"/>
+      <c r="D50" s="73"/>
+      <c r="E50" s="104"/>
+      <c r="F50" s="104"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
+      <c r="J50" s="98"/>
       <c r="K50" s="107"/>
       <c r="L50" s="107"/>
       <c r="M50" s="107"/>
@@ -9187,27 +9327,18 @@
       <c r="BN50" s="107"/>
     </row>
     <row r="51" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A51" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
-        <v>1.1.1</v>
-      </c>
-      <c r="B51" s="82" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" s="81"/>
-      <c r="D51" s="79"/>
-      <c r="E51" s="100"/>
-      <c r="F51" s="101" t="str">
-        <f t="shared" si="71"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G51" s="62"/>
-      <c r="H51" s="63"/>
-      <c r="I51" s="80" t="str">
-        <f t="shared" si="72"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J51" s="99"/>
+      <c r="A51" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="77"/>
+      <c r="C51" s="77"/>
+      <c r="D51" s="77"/>
+      <c r="E51" s="105"/>
+      <c r="F51" s="105"/>
+      <c r="G51" s="77"/>
+      <c r="H51" s="77"/>
+      <c r="I51" s="77"/>
+      <c r="J51" s="98"/>
       <c r="K51" s="107"/>
       <c r="L51" s="107"/>
       <c r="M51" s="107"/>
@@ -9266,24 +9397,24 @@
       <c r="BN51" s="107"/>
     </row>
     <row r="52" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A52" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
-        <v>1.1.1.1</v>
-      </c>
-      <c r="B52" s="82" t="s">
-        <v>66</v>
-      </c>
-      <c r="C52" s="81"/>
+      <c r="A52" s="130" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>1</v>
+      </c>
+      <c r="B52" s="131" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="78"/>
       <c r="D52" s="79"/>
       <c r="E52" s="100"/>
       <c r="F52" s="101" t="str">
-        <f t="shared" si="71"/>
+        <f t="shared" ref="F52:F55" si="73">IF(ISBLANK(E52)," - ",IF(G52=0,E52,E52+G52-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G52" s="62"/>
       <c r="H52" s="63"/>
       <c r="I52" s="80" t="str">
-        <f t="shared" si="72"/>
+        <f>IF(OR(F52=0,E52=0)," - ",NETWORKDAYS(E52,F52))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J52" s="99"/>
@@ -9344,86 +9475,330 @@
       <c r="BM52" s="107"/>
       <c r="BN52" s="107"/>
     </row>
-    <row r="53" spans="1:66" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="30"/>
-      <c r="B53" s="31"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="31"/>
-      <c r="F53" s="31"/>
-      <c r="G53" s="31"/>
-      <c r="H53" s="31"/>
-      <c r="I53" s="31"/>
-      <c r="J53" s="31"/>
-      <c r="K53" s="31"/>
-      <c r="L53" s="31"/>
-      <c r="M53" s="31"/>
-      <c r="N53" s="31"/>
-      <c r="O53" s="31"/>
-      <c r="P53" s="31"/>
-      <c r="Q53" s="31"/>
-      <c r="R53" s="31"/>
-      <c r="S53" s="31"/>
-      <c r="T53" s="31"/>
-      <c r="U53" s="31"/>
-      <c r="V53" s="31"/>
-      <c r="W53" s="31"/>
-      <c r="X53" s="31"/>
-      <c r="Y53" s="31"/>
-      <c r="Z53" s="31"/>
-      <c r="AA53" s="31"/>
-      <c r="AB53" s="31"/>
-      <c r="AC53" s="31"/>
-      <c r="AD53" s="31"/>
-      <c r="AE53" s="31"/>
-      <c r="AF53" s="31"/>
-      <c r="AG53" s="31"/>
-      <c r="AH53" s="31"/>
-      <c r="AI53" s="31"/>
-      <c r="AJ53" s="31"/>
-      <c r="AK53" s="31"/>
-      <c r="AL53" s="31"/>
-      <c r="AM53" s="31"/>
-      <c r="AN53" s="31"/>
-      <c r="AO53" s="31"/>
-      <c r="AP53" s="31"/>
-      <c r="AQ53" s="31"/>
-      <c r="AR53" s="31"/>
-      <c r="AS53" s="31"/>
-      <c r="AT53" s="31"/>
-      <c r="AU53" s="31"/>
-      <c r="AV53" s="31"/>
-      <c r="AW53" s="31"/>
-      <c r="AX53" s="31"/>
-      <c r="AY53" s="31"/>
-      <c r="AZ53" s="31"/>
-      <c r="BA53" s="31"/>
-      <c r="BB53" s="31"/>
-      <c r="BC53" s="31"/>
-      <c r="BD53" s="31"/>
-      <c r="BE53" s="31"/>
-      <c r="BF53" s="31"/>
-      <c r="BG53" s="31"/>
-      <c r="BH53" s="31"/>
-      <c r="BI53" s="31"/>
-      <c r="BJ53" s="31"/>
-      <c r="BK53" s="31"/>
-      <c r="BL53" s="31"/>
-      <c r="BM53" s="31"/>
-      <c r="BN53" s="31"/>
+    <row r="53" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A53" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>1.1</v>
+      </c>
+      <c r="B53" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="81"/>
+      <c r="D53" s="79"/>
+      <c r="E53" s="100"/>
+      <c r="F53" s="101" t="str">
+        <f t="shared" si="73"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G53" s="62"/>
+      <c r="H53" s="63"/>
+      <c r="I53" s="80" t="str">
+        <f t="shared" ref="I53:I55" si="74">IF(OR(F53=0,E53=0)," - ",NETWORKDAYS(E53,F53))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J53" s="99"/>
+      <c r="K53" s="107"/>
+      <c r="L53" s="107"/>
+      <c r="M53" s="107"/>
+      <c r="N53" s="107"/>
+      <c r="O53" s="107"/>
+      <c r="P53" s="107"/>
+      <c r="Q53" s="107"/>
+      <c r="R53" s="107"/>
+      <c r="S53" s="107"/>
+      <c r="T53" s="107"/>
+      <c r="U53" s="107"/>
+      <c r="V53" s="107"/>
+      <c r="W53" s="107"/>
+      <c r="X53" s="107"/>
+      <c r="Y53" s="107"/>
+      <c r="Z53" s="107"/>
+      <c r="AA53" s="107"/>
+      <c r="AB53" s="107"/>
+      <c r="AC53" s="107"/>
+      <c r="AD53" s="107"/>
+      <c r="AE53" s="107"/>
+      <c r="AF53" s="107"/>
+      <c r="AG53" s="107"/>
+      <c r="AH53" s="107"/>
+      <c r="AI53" s="107"/>
+      <c r="AJ53" s="107"/>
+      <c r="AK53" s="107"/>
+      <c r="AL53" s="107"/>
+      <c r="AM53" s="107"/>
+      <c r="AN53" s="107"/>
+      <c r="AO53" s="107"/>
+      <c r="AP53" s="107"/>
+      <c r="AQ53" s="107"/>
+      <c r="AR53" s="107"/>
+      <c r="AS53" s="107"/>
+      <c r="AT53" s="107"/>
+      <c r="AU53" s="107"/>
+      <c r="AV53" s="107"/>
+      <c r="AW53" s="107"/>
+      <c r="AX53" s="107"/>
+      <c r="AY53" s="107"/>
+      <c r="AZ53" s="107"/>
+      <c r="BA53" s="107"/>
+      <c r="BB53" s="107"/>
+      <c r="BC53" s="107"/>
+      <c r="BD53" s="107"/>
+      <c r="BE53" s="107"/>
+      <c r="BF53" s="107"/>
+      <c r="BG53" s="107"/>
+      <c r="BH53" s="107"/>
+      <c r="BI53" s="107"/>
+      <c r="BJ53" s="107"/>
+      <c r="BK53" s="107"/>
+      <c r="BL53" s="107"/>
+      <c r="BM53" s="107"/>
+      <c r="BN53" s="107"/>
+    </row>
+    <row r="54" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A54" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <v>1.1.1</v>
+      </c>
+      <c r="B54" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="C54" s="81"/>
+      <c r="D54" s="79"/>
+      <c r="E54" s="100"/>
+      <c r="F54" s="101" t="str">
+        <f t="shared" si="73"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G54" s="62"/>
+      <c r="H54" s="63"/>
+      <c r="I54" s="80" t="str">
+        <f t="shared" si="74"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J54" s="99"/>
+      <c r="K54" s="107"/>
+      <c r="L54" s="107"/>
+      <c r="M54" s="107"/>
+      <c r="N54" s="107"/>
+      <c r="O54" s="107"/>
+      <c r="P54" s="107"/>
+      <c r="Q54" s="107"/>
+      <c r="R54" s="107"/>
+      <c r="S54" s="107"/>
+      <c r="T54" s="107"/>
+      <c r="U54" s="107"/>
+      <c r="V54" s="107"/>
+      <c r="W54" s="107"/>
+      <c r="X54" s="107"/>
+      <c r="Y54" s="107"/>
+      <c r="Z54" s="107"/>
+      <c r="AA54" s="107"/>
+      <c r="AB54" s="107"/>
+      <c r="AC54" s="107"/>
+      <c r="AD54" s="107"/>
+      <c r="AE54" s="107"/>
+      <c r="AF54" s="107"/>
+      <c r="AG54" s="107"/>
+      <c r="AH54" s="107"/>
+      <c r="AI54" s="107"/>
+      <c r="AJ54" s="107"/>
+      <c r="AK54" s="107"/>
+      <c r="AL54" s="107"/>
+      <c r="AM54" s="107"/>
+      <c r="AN54" s="107"/>
+      <c r="AO54" s="107"/>
+      <c r="AP54" s="107"/>
+      <c r="AQ54" s="107"/>
+      <c r="AR54" s="107"/>
+      <c r="AS54" s="107"/>
+      <c r="AT54" s="107"/>
+      <c r="AU54" s="107"/>
+      <c r="AV54" s="107"/>
+      <c r="AW54" s="107"/>
+      <c r="AX54" s="107"/>
+      <c r="AY54" s="107"/>
+      <c r="AZ54" s="107"/>
+      <c r="BA54" s="107"/>
+      <c r="BB54" s="107"/>
+      <c r="BC54" s="107"/>
+      <c r="BD54" s="107"/>
+      <c r="BE54" s="107"/>
+      <c r="BF54" s="107"/>
+      <c r="BG54" s="107"/>
+      <c r="BH54" s="107"/>
+      <c r="BI54" s="107"/>
+      <c r="BJ54" s="107"/>
+      <c r="BK54" s="107"/>
+      <c r="BL54" s="107"/>
+      <c r="BM54" s="107"/>
+      <c r="BN54" s="107"/>
+    </row>
+    <row r="55" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A55" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
+        <v>1.1.1.1</v>
+      </c>
+      <c r="B55" s="82" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" s="81"/>
+      <c r="D55" s="79"/>
+      <c r="E55" s="100"/>
+      <c r="F55" s="101" t="str">
+        <f t="shared" si="73"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G55" s="62"/>
+      <c r="H55" s="63"/>
+      <c r="I55" s="80" t="str">
+        <f t="shared" si="74"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J55" s="99"/>
+      <c r="K55" s="107"/>
+      <c r="L55" s="107"/>
+      <c r="M55" s="107"/>
+      <c r="N55" s="107"/>
+      <c r="O55" s="107"/>
+      <c r="P55" s="107"/>
+      <c r="Q55" s="107"/>
+      <c r="R55" s="107"/>
+      <c r="S55" s="107"/>
+      <c r="T55" s="107"/>
+      <c r="U55" s="107"/>
+      <c r="V55" s="107"/>
+      <c r="W55" s="107"/>
+      <c r="X55" s="107"/>
+      <c r="Y55" s="107"/>
+      <c r="Z55" s="107"/>
+      <c r="AA55" s="107"/>
+      <c r="AB55" s="107"/>
+      <c r="AC55" s="107"/>
+      <c r="AD55" s="107"/>
+      <c r="AE55" s="107"/>
+      <c r="AF55" s="107"/>
+      <c r="AG55" s="107"/>
+      <c r="AH55" s="107"/>
+      <c r="AI55" s="107"/>
+      <c r="AJ55" s="107"/>
+      <c r="AK55" s="107"/>
+      <c r="AL55" s="107"/>
+      <c r="AM55" s="107"/>
+      <c r="AN55" s="107"/>
+      <c r="AO55" s="107"/>
+      <c r="AP55" s="107"/>
+      <c r="AQ55" s="107"/>
+      <c r="AR55" s="107"/>
+      <c r="AS55" s="107"/>
+      <c r="AT55" s="107"/>
+      <c r="AU55" s="107"/>
+      <c r="AV55" s="107"/>
+      <c r="AW55" s="107"/>
+      <c r="AX55" s="107"/>
+      <c r="AY55" s="107"/>
+      <c r="AZ55" s="107"/>
+      <c r="BA55" s="107"/>
+      <c r="BB55" s="107"/>
+      <c r="BC55" s="107"/>
+      <c r="BD55" s="107"/>
+      <c r="BE55" s="107"/>
+      <c r="BF55" s="107"/>
+      <c r="BG55" s="107"/>
+      <c r="BH55" s="107"/>
+      <c r="BI55" s="107"/>
+      <c r="BJ55" s="107"/>
+      <c r="BK55" s="107"/>
+      <c r="BL55" s="107"/>
+      <c r="BM55" s="107"/>
+      <c r="BN55" s="107"/>
+    </row>
+    <row r="56" spans="1:66" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="30"/>
+      <c r="B56" s="31"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="31"/>
+      <c r="G56" s="31"/>
+      <c r="H56" s="31"/>
+      <c r="I56" s="31"/>
+      <c r="J56" s="31"/>
+      <c r="K56" s="31"/>
+      <c r="L56" s="31"/>
+      <c r="M56" s="31"/>
+      <c r="N56" s="31"/>
+      <c r="O56" s="31"/>
+      <c r="P56" s="31"/>
+      <c r="Q56" s="31"/>
+      <c r="R56" s="31"/>
+      <c r="S56" s="31"/>
+      <c r="T56" s="31"/>
+      <c r="U56" s="31"/>
+      <c r="V56" s="31"/>
+      <c r="W56" s="31"/>
+      <c r="X56" s="31"/>
+      <c r="Y56" s="31"/>
+      <c r="Z56" s="31"/>
+      <c r="AA56" s="31"/>
+      <c r="AB56" s="31"/>
+      <c r="AC56" s="31"/>
+      <c r="AD56" s="31"/>
+      <c r="AE56" s="31"/>
+      <c r="AF56" s="31"/>
+      <c r="AG56" s="31"/>
+      <c r="AH56" s="31"/>
+      <c r="AI56" s="31"/>
+      <c r="AJ56" s="31"/>
+      <c r="AK56" s="31"/>
+      <c r="AL56" s="31"/>
+      <c r="AM56" s="31"/>
+      <c r="AN56" s="31"/>
+      <c r="AO56" s="31"/>
+      <c r="AP56" s="31"/>
+      <c r="AQ56" s="31"/>
+      <c r="AR56" s="31"/>
+      <c r="AS56" s="31"/>
+      <c r="AT56" s="31"/>
+      <c r="AU56" s="31"/>
+      <c r="AV56" s="31"/>
+      <c r="AW56" s="31"/>
+      <c r="AX56" s="31"/>
+      <c r="AY56" s="31"/>
+      <c r="AZ56" s="31"/>
+      <c r="BA56" s="31"/>
+      <c r="BB56" s="31"/>
+      <c r="BC56" s="31"/>
+      <c r="BD56" s="31"/>
+      <c r="BE56" s="31"/>
+      <c r="BF56" s="31"/>
+      <c r="BG56" s="31"/>
+      <c r="BH56" s="31"/>
+      <c r="BI56" s="31"/>
+      <c r="BJ56" s="31"/>
+      <c r="BK56" s="31"/>
+      <c r="BL56" s="31"/>
+      <c r="BM56" s="31"/>
+      <c r="BN56" s="31"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="35">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="DL4:DR4"/>
+    <mergeCell ref="DL5:DR5"/>
+    <mergeCell ref="CQ4:CW4"/>
+    <mergeCell ref="CQ5:CW5"/>
+    <mergeCell ref="CX4:DD4"/>
+    <mergeCell ref="CX5:DD5"/>
+    <mergeCell ref="DE4:DK4"/>
+    <mergeCell ref="DE5:DK5"/>
+    <mergeCell ref="CJ4:CP4"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BO4:BU4"/>
+    <mergeCell ref="BV4:CB4"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="CC5:CI5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -9434,26 +9809,19 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="CJ4:CP4"/>
-    <mergeCell ref="CJ5:CP5"/>
-    <mergeCell ref="BO5:BU5"/>
-    <mergeCell ref="BO4:BU4"/>
-    <mergeCell ref="BV4:CB4"/>
-    <mergeCell ref="BV5:CB5"/>
-    <mergeCell ref="CC4:CI4"/>
-    <mergeCell ref="CC5:CI5"/>
-    <mergeCell ref="DL4:DR4"/>
-    <mergeCell ref="DL5:DR5"/>
-    <mergeCell ref="CQ4:CW4"/>
-    <mergeCell ref="CQ5:CW5"/>
-    <mergeCell ref="CX4:DD4"/>
-    <mergeCell ref="CX5:DD5"/>
-    <mergeCell ref="DE4:DK4"/>
-    <mergeCell ref="DE5:DK5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H8:H9 H39:H52 H11:H12 H14 H16:H28">
-    <cfRule type="dataBar" priority="40">
+  <conditionalFormatting sqref="H8:H9 H42:H55 H11:H12 H14 H16:H20 H22 H25:H31">
+    <cfRule type="dataBar" priority="52">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -9467,65 +9835,65 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN7">
-    <cfRule type="expression" dxfId="31" priority="83">
+    <cfRule type="expression" dxfId="43" priority="95">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BN9 K11:BN12 BO24:CL24 K14:BN14 K16:BN52">
-    <cfRule type="expression" dxfId="30" priority="86">
+  <conditionalFormatting sqref="K8:BN9 K11:BN12 BO27:CL27 K14:BN14 K16:BN20 K22:BN22 K25:BN55">
+    <cfRule type="expression" dxfId="42" priority="98">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="87">
+    <cfRule type="expression" dxfId="41" priority="99">
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:BN9 K39:BN52 BO24:CL24 K11:BN12 K14:BN14 K16:BN28">
-    <cfRule type="expression" dxfId="28" priority="46">
+  <conditionalFormatting sqref="K6:BN9 K42:BN55 BO27:CL27 K11:BN12 K14:BN14 K16:BN20 K22:BN22 K25:BN31">
+    <cfRule type="expression" dxfId="40" priority="58">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO6:BU7">
-    <cfRule type="expression" dxfId="27" priority="38">
+    <cfRule type="expression" dxfId="39" priority="50">
       <formula>BO$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO6:BU7">
-    <cfRule type="expression" dxfId="26" priority="37">
+    <cfRule type="expression" dxfId="38" priority="49">
       <formula>BO$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV6:CB7">
-    <cfRule type="expression" dxfId="25" priority="36">
+    <cfRule type="expression" dxfId="37" priority="48">
       <formula>BV$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV6:CB7">
-    <cfRule type="expression" dxfId="24" priority="35">
+    <cfRule type="expression" dxfId="36" priority="47">
       <formula>BV$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC6:CI7">
-    <cfRule type="expression" dxfId="23" priority="34">
+    <cfRule type="expression" dxfId="35" priority="46">
       <formula>CC$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC6:CI7">
-    <cfRule type="expression" dxfId="22" priority="33">
+    <cfRule type="expression" dxfId="34" priority="45">
       <formula>CC$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ6:CP7">
-    <cfRule type="expression" dxfId="21" priority="32">
+    <cfRule type="expression" dxfId="33" priority="44">
       <formula>CJ$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ6:CP7">
-    <cfRule type="expression" dxfId="20" priority="31">
+    <cfRule type="expression" dxfId="32" priority="43">
       <formula>CJ$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H29:H32">
-    <cfRule type="dataBar" priority="25">
+  <conditionalFormatting sqref="H32:H35">
+    <cfRule type="dataBar" priority="37">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -9538,13 +9906,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K29:BN32">
-    <cfRule type="expression" dxfId="19" priority="26">
+  <conditionalFormatting sqref="K32:BN35">
+    <cfRule type="expression" dxfId="31" priority="38">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H33:H36">
-    <cfRule type="dataBar" priority="21">
+  <conditionalFormatting sqref="H36:H39">
+    <cfRule type="dataBar" priority="33">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -9557,8 +9925,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H37:H38">
-    <cfRule type="dataBar" priority="23">
+  <conditionalFormatting sqref="H40:H41">
+    <cfRule type="dataBar" priority="35">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -9571,58 +9939,58 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K37:BN38">
-    <cfRule type="expression" dxfId="18" priority="24">
+  <conditionalFormatting sqref="K40:BN41">
+    <cfRule type="expression" dxfId="30" priority="36">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K33:BN36">
-    <cfRule type="expression" dxfId="17" priority="22">
+  <conditionalFormatting sqref="K36:BN39">
+    <cfRule type="expression" dxfId="29" priority="34">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CQ6:CW7">
-    <cfRule type="expression" dxfId="16" priority="20">
+    <cfRule type="expression" dxfId="28" priority="32">
       <formula>CQ$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CQ6:CW7">
-    <cfRule type="expression" dxfId="15" priority="19">
+    <cfRule type="expression" dxfId="27" priority="31">
       <formula>CQ$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CX6:DD7">
-    <cfRule type="expression" dxfId="14" priority="18">
+    <cfRule type="expression" dxfId="26" priority="30">
       <formula>CX$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CX6:DD7">
-    <cfRule type="expression" dxfId="13" priority="17">
+    <cfRule type="expression" dxfId="25" priority="29">
       <formula>CX$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DE6:DK7">
-    <cfRule type="expression" dxfId="12" priority="16">
+    <cfRule type="expression" dxfId="24" priority="28">
       <formula>DE$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DE6:DK7">
-    <cfRule type="expression" dxfId="11" priority="15">
+    <cfRule type="expression" dxfId="23" priority="27">
       <formula>DE$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DL6:DR7">
-    <cfRule type="expression" dxfId="10" priority="14">
+    <cfRule type="expression" dxfId="22" priority="26">
       <formula>DL$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DL6:DR7">
-    <cfRule type="expression" dxfId="9" priority="13">
+    <cfRule type="expression" dxfId="21" priority="25">
       <formula>DL$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -9636,7 +10004,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -9650,33 +10018,33 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10:BN10">
-    <cfRule type="expression" dxfId="8" priority="11">
+    <cfRule type="expression" dxfId="20" priority="23">
       <formula>AND($E10&lt;=K$6,ROUNDDOWN(($F10-$E10+1)*$H10,0)+$E10-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="12">
+    <cfRule type="expression" dxfId="19" priority="24">
       <formula>AND(NOT(ISBLANK($E10)),$E10&lt;=K$6,$F10&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10:BN10">
-    <cfRule type="expression" dxfId="6" priority="10">
+    <cfRule type="expression" dxfId="18" priority="22">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:BN13">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="17" priority="19">
       <formula>AND($E13&lt;=K$6,ROUNDDOWN(($F13-$E13+1)*$H13,0)+$E13-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="16" priority="20">
       <formula>AND(NOT(ISBLANK($E13)),$E13&lt;=K$6,$F13&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:BN13">
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="15" priority="18">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -9690,14 +10058,95 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:BN15">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>AND($E15&lt;=K$6,ROUNDDOWN(($F15-$E15+1)*$H15,0)+$E15-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="13" priority="16">
       <formula>AND(NOT(ISBLANK($E15)),$E15&lt;=K$6,$F15&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:BN15">
+    <cfRule type="expression" dxfId="12" priority="14">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0F5B7656-4F83-4441-AC84-84F3141DCA60}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21:BN21">
+    <cfRule type="expression" dxfId="11" priority="11">
+      <formula>AND($E21&lt;=K$6,ROUNDDOWN(($F21-$E21+1)*$H21,0)+$E21-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="12">
+      <formula>AND(NOT(ISBLANK($E21)),$E21&lt;=K$6,$F21&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21:BN21">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{03ADCB47-F475-4C42-BCA7-F36BB5C4C1BA}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23:BN23">
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>AND($E23&lt;=K$6,ROUNDDOWN(($F23-$E23+1)*$H23,0)+$E23-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="8">
+      <formula>AND(NOT(ISBLANK($E23)),$E23&lt;=K$6,$F23&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23:BN23">
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A23A511D-2312-49ED-A413-04A22FC92768}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K24:BN24">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>AND($E24&lt;=K$6,ROUNDDOWN(($F24-$E24+1)*$H24,0)+$E24-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>AND(NOT(ISBLANK($E24)),$E24&lt;=K$6,$F24&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K24:BN24">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>K$6=TODAY()</formula>
     </cfRule>
@@ -9712,8 +10161,8 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 A45:B46 B40 B41:B43 A48:B48 B47 E17 E23 E39 E45:H48 G17:H17 G23:H23 G39:H43 G49 G50:G51 G52 H25:H27" unlockedFormula="1"/>
-    <ignoredError sqref="A39 A23 A17" formula="1"/>
+    <ignoredError sqref="H9 A48:B49 B43 B44:B46 A51:B51 B50 E17 E26 E42 E48:H51 G17:H17 G26:H26 G42:H46 G52 G53:G54 G55 H28:H30" unlockedFormula="1"/>
+    <ignoredError sqref="A42 A26 A17" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
@@ -9761,7 +10210,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H8:H9 H39:H52 H11:H12 H14 H16:H28</xm:sqref>
+          <xm:sqref>H8:H9 H42:H55 H11:H12 H14 H16:H20 H22 H25:H31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{FE744373-948F-4DF4-9B3E-95C2E34DC4FE}">
@@ -9776,7 +10225,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H29:H32</xm:sqref>
+          <xm:sqref>H32:H35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{D1031EA8-9A20-464F-8924-40F8769CD1E1}">
@@ -9791,7 +10240,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H33:H36</xm:sqref>
+          <xm:sqref>H36:H39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{5DB45CD5-8AFF-4405-9C9C-03F0C97B1A7F}">
@@ -9806,7 +10255,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H37:H38</xm:sqref>
+          <xm:sqref>H40:H41</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{8D6FF62A-898B-410F-8228-8CA900FC2DAE}">
@@ -9853,6 +10302,51 @@
           </x14:cfRule>
           <xm:sqref>H15</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0F5B7656-4F83-4441-AC84-84F3141DCA60}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H21</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{03ADCB47-F475-4C42-BCA7-F36BB5C4C1BA}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H23</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A23A511D-2312-49ED-A413-04A22FC92768}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H24</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -10119,10 +10613,10 @@
     </row>
     <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="172" t="s">
+      <c r="A13" s="174" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="172"/>
+      <c r="B13" s="174"/>
     </row>
     <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:3" s="134" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -10184,10 +10678,10 @@
       <c r="B23" s="10"/>
     </row>
     <row r="24" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="172" t="s">
+      <c r="A24" s="174" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="172"/>
+      <c r="B24" s="174"/>
     </row>
     <row r="25" spans="1:3" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A25" s="144"/>
@@ -10260,10 +10754,10 @@
       <c r="B37" s="10"/>
     </row>
     <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A38" s="172" t="s">
+      <c r="A38" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="172"/>
+      <c r="B38" s="174"/>
     </row>
     <row r="39" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B39" s="141" t="s">
@@ -10300,10 +10794,10 @@
       <c r="B48" s="11"/>
     </row>
     <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A49" s="172" t="s">
+      <c r="A49" s="174" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="172"/>
+      <c r="B49" s="174"/>
     </row>
     <row r="50" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B50" s="141" t="s">
@@ -10401,10 +10895,10 @@
       <c r="B64" s="12"/>
     </row>
     <row r="65" spans="1:2" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A65" s="172" t="s">
+      <c r="A65" s="174" t="s">
         <v>10</v>
       </c>
-      <c r="B65" s="172"/>
+      <c r="B65" s="174"/>
     </row>
     <row r="66" spans="1:2" s="20" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B66" s="141" t="s">
@@ -10415,10 +10909,10 @@
       <c r="B67" s="13"/>
     </row>
     <row r="68" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A68" s="172" t="s">
+      <c r="A68" s="174" t="s">
         <v>5</v>
       </c>
-      <c r="B68" s="172"/>
+      <c r="B68" s="174"/>
     </row>
     <row r="69" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="156" t="s">

</xml_diff>

<commit_message>
Added Archive for mode 2->3 demo
</commit_message>
<xml_diff>
--- a/Gantt_Diagram_Robot_Project_2018.xlsx
+++ b/Gantt_Diagram_Robot_Project_2018.xlsx
@@ -3011,6 +3011,24 @@
     <xf numFmtId="0" fontId="42" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3018,27 +3036,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3090,33 +3090,7 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="44">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="41">
     <dxf>
       <border>
         <left style="thin">
@@ -3609,7 +3583,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="8"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="5"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4269,7 +4243,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="BH22" sqref="BH22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4346,29 +4320,29 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
       <c r="I1" s="132"/>
-      <c r="K1" s="165" t="s">
+      <c r="K1" s="171" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="165"/>
-      <c r="M1" s="165"/>
-      <c r="N1" s="165"/>
-      <c r="O1" s="165"/>
-      <c r="P1" s="165"/>
-      <c r="Q1" s="165"/>
-      <c r="R1" s="165"/>
-      <c r="S1" s="165"/>
-      <c r="T1" s="165"/>
-      <c r="U1" s="165"/>
-      <c r="V1" s="165"/>
-      <c r="W1" s="165"/>
-      <c r="X1" s="165"/>
-      <c r="Y1" s="165"/>
-      <c r="Z1" s="165"/>
-      <c r="AA1" s="165"/>
-      <c r="AB1" s="165"/>
-      <c r="AC1" s="165"/>
-      <c r="AD1" s="165"/>
-      <c r="AE1" s="165"/>
+      <c r="L1" s="171"/>
+      <c r="M1" s="171"/>
+      <c r="N1" s="171"/>
+      <c r="O1" s="171"/>
+      <c r="P1" s="171"/>
+      <c r="Q1" s="171"/>
+      <c r="R1" s="171"/>
+      <c r="S1" s="171"/>
+      <c r="T1" s="171"/>
+      <c r="U1" s="171"/>
+      <c r="V1" s="171"/>
+      <c r="W1" s="171"/>
+      <c r="X1" s="171"/>
+      <c r="Y1" s="171"/>
+      <c r="Z1" s="171"/>
+      <c r="AA1" s="171"/>
+      <c r="AB1" s="171"/>
+      <c r="AC1" s="171"/>
+      <c r="AD1" s="171"/>
+      <c r="AE1" s="171"/>
     </row>
     <row r="2" spans="1:122" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
@@ -4413,356 +4387,356 @@
       <c r="B4" s="114" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="170">
+      <c r="C4" s="173">
         <v>43340</v>
       </c>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="173"/>
       <c r="F4" s="111"/>
       <c r="G4" s="114" t="s">
         <v>75</v>
       </c>
       <c r="H4" s="129">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I4" s="112"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="167" t="str">
+      <c r="K4" s="165" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 5</v>
+      </c>
+      <c r="L4" s="166"/>
+      <c r="M4" s="166"/>
+      <c r="N4" s="166"/>
+      <c r="O4" s="166"/>
+      <c r="P4" s="166"/>
+      <c r="Q4" s="167"/>
+      <c r="R4" s="165" t="str">
+        <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 6</v>
+      </c>
+      <c r="S4" s="166"/>
+      <c r="T4" s="166"/>
+      <c r="U4" s="166"/>
+      <c r="V4" s="166"/>
+      <c r="W4" s="166"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="165" t="str">
+        <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 7</v>
+      </c>
+      <c r="Z4" s="166"/>
+      <c r="AA4" s="166"/>
+      <c r="AB4" s="166"/>
+      <c r="AC4" s="166"/>
+      <c r="AD4" s="166"/>
+      <c r="AE4" s="167"/>
+      <c r="AF4" s="165" t="str">
+        <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="L4" s="168"/>
-      <c r="M4" s="168"/>
-      <c r="N4" s="168"/>
-      <c r="O4" s="168"/>
-      <c r="P4" s="168"/>
-      <c r="Q4" s="169"/>
-      <c r="R4" s="167" t="str">
-        <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AG4" s="166"/>
+      <c r="AH4" s="166"/>
+      <c r="AI4" s="166"/>
+      <c r="AJ4" s="166"/>
+      <c r="AK4" s="166"/>
+      <c r="AL4" s="167"/>
+      <c r="AM4" s="165" t="str">
+        <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="S4" s="168"/>
-      <c r="T4" s="168"/>
-      <c r="U4" s="168"/>
-      <c r="V4" s="168"/>
-      <c r="W4" s="168"/>
-      <c r="X4" s="169"/>
-      <c r="Y4" s="167" t="str">
-        <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AN4" s="166"/>
+      <c r="AO4" s="166"/>
+      <c r="AP4" s="166"/>
+      <c r="AQ4" s="166"/>
+      <c r="AR4" s="166"/>
+      <c r="AS4" s="167"/>
+      <c r="AT4" s="165" t="str">
+        <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="Z4" s="168"/>
-      <c r="AA4" s="168"/>
-      <c r="AB4" s="168"/>
-      <c r="AC4" s="168"/>
-      <c r="AD4" s="168"/>
-      <c r="AE4" s="169"/>
-      <c r="AF4" s="167" t="str">
-        <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AU4" s="166"/>
+      <c r="AV4" s="166"/>
+      <c r="AW4" s="166"/>
+      <c r="AX4" s="166"/>
+      <c r="AY4" s="166"/>
+      <c r="AZ4" s="167"/>
+      <c r="BA4" s="165" t="str">
+        <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="AG4" s="168"/>
-      <c r="AH4" s="168"/>
-      <c r="AI4" s="168"/>
-      <c r="AJ4" s="168"/>
-      <c r="AK4" s="168"/>
-      <c r="AL4" s="169"/>
-      <c r="AM4" s="167" t="str">
-        <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="BB4" s="166"/>
+      <c r="BC4" s="166"/>
+      <c r="BD4" s="166"/>
+      <c r="BE4" s="166"/>
+      <c r="BF4" s="166"/>
+      <c r="BG4" s="167"/>
+      <c r="BH4" s="165" t="str">
+        <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="AN4" s="168"/>
-      <c r="AO4" s="168"/>
-      <c r="AP4" s="168"/>
-      <c r="AQ4" s="168"/>
-      <c r="AR4" s="168"/>
-      <c r="AS4" s="169"/>
-      <c r="AT4" s="167" t="str">
-        <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="BI4" s="166"/>
+      <c r="BJ4" s="166"/>
+      <c r="BK4" s="166"/>
+      <c r="BL4" s="166"/>
+      <c r="BM4" s="166"/>
+      <c r="BN4" s="167"/>
+      <c r="BO4" s="165" t="str">
+        <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 13</v>
       </c>
-      <c r="AU4" s="168"/>
-      <c r="AV4" s="168"/>
-      <c r="AW4" s="168"/>
-      <c r="AX4" s="168"/>
-      <c r="AY4" s="168"/>
-      <c r="AZ4" s="169"/>
-      <c r="BA4" s="167" t="str">
-        <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="BP4" s="166"/>
+      <c r="BQ4" s="166"/>
+      <c r="BR4" s="166"/>
+      <c r="BS4" s="166"/>
+      <c r="BT4" s="166"/>
+      <c r="BU4" s="167"/>
+      <c r="BV4" s="165" t="str">
+        <f>"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 14</v>
       </c>
-      <c r="BB4" s="168"/>
-      <c r="BC4" s="168"/>
-      <c r="BD4" s="168"/>
-      <c r="BE4" s="168"/>
-      <c r="BF4" s="168"/>
-      <c r="BG4" s="169"/>
-      <c r="BH4" s="167" t="str">
-        <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="BW4" s="166"/>
+      <c r="BX4" s="166"/>
+      <c r="BY4" s="166"/>
+      <c r="BZ4" s="166"/>
+      <c r="CA4" s="166"/>
+      <c r="CB4" s="167"/>
+      <c r="CC4" s="165" t="str">
+        <f>"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 15</v>
       </c>
-      <c r="BI4" s="168"/>
-      <c r="BJ4" s="168"/>
-      <c r="BK4" s="168"/>
-      <c r="BL4" s="168"/>
-      <c r="BM4" s="168"/>
-      <c r="BN4" s="169"/>
-      <c r="BO4" s="167" t="str">
-        <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="CD4" s="166"/>
+      <c r="CE4" s="166"/>
+      <c r="CF4" s="166"/>
+      <c r="CG4" s="166"/>
+      <c r="CH4" s="166"/>
+      <c r="CI4" s="167"/>
+      <c r="CJ4" s="165" t="str">
+        <f>"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 16</v>
       </c>
-      <c r="BP4" s="168"/>
-      <c r="BQ4" s="168"/>
-      <c r="BR4" s="168"/>
-      <c r="BS4" s="168"/>
-      <c r="BT4" s="168"/>
-      <c r="BU4" s="169"/>
-      <c r="BV4" s="167" t="str">
-        <f>"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="CK4" s="166"/>
+      <c r="CL4" s="166"/>
+      <c r="CM4" s="166"/>
+      <c r="CN4" s="166"/>
+      <c r="CO4" s="166"/>
+      <c r="CP4" s="167"/>
+      <c r="CQ4" s="165" t="str">
+        <f>"Week "&amp;(CQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 17</v>
       </c>
-      <c r="BW4" s="168"/>
-      <c r="BX4" s="168"/>
-      <c r="BY4" s="168"/>
-      <c r="BZ4" s="168"/>
-      <c r="CA4" s="168"/>
-      <c r="CB4" s="169"/>
-      <c r="CC4" s="167" t="str">
-        <f>"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="CR4" s="166"/>
+      <c r="CS4" s="166"/>
+      <c r="CT4" s="166"/>
+      <c r="CU4" s="166"/>
+      <c r="CV4" s="166"/>
+      <c r="CW4" s="167"/>
+      <c r="CX4" s="165" t="str">
+        <f>"Week "&amp;(CX6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 18</v>
       </c>
-      <c r="CD4" s="168"/>
-      <c r="CE4" s="168"/>
-      <c r="CF4" s="168"/>
-      <c r="CG4" s="168"/>
-      <c r="CH4" s="168"/>
-      <c r="CI4" s="169"/>
-      <c r="CJ4" s="167" t="str">
-        <f>"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="CY4" s="166"/>
+      <c r="CZ4" s="166"/>
+      <c r="DA4" s="166"/>
+      <c r="DB4" s="166"/>
+      <c r="DC4" s="166"/>
+      <c r="DD4" s="167"/>
+      <c r="DE4" s="165" t="str">
+        <f>"Week "&amp;(DE6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 19</v>
       </c>
-      <c r="CK4" s="168"/>
-      <c r="CL4" s="168"/>
-      <c r="CM4" s="168"/>
-      <c r="CN4" s="168"/>
-      <c r="CO4" s="168"/>
-      <c r="CP4" s="169"/>
-      <c r="CQ4" s="167" t="str">
-        <f>"Week "&amp;(CQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="DF4" s="166"/>
+      <c r="DG4" s="166"/>
+      <c r="DH4" s="166"/>
+      <c r="DI4" s="166"/>
+      <c r="DJ4" s="166"/>
+      <c r="DK4" s="167"/>
+      <c r="DL4" s="165" t="str">
+        <f>"Week "&amp;(DL6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="CR4" s="168"/>
-      <c r="CS4" s="168"/>
-      <c r="CT4" s="168"/>
-      <c r="CU4" s="168"/>
-      <c r="CV4" s="168"/>
-      <c r="CW4" s="169"/>
-      <c r="CX4" s="167" t="str">
-        <f>"Week "&amp;(CX6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 21</v>
-      </c>
-      <c r="CY4" s="168"/>
-      <c r="CZ4" s="168"/>
-      <c r="DA4" s="168"/>
-      <c r="DB4" s="168"/>
-      <c r="DC4" s="168"/>
-      <c r="DD4" s="169"/>
-      <c r="DE4" s="167" t="str">
-        <f>"Week "&amp;(DE6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 22</v>
-      </c>
-      <c r="DF4" s="168"/>
-      <c r="DG4" s="168"/>
-      <c r="DH4" s="168"/>
-      <c r="DI4" s="168"/>
-      <c r="DJ4" s="168"/>
-      <c r="DK4" s="169"/>
-      <c r="DL4" s="167" t="str">
-        <f>"Week "&amp;(DL6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 23</v>
-      </c>
-      <c r="DM4" s="168"/>
-      <c r="DN4" s="168"/>
-      <c r="DO4" s="168"/>
-      <c r="DP4" s="168"/>
-      <c r="DQ4" s="168"/>
-      <c r="DR4" s="169"/>
+      <c r="DM4" s="166"/>
+      <c r="DN4" s="166"/>
+      <c r="DO4" s="166"/>
+      <c r="DP4" s="166"/>
+      <c r="DQ4" s="166"/>
+      <c r="DR4" s="167"/>
     </row>
     <row r="5" spans="1:122" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="110"/>
       <c r="B5" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="166" t="s">
+      <c r="C5" s="172" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="166"/>
-      <c r="E5" s="166"/>
+      <c r="D5" s="172"/>
+      <c r="E5" s="172"/>
       <c r="F5" s="113"/>
       <c r="G5" s="113"/>
       <c r="H5" s="113"/>
       <c r="I5" s="113"/>
       <c r="J5" s="50"/>
-      <c r="K5" s="171">
+      <c r="K5" s="168">
         <f>K6</f>
+        <v>43367</v>
+      </c>
+      <c r="L5" s="169"/>
+      <c r="M5" s="169"/>
+      <c r="N5" s="169"/>
+      <c r="O5" s="169"/>
+      <c r="P5" s="169"/>
+      <c r="Q5" s="170"/>
+      <c r="R5" s="168">
+        <f>R6</f>
+        <v>43374</v>
+      </c>
+      <c r="S5" s="169"/>
+      <c r="T5" s="169"/>
+      <c r="U5" s="169"/>
+      <c r="V5" s="169"/>
+      <c r="W5" s="169"/>
+      <c r="X5" s="170"/>
+      <c r="Y5" s="168">
+        <f>Y6</f>
+        <v>43381</v>
+      </c>
+      <c r="Z5" s="169"/>
+      <c r="AA5" s="169"/>
+      <c r="AB5" s="169"/>
+      <c r="AC5" s="169"/>
+      <c r="AD5" s="169"/>
+      <c r="AE5" s="170"/>
+      <c r="AF5" s="168">
+        <f>AF6</f>
         <v>43388</v>
       </c>
-      <c r="L5" s="172"/>
-      <c r="M5" s="172"/>
-      <c r="N5" s="172"/>
-      <c r="O5" s="172"/>
-      <c r="P5" s="172"/>
-      <c r="Q5" s="173"/>
-      <c r="R5" s="171">
-        <f>R6</f>
+      <c r="AG5" s="169"/>
+      <c r="AH5" s="169"/>
+      <c r="AI5" s="169"/>
+      <c r="AJ5" s="169"/>
+      <c r="AK5" s="169"/>
+      <c r="AL5" s="170"/>
+      <c r="AM5" s="168">
+        <f>AM6</f>
         <v>43395</v>
       </c>
-      <c r="S5" s="172"/>
-      <c r="T5" s="172"/>
-      <c r="U5" s="172"/>
-      <c r="V5" s="172"/>
-      <c r="W5" s="172"/>
-      <c r="X5" s="173"/>
-      <c r="Y5" s="171">
-        <f>Y6</f>
+      <c r="AN5" s="169"/>
+      <c r="AO5" s="169"/>
+      <c r="AP5" s="169"/>
+      <c r="AQ5" s="169"/>
+      <c r="AR5" s="169"/>
+      <c r="AS5" s="170"/>
+      <c r="AT5" s="168">
+        <f>AT6</f>
         <v>43402</v>
       </c>
-      <c r="Z5" s="172"/>
-      <c r="AA5" s="172"/>
-      <c r="AB5" s="172"/>
-      <c r="AC5" s="172"/>
-      <c r="AD5" s="172"/>
-      <c r="AE5" s="173"/>
-      <c r="AF5" s="171">
-        <f>AF6</f>
+      <c r="AU5" s="169"/>
+      <c r="AV5" s="169"/>
+      <c r="AW5" s="169"/>
+      <c r="AX5" s="169"/>
+      <c r="AY5" s="169"/>
+      <c r="AZ5" s="170"/>
+      <c r="BA5" s="168">
+        <f>BA6</f>
         <v>43409</v>
       </c>
-      <c r="AG5" s="172"/>
-      <c r="AH5" s="172"/>
-      <c r="AI5" s="172"/>
-      <c r="AJ5" s="172"/>
-      <c r="AK5" s="172"/>
-      <c r="AL5" s="173"/>
-      <c r="AM5" s="171">
-        <f>AM6</f>
+      <c r="BB5" s="169"/>
+      <c r="BC5" s="169"/>
+      <c r="BD5" s="169"/>
+      <c r="BE5" s="169"/>
+      <c r="BF5" s="169"/>
+      <c r="BG5" s="170"/>
+      <c r="BH5" s="168">
+        <f>BH6</f>
         <v>43416</v>
       </c>
-      <c r="AN5" s="172"/>
-      <c r="AO5" s="172"/>
-      <c r="AP5" s="172"/>
-      <c r="AQ5" s="172"/>
-      <c r="AR5" s="172"/>
-      <c r="AS5" s="173"/>
-      <c r="AT5" s="171">
-        <f>AT6</f>
+      <c r="BI5" s="169"/>
+      <c r="BJ5" s="169"/>
+      <c r="BK5" s="169"/>
+      <c r="BL5" s="169"/>
+      <c r="BM5" s="169"/>
+      <c r="BN5" s="170"/>
+      <c r="BO5" s="168">
+        <f>BO6</f>
         <v>43423</v>
       </c>
-      <c r="AU5" s="172"/>
-      <c r="AV5" s="172"/>
-      <c r="AW5" s="172"/>
-      <c r="AX5" s="172"/>
-      <c r="AY5" s="172"/>
-      <c r="AZ5" s="173"/>
-      <c r="BA5" s="171">
-        <f>BA6</f>
+      <c r="BP5" s="169"/>
+      <c r="BQ5" s="169"/>
+      <c r="BR5" s="169"/>
+      <c r="BS5" s="169"/>
+      <c r="BT5" s="169"/>
+      <c r="BU5" s="170"/>
+      <c r="BV5" s="168">
+        <f>BV6</f>
         <v>43430</v>
       </c>
-      <c r="BB5" s="172"/>
-      <c r="BC5" s="172"/>
-      <c r="BD5" s="172"/>
-      <c r="BE5" s="172"/>
-      <c r="BF5" s="172"/>
-      <c r="BG5" s="173"/>
-      <c r="BH5" s="171">
-        <f>BH6</f>
+      <c r="BW5" s="169"/>
+      <c r="BX5" s="169"/>
+      <c r="BY5" s="169"/>
+      <c r="BZ5" s="169"/>
+      <c r="CA5" s="169"/>
+      <c r="CB5" s="170"/>
+      <c r="CC5" s="168">
+        <f>CC6</f>
         <v>43437</v>
       </c>
-      <c r="BI5" s="172"/>
-      <c r="BJ5" s="172"/>
-      <c r="BK5" s="172"/>
-      <c r="BL5" s="172"/>
-      <c r="BM5" s="172"/>
-      <c r="BN5" s="173"/>
-      <c r="BO5" s="171">
-        <f>BO6</f>
+      <c r="CD5" s="169"/>
+      <c r="CE5" s="169"/>
+      <c r="CF5" s="169"/>
+      <c r="CG5" s="169"/>
+      <c r="CH5" s="169"/>
+      <c r="CI5" s="170"/>
+      <c r="CJ5" s="168">
+        <f>CJ6</f>
         <v>43444</v>
       </c>
-      <c r="BP5" s="172"/>
-      <c r="BQ5" s="172"/>
-      <c r="BR5" s="172"/>
-      <c r="BS5" s="172"/>
-      <c r="BT5" s="172"/>
-      <c r="BU5" s="173"/>
-      <c r="BV5" s="171">
-        <f>BV6</f>
+      <c r="CK5" s="169"/>
+      <c r="CL5" s="169"/>
+      <c r="CM5" s="169"/>
+      <c r="CN5" s="169"/>
+      <c r="CO5" s="169"/>
+      <c r="CP5" s="170"/>
+      <c r="CQ5" s="168">
+        <f>CQ6</f>
         <v>43451</v>
       </c>
-      <c r="BW5" s="172"/>
-      <c r="BX5" s="172"/>
-      <c r="BY5" s="172"/>
-      <c r="BZ5" s="172"/>
-      <c r="CA5" s="172"/>
-      <c r="CB5" s="173"/>
-      <c r="CC5" s="171">
-        <f>CC6</f>
+      <c r="CR5" s="169"/>
+      <c r="CS5" s="169"/>
+      <c r="CT5" s="169"/>
+      <c r="CU5" s="169"/>
+      <c r="CV5" s="169"/>
+      <c r="CW5" s="170"/>
+      <c r="CX5" s="168">
+        <f>CX6</f>
         <v>43458</v>
       </c>
-      <c r="CD5" s="172"/>
-      <c r="CE5" s="172"/>
-      <c r="CF5" s="172"/>
-      <c r="CG5" s="172"/>
-      <c r="CH5" s="172"/>
-      <c r="CI5" s="173"/>
-      <c r="CJ5" s="171">
-        <f>CJ6</f>
+      <c r="CY5" s="169"/>
+      <c r="CZ5" s="169"/>
+      <c r="DA5" s="169"/>
+      <c r="DB5" s="169"/>
+      <c r="DC5" s="169"/>
+      <c r="DD5" s="170"/>
+      <c r="DE5" s="168">
+        <f>DE6</f>
         <v>43465</v>
       </c>
-      <c r="CK5" s="172"/>
-      <c r="CL5" s="172"/>
-      <c r="CM5" s="172"/>
-      <c r="CN5" s="172"/>
-      <c r="CO5" s="172"/>
-      <c r="CP5" s="173"/>
-      <c r="CQ5" s="171">
-        <f>CQ6</f>
+      <c r="DF5" s="169"/>
+      <c r="DG5" s="169"/>
+      <c r="DH5" s="169"/>
+      <c r="DI5" s="169"/>
+      <c r="DJ5" s="169"/>
+      <c r="DK5" s="170"/>
+      <c r="DL5" s="168">
+        <f>DL6</f>
         <v>43472</v>
       </c>
-      <c r="CR5" s="172"/>
-      <c r="CS5" s="172"/>
-      <c r="CT5" s="172"/>
-      <c r="CU5" s="172"/>
-      <c r="CV5" s="172"/>
-      <c r="CW5" s="173"/>
-      <c r="CX5" s="171">
-        <f>CX6</f>
-        <v>43479</v>
-      </c>
-      <c r="CY5" s="172"/>
-      <c r="CZ5" s="172"/>
-      <c r="DA5" s="172"/>
-      <c r="DB5" s="172"/>
-      <c r="DC5" s="172"/>
-      <c r="DD5" s="173"/>
-      <c r="DE5" s="171">
-        <f>DE6</f>
-        <v>43486</v>
-      </c>
-      <c r="DF5" s="172"/>
-      <c r="DG5" s="172"/>
-      <c r="DH5" s="172"/>
-      <c r="DI5" s="172"/>
-      <c r="DJ5" s="172"/>
-      <c r="DK5" s="173"/>
-      <c r="DL5" s="171">
-        <f>DL6</f>
-        <v>43493</v>
-      </c>
-      <c r="DM5" s="172"/>
-      <c r="DN5" s="172"/>
-      <c r="DO5" s="172"/>
-      <c r="DP5" s="172"/>
-      <c r="DQ5" s="172"/>
-      <c r="DR5" s="173"/>
+      <c r="DM5" s="169"/>
+      <c r="DN5" s="169"/>
+      <c r="DO5" s="169"/>
+      <c r="DP5" s="169"/>
+      <c r="DQ5" s="169"/>
+      <c r="DR5" s="170"/>
     </row>
     <row r="6" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A6" s="49"/>
@@ -4777,451 +4751,451 @@
       <c r="J6" s="50"/>
       <c r="K6" s="92">
         <f>C4-WEEKDAY(C4,1)+2+7*(H4-1)</f>
-        <v>43388</v>
+        <v>43367</v>
       </c>
       <c r="L6" s="83">
         <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
-        <v>43389</v>
+        <v>43368</v>
       </c>
       <c r="M6" s="83">
         <f t="shared" si="0"/>
-        <v>43390</v>
+        <v>43369</v>
       </c>
       <c r="N6" s="83">
         <f t="shared" si="0"/>
-        <v>43391</v>
+        <v>43370</v>
       </c>
       <c r="O6" s="83">
         <f t="shared" si="0"/>
-        <v>43392</v>
+        <v>43371</v>
       </c>
       <c r="P6" s="83">
         <f t="shared" si="0"/>
-        <v>43393</v>
+        <v>43372</v>
       </c>
       <c r="Q6" s="93">
         <f t="shared" si="0"/>
-        <v>43394</v>
+        <v>43373</v>
       </c>
       <c r="R6" s="92">
         <f t="shared" si="0"/>
-        <v>43395</v>
+        <v>43374</v>
       </c>
       <c r="S6" s="83">
         <f t="shared" si="0"/>
-        <v>43396</v>
+        <v>43375</v>
       </c>
       <c r="T6" s="83">
         <f t="shared" si="0"/>
-        <v>43397</v>
+        <v>43376</v>
       </c>
       <c r="U6" s="83">
         <f t="shared" si="0"/>
-        <v>43398</v>
+        <v>43377</v>
       </c>
       <c r="V6" s="83">
         <f t="shared" si="0"/>
-        <v>43399</v>
+        <v>43378</v>
       </c>
       <c r="W6" s="83">
         <f t="shared" si="0"/>
-        <v>43400</v>
+        <v>43379</v>
       </c>
       <c r="X6" s="93">
         <f t="shared" si="0"/>
-        <v>43401</v>
+        <v>43380</v>
       </c>
       <c r="Y6" s="92">
         <f t="shared" si="0"/>
-        <v>43402</v>
+        <v>43381</v>
       </c>
       <c r="Z6" s="83">
         <f t="shared" si="0"/>
-        <v>43403</v>
+        <v>43382</v>
       </c>
       <c r="AA6" s="83">
         <f t="shared" si="0"/>
-        <v>43404</v>
+        <v>43383</v>
       </c>
       <c r="AB6" s="83">
         <f t="shared" si="0"/>
-        <v>43405</v>
+        <v>43384</v>
       </c>
       <c r="AC6" s="83">
         <f t="shared" si="0"/>
-        <v>43406</v>
+        <v>43385</v>
       </c>
       <c r="AD6" s="83">
         <f t="shared" si="0"/>
-        <v>43407</v>
+        <v>43386</v>
       </c>
       <c r="AE6" s="93">
         <f t="shared" si="0"/>
-        <v>43408</v>
+        <v>43387</v>
       </c>
       <c r="AF6" s="92">
         <f t="shared" si="0"/>
-        <v>43409</v>
+        <v>43388</v>
       </c>
       <c r="AG6" s="83">
         <f t="shared" si="0"/>
-        <v>43410</v>
+        <v>43389</v>
       </c>
       <c r="AH6" s="83">
         <f t="shared" si="0"/>
-        <v>43411</v>
+        <v>43390</v>
       </c>
       <c r="AI6" s="83">
         <f t="shared" si="0"/>
-        <v>43412</v>
+        <v>43391</v>
       </c>
       <c r="AJ6" s="83">
         <f t="shared" si="0"/>
-        <v>43413</v>
+        <v>43392</v>
       </c>
       <c r="AK6" s="83">
         <f t="shared" si="0"/>
-        <v>43414</v>
+        <v>43393</v>
       </c>
       <c r="AL6" s="93">
         <f t="shared" si="0"/>
-        <v>43415</v>
+        <v>43394</v>
       </c>
       <c r="AM6" s="92">
         <f t="shared" si="0"/>
-        <v>43416</v>
+        <v>43395</v>
       </c>
       <c r="AN6" s="83">
         <f t="shared" si="0"/>
-        <v>43417</v>
+        <v>43396</v>
       </c>
       <c r="AO6" s="83">
         <f t="shared" si="0"/>
-        <v>43418</v>
+        <v>43397</v>
       </c>
       <c r="AP6" s="83">
         <f t="shared" si="0"/>
-        <v>43419</v>
+        <v>43398</v>
       </c>
       <c r="AQ6" s="83">
         <f t="shared" si="0"/>
-        <v>43420</v>
+        <v>43399</v>
       </c>
       <c r="AR6" s="83">
         <f t="shared" ref="AR6:BN6" si="1">AQ6+1</f>
-        <v>43421</v>
+        <v>43400</v>
       </c>
       <c r="AS6" s="93">
         <f t="shared" si="1"/>
-        <v>43422</v>
+        <v>43401</v>
       </c>
       <c r="AT6" s="92">
         <f t="shared" si="1"/>
-        <v>43423</v>
+        <v>43402</v>
       </c>
       <c r="AU6" s="83">
         <f t="shared" si="1"/>
-        <v>43424</v>
+        <v>43403</v>
       </c>
       <c r="AV6" s="83">
         <f t="shared" si="1"/>
-        <v>43425</v>
+        <v>43404</v>
       </c>
       <c r="AW6" s="83">
         <f t="shared" si="1"/>
-        <v>43426</v>
+        <v>43405</v>
       </c>
       <c r="AX6" s="83">
         <f t="shared" si="1"/>
-        <v>43427</v>
+        <v>43406</v>
       </c>
       <c r="AY6" s="83">
         <f t="shared" si="1"/>
-        <v>43428</v>
+        <v>43407</v>
       </c>
       <c r="AZ6" s="93">
         <f t="shared" si="1"/>
-        <v>43429</v>
+        <v>43408</v>
       </c>
       <c r="BA6" s="92">
         <f t="shared" si="1"/>
-        <v>43430</v>
+        <v>43409</v>
       </c>
       <c r="BB6" s="83">
         <f t="shared" si="1"/>
-        <v>43431</v>
+        <v>43410</v>
       </c>
       <c r="BC6" s="83">
         <f t="shared" si="1"/>
-        <v>43432</v>
+        <v>43411</v>
       </c>
       <c r="BD6" s="83">
         <f t="shared" si="1"/>
-        <v>43433</v>
+        <v>43412</v>
       </c>
       <c r="BE6" s="83">
         <f t="shared" si="1"/>
-        <v>43434</v>
+        <v>43413</v>
       </c>
       <c r="BF6" s="83">
         <f t="shared" si="1"/>
-        <v>43435</v>
+        <v>43414</v>
       </c>
       <c r="BG6" s="93">
         <f t="shared" si="1"/>
-        <v>43436</v>
+        <v>43415</v>
       </c>
       <c r="BH6" s="92">
         <f t="shared" si="1"/>
-        <v>43437</v>
+        <v>43416</v>
       </c>
       <c r="BI6" s="83">
         <f t="shared" si="1"/>
-        <v>43438</v>
+        <v>43417</v>
       </c>
       <c r="BJ6" s="83">
         <f t="shared" si="1"/>
-        <v>43439</v>
+        <v>43418</v>
       </c>
       <c r="BK6" s="83">
         <f t="shared" si="1"/>
-        <v>43440</v>
+        <v>43419</v>
       </c>
       <c r="BL6" s="83">
         <f t="shared" si="1"/>
-        <v>43441</v>
+        <v>43420</v>
       </c>
       <c r="BM6" s="83">
         <f t="shared" si="1"/>
-        <v>43442</v>
+        <v>43421</v>
       </c>
       <c r="BN6" s="93">
         <f t="shared" si="1"/>
-        <v>43443</v>
+        <v>43422</v>
       </c>
       <c r="BO6" s="92">
         <f t="shared" ref="BO6" si="2">BN6+1</f>
-        <v>43444</v>
+        <v>43423</v>
       </c>
       <c r="BP6" s="83">
         <f t="shared" ref="BP6" si="3">BO6+1</f>
-        <v>43445</v>
+        <v>43424</v>
       </c>
       <c r="BQ6" s="83">
         <f t="shared" ref="BQ6" si="4">BP6+1</f>
-        <v>43446</v>
+        <v>43425</v>
       </c>
       <c r="BR6" s="83">
         <f t="shared" ref="BR6" si="5">BQ6+1</f>
-        <v>43447</v>
+        <v>43426</v>
       </c>
       <c r="BS6" s="83">
         <f t="shared" ref="BS6" si="6">BR6+1</f>
-        <v>43448</v>
+        <v>43427</v>
       </c>
       <c r="BT6" s="83">
         <f t="shared" ref="BT6" si="7">BS6+1</f>
-        <v>43449</v>
+        <v>43428</v>
       </c>
       <c r="BU6" s="93">
         <f t="shared" ref="BU6" si="8">BT6+1</f>
-        <v>43450</v>
+        <v>43429</v>
       </c>
       <c r="BV6" s="92">
         <f t="shared" ref="BV6" si="9">BU6+1</f>
-        <v>43451</v>
+        <v>43430</v>
       </c>
       <c r="BW6" s="83">
         <f t="shared" ref="BW6" si="10">BV6+1</f>
-        <v>43452</v>
+        <v>43431</v>
       </c>
       <c r="BX6" s="83">
         <f t="shared" ref="BX6" si="11">BW6+1</f>
-        <v>43453</v>
+        <v>43432</v>
       </c>
       <c r="BY6" s="83">
         <f t="shared" ref="BY6" si="12">BX6+1</f>
-        <v>43454</v>
+        <v>43433</v>
       </c>
       <c r="BZ6" s="83">
         <f t="shared" ref="BZ6" si="13">BY6+1</f>
-        <v>43455</v>
+        <v>43434</v>
       </c>
       <c r="CA6" s="83">
         <f t="shared" ref="CA6" si="14">BZ6+1</f>
-        <v>43456</v>
+        <v>43435</v>
       </c>
       <c r="CB6" s="93">
         <f t="shared" ref="CB6" si="15">CA6+1</f>
-        <v>43457</v>
+        <v>43436</v>
       </c>
       <c r="CC6" s="92">
         <f t="shared" ref="CC6" si="16">CB6+1</f>
-        <v>43458</v>
+        <v>43437</v>
       </c>
       <c r="CD6" s="83">
         <f t="shared" ref="CD6" si="17">CC6+1</f>
-        <v>43459</v>
+        <v>43438</v>
       </c>
       <c r="CE6" s="83">
         <f t="shared" ref="CE6" si="18">CD6+1</f>
-        <v>43460</v>
+        <v>43439</v>
       </c>
       <c r="CF6" s="83">
         <f t="shared" ref="CF6" si="19">CE6+1</f>
-        <v>43461</v>
+        <v>43440</v>
       </c>
       <c r="CG6" s="83">
         <f t="shared" ref="CG6" si="20">CF6+1</f>
-        <v>43462</v>
+        <v>43441</v>
       </c>
       <c r="CH6" s="83">
         <f t="shared" ref="CH6" si="21">CG6+1</f>
-        <v>43463</v>
+        <v>43442</v>
       </c>
       <c r="CI6" s="93">
         <f t="shared" ref="CI6" si="22">CH6+1</f>
-        <v>43464</v>
+        <v>43443</v>
       </c>
       <c r="CJ6" s="92">
         <f t="shared" ref="CJ6" si="23">CI6+1</f>
-        <v>43465</v>
+        <v>43444</v>
       </c>
       <c r="CK6" s="83">
         <f t="shared" ref="CK6" si="24">CJ6+1</f>
-        <v>43466</v>
+        <v>43445</v>
       </c>
       <c r="CL6" s="83">
         <f t="shared" ref="CL6" si="25">CK6+1</f>
-        <v>43467</v>
+        <v>43446</v>
       </c>
       <c r="CM6" s="83">
         <f t="shared" ref="CM6" si="26">CL6+1</f>
-        <v>43468</v>
+        <v>43447</v>
       </c>
       <c r="CN6" s="83">
         <f t="shared" ref="CN6" si="27">CM6+1</f>
-        <v>43469</v>
+        <v>43448</v>
       </c>
       <c r="CO6" s="83">
         <f t="shared" ref="CO6" si="28">CN6+1</f>
-        <v>43470</v>
+        <v>43449</v>
       </c>
       <c r="CP6" s="93">
         <f t="shared" ref="CP6" si="29">CO6+1</f>
-        <v>43471</v>
+        <v>43450</v>
       </c>
       <c r="CQ6" s="92">
         <f t="shared" ref="CQ6" si="30">CP6+1</f>
-        <v>43472</v>
+        <v>43451</v>
       </c>
       <c r="CR6" s="83">
         <f t="shared" ref="CR6" si="31">CQ6+1</f>
-        <v>43473</v>
+        <v>43452</v>
       </c>
       <c r="CS6" s="83">
         <f t="shared" ref="CS6" si="32">CR6+1</f>
-        <v>43474</v>
+        <v>43453</v>
       </c>
       <c r="CT6" s="83">
         <f t="shared" ref="CT6" si="33">CS6+1</f>
-        <v>43475</v>
+        <v>43454</v>
       </c>
       <c r="CU6" s="83">
         <f t="shared" ref="CU6" si="34">CT6+1</f>
-        <v>43476</v>
+        <v>43455</v>
       </c>
       <c r="CV6" s="83">
         <f t="shared" ref="CV6" si="35">CU6+1</f>
-        <v>43477</v>
+        <v>43456</v>
       </c>
       <c r="CW6" s="93">
         <f t="shared" ref="CW6" si="36">CV6+1</f>
-        <v>43478</v>
+        <v>43457</v>
       </c>
       <c r="CX6" s="92">
         <f t="shared" ref="CX6" si="37">CW6+1</f>
-        <v>43479</v>
+        <v>43458</v>
       </c>
       <c r="CY6" s="83">
         <f t="shared" ref="CY6" si="38">CX6+1</f>
-        <v>43480</v>
+        <v>43459</v>
       </c>
       <c r="CZ6" s="83">
         <f t="shared" ref="CZ6" si="39">CY6+1</f>
-        <v>43481</v>
+        <v>43460</v>
       </c>
       <c r="DA6" s="83">
         <f t="shared" ref="DA6" si="40">CZ6+1</f>
-        <v>43482</v>
+        <v>43461</v>
       </c>
       <c r="DB6" s="83">
         <f t="shared" ref="DB6" si="41">DA6+1</f>
-        <v>43483</v>
+        <v>43462</v>
       </c>
       <c r="DC6" s="83">
         <f t="shared" ref="DC6" si="42">DB6+1</f>
-        <v>43484</v>
+        <v>43463</v>
       </c>
       <c r="DD6" s="93">
         <f t="shared" ref="DD6" si="43">DC6+1</f>
-        <v>43485</v>
+        <v>43464</v>
       </c>
       <c r="DE6" s="92">
         <f t="shared" ref="DE6" si="44">DD6+1</f>
-        <v>43486</v>
+        <v>43465</v>
       </c>
       <c r="DF6" s="83">
         <f t="shared" ref="DF6" si="45">DE6+1</f>
-        <v>43487</v>
+        <v>43466</v>
       </c>
       <c r="DG6" s="83">
         <f t="shared" ref="DG6" si="46">DF6+1</f>
-        <v>43488</v>
+        <v>43467</v>
       </c>
       <c r="DH6" s="83">
         <f t="shared" ref="DH6" si="47">DG6+1</f>
-        <v>43489</v>
+        <v>43468</v>
       </c>
       <c r="DI6" s="83">
         <f t="shared" ref="DI6" si="48">DH6+1</f>
-        <v>43490</v>
+        <v>43469</v>
       </c>
       <c r="DJ6" s="83">
         <f t="shared" ref="DJ6" si="49">DI6+1</f>
-        <v>43491</v>
+        <v>43470</v>
       </c>
       <c r="DK6" s="93">
         <f t="shared" ref="DK6" si="50">DJ6+1</f>
-        <v>43492</v>
+        <v>43471</v>
       </c>
       <c r="DL6" s="92">
         <f t="shared" ref="DL6" si="51">DK6+1</f>
-        <v>43493</v>
+        <v>43472</v>
       </c>
       <c r="DM6" s="83">
         <f t="shared" ref="DM6" si="52">DL6+1</f>
-        <v>43494</v>
+        <v>43473</v>
       </c>
       <c r="DN6" s="83">
         <f t="shared" ref="DN6" si="53">DM6+1</f>
-        <v>43495</v>
+        <v>43474</v>
       </c>
       <c r="DO6" s="83">
         <f t="shared" ref="DO6" si="54">DN6+1</f>
-        <v>43496</v>
+        <v>43475</v>
       </c>
       <c r="DP6" s="83">
         <f t="shared" ref="DP6" si="55">DO6+1</f>
-        <v>43497</v>
+        <v>43476</v>
       </c>
       <c r="DQ6" s="83">
         <f t="shared" ref="DQ6" si="56">DP6+1</f>
-        <v>43498</v>
+        <v>43477</v>
       </c>
       <c r="DR6" s="93">
         <f t="shared" ref="DR6" si="57">DQ6+1</f>
-        <v>43499</v>
+        <v>43478</v>
       </c>
     </row>
     <row r="7" spans="1:122" s="124" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -6738,21 +6712,20 @@
       </c>
       <c r="D20" s="127"/>
       <c r="E20" s="100">
-        <v>43374</v>
+        <v>43367</v>
       </c>
       <c r="F20" s="101">
         <f t="shared" si="65"/>
-        <v>43392</v>
+        <v>43385</v>
       </c>
       <c r="G20" s="62">
         <v>19</v>
       </c>
       <c r="H20" s="63">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I20" s="64">
-        <f t="shared" si="62"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J20" s="95"/>
       <c r="K20" s="107"/>
@@ -6822,21 +6795,21 @@
       </c>
       <c r="D21" s="127"/>
       <c r="E21" s="100">
-        <v>43364</v>
+        <v>43381</v>
       </c>
       <c r="F21" s="101">
         <f>IF(ISBLANK(E21)," - ",IF(G21=0,E21,E21+G21-1))</f>
-        <v>43367</v>
+        <v>43384</v>
       </c>
       <c r="G21" s="62">
         <v>4</v>
       </c>
       <c r="H21" s="63">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="I21" s="64">
         <f t="shared" ref="I21" si="68">IF(OR(F21=0,E21=0)," - ",NETWORKDAYS(E21,F21))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J21" s="95"/>
       <c r="K21" s="107"/>
@@ -9783,22 +9756,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="35">
-    <mergeCell ref="DL4:DR4"/>
-    <mergeCell ref="DL5:DR5"/>
-    <mergeCell ref="CQ4:CW4"/>
-    <mergeCell ref="CQ5:CW5"/>
-    <mergeCell ref="CX4:DD4"/>
-    <mergeCell ref="CX5:DD5"/>
-    <mergeCell ref="DE4:DK4"/>
-    <mergeCell ref="DE5:DK5"/>
-    <mergeCell ref="CJ4:CP4"/>
-    <mergeCell ref="CJ5:CP5"/>
-    <mergeCell ref="BO5:BU5"/>
-    <mergeCell ref="BO4:BU4"/>
-    <mergeCell ref="BV4:CB4"/>
-    <mergeCell ref="BV5:CB5"/>
-    <mergeCell ref="CC4:CI4"/>
-    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -9809,15 +9775,22 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="CJ4:CP4"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BO4:BU4"/>
+    <mergeCell ref="BV4:CB4"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="DL4:DR4"/>
+    <mergeCell ref="DL5:DR5"/>
+    <mergeCell ref="CQ4:CW4"/>
+    <mergeCell ref="CQ5:CW5"/>
+    <mergeCell ref="CX4:DD4"/>
+    <mergeCell ref="CX5:DD5"/>
+    <mergeCell ref="DE4:DK4"/>
+    <mergeCell ref="DE5:DK5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8:H9 H42:H55 H11:H12 H14 H16:H20 H22 H25:H31">
@@ -9835,60 +9808,60 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN7">
-    <cfRule type="expression" dxfId="43" priority="95">
+    <cfRule type="expression" dxfId="40" priority="95">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:BN9 K11:BN12 BO27:CL27 K14:BN14 K16:BN20 K22:BN22 K25:BN55">
-    <cfRule type="expression" dxfId="42" priority="98">
+    <cfRule type="expression" dxfId="39" priority="98">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="99">
+    <cfRule type="expression" dxfId="38" priority="99">
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN9 K42:BN55 BO27:CL27 K11:BN12 K14:BN14 K16:BN20 K22:BN22 K25:BN31">
-    <cfRule type="expression" dxfId="40" priority="58">
+    <cfRule type="expression" dxfId="37" priority="58">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO6:BU7">
-    <cfRule type="expression" dxfId="39" priority="50">
+    <cfRule type="expression" dxfId="36" priority="50">
       <formula>BO$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO6:BU7">
-    <cfRule type="expression" dxfId="38" priority="49">
+    <cfRule type="expression" dxfId="35" priority="49">
       <formula>BO$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV6:CB7">
-    <cfRule type="expression" dxfId="37" priority="48">
+    <cfRule type="expression" dxfId="34" priority="48">
       <formula>BV$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV6:CB7">
-    <cfRule type="expression" dxfId="36" priority="47">
+    <cfRule type="expression" dxfId="33" priority="47">
       <formula>BV$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC6:CI7">
-    <cfRule type="expression" dxfId="35" priority="46">
+    <cfRule type="expression" dxfId="32" priority="46">
       <formula>CC$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC6:CI7">
-    <cfRule type="expression" dxfId="34" priority="45">
+    <cfRule type="expression" dxfId="31" priority="45">
       <formula>CC$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ6:CP7">
-    <cfRule type="expression" dxfId="33" priority="44">
+    <cfRule type="expression" dxfId="30" priority="44">
       <formula>CJ$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ6:CP7">
-    <cfRule type="expression" dxfId="32" priority="43">
+    <cfRule type="expression" dxfId="29" priority="43">
       <formula>CJ$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9907,7 +9880,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:BN35">
-    <cfRule type="expression" dxfId="31" priority="38">
+    <cfRule type="expression" dxfId="28" priority="38">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9940,52 +9913,52 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K40:BN41">
-    <cfRule type="expression" dxfId="30" priority="36">
+    <cfRule type="expression" dxfId="27" priority="36">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36:BN39">
-    <cfRule type="expression" dxfId="29" priority="34">
+    <cfRule type="expression" dxfId="26" priority="34">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CQ6:CW7">
-    <cfRule type="expression" dxfId="28" priority="32">
+    <cfRule type="expression" dxfId="25" priority="32">
       <formula>CQ$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CQ6:CW7">
-    <cfRule type="expression" dxfId="27" priority="31">
+    <cfRule type="expression" dxfId="24" priority="31">
       <formula>CQ$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CX6:DD7">
-    <cfRule type="expression" dxfId="26" priority="30">
+    <cfRule type="expression" dxfId="23" priority="30">
       <formula>CX$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CX6:DD7">
-    <cfRule type="expression" dxfId="25" priority="29">
+    <cfRule type="expression" dxfId="22" priority="29">
       <formula>CX$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DE6:DK7">
-    <cfRule type="expression" dxfId="24" priority="28">
+    <cfRule type="expression" dxfId="21" priority="28">
       <formula>DE$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DE6:DK7">
-    <cfRule type="expression" dxfId="23" priority="27">
+    <cfRule type="expression" dxfId="20" priority="27">
       <formula>DE$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DL6:DR7">
-    <cfRule type="expression" dxfId="22" priority="26">
+    <cfRule type="expression" dxfId="19" priority="26">
       <formula>DL$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DL6:DR7">
-    <cfRule type="expression" dxfId="21" priority="25">
+    <cfRule type="expression" dxfId="18" priority="25">
       <formula>DL$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10018,28 +9991,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10:BN10">
-    <cfRule type="expression" dxfId="20" priority="23">
+    <cfRule type="expression" dxfId="17" priority="23">
       <formula>AND($E10&lt;=K$6,ROUNDDOWN(($F10-$E10+1)*$H10,0)+$E10-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="24">
+    <cfRule type="expression" dxfId="16" priority="24">
       <formula>AND(NOT(ISBLANK($E10)),$E10&lt;=K$6,$F10&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10:BN10">
-    <cfRule type="expression" dxfId="18" priority="22">
+    <cfRule type="expression" dxfId="15" priority="22">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:BN13">
-    <cfRule type="expression" dxfId="17" priority="19">
+    <cfRule type="expression" dxfId="14" priority="19">
       <formula>AND($E13&lt;=K$6,ROUNDDOWN(($F13-$E13+1)*$H13,0)+$E13-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="20">
+    <cfRule type="expression" dxfId="13" priority="20">
       <formula>AND(NOT(ISBLANK($E13)),$E13&lt;=K$6,$F13&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:BN13">
-    <cfRule type="expression" dxfId="15" priority="18">
+    <cfRule type="expression" dxfId="12" priority="18">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10058,15 +10031,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:BN15">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="11" priority="15">
       <formula>AND($E15&lt;=K$6,ROUNDDOWN(($F15-$E15+1)*$H15,0)+$E15-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="16">
+    <cfRule type="expression" dxfId="10" priority="16">
       <formula>AND(NOT(ISBLANK($E15)),$E15&lt;=K$6,$F15&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:BN15">
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="9" priority="14">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10085,15 +10058,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21:BN21">
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="8" priority="11">
       <formula>AND($E21&lt;=K$6,ROUNDDOWN(($F21-$E21+1)*$H21,0)+$E21-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="7" priority="12">
       <formula>AND(NOT(ISBLANK($E21)),$E21&lt;=K$6,$F21&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21:BN21">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="6" priority="10">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>